<commit_message>
update users and data
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -28,49 +28,49 @@
     <t>texts</t>
   </si>
   <si>
-    <t>elicoh1</t>
-  </si>
-  <si>
-    <t>assafrl</t>
-  </si>
-  <si>
-    <t>OfirAkunis</t>
+    <t>michael_dvorin</t>
+  </si>
+  <si>
+    <t>YairGolan1</t>
+  </si>
+  <si>
+    <t>yoavr</t>
+  </si>
+  <si>
+    <t>gidonsaar</t>
+  </si>
+  <si>
+    <t>tamarzandberg</t>
+  </si>
+  <si>
+    <t>Nefolet</t>
+  </si>
+  <si>
+    <t>ruth_elbaz</t>
+  </si>
+  <si>
+    <t>Michal_Rozin</t>
+  </si>
+  <si>
+    <t>haggai_segal</t>
+  </si>
+  <si>
+    <t>meretzparty</t>
+  </si>
+  <si>
+    <t>galidalal</t>
   </si>
   <si>
     <t>barak_ehud</t>
   </si>
   <si>
-    <t>FateenMulla</t>
-  </si>
-  <si>
-    <t>shireuven</t>
-  </si>
-  <si>
-    <t>nadavabeksis</t>
-  </si>
-  <si>
-    <t>mikiros1</t>
-  </si>
-  <si>
-    <t>AviNissenkorn</t>
-  </si>
-  <si>
-    <t>BarakRavid</t>
-  </si>
-  <si>
-    <t>MakorRishon</t>
-  </si>
-  <si>
-    <t>IlanLukatch</t>
-  </si>
-  <si>
-    <t>AvishayBenHaim</t>
-  </si>
-  <si>
-    <t>GadiAleks</t>
-  </si>
-  <si>
-    <t>GabbayAvi</t>
+    <t>erancherpak</t>
+  </si>
+  <si>
+    <t>YairNetanyahu</t>
+  </si>
+  <si>
+    <t>Likud_Party</t>
   </si>
   <si>
     <t>R</t>
@@ -79,49 +79,49 @@
     <t>L</t>
   </si>
   <si>
-    <t xml:space="preserve">הרוצה בשלום יכון למלחמה העליונות הצבאית של ישראל תישמר בזכות הברית ביננו לארהב אך מעל הכל בזכות יכולות ביטחוניות…  ההתאבדות של חברי כחול לבן על קיום ההפגנות היא פשוט בלתי נתפסת המגיפה מתפשטת בכל העולם אנשים מאבדים במקרה הטוב את…  ידעתם שהעובד הישראלי עובד בממוצע 42 שעות בשבוע ובמדינות הOECD כ40 שעות בלבד אני מתכוון כעת להמשיך בקידום המהלך…  יוזמת סוף שבוע ארוך חוזרת במיוחד בתקופה של משבר הקורונה כשהפעילות במשק יורדת והאבטלה עולה זוהי בשורה חשובה לכלכל…  33 אני רוצה לברך גם את שייח מוחמד בן זאיד מנהיג איחוד האמירויות ואת מלך בחריין חמד בן עיסא על תרומתם להסכם פורץ ה…  23 לאחר 26 שנה אנו חותמים היום על הסכם שלום נוסף עם שתי מדינות ערביות הסכם שיחזק את ישראל מבחינה ביטחונית וכלכלי…  13 שֶׁהֶחֱיָנוּ וְקִיְּמָנוּ וְהִגִּיעָנוּ לַזְמַן הַזֶּה  יש רגעים שנחרטים לעד על לוח ההיסטוריה של מדינת…  simonarann ⁦⁩⁦⁩ وزير الاستخبارات ⁩ إيلي كوهن لقناة سكاي نيوز عربية من الإمارات⁦ ⁩ تحدياتنا الأمنية مشتركة ومعاهدة السلام الإس… באמת היתה שבת שלום כפי שאמרתי הסכמים נוספים על הפרק מברך את ראש הממשלה נתניהו ואת והנשיא טראמפ על הסכם שלום הי…  המשטר האיסלאמי בטהראן שוב הוכיח שהאויב הגדול בעיניהם הוא העם הפרסי אני עם העם הפרסי אני עם נביד אפקרי יגיע יום ש…  جمهوری اسلامی ثابت کرده که بزرگ‌ترین دشمن مردم ایران است من در کنار ایرانیان هستم، من در کنار زنده‌یاد،…  simonarann   שר המודיעין אלי כהן elicoh1 נועד עם משלחת של צאד בראשות בנו של הנשיא וראש הקבינט הגנרל עבד אלכרים דבי אשר הביע א… מחזקים את היחסים עם צאד פגישה חשובה עם יור הקבינט של צאד גנרל עבד אל כרים דבי ועם מנהל הסוכנות לביטחון לאומ…  נורות האזהרה הבהבו מעל חקירות נתניהו לכל אורך הדרך כל מי שעיניו בראשו יכל לראות את שלל החורים וסימני השאלה בתיקים…  השבכ בעוד פעולה מוצלחת חשף היום ניסיון של חמאס לגייס אזרח ישראלי לבצע פיגוע בשטח מדינת ישראל  אני מודה לאנשי השב…  radios100 השבוע בתוכנית הנבחרים עם דוד בן בסט ראיון עם שר המודיעין elicoh1 LikudParty שישי 1000 בבוקר ברדיוס 100FM  באפל… ברוכה הבאה לליכוד שולי קידמנו ביחד פרויקטים בעבר ואני יכול לומר שהליכוד הרוויח חברה מוכשרת חדורת תחושת שליחות ומ…  שלום כיתה ב בהצלחה לבתי עמנואל שמתחילה היום את כיתה ב ובהצלחה לכל ילדות וילדי ישראל  שהחיינו מברך על המראת הטיסה הראשונה וההיסטורית מישראל לאבו דאבי חשיבות ההסכם בין ישראל לאמירויות מעבר ליצירת חזי…  gershuni AmalyaDuek 3 במקביל פעלתי לפתוח את השוק להקל בייבוא ולעודד ייצור מקומי משום שהיה קושי זמני בהשגת המ…  gershuni AmalyaDuek 2 בזמנו כשהמסכות עלו מעל ל10 שח ליחידה פעלתי באמצעות משא ומתן וגם באמצעות איום הפיקוח…  gershuni AmalyaDuek 1 כאחד שהגיע לפוליטיקה מהדרגות הבכירות ביותר במגזר העסקי אני לא חושב שאני צריך שיעורים בכלכ…  שולח את תנחומיי למשפחתו של הנרצח בפיגוע הדקירה בפת על ידי בן עוולה עלינו להחריב עד היסוד את הבית ממנו יצאה חיית…  I welcome our true friend Secretary of State mikepompeo on his arrival to Israel The relationship between Israel…  בחירות בעת הנוכחית הן לא דבר רצוי עבור מדינת ישראל ראש הממשלה נתניהו הוכיח שרק טובת המדינה לנגד עיניו נמשיך לעבוד…  השמאל מוכן להכפיש מפקד חיל אוויר עתיר זכויות כדי לנסות לפגוע ברוה״מ נתניהו הגם שמפקד ח״א כמו הרמטכ״ל משרד הביטח…  arutz20 שר המודיעין אלי כהן הסכם השלום שלנו עם איחוד האמירויות בחסות ארהב לא כולל שום סעיף שמדבר על מכירת נשק לא סעיף גלוי ולא סמוי… אונס הנערה שהתרחש השבוע באילת הוא מזעזע ומחריד איך ניתן לאבד כך צלם אנוש אין לחלאות האלה אמא בת אחות אני קורא…  ההסכם עם איחוד האמירויות הוא הסנונית הראשונה ואין לי ספק שלאחריו תגענה מדינות נוספות מהמפרץ ומאפריקה הסכם שלום בין…  תקופת הצונאמי המדיני הזאת תירשם בדפי ההיסטוריה של מדינת ישראל כפי שאמרנו ההסכם מול איחוד האמירויות הוא רק הסנונית…  ההסכם עם האמירויות אינו כולל הסכמה  ישראלית למכירת ציוד צבאי שיפר את העליונות הצבאית האזורית של ישראל מציע לחברי כ…  simonarann ⁦⁦⁩⁩⁦⁦⁩  وزير الاستخبارات الإسرائيلي elicoh1 إيلى كوهين يتوقع بأن يتم قريباً التوصل إلى اتفاقسلام بين إسرائيل و ال… simonarann ⁦⁩⁦⁩  שר המודיעין אלי כהן elicoh1  מעריך שסודן תחתום בקרוב על הסכם שלום עם ישראל  מקורות מדיניים המגעים בין המדינות… יום היסטורי ליחסי ישראל ומדינות ערב עם חתימה על הסכם שעוד רבים יגיעו בעקבותיו מברך את ראש הממשלה והנשיא טראמפ שהפ…  עמית בן יגאל זל נרצח על ידי מחבל מתועב במהלך פעילות צהל היום דחו שופטי העליון את הריסת בית המחבל בטיעון מקומם ו…  כל הכבוד לשבכ על לכידת המחבל שתכנן את הפיגוע בו נפלו חיילי צהל אלירז פרץ ואילן סביאטקובסטקי לפני כעשור מדינת ישר…  ברוך דיין האמת כואבים את פטירתו של הרב עדין שטיינזלץ שהקדיש את חייו להנגשת ארון הספרים היהודי לעם ישראל ולקירוב…  Oui M le Président pas seul car l’Iran est avec lui Depuis 30 ans le Hezbollah envoyé de l’Iran détruit le pay…  נכון אדוני הנשיא לבנון לא לבד כי איראן לא עוזבת אותה כבר 30 שנה שחיזבאללה השלוחה הקדמית של איראן הורסת כל חלקה…  שבוע טוב ביום שישי קיבלתי הודעה ממשרד הבריאות על כך שאחד מהנוכחים בפגישה שקיימתי בשבוע שעבר התגלה כחולה קורונה וע…  Menachemcohen1 קיבלת שבת שלום שבת שלום לחיילי וחיילות צהל היקרים לכוחות הביטחון ולכל עם ישראל  התמונה מלפני הקורונה  מיקי יקירי כשאיש קטן מטיל צל ענק זה אומר שהשמש שוקעת מקווה שתפעל למלא את שליחותך ולאחד את הסיעה zoharm7…  כל ניסיון של חיזבאללה לפגוע במדינת ישראל ייענה בתגובה נחושה ועוצמתית מחזק את חיילי צהל על התגובה המהירה ובמיוחד…  שיעור על כוח רצון אמונה בעצמנו והגשמת חלומות ביום חמישי שעבר ליוויתי לבקום 9 צעירים עם צרכים מיוחדים שלא נתנו…  arutz20 שר המודיעין אלי כהן במהלך ההפגנות האחרונות אין שום קשר לסוגיות כלכליות יש פשוט אנשים שלא מקבלים דבר אחד את בחירת העם את ה… arutz20 שר המודיעין אלי כהן יגיע בשעה 1800 לתכנית הכלכלית  יש לכם שאלה עבורו ספרו לנו  ErezZadok1 elicoh1  מחאת הדגלים השחורים אתמול הייתה מפגן צביעות של קבוצה אלימה ואנרכיסטית שלא הפנימה את ההפסד בבחירות אבל מה הפלא כשח…  simonarann שר המודיעין אלי כהן elicoh1  בראיון עמנו  בקרוב תעלה האפליקציה המגן 2 לזיהוי ואיתור נדבקים בתקווה להשטחת עקומת הנדבקי… radio103fm השר אלי כהן elicoh1 ליכוד סגר הוא צעד דרסטי מדי כרגע הקורונה תישאר איתנו גם אחרי הסגר שמציע השר steinitzyuval הנדב… למי שעוד היה ספק עכשיו אין ספק הכלים של השבכ מצילים חיים מונעים סגר ומסייעים להשטיח מחדש את העקומה מי שמתנגד ל…  GolanMay הגיע הזמן לעשות צדק עם תושבי העיר אשקלון שחיים במציאות בטחונית מורכבת המקשה עליהם ועל חיי השגרה הצ״ח שהגשתי בשיתוף עם השר אל… כולם שווים בפני החוק נבחרי ציבור פקידים וכן גם שופטים מניעת ניגודי עניינים תחזק את מערכת המשפט ואת אמון הציבור…  ArielKallner בהצלחה אריאל  OsnathilaMark בהצלחה  עוד הישג גדול למערכת הביטחון הישראלית השיגור המוצלח של לווין אופק 16 הוא הוכחה נוספת לעליונות הטכנולוגית והמודיעינ…  simonarann שר המודיעין elicoh1 אלי כהן ירכז את ועדת השרים לבחינת הצורך בהמשך ההסתייעות בשרות הביטחון הכללי לצמצום התפשטות נגיף קורונ… Just another example of the Arab world being interested in normalizing its relations with the Jewish State just li…  מיכאל בן זיקרי  גיבור הלב מתרחב שיש אנשים כאלו שעושים את הכל על מנת להציל מטביעה אם וילדים והלב נקרע כשגיבור כז…  להזכירכם הקונצנזוס בישראל נקבע באמצעות בחירות דמוקרטיות אתם מוזמנים להתמודד אגב בישראל כל קול שווה בין אם אתה…  כל הכבוד לשבכ שחשף היום ניסיון של חיזבאללה לגייס אזרחים ישראלים מהגליל לפעילות כנגד מדינת ישראל  אנשי השבכ עובד…  UriKarzen שמחנו לארח היום את  ידיד חברון שר המודיעין אלי כהן elicoh1  ראש ממשלה חכם אמר פעם עתידנו תלוי לא במה שיאמרו הגויים אלא במה שיעשו היהודים אני מציע להפסיק עם הנסיונות לזרוע…  GLZRadio שר המודיעין elicoh1 מגיב את הריבונות על שטחי אבותינו נחיל על אפו וחמתו של החמאס שיודע שמי ששילם את המחיר על הרפתקאותיו הם… ברוך דיין האמת הצטערתי לשמוע על מותו של יהודה אביו של נחשון וקסמן שנלקח כבן ערובה ונרצח בידי החמאס לפני 26 שנים…  בשביל טיבי פלסטיני שניסה לרצוח יהודים זוהי רק תקלה אז טיבי בתקלות צריך לטפל בזריזות ובנחישות מחזק את חיילי…  מועצת הביטחון של האום תדון בהצעת ארהב להאריך את אמברגו הנשק על איראן ללא הגבלת זמן  איראן היא סכנה לא רק לישראל…  amirbohbot פרסום ראשון ההצעה להעלאת נושא לסדר היום של ישיבת הממשלה על העברת יחידות אמן לנגב מאת שר המודיעין חכ אלי כהן   idfonlin… elicoh1 להגיד שהטלת היצף לא תשפיע על מחירי הדיור זה כמו להגיד שמחירי החלב לא ישפיעו על מחירי הגבינה  לנופף בסיסמה ריקה מתוכן של כלכל… IsraelHayomHeb ניתוח שנערך במשרד לענייני מודיעין קובע כי העת הנוכחית היא המתאימה ביותר ליישם את מהלך הריבונות ביהודה שומרון ובקעת היר… שוק חופשי עם רגישות חברתית פתיחת השווקים והגברת התחרות היא טובה למשק טובה לאזרחים והיא מה שהצעיד קדימה את הכלכ…  להגיד שהטלת היצף לא תשפיע על מחירי הדיור זה כמו להגיד שמחירי החלב לא ישפיעו על מחירי הגבינה  לנופף בסיסמה ריקה מת…  Joined PrimeministerGR during his visit at YadVashem Mitsotakis’ family saved a Jewish girl during the Holocaust…  ביד ושם יחד עם ראש ממשלת יוון קיריאקוס מיצוטקיס במסגרת ביקורו הרשמי בישראל קרובת משפחתו של מיצוטקיס הצילה בשואה…  אם גנץ ואשכנזי יתקעו מקלות בגלגלי הריבונות הם יהיו חתומים על פספוס בקנה מידה היסטורי שעשויות להיות לו השלכות גם ע…  מקום הצדק שמה הרשע בית הדין האנטישמי בהאג מתעלם מפשעי המשטר בוונצואלה מרצח העם בסוריה ומזוועות נוספות שמתרחשות ב…  JamesCleverly Congratulated elicoh1 today on his appointment as Israel  Minister of Intelligence  We discussed Israeli security… Had a great Zoom meeting w Minister JamesCleverly We discussed Iranian malign actions in the region and the „Tru…  שוחחתי הבוקר עם השר הבריטי לענייני המזרח התיכון ידיד ישראל JamesCleverly שוחחנו על החלת הריבונות האיום האיראני…  ההסדרה שחייבים לקדם היא פסקת התגברות הפקעת קרקע תוך שמירה על זכות הקניין מותרת עבור יהודים באריאל ברעננה ובכל מק…  אֶרְדּוֹף אוֹיְבַי וְאַשִּׂיגֵם וְלֹא אָשׁוּב עַד כַּלּוֹתָם יידע כל טרוריסט כי זרועה של מדינת ישראל מגיעה לכל…  ארגוני השמאל שהפגינו היום נגד הסיפוח עם דגלי אשף ושלטים נגד צהל חשפו את כוונותם האמיתית לא נרתע מתומכי מחבלים…  DanWilliams Israel’s Intelligence Ministry says flights should resume to these countries Seychelles Cyprus Greece South Korea Slo… למי שרוצה תמונה מהימנה ופחות לזרוע פאניקה מיותרת שיסתכל בעיקר על שיעור הבדיקות החיוביות שהוא נתון חשוב יותר מכמות…  ynetalerts המלצת משרד המודיעין אלה המדינות שאליהן ניתן יהיה לטוס בקרוב   התחקיר המצוין של כאן 11 מאתמול מוכיח עד כמה חשובה השקיפות במערכת המשפט ועד כמה היא הוזנחה עד היום כפי שכבר אמרתי…  YakiAdamker יקי היקר שלא תדעו עוד צער בטיעון מקומם ובניגוד לעמדת מערכת הביטחון שהריסת בתים מרתיעה מחבלים דחו שופטי בגץ הריסת בית מחבל משום שמשפחתו חפה…  דברי הרהב של חימינאי נועדו להסית את תשומת הלב של העם האיראני מהבוץ בו הם שקועים הוא יודע היטב כי ניסיון לממש את ה…  היום בטקס חילופי שרים במשרד הכלכלה והתעשייה במהלך שלוש וחצי השנים האחרונות פעלנו ללא ליאות למען הכלכלה הישראלית ו…  akibigman שבוע טוב יקירי מערך המודיעין הישראלי הוא בעל שם בינלאומי ובעל חשיבות עצומה לביטחון המדינה  אפעל באחריות ובמסירות לחיזוק ולשדרוג מ…  שבוע טוב אני רוצה להודות לראש הממשלה netanyahu על האמון שנתן בי לכהן כשר המודיעין בממשלה הבאה הייתה לי הזכות לש…  netanyahu אני שמח לבשר כי החלטתי למנות את השר elicoh1 לתפקיד שר המודיעין בתפקידו כשר הכלכלה השר כהן פעל רבות להצלחה ולשגשוג הכלכלה… chaimlevinson לוינסון להבא רק תתייג elicoh1 שבוע טוב ItaiHoffman uriyaelk JoshBreiner איתי שלום תחום זה שייך למשרד העבודה תודה רני  פתיחת הכלכלה היא צו השעה בשבילי כל עסק זה עולם ומלואו ואני אמשיך להילחם למענם RahavRan  ikicohen RahavRan IsraelHayomHeb misradcalcala IsraelMOH תודה אח יקר בוקר קשה וכואב שולח את תנחומיי למשפחתו ולהוריו של עמית בן יגאל לוחם סיירת גולני שנפל בעת מילוי תפקידו מחבק את הה…  GLZRadio הפרופ איתמר גרוטו המשנה למנכל משרד הבריאות על פתיחת המסעדות מיום רביעי הבא ככל שנראה שהמצב יותר טוב אפשר לדון על התאריכ… giladerdan1 בהצלחה גלעד מדינת ישראל זכתה  shlomokarhi השר elicoh1 ואני מברכים את בנק ישראל על מתווה הסיוע למשקי הבית ולעסקים על רקע הקורונה בהמשך להצח שלנו ולשיחות עם הנגיד… p08bK41UHtjDpcN פועלים מולם שיקדימו כמה שיותר חשוב לעולם לא נתפשר על ביטחוננו  ביטחונה של מדינת ישראל זוהי חובתנו לנופלים זוהי חובתנו לאזרחי ישראל זוהי חובתנו לדו…  zviashkenazi ShaikeKatz NaftaliSariel1 amsterdamski2 naftalibennett אכן צבי ידידות  שלא תלויה בדבר  נב נפגשת…  עכשיו אפשר להגיד שמתחילים לחזור לשגרה אחרי יותר מחודש עם אחת המנות הטובות בחולון פלאפל בטעם של עוד🥙 שלחו תמונה…  כואב הלב הרב הבר הציל במו ידיו חיים של מאות אנשים שולח את תנחומיי למשפחה ולחברים ברוך דיין האמת יום העצמאות מתקרב וזה הזמן לפרגן לתוצרת ישראלית להפגין ערבות הדדית שכל כך מאפיינת את העם שלנו ולתמוך בישראלים הרבי…  ברוך רופא חולים שמחתי לשמוע שמצבו של אלי ביר נשיא ומייסד איחוד הצלה משתפר ושהוא שב הביתה לישראל מאחל לו שימשיך…  benirabin הבנקים שחשוב שיגלו רגישות בשעה זו ללקוחות שלהם שלמה היקר מה שלא הולך בטוב יתקדם בחקיקה  shlomokarhi gtgt  3 הבנקים יחוייבו לאפשר ללקוחות לדחות תשלומי הלוואות עד חצי שנה ולהעבירן לסוף התקופה הפעולה לא תהיה כרוכה בעמלה ותנא… 10elilevi מיד אצלנו ב news1075  שר הכלכלה elicoh1 אלוף משנה רלי מרגלית מנכ״ל רמב״ם ד״ר מיקי הלברטל bokeralmog דיווח מאיטליה ראש הע… אתמול אישרנו תכנית ראשונית לסיוע כלכלי לנפגעים מהקורונה כולל מענק של 500 שח להורים על כל ילד וגם לקשישים ונכים ר…  amirbohbot לכן סגרנו עם הרשתות הגדולות מחירי מכירה של מסכות ואלכוג׳ל BorisJohnson is a great friend of Israel I wish him a full and quick recovery  Photo by Flash 90  amirbohbot אמיר מציע שתעקוב אחר הפרסומים של משרד הכלכלה וגם בפייס אצלי כבר הכשרנו 2 מפעלים בשדרות ובאלון תבור שמיי…  SamerBarhamS hadover1 תקנה רק ברשתות הגדולות שהתחייבו על מחיר 3 ב10 שח מקסימום GLZRadio השר elicoh1 לירון וילנסקי וbardugojacob מצפה מנגיד בנק ישראל להורות לבנקים להקפיא את תשלומי הקרן לשלושה חודשים ולא להעלו… NitayAnavi שר הכלכלה elicoh1 מאיים על הבנקים  היכנסו מתחת לאלונקה או שנפעל נגדכם בחקיקה שבוע טוב לצערי שמענו השבוע הרבה הכפשות והכללות שלא בצדק נגד המגזר החרדי הכפשות אלה מבוססות על דעות קדומות ומבזו…  Idaneretz עידן אין קשר בפוסט שרשמת למשרד הכלכלה אולי לחקלאות לכן לכן לא חתמתי על צו מוצרי חקלאות לא בכלכלהמציע מנסיונך שתתקן שולח איחולי החלמה מהירה לידידי שר הבריאות יעקב ליצמן ורעייתו יחד עם כל חולי ישראל בהזדמנות זו אני רוצה להזכיר לכו…  newsisrael13 מגפת הקורונה  שר הכלכלה והתעשייה elicoh1 פנה לנגיד בנק ישראל אמיר ירון במטרה להנחות את הבנקים לדחות את תשלומי קרן הה… מאיר בן שבת ראש המלל הקדיש ומקדיש את חייו ימיו ולילותיו למען מדינת ישראל זכיתי להכיר אותו במסגרת פעילותי בקבינט…  יור הכנסת יולי אדלשטיין פעל בצורה ממלכתית ומכבדת אל מול ההתערבות הבוטה של בגץ שמהווה פגיעה קשה בעקרון הפרדת הרשו…  אתם שם בקוקפיט טיפת כבוד לא נשארה לכם אתם מפקידים וועדה שעוסקת גם בנפגעי טרור בידי תומכי טרור אתם שהובלתם חייל…  liatron שר הכלכלה elicoh1 להיזהר משרלטנים  שמציעים ליווי עסקי למילוי הטפסים באלפי שקלים מרכזי המעוף נותנים ייעוץ כזה ב 100 שקלים ב… אנחנו כאן בשבילכם עסקים קטנים ובינוניים יש לכם שאלה חייגו 6680 ומוקד החירום של משרד הכלכלה ייענה לכם על כל שאלה…  sivanhakolkalul מקבלת אינספור תלונות על רשתות שיווק וחנויות שמנצלות את המצב ומפקיעות מחירים מאיפה בכל הארץ אבל בעיקר בפריפריה גייסנו… omeraricha לא רק בנט גם שר הכלכלה elicoh1 יפתח בסבב מענה משודר  שפל חדש בתולדות המפלגות הציוניות תראו מי תומך היום בגנץ אחמד טיבי יועץ רב המרצחים ערפאת שלפיו ארץ ישראל היא ביט…  שוחחתי עם ראשי הרשתות הגדולות וסיכמתי איתם שמחירי האלכוגל לא יעלו על 990 שח ל100 מל העלאת מחירים של מוצרים הכ…  בושה וחרפה שבשעה שמדינת ישראל מתמודדת עם אתגר הקורונה שמשפיע על חיי כולנו הפוליטיקאים של כחול לבן ממשיכים במשחקי…  newsisrael13 הקורונה  משבר עולמי  שר הכלכלה elicoh1 זה משבר חמור מאוד במהלך 48 השעות הקרובות נציג את התוכנית להתמודדות עם משבר… לא משנה מה יש לכם על הראש פורים שמח לכל עם ישראל dudiamsalem avidichter  radio103fm האם הליכוד פנה לרעמ בבחירות אפריל 2019 שר הכלכלה אלי כהן elicoh1 ליכוד לא מני ולא מקצתי לא באישור ולא בידיעת רהמ… הדבר היחיד שמעניין את כחול לבן זה להחליף את ראש הממשלה וכל האמצעים כשרים לשם כך כולל שיתוף פעולה עם תומכי טרור וחק…  מי שהיה אתמול בלילה בגני התערוכה בחגיגות הניצחון של הליכוד ראה את עם ישראל לגווניו בשיא תפארתו חילונים דתיים וח…  תודה ענקית לכל הליכודניקים שייצאו להצביע ולפעילים והמתנדבים שנתנו את הנשמה  ב״ה נקים ממשלה לאומית טובה לעם ישראל אני כבר הצבעתי עכשיו תורכם אלו בחירות שיוכרעו על חודו של מנדט וכל קול קובע צאו להצביע מחל והביאו איתכם לקלפי את…  לגבי ההבדלה אני לא יודע אבל מצב האבטלה הוא הטוב ביותר שהיה מקום המדינה מי שרוצה בהמשך הצמיחה הכלכלית של ישראל אס…  עסקים קטנים זה העסק שלנו העסקים הקטנים והבינוניים הם מנוע הצמיחה של המשק הישראלי עשינו הרבה לטובת העסקים הקטנים…  elicoh1 בידוד כלכלי או סיפור הצלחה בינלאומי צפו ותשפטו בעצמכםgtgt  MaarivOnline ועידת מעריב עסקים 2030  השר elicoh1 אין שום הצדקה להעלאת מיסים המדיניות הכלכלית שתוביל כחול לבן תהיה מסוכנת למדינת י… MidaWebsite משבר הדיור והמחסור בחמאה ההסתדרות והאיום של ניסנקורן במשרד האוצר רגע לפני הבחירות שר הכלכלה אלי כהן elicoh1 עונה על כל… בידוד כלכלי או סיפור הצלחה בינלאומי צפו ותשפטו בעצמכםgtgt  Israelcohen911 ביטחון ואמונה בין דיוני הקבינט על המתיחות בדרום נפגש חבר הקבינט ושר הכלכלה אלי כהן עם הראשלצ הגרי יוסף בסיום הפגישה… התזמון של ארגוני הטרור בעזה לירי על ישראל אינו מקרי הם מעדיפים לראות את גנץ בראשות הממשלה במקום נתניהו כמו בעבר…  GLZRadio חבר הקבינט elicoh1 מצהיר בנכוןלהבוקר מי שנתן את ההוראה לירות ישלם בחייו מערכה צבאית תהיה בעיתוי שאנחנו נחליט  צילום… GolanMay ממשיכים להגיע לכל עיר ופוגשים את ארץ ישראל היפה  הערב עם השר elicoh1 וחכ MKOfirKatz הבהרנו כי  כל קול קובע ולכן לא מוותר… עם כל הכבוד לקורונה ויש כבוד מגיפת הרק לא ביבי מפחידה הרבה יותר לא נורא עד ה23 זה יעבור רק מחל  DayanUzi וכבר אנחנו בכנס בבאר שבע עם רוהם בתמונה עם השר אלי כהן והקהל הבאר שבעי החם והאוהב  כך כל יום עד הניצחון  מי שמאמין לא מפחד מי שיש לו אידאולוגיה לא מפחד מי שיודע מה הדעות שלו לא מפחד מי שלא תלוי ברשימה המשותפת לא מפחד…  netanyahu עברנו את בריטניה עברנו את צרפת ישראל מהמדינות החזקות בעולם  ניסיון החרם המביש של האום רחוק מלעודד דו קיום ואף עלול להותיר אלפי פלשתינאים מובטלים זהו צעד של אנטישמיות מודרנית…  בשנות ה80 היו שתי מעצמות ששלטו בעולם ברית המועצות וארהב מאז אחת מהם התפרקה והשניה שגשגה הסיבה היחידה שארצות הב…  KoheletForum מחר יתקיים כנסקהלת לכלכלה בהשתתפות bezalelsm elicoh1  NadavEyalDesk  SharrenHaskel  NirBarkat  RoyIddan  OriKat… FateenMulla השתתפתי היום בחוג בית בישוב ביר אלמקסור אצל חבירנו חסין עדיר בראשותו של שר הכלכלה חכ elicoh1  חברי מרכז ומכובדים מהמג… בהחלטה צפויה הכשיר העליון את יזבק תומכת הטרור להתמודד לכנסת זוהי בושה שכף רגלה של אשה כזו תהיה חלק מכנסת ישראל וס…  10elilevi תמונת היום   הלך הזרזיר אצל העורב זה שרצה לתת את הכותל תמורת כלום וזה שתומך בטרור ולא מכיר בישראל כמדינה יהודית פועלים יחד נג…  גולני שלי יחד עם כל עם ישראל מתפלל לרפואת חיילי גולני היקרים שנפצעו בפיגוע הדריסה בירושלים אני סמוך ובטוח שכוחו…  בושה שאלה הם פני השמאל הישראלי מחבל מתועב ניסה לרצוח חייל באמצעות בקבוק תבערה ועל מי מרחם מוסי רז על הטרוריסט הק…  ריבונות הלכה למעשה קובעים עובדות בשטח אישרנו השבוע הקמת 6 מפעלים חדשים באיזור התעשייה במעלה אדומים עוד מפעל ועוד…  צביעות אירופאית קווים לדמותה כאילו אין עוד סכסוכים בעולם כאילו אין סכסוכים באירופה כל הזזת אבן כאן מוציאה אותם מ…  מחזקים את הקשרים עם הולנד  נפגשתי כעת עם מקבילתי ההולנדית שרת הסחר זיגריך קאך ויחד סיכמנו על חיזוק שיתופי הפעו…  מדינה הקוראת להשמדת מדינה אחרת לא יכולה להיות חברה באום בטח שלא לייצר נשק גרעיני זה המסר שהעברתי למנכל הנכנס של…  לא עוצרים הנחתי הבוקר אבן פינה לשני מפעלים חדשים בנוף הגליל יחד עם ידידי ראש העיר רונן פלוט  בזכות השקעה אדירה ב…  תכניתו של הנשיא טראמפ מכירה בזכות העם היהודי לחיות במולדתו ההיסטורית ומבטיחה את המשך השמירה על האינטרסים הבטחוניים…  likudnik1 elicoh1 LikudParty  RodgoldMD  Minister of Economy elicoh1 held a warning speech at the Internl Commemoration Day in Memory of the Holocaust UNVienn… מחכים לך בבית נעמה  תודה לראש הממשלה netanyahu שפעל מאחורי הקלעים והוכיח שבשבילו אזרחי ישראל מעל הכל  RodgoldMD עם שר הכלכלה אלי כהן elicoh1 ודוד אונגרכהן יוזם קונגרס וינה אשר מתמקד השנה על אתגרי הדיגיטליזציה של הכלכלה והחברה לא עוצרים חתמתי היום על הסכם להקמת איזור תעשייה חדש יחד עם יוחאי דמרי רמ דרום הר חברון דני מורביה רמ לכיש וניב…  הבלאגנץ חוגג כך נראית מפלגה שרק לא ביבי זו האגנדה היחידה שלה מציע שקודם תגיעו להסכמות ביניכם ואז תחזרו אלינו  נתוני האבטלה הטובים ביותר מקום המדינה השכר הראלי בעלייה הייצוא בשיא התיירות בשיא הקשרים עם ארה״ב ומדינות העולם…  radios100 השבוע בתוכנית הנבחרים עם דוד בן בסט ראיון עם שר הכלכלה והתעשייה elicoh1 LikudParty  מחר שישי 1000 בבוקר ברדיוס 10… איך אומרים פינטק בעברית  מספר חברות הפינטק שנפתחות בישראל מזנק משנה לשנה לאחר שבמשרד הכלכלה הבנו את הפוטנציאל האד…  elicoh1 בכחול לבן מנסים להסתיר את זה שהם מפלגת שמאל אך הם פעלו לאיחוד בין מרצ והעבודה וכיום הם מברכים עליו כי הם מפלגת שמאל  מפלגת… GLZRadio השר elicoh1 על האיחוד בשמאל אצל amirivgi שושבין האיחוד בין מרצ לעבודה הייתה כחול לבן אם למישהו היה ספק ראינו שהיא מפלגת… בכחול לבן מנסים להסתיר את זה שהם מפלגת שמאל אך הם פעלו לאיחוד בין מרצ והעבודה וכיום הם מברכים עליו כי הם מפלגת שמ…  yayafink סיימנו כעת פגישה טובה במשרד הכלכלה עם elicoh1 וצוותו עד ה 152 רשתות השיווק התחייבו להשוות בין המחירים שלהם בפריפריה לאלו ב… newsisrael13 בחירות 2020  שר הכלכלה והתעשייה elicoh1 התייחס לחקירות ראש הממשלה netanyahu ותקף את התנהלות בכירי מפלגת כחול לבן כשה… kannnews השר elicoh1 בשבתרבות בגבעתיים אם רוצים להימנע ממערכת בחירות רביעית – הדרך היא אחת מי שבעד ממשלת ימין לאומי צריך להצביע… תודה על הרעיון בני אבל אנחנו מסתדרים מצוין בלעדיך בטח תשמח לשמוע שממש לפני שבועיים הודענו על השקעה של 80 מיליון…  yayafink מחמאה לליכודניקית שר הכלכלה elicoh1 נפגש בימים האחרונים עם מנכלי רשתות השיווק ודרש מהם להשוות את מחירי הסופרים בפריפריה לאל… מוזמנים לצפות הערב קצת אחרי השעה שש בראיון שקיימתי עם אופירה וברקו יש למה לחכות שבת שלום  סך הכל שותפה קואליציונית לגיטימית🤦‍  סיכום העשור שלי  עם ישראל כולו כואב יחד את ההתקפה האנטישמית הנוראית על הקהילה היהודית במונסי ארהב ומתפלל לרפואת הפצועים ימי החנו…  עוד עסקת ענק שהיא גאווה לתעשייה הישראלית מאות מקומות עבודה נוספים מאות משפחות שיוכלו להתפרנס בכבוד נמשיך למשוך ח…  חברים וחברות יקרים היום הוא יום חג לדמוקרטיה ולתנועת הליכוד  למרות מזג האוויר הלא נוח אני מבקש מכם לצאת ולהצביע…  YairRevivo נפגשתי עם שר הכלכלה והתעשייה אלי כהן שמשרדו פותח מסלול יזמות טכנולוגית לצעירי לוד שנועד לתמרץ סטארטפים בתחילת הדרך ולתת… עכשיו זה כבר ברור בחירה בליברמן היא בחירה בבחירות רביעיות  מי שרוצה למנוע בחירות חייב להחליט ימין או שמאל ומי ש…  gershuni חשבתי לתומי שתדע לזהות הערה מעט צינית דבריי היו ברורים חסמי הרגולציה הוסרו ואם יש עוד משהו לא נהסס מנגד…  gershuni תשומת לבך עברנו לתקינה בינלאומית הורדנו מכסים לא נדרש כשרות בגין רהיטיםאת החלק שלנו עשינו ואם נ…  הבוקר בכנס התעשיינים בצפת יחד עם ידידי ראש העיר shooki32  משיקים פארק תעשיות חדש בשורה לצפת בשורה לצפון בשורה…  גאולה כהן הייתה חלק מדור הנפילים של הציונות לוחמת אמיצה מבוני יסודותיה של מדינת ישראל לעד נזכור את קולה הייחודי…  גאווה ישראלית   עוד אקזיט מוצלח עוד השקעה של חברת הענק intel בחברה ישראלית ישראל היא שחקנית מובילה בזירת הטכנו… </t>
-  </si>
-  <si>
-    <t xml:space="preserve">yigalc73 מחזק את מה שאני אומר לך כל פעם רק אנשים מעניינים יכולים לכתוב סדרות מעניינות אין מה לראות סדרות של אנשים שלא מעניינים אותך N12News מי היה כאן ראש הממשלה בחצי השנה האחרונה אולי גם לו יש אחריות כך הגיבה KerenMarc  להצהרת ראש הממשלה  dovbsin roysharon11 גם לך רק אומר yanivbiton99  rumblevcrumble נראה לי לא זול בכלל כולל הייבוא והכל ShaniAshkenazi RonHuldai הבעיה שלנו היא לא מחסור באומץ אלא מחסור במרחב ציבורי לפעול בו הכל קטן הכל צפוף והרוב…  est987 אי אפשר גם להגיד טקטי ומהיר וגם לדבר על מצב הכביש והתשתיות זה או או או קומנדו או חטיבת שריון ShaniAshkenazi RonHuldai לגבי הכרם ונווה צדק אני מסכים איתך  החזון לשכונות האלה צריך להיות עם מינימום רכבים בש…  ShaniAshkenazi RonHuldai נכון נחלת בנימין למשל פועל כרחוב בבוקר על מנת להקל על הסוחרים זו אוכלוסיה חשובה לא פ…  ShaniAshkenazi RonHuldai ויחד עם זאת  אם יש מקום שאת חושבת שאפשר לעשות בו התערבות נשמח לשמוע היה גל ראשון של…  ShaniAshkenazi RonHuldai כמעט כל הצירים הראשיים בעיר ייסגרו כל צירי המשנה יהפכו לעמוסים בתחבורה ציבורית המרחב…  ShaniAshkenazi RonHuldai אפשר למצוא גם בת״א כמה תמונות  שיראו שדווקא כן עושים פה ״סטוקהולם״ אבל אם לרדת לשורש ה…  DorLasker avishaysela געגועים גם מהצד השני abaleh העיקר שהצעתי התקבלה לא whatevergever 1 ZRTZR ברור שזה מבוים guylerer תהיה חזק חבר דיברנו על זה שזה יהיה רגע קשה עשיתם המון טוב לעולם זה לא יספיק  stagadouch בתל אביב במקרה כולם מדברים על אלשיך  אף אחד לא מדבר על ארדן השר לבטחון פנים שהגיע למקום באותו הבוקר קבע שמדובר במחבל והאשים את…  jony4212 לא יודע אבל אם היה פתרון זמין אני די משוכנע שהיינו כבר מזמן מאמצים אותו jony4212 רק בן אדם שכל כך איכפת לו כל כך מתעצבן מהדברים האלה רובם באמת מטריפים אבל הם חלק מהמכלול שכולנו אוהבים…  tamarlask טופל  Yashar2U  barakbl אודיסאה yoavr  mtklng קיקה אלמודובר 1993 גרסה מוקדמת יותר  mtklng eyaldatz ממש לא אבל אם הוא ירוץ וייבחר  זה חדשות נפלאות למדינה therealnirs TelAviv  Oelster zviashkenazi  zviashkenazi תודה אכן הבטחתי ושמח שזה עזר בהלם שזכרת את זה בפועל הקרדיט ליועצת רה״ע למעמד האשה  אפרת מייקין כנפו abaleh מנחש שעוד מגדל אבל לא בדקתי SecPompeo The people of Israel recently made a beautiful demonstration of solidarity with the people of  Lebanon  by illuminating the… DoroniP RIP freyisrael1 עצה ידידותית אם אתה לא רוצה שיזכירו שאבא שלך טרוריסט אל תמזער את סיקור האלימות הפוליטית מימין על ידי סימטריה שקרית מה ל… spez RonHuldai EINATkalisch kunikran השלושה האחרים לא באמת מסורים robertrabin ברוך הבא  כן יירבו dudiLift מושלם EliBarbel 1 Elinorigby היי חברות וחברים מדובר באותו אדם שפגע גם בי אם זה לא רלוונטי אליכם ומקווה שלא בבקשה בבקשה בבקשה שתפו אולי ביחד נצליח ל… noalandau Live from Tel Aviv A rare moment of solidarity   TelAviv  סינמטק תל אביב מחפש מנהלת אמנותית  דרישות המכרז גמישות למדי אבל הכי חשוב  מישהוי שמאוד אוהבת קולנוע ישראלי ו…  elad3 spez jimmyjazz0123 אלה בדיוק הגבולות של הפעימה הראשונה שאני מציע קטע בואו נדסקס ברצינות בשבוע הבא spez elad3 jimmyjazz0123 תשמע זה ממש דומה למתווה שאני עובד עליו סמול מיינדס  שווה לדסקס קצת יותר לעומק במהלך שבוע הבא spez האפשרות השנייה היתה שביל דו סיטרי בצד אחד אבל אז נכנסים לבעיה בצמתים spez זאת גם היתה עמדתי אבל זה נפל מטעמי בטיחות הסיבה המרכזית היא רוחב השביל יש מקטעים צרים ברחוב ואם רוצים שב…  Nirpetel לשכנע את אבי ניר אבל זה יהיה קשה כי זה פרוייקט קצת יקר ביחס למה שקורה היום שלא לדבר על זה שזה נולד בתקו…  drgilitamir LeonSlepyan DavidAgaev3 מכיר ומוקיר מאוד את פועלו מהאנשים שיקבלו פרס ישראל צדיק בעירו LilacBL zviashkenazi TogetherKulan iTelAvivYafo אנסה ruthelbaz ״תפקידה הראשון על המסך״ חצופים לא יהיה פה שום קלוז׳ר עד שלא אזכה בתביעת הדיבה נגד ישראל היום considerthefish ואין אוטובוסים  חלק מהקסםשקט considerthefish פידתחבורה בעלי עסקים נוטים להתנגד לביטול מקומות חניה בטענה שזה יפגע בהם אבל סקירה של 12 מחקרים מהעולם מוצאת שלסלילת… ronasherov considerthefish iTelAvivYafo MeitalLehavi אוקיי אעבור שם בשבוע הבא ואחפש מקום  תודה considerthefish iTelAvivYafo MeitalLehavi צודק יטופל est987 MeitalLehavi בקיצור צריך להתחיל מדידות ותכנון ואז נדע איפה אנחנו עומדים לא הייתי בונה על 2020 מקווה שנצליח ל2021 est987 MeitalLehavi מצד שני כיוון שהתכניות העתידיות הן להרחיב את הרחוב להגדיל את המדרכות לייצר מסחר ושבילי אופ…  est987 MeitalLehavi לא ״אמור״ להיות מסובך אבל גם לא לגמרי פשוט כי יש תחבורה ציבורית משני הצדדים מה שדורש תכנון ש…  est987 MeitalLehavi בהחלט חייבים שם שביל גם מתוכנן אחד מבטיח לנסות להקדים את הביצוע שלו ZRTZR וואו מקרה קיצוני אם הוא קורה הרבה בשלב ראשון הייתי מגביר אכיפה לפעמים זה מספיק rahelibindman גם חלק מהתכנית spez בינתיים אין תכנון כזה eliavl תבוא לשיתוף ציבור יוסבר שם eliavl האדומים  שבילים ראשיים הירוקים בהירים  שבילים משניים talrabinovsky ittaishick הטיפול בצמתים הוא חלק מרכזי בתכנית בשיתוף הציבור נרחיב על הפתרונות ilalevy בבקשה   nirmatara בבקשה   ronasherov בשנה הבאה אמורות להתחיל שם עבודות הרכבת הקלה ואז סוף סוף יהיה שביל ofekzemach בבקשה   IllBrains בבקשה    ShayLibrowski יהיו עוד כמובן yuvalvar בבקשה    DorVardi צמתים הם חלק משמעותי מהתכנית TheMokagi בבקשה   yguyyyy AssafShtauber הכל תלוי ברוחב הרחוב השאיפה היא שבילים דו סטריים משני עברי הכביש אבל זה רק בכבישים ראשיים…  RosinJonathan 1 תודה 2 לינק למפה ברזולוציה גבוהה   3 המפה פתוחה לשינויים רצינו להביא משהו קונקרטי לשיתוף ציבור assafon 5 שנים  אם הכל הולך חלק בטח ייקח קצת יותר isrPiccolo מסכים כל עוד כל ערי המטרופולין לא ייקחו חלק בשינוי סדר העדיפויות יהיה קשה לייצר מהפיכה אמיתית AssafShtauber אמור לרדת בסוף השנה נובמברדצמבר isrPiccolo לצערי בינתיים רק דיבורים Idan68492838 אם תשלח מייל מסודר לפה assafhareltlvgmailcom מבטיח להעביר לגורמים הרלוונטים yosefmatan עושים ריסטארט בתחבורה תכנית האופניים שלנו יוצאת לדרך כבר השנה נסלול שני שבילים היסטוריים  בדיזנגוף ובהרצל נוריד לכביש את השבילים שמצוי…  itaihyman הלילה צובעים בנווה שאנן רח׳ סלומון chaluny therealnirs שמנו עמודונים isrPiccolo בהחלט מקווה שממש בקרוב יש שופטים בירושלים ויש שבילים טקטים בתל אביב  פינסקר  בין בוגרשוב לכיכר  yigalc73  yigalc73  היתה לי תחושה שהטלפונים שאני עושה לזקני העיר לא ממש פועלים לטובתי  gotomichal Alikfinkelstein ShaniAshkenazi naamuli84 אני לא חושב שיש פה היתממות אלא כאמור משאב מוגבל ברור שיש א…  telavivacation צריכים פה עזרה של הממשלה כי מבחינת החקיקה הקיימת לעירייה אין מספיק כלים לאכוף העלנו את הארנונה אב…  telavivacation זה קורה מעצמו זה היופי הן מתחילות לחזור לשוק בגלל הקורונה ״השוק החופשי נתן השוק החופשי לקח יהא השוק החופשי מבורך״ NeumanRoee מצטער על זה SagiShyovitz אני מציע בעניין כיכר אתרים לשפוט אותי לפי התוצאה הסופית ולא לפי כל מני כותרות ופרשנויות לא שיניתי את…  everytinisfine אתה צודק הקדשתי את רוב הזמן ללמוד את החומר ואת המערכת אשתדל להשתפר ולשתף יותר NeumanRoee יש מיקרו ויש מקרו במיקרו יש צוותי עבודה לכל נושא אופניים מדרחובים שמגבשים תכניות עבודה ואני חלק מהם…  ExteriorMusic עובדים גם על זה naamuli84 הגיעו ימות המשיח עיריית תל אביב מאפשרת להוציא כיסאות ושולחנות על חשבון חניה עושים את זה קצת מכוער לא יכלו להעתיק מברצלונה… אם יש לכם המלצות למדרחובים נוספים  אשמח לשמוע  assafhareltlvgmailcom מדרחובים שבילי אופניים הצללות ומרחבים להולכי רגל שנה שלמה אנחנו מגבשים הכל וסוף סוף אפשר לראות קצת תוצאות יש עו…  abuhobbit הבוט הבטיח בקרוב בשלב הבא  תכנית האופניים abuhobbit וריאציות שונות של בקרוב אצלנו ltltltRLbotgtgtgt therealnirs chaluny בקרוב עובדים על זה במלוא הכח aaronaaronmt dovalfon RonHuldai TelAviv מקווה שבקרוב מאוד עובדים על זה ReutMor  GadeerMreeh היום בכנסת israelrosner MattiFriedman kann מגיע לכם כל מי שעשה פעם דוקו היסטורי יידע להעריך את העבודה שלכם  מהעריכה המעו…  מלחמה בלי שם  סדרת דוקו נפלאה על הבוץ הלבנוני שבמשך שני עשורים היה חלק הזוי משגרת החיים פה מאות הרוגים אלפי פצו…  ShaiCohen13 גם אני ביחד עם ירון ניסקי ודורון צור    DavidLifshitz מעולה AsafZagrizak yoavr בעבודה בימים אלה ממש פרטים בקרוב yoavr זה אנחנו צובעים לא מע״צ נכון יפה  חוץ מזה כבר אין מע״צ RTsipris  RTsipris קייס לתפארת eyaldatz 1 לאוהבים את האביב ומילים מוזרות כמו דינגה דינג  SaHreports Day 13 of lockdown  yigalc73 בדרך avishaysela וואו אתה היחיד שזוכר את זה AsafCarmel1 roykatz ואליהו שפייזר כמובן ashavit23 AsafCarmel1 roykatz מאשר רשמית ברוך הבא מספר 3 ברשימה שלנו  eyaldatz אסור ShaniAshkenazi barakbl RonHuldai פינו את הכלים  תודה לפקחים שעובדים בשבת תודה למחלקת התפעול ותודה לסוכנת שלי שמלווה אותי מתחילת הדרך barakbl ShaniAshkenazi RonHuldai מסכים בודק OriBenDov Yashar2U ואכן לאור הגידול המבורך במספר הילדים בשכונה העירייה מבקשת להשתמש במבנה כבית ספר עם זאת מתו…  OriBenDov Yashar2U ההסבר הרשמי סניף הנוער העובד והלומד ביפו מקיים את הפעילות השוטפת שלו בבי״ס ויצמן שנסגר לפ…  OriBenDov Yashar2U אין לי מושג שומע על זה בפעם הראשונה אבדוק תודה barakbl eyal6699 צריך להבין שההגדרה הסטטוטורית של שטח בית הספר היא שטח חום  שטח לצרכי ציבור בעבר היה שם בית ספר…  eyal6699 בוא נתחיל מזה שתהיה ממשלה barakbl eyal6699 החלטה קשה שהתקבלה בלב כבד אבל לצערי לא נמצאה באמת חלופה עדיפה כל נושא הזרים בעיר מורכב מאוד במ…  eyal6699 לצערנו התשתיות בעיר רחוקות  מלהתמודד עם משבר האקלים מבחינת תקציבים כבר עכשיו אנחנו עושים את המקסימום אבל…  abaleh שכחת לתייג אותי הכל בסדר נשמה אלה חוקי הפורמט  לא יודע מי עשה אבל מדויק  YTB2018 shaulig theakerman RoeiGalnor עובדים על זה כבר כמה חודשים ממש לא שבועיים התקציב הוא 125 מיליון למיט…  yigalc73 אלק  בולדווין yigalc73 מותר האדם עלק  drornissan mayasel רעיון שכשל גם במקרה של האסיר איקס mayasel אינדיד ובגלל זה עד היום לא יודעים mayasel המעורבות של האדם השלישי לא הוכחה ולא נחקרה לעומקה סימני השאלה שם גדולים ורבים לא ברור האם נשבר בחקירה ש…  דרוש גרפיקאי של שבת עבודה קטנה שעתיים כזה שמערבת פוטושופ ופאוורפוינט חייב להיות מחר בתשלום כמובן מי פנוי ברוטשילד yuvalrub barakbl אנחנו רק בתחילת הדרך תן כמה שנים להוכיח את עצמי מקווה שתוך כמה שנים תחשוב אחרת תהליכים רציניים לוקחים זמן EstyS אעלה בקרוב מונולוג שמסביר את כל הסיטואציה עברהווהעתיד מחכה להחלטת הוולחוף EstyS ולעניות דעתי  זה לא הדיון המכריע אני סבור שהדיון המכריע עוד לפנינו פה אני חלוק על העמותה EstyS אני פה בדיון נלחם במגדלים בדרכי גם אם היא שונה מזו של העמותה זה לא אומר שאנחנו לא פועלים למען אותה מטרה ruthelbaz מה לא היה כיף OmerLubi ביבי  רוצה  שתדברו  על  הבחירות  החוזרות  במקום  על  ההפגנה  אתמול  סתם שתדעו  נב  לא יהיו בחירות חוזרות abaleh שולה קשת ואני דווקא מתואמים בעניין הזה אבל גם אם דעותנו היו שונות אני מעדיף רשימה שבה מותר לכל אחד להחזיק…  abaleh ספציפית זה אומר שבמקביל להקמת מרכז התרבות שהוא כאמור מבורך בעיני צריך לדאוג שיהיו מאות יחידות של דיור בר…  abaleh ג׳נטריפיקציה היא מילה שקל לזרוק אבל במציאות גם אם תיקח שכונה במצב קשה ורק תשפץ את הרחובות תוסיף גינות תא…  abaleh הדבר החשוב בעיני הוא כיצד יתפקד מרכז התרבות והאם תהיה בו רק ״תרבות לבנה״ או גם ״תרבות שחורה״ ויצוג לקהילות…  abaleh המציאות רחוקה ממה שאתה מתאר אבל כיוון שקמת מהספה ושרפת את הקול עלי מגיע לך הסבר מפורט  שולה קשת לא מתנגד…  ruthelbaz היי לכולם אני יוצאת לדרך עצמאית ומחפשת עבודה בניהול תוכן ודיגיטל קריאיטיב כתיבה וכו יש לי ניסיון בניהול דיגיטל וכתיבת…  במסגרת חגיגות העצמאות בבית הנשיא ציפי שביט נשיא המדינה וכל הקהל שרים יחד ״ברבאבא ברבאבא אוהבים אותך כולם״ ורק ראש…  לטוס לחו״ל עם תינוק זה מאתגר אבל גם להגיע לנתב״ג עם תינוק זה לא פשוט השבוע גיליתי את הסטארטאפ הישראלי החדש  מונית…  Lazyishai נכון אבל הסדרה החדשה שלו סתמית ובינונית ArielBH ברור  בוא נמשיך בפרטי ולגבי הבחור שבתמונה באופן מפתיע אנחנו מסכימים על הרבה יותר דברים ממה שחשבתי הדיאלוג מאוד ענייני רציני ומקצועי…  מקווה להתחיל לעדכן לעיתים תכופות יותר ולישון יותר הטלפון במשרד שיהיה לכם 037244605 פלאפון 0547324732 המייל assafhareltlvgmailcom תכלס הרבה מאוד נושאים קריטיים בעיר מחכים לשר תחבורה חדש ושר פנים חדש שיכולים לעשות שינוי אמיתי בנוגע לתחנה המרכזית…  נושאים נוספים שהתחלתי לעסוק בהם הגדלת כמות בתי השימוש הציבוריים ברחבי העיר ובגינות הסעות לים בשבתות הפחתת תקן הח…  המאבק על ציר שלבים גם כאן נשמעים קולות חדשים בעירייה תחזיקו לנו אצבעות  עובד על זה ביחד עם שלי דביר וגם כאן אני…  אני מנסה לעזור מבפנים למאבקים החשובים בעיר המאבק להצלת העצים שנותרו בארלוזורוב ממערב לאבן גבירול נעשים ניסיונות…  ביחד עם שותפי לסיעה אמיר בדראן אנחנו מלווים את הנסיונות להסדרת נמל הדייגים הפרדסים ובתי הקברות בפרוייקטים החדשים…  מגדלים בני השגה  ביחד עם יו״ר ועדת התכנון והבנייה דורון ספיר מתחילים לשנות את תמהיל הדירות במגדלים החדשים בעיר וב…  תכנית האופניים הגדולה  כאחראי על תחום התשתיות של שבילי האופניים אנחנו מתחילים לגבש  ביחד עם צוות התחבורה הרציני…  פינויים בעיר  בחודש האחרון הגישו יותר מ200 משפחות בקשה להצטרף למתווה הפינוי של שכונת הארגזים מדובר במתווה פינוי…  ברגע שכל הפרטים ייסגרו אציג לכם אותו במונולוג מיוחד שיפרט את כל ההסכמות המחלוקות והסטטוס העדכני בכל מקרה אני מאמ…  רוב הזמן מוקדש לפגישות ישיבות ושיעורי בית אני עוד רחוק מלהציג הישגים ממשיים מדובר בתהליכים ארוכים אבל אשמח לשת…  מבזק עדכונים דבר ראשון אני מתנצל שאני לא מעדכן בתדירות גדולה יותר השילוב של תפקיד חדש ורציני ביחד עם תינוק…  ruthelbaz נחמד שכחתי את זה odedkramer נחיתה הבאה  רק עם מאמן זר zviashkenazi תודה צבי mtklng ברצוני להתנצל בשם מחלקת הקריאייטיב העירונית משחק המילים אינו ראוי ואינו מכבד את התושבים נותר לנו רק להתנח…  1 המערכון לא צחק על יוני אלא על מסע היח״צ ההזוי שאירגנת לעצמך באנטבה  2 יש הבדל קטן בין תכנית סאטירה לתשדיר בחיר…  drorfo יפה כתבת לזכר הזוגיות המופלאה של יונה עטרי ז״ל ואילי גורליצקי  Lazyishai תהיה בשקט תהיה בשקט תהיה בשקט תהיה בשקט תהיה בשקט תהיה בשקט תהיה בשקט תהיה בשקט תהיה בשקט תהיה…  תקשיבו לרותם סלע בסרטון מ2014  הבחורה יודעת על מה היא מדברת   כשיש לך כרטיס קופת חולים לפני שיש לך שם  mulisegev odedkramer היו ימים שהיה מותר לעשן בחדר כותבים ליד החלון swedishkeren  כבוד גדול להיות מוזכר בכתב האישום נגד נתניהו סעיף 195 מספר איך הפך ״מערכון ביקורתי״ הגדרה של היועמ״ש על מסעות נ…  קצת מוזר שכולם מדברים על איחודים בשמאל ואף אחד לא מציע את האופציה של איחוד עם חד״ש מילא העבודה אבל גם למרצ יש בעי…  AviBenayahu זה לא עניין של שמאל וימין  הכיבוש משחיתזו עובדהאמרו זאת לפנייגם שרון  גם בצה״ל מודעים לכך ומשקיעים רבות בחינוך והכנה… hagaykr igalmosko אהה אז שמתם לב שמתם לב שהכתבות של igalmosko מתחילות למלא את החלל הגדול שהותיר אחריו  קירשנבאום עם טון מדויק ומשעשע הוא הופך את ג…  elidukorski כשאנו נכנסים לכיתה או לגן מתנוססות מולנו תמונות נשיא המדינה ראש הממשלה והרמטכל  דמויות גבריות כאילו רק גברים יכולים להצ… לא מצליח להבין מה הטמפרטורה בחדר  לפני שנה נסעתי ליום כיף במתקן הכליאה עופר בשטחים רציתי להתרשם כמה אנחנו מוסריים לשבת קצת בדיונים לראות איך הסיס…  NitzanHorowitz אני רואה שמתפתח מיני קמפיין נגד אסף הראל ״הציני והאופורטוניסט״ אז ככה הוא לא הראשון ולא האחרון שמשנה כיוון בניגוד ל… asaflib שמתי לב שיש זעזוע בפיד מההחלטה של אסף הראל להיכנס לקואליציה של חולדאי עוד שמתי לב שאיש מהמזועזעים אלה שראיתי לא תמך באסף ה… dovhanin עוזב את הכנסת אבל לא מוותר על עשייה בשטח  hapoella זה לא אני זה פופטיץ תכלס מהפייסבוק של דניאל מירן  faniaoz איזה יפה כתבת ודיברת ושרת בציבור היה מרגש במשך 13 שנים היה dovhanin חבר הכנסת האהוב עלי להצביע לו היה מניה בטוחה הוא אף פעם לא הביך אותך או גרם לך להתחרט…  lironk1 שלא תדעי עוד צער odedkramer כשהיינו בסוף היסודי הבילוי של שישי בערב היה לנסוע לסעיד לאכול לאפה הקושי הגדול היה למצוא מונית של 7 ונהג שיסכים לדחוף אליה 8 המנוח ואני אחד הפרקים האהובים עלי בשוטטות היה לאיש הומור עצמי </t>
-  </si>
-  <si>
-    <t xml:space="preserve">הסתיים ביקור עבודה בצ׳כיה  ובשעה טובה נחתנו לפני זמן קצר בארצנו הטובה והיפה      ידידות מופלאה של שנים ארוכות  תודה לך צ׳כיה על התמיכה בישראל                                     הצטרפו לשידור החי של של מסע״ת עם סגן ראש  עם ישראל חי                                             הנחתי עכשיו את זר הממשלה למרגלות האנדרטה בגטו טרזנישטט  שבוע מצוין שיהיה וחודש טוב מאוד לכולכם ‼  לכם לבני ביתכם לחיילינו הגיבורים והאהובים בכל הגזרות ולכל אזרחי ישראל שבת שלום וסופ״ש מעולה   ממעלות זמן קצר לפני סיומו של שבוע אינטנסיבי מאוד ברחבי הארץ שבו המשכתי במימוש היעד הראשון שהצבתי כשר מדע הנגשת  ממעלות זמן קצר לפני סיומו של שבוע אינטנסיבי מאוד ברחבי הארץ שבו המשכתי במימוש היעד הראשון שהצבתי כשר מדע הנגשת  יש שאומרים לי שאני ״קיצוני״ משום שאני מתנגד למדינת טרור פלשתינית בלב הארץ שלנו אמרו לי כבר שאני ״איש האתמול״  חיילינו האהובים והגיבורים אתם כבר מכירים את הנוסח                                                   והערב  בשמכם ובשם המדינה ליוויתי אתמול את סמל יובל ז״ל למנוחת עולמים את יובל לא הכרתי שעה אחת במהלך הלוויתו ישבתי  הדס מלכא הי״ד נרצחה בידי חיות דו רגליות ששאבו עידוד מההסתה של ה ״רשות הפלשתינית״ זהו כפל הלשון והצביעות של אבו  הרגעים העוצמתיים והמרגשים ביותר                                        כל הקהל שבא אתמול בלילה לבית הכנסת של  עכשיו בסלוניקי  ישיבת ממשלה משותפת עם ממשלת יוון ואחרי חתימה על עוד הסכם לשת״פ במדע טכנולוגיה וחדשנות  מתחילים ביקור עבודה בסלוניקי ולי כנצר ליהודי העיר שכונתה ״ירושלים דה בלקן״ הפעם זאת לא רק נסיעה להידוק הקשרים  מקרית שמונה אני מבקש לבשר לכולכם      הוריתי להוסיף עוד מיליון שקלים לקייטנות הקיץ של משרד המדע  שבוע טוב מאוד לכולכם   לפנק לפנק אז מסתבר שמי שמפעיל את הקייטנות הזולות ביותר בישראל הוא משרד המדע נרשמים עכשיו אפילו ב תוכנית  לפנק לפנק נרשמים עכשיו לקייטנות הקיץ של משרד המדע                                      הזולות ביותר בישראל  בעולם של צביעות היית מגדלור של ישירות וכנות בעולם שברובו העמדת פנים תמיד עמדת על האמת  בעיקר על האמת שלך  בתוך ״הבידוד המדיני״ שישראל נמצאת בו אנחנו ממשיכים לחתום על הסכמים לשת״פ במדע טכנולוגיה וחדשנות עם עוד ועוד  בדרך לאירועי שבוע המצויינות בשדרות תמיד נפעם מיופיה של ארצנו   טרור בלונדון או טילים מעזה אין שום הבדל חבורה של מופרעים שרוצים להחריב את העולם החופשי כולו  שבוע טוב מאוד יקיריי                                    הצלחה רבה מאוד לראש הממשלה שיוצא הערב לביקור במערב  שבוע טוב מאוד יקיריי                                   נשלח הערב ברכת הדרך לראש הממשלה שיוצא לביקור חשוב במערב  סליחה שניצחנו                                       אז זהו שלא  כשחזרתי מביקור העבודה האחרון שלי בארה״ב אמרתי שאני מעריך  שלצערי  הפעם השגרירות לא תעבור לירושלים     אבל  לכם לבני ביתכם לחיילנו הגיבורים והאהובים בכל הגזרות ולכל אזרחי ישראל חג שמח       ולכל המטיילים בארצנו הטובה  הברכות שיצאו מן הלב  נכנסו אל הלב       תודה רבה לכולכם שימחתם וריגשתם  השר שלנו עשינו לך השתלטות עוינת על הפייסבוק  אל תדאג לא מתרגלים זה אך ורק לרגל יום הולדתך ה 44   עשינו דרך  בדרך לישיבת ממשלה היסטורית בכותל המערבי  לכולכם יקיריי שבת שלום סופ״ש מצוין וחודש טוב מאוד   תכירו את ונוס ותאחלו לו דרך צלחה                                            לווין המחקר הישראליצרפתי עוזב  מירושלים חג שמח מאוד ירושלים   תודה לך הנשיא טראמפ             תודה על אהבה אמיתית לישראל לירושלים תודה על ביקור היסטורי בכותל המערבי תודה  נצחון גדול למתנגדי המדינה הפלשתינית הנשיא טראמפ לא חזר בנאומו בבית לחם על האיוולת של ״שתי מדינות״ עקביות ועמידה  מה אמרתי לנשיא טראמפ  ומה הוא השיב לי                            ולמה שהפלשתינים לא יעשו לנו מחוות  ולא אנחנו  ברוך הבא לישראל כבוד הנשיא  ברוך הבא לישראל כבוד הנשיא  ברוך הבא לישראל כבוד הנשיא  ברוך הבא כבוד הנשיא               שבוע טוב מאוד יקיריי פגשתי את העיתונות הערב והסברתי מדוע זה דרמטי שלראשונה  בארץ אהבתי מחכים לאורח                     לכם לבני ביתכם לחיילנו הגיבורים והאהובים בכל הגזרות לכל אזרחי  איזו שערורייה זאת שבטקס סיום באוניברסיטה העברית בירושלים לא ישירו היום את ״התקווה״ כדי לא לפגוע ברגשות של  תודה רבה מאוד לצוות הנהדר שלי על ארגון מופתי של כנס ״סל מדע 2״ שיחקתם אותה בענק  17 במאי היום לפני 40 שנה קיבלנו מנדט ברור מהעם להוביל  בדרך הליכוד  אפשר לכתוב הרבה מאוד מאוד דברים על היום  השלום עם ירדן  חשוב מאוד מיזמים מדעיים  חשובים מאוד כבודנו הלאומי ועמידה על עקרונות  חשובים הרבה יותר מהכל  התגעגעתי אז באתי   ככה מפריכים את השקר הפלשתיני של הכיבוש גם בתקשורת האמריקאית 97 מהפלשתינים חיים תחת שליטתה של הרשפ ולא תחת  לכולכם יקיריי שבת שלום שבת מנוחה וסופ״ש מצוין   תגידו בהצלחה וברוך הבא לדייויד פרידמן שגרירה החדש של ארה״ב בישראל                             סיימנו פגישה  רוחות של שינוי נושבות עכשיו בוושינגטון למען ישראל                                                 אני מאמין  תראו את מי פגשתי ברכבת לוושינגטון איילת שקד  הנה שתי סיבות מתוך רבות שבגללן כולנו צריכים להתנגד ל״שתי מדינות לשני עמים״         1 זאת הארץ שלנו תמיד  כל עוד אני משרת אתכם תמיד אתנגד להקמת מדינת טרור פלשתינית ביו״ש התחיל ביקור העבודה בארה״ב בנאום בפני אלף אורחי  לכולכם יקיריי שבוע טוב מאוד                      בעוד שעות אחדות אמריא בשליחותכם לביקור עבודה בארה״ב מבטיח  מיהונתן מרוני וממני שבת שלום חברים יקרים שבת מנוחה וסופ״ש מצוין   תראו מה זה נשיא ארה״ב לא דקלם ״שתי מדינות לשני עמים״ בסיום פגישתו עם ״אבו מאזן״ שנים אני אומר לכם שמדינה  אונס״קו לא מכירים בריבונות ישראל בירושלים                                                   אז תשמעו ההחלטות  לכולכם חג עצמאות שמח מירושלים   מירושלים לכולכם חג עצמאות שמח   בתום היום הזה בטרם יונפו הערב דגלי ישראל לראש התורן המדינה כולה עוצרת מרכינה ראש  ומצדיעה לנופלים את  בהצדעה ובהרכנת ראש היום כולנו משפחת השכול  מאיתנו שבוע טוב מאוד לכם ולכל עם ישראל   לכם לבני ביתכם לחיילנו האהובים והגיבורים בכל הגזרות ולכל אזרחי ישראל שבת שלום וסופ״ש מצוין   האופוזיציה שלנו אומרים כל הזמן ש הדמוקרטיה בסכנה אבל מי שבאמת בסכנה היא האופוזיציה עצמה עם העמדות הבלתי  חג שמח לאחים היקרים שלנו בני העדה הדרוזית החוגגים את חג הנביא שועייב מי שהולך איתנו  אנחנו הולכים איתו  תגידו להם מזל טוב אלופי עולם נבחרת הרובוטיקה של דימונה                              בזמן שישנתם קיבלתי  שר החוץ של גרמניה כבר אמר את האיוולת והשקר הגס ש״ישראל מקיימת ממשל אפרטהייד״  הוא גם יודע היטב שקרנות גרמניות  מאודים מוצלים בשמי אירופה  למדינה חזקה ומפוארת               מרכינים ראש לזכרם שישה מיליון יהודים מהם מיליון  הייה לי חברהייה לי אח              גיסי האהוב שי מוצפי ז״ל  נפרדנו אתמול משי אהוב ליבנו אחיה של רעייתי  לכולכם יקיריי מאיתנו חג שמח ושתמיד נחייך   תגידו מזל טוב ליהורם גאון                        התקשרתי עכשיו לברך אותו על ההחלטה הנבונה לפיה הוא יהיה אחד מ12  ההבדל בין יוסי קליין לרועי קליין הי״ד יוסי קליין מעיתון ״הארץ״ פרסם אמש מאמר מבחיל נוטף ארס ושנאה בו כתב בין  אנחנו נשארים בארץ                  טיפסנו היום לפסגת הסרטבה שבבקעת הירדן כדי להזיז הרים גם בחופשה   תגידו לאן נעלמו כל אלה שלא הפסיקו להתראיין לדבר לחתום על מודעות בעיתונים ולשכנע אותנו שצריך לסגת מרמת הגולן  לכולכם יקיריי שבת שלום שבת מנוחה וסופ״ש מצוין   הַצְּבִי יִשְׂרָאֵל עַלבָּמוֹתֶיךָ חָלָל אֵיךְ נָפְלוּ גִבּוֹרִים תנחומים למשפחתו של החייל  אלחי טהרלב הי״ד  עכשיו אני רוצה לראות את מהירות הגינויים הבינלאומיים הכינוסים הבהולים ו״העצרת הכללית של האו״ם״ בעקבות הטרגדיה  אתמול בערב בשעות אלה ממש ממש ממש התרגשתי       מאות אנשים הגיעו להרמת הכוסית לפסח והם עשו זאת מכל קצות הארץ  אני רוצה להגיד לכם מילה אחת תודה התרגשתי ושמחתי לראות אתכם בהרמת הכוסית לחג         אנחנו הולכים ביחד כברת דרך  שבוע טוב מאוד יקיריי                  קבלו ספויילר  בלעדי לקראת ישיבת הממשלה מחר שבה אסקור את פעילות משרד המדע  יקיריי שתהיה לכולכם שבת שלום שבת מנוחה וסופ״ש אביבי   צמצום פערים חיזוק הפריפריה הנגשת המדע הטכנולוגיה והחדשנות לכל אזרחי ישראל  במעשים לא בדיבורים ולא בציוצים  תגידו מזל טוב ליהודה ברקן             התקשרתי עכשיו לברך אותו לכבוד יום הולדתו שחל היום ואמרתי לו שמיליוני  הבטחתי  וקיימתי את הרמת הכוסית לפסח לעובדי משרד המדע סיימנו עכשיו בשילה הקדומה שבחבל בנימין  הבטחתי  וקיימתי הרמת כוסית לחג הפסח לעובדי משרד המדע בשילה הקדומה שבחבל בנימין היפה זאת הארץ שלנו ואנחנו כאן  כשאני רואה את מיטב הנוער שלנו  אני רואה את העתיד המזהיר של ישראל כשאני פוגש אותם בכל הארץ  והיום בעכו  אני  אין כמו בבית  אין אבל ממש אין כמו בבית  במזרח הרחוק השבת תכף נכנסת אז לכולכם מטוקיו                                              שבת שלום וסופ״ש מצוין  מטוקיו בוקר טוב ישראל                                 החיבוק של ארצות המזרח הרחוק את מדינתנו הוא פשוט מחמם לב  אני ממשיך בביקור העבודה במזרח הרחוק                           שלום לכולכם מטוקיו אחרי יום ארוך ופורה שכלל  גאווה והתרגשות דגלי ישראל מתנופפים בכיכר טיאנאנמן בבייג׳ינג                             אני מסיים עכשיו את  הבטחתי לכם  וקיימתי עוד הסכם עם סין נחתם עכשיו          ראש ממשלת סין וראש ממשלת ישראל באו לראות מקרוב   בוקר טוב ישראל                          בזמן שישנתם התחלנו כאן את היום בכנס משותף למדענים ישראלים וסינים  עוד  נחנתנו בשלום בבייג׳ינג מתחיל ביקור העבודה  יְהִי רָצוֹן מִלְּפָנֶיךָ יְהֹוָה אֱלֹהֵנוּ וֵאֱלֹהֵי אֲבוֹתֵנוּ שֶׁתּוֹלִיכֵנוּ לְשָׁלוֹם וְתַגִּיעֵנוּ  השבוע לפני שאברך אתכם בברכת שבת שלום המסורתית אני רוצה להגיד לכם מילה אחת תודה  יום המדע הישראלי הפך לשבוע של חגיגות מסיים אותו עכשיו בכינוס השגרירים הזרים שנמצאים בישראל כדי לספר גם להם על  יום המדע הישראלי הפך לשבוע של חגיגות מסיים אותו עכשיו בכינוס השגרירים הזרים שנמצאים בישראל כדי לספר גם להם על  קחו בבקשה שלוש דקות מזמנכם וצפו בקליפ המטורף שהכנתי לכם עם זוכי פרס נובל לכבוד יום המדע מקום ראשון במצעדים  יום מדע ישראלי שמח לנו מתחילים עכשיו בשורה של אירועים ופעילויות בחינם  בכל הארץ מציינים את פאר היצירה שלנו  תגידו כמה פעמים כבר אמרתי לכם שישראל היא מעצמה עולמית של מדע וחדשנות          הרבה נכון היום קיבלנו הוכחה  שבוע טוב מאוד חג שמח וKeep on running my friends   מתל אביב שבת שלום לכולכם וסופ״ש מצוין  Shabbat Shalom from Tel Aviv  איפה יהיו כולם ב  2 באפריל בשבע בערב כנסו לסרטון  ותדעו  איזה כיף לצאת מהופעה בפני אנשי היי טק באוניברסיטת תל אביב  ולפגוש את האישה שאיתי  ישראל מעצמת מדע וחדשנות דימונה מעצמת רובוטיקה וסייבר  אני מסיים עכשיו ביקור עבודה משמח מאוד בדימונה למה  לפנק לפנק                     בוקר אור יקיריי יום המדע הישראלי מתקרב ואנחנו מכינים לכם אירועים בכל הארץ   יקיריי לכולכם שבת שלום וסופ״ש מצוין מירושלים                                            Shabbat Shalom from  אני יהודי פשוט העיד על עצמו מנחם בגין                                   בצוואתו הורה לקבור אותו בהר הזיתים  ״הביאו לי את יהודי אתיופיה״ כך הורה ראש הממשלה מנחם בגין לראשי המוסד זמן קצר אחרי כניסתו לתפקיד ראש הממשלה   שלום לכם ממליאת הכנסת         הארכנו עכשיו את חופשת הלידה לנשים מ14 ל16 שבועות  עיתונאי באיזה סגנון אתה מתכוון להיות ראש ממשלה  בגין בסגנון יהודי טוב                   שבת שלום וסופ״ש מצוין לכולכם  Shabbat Shalom from Israel  כבוד השר זאת ישראל  עבר מפואר  עתיד גדול                                                    כך סיימתי את  אני גאה בדגל שלנו תמיד  ובכל מקום  אני מקיים ביקור עבודה קצר בשוויץ גם כאן המדע הטכנולוגיה והחדשנות  יש הרבה מאוד תשובות טובות לשאלה למה אני מתנגד למדינה פלשתינית אבל הטובה מכולן היא הכי בסיסית אין עם בעולם שמוסר  מאיתנו שבוע טוב מאוד לכולכם  בארץ אהבתי השקד פורח  השבוע עוד לפני הברכה המסורתית אני מזמין אתכם לצפות בראיון נרחב איתי בערוץ 20 החל  כל חיי התנגדתי למדינה פלשתינית                                  מאז שנבחרתי לכנסת אמרתי בכל מקום  לפני ואחרי  הערב הושם הקץ על פתרון שתי המדינות הצטרפו אליי עכשיו לשידור חי מאולפן מבט  מדעניות העתיד העתיד שלנו      הצטרפו אליי לשידור חי מהכנס השנתי של פרוייקט הדגל שלנו שמבטיח שישראל תמשיך להיות  יקיריי לכולכם לבני ביתכם לחיילינו הגיבורים והאמיצים בכל הגזרות ולכל אזרחי ישראל שבת שלום וט״ו בשבט שמח  בהתרגשות ובגאווה ליווינו  הבוקר את יהונתן למצוות  בבית הכנסת ״בית תפילה״ בשכונת שפירא בתל אביב שימש עובדיה  זה יום קשה לכל ישראלי שאוהב את ארצו  שאוהב את עמו  אבל זהו היום הקשה ביותר ל40 משפחות יקרות תושבות ותושבי  אני מייצג עכשיו את הממשלה בטקס לציון 25 שנה לחידוש היחסים בין ישראל לסין                   אבל הכי מרגש היה  יקיריי לכולכם לבני ביתכם לחיילנו ושוטרינו הגיבורים ולכל אזרחי ישראל  שבת שלום שבת מנוחה וסופ״ש מצוין   רס״ל ארז לוי הי״ד נרצח הבוקר על ידי מחבל מתועב  כשח״כים מסיתים בכנסת ומדברים על ״הכרזת מלחמה״ יש קנאים  רס״ל ארז לוי הי״ד נרצח הבוקר על ידי מחבל מתועב  כשח״כים מסיתים בכנסת ומדברים על ״הכרזת מלחמה״ יש קנאים  הם מחרימים  אנחנו קונים  לקראת סיום ביקור בבנימין אני נמצא עכשיו ביקב ״גבעות״ וקונה יין שמיוצר כאן היישר  אל תפחדו מההפחדות של השמאל                                          מצחיקים אותי אלה שאמרו לנו שאוסלו יביא  אומרים לי 70 מדינות התכנסו בפריז כדי לתמוך במדינה פלשתינית אז אני אומר להם הבוקר מירושלים יכולות להתכנס גם  גאווה של אבא לסופ״ש  102 במדעים אלא מה   לכם לבני ביתכם לכל חיילנו הגיבורים והאהובים ולכל אזרחי ישראל  מה אני אני רק בן אדםאני חי ועובד כמו כולם  בקיץ 1985 שמעתי לראשונה על מאיר בנאי  ואותו שירו של שפשף״  סוף להופעות ״שוברים שתיקה״ בבתי הספר  מליאת הכנסת אישרה עכשיו בקריאה טרומית את הצעת החוק שתאסור עליהם ועל  שיר חג׳אג׳ יעל יקותיאל שירה צור ארז אורבך הי״ד  כן כמו כל חיילות וחיילי צה״ל  של כולנו  יקיריי לכל אחת ואחד מכם שבוע טוב מאוד  לאור דרישת הקהל אני מצרף מסמך תקשורתי נדיר בארצנו ראיון מראיינת  לכולכם יקיריי מעדי וממני שבת שלום שבת מנוחה וסופ״ש מצוין  Shabbat Shalom from Israel  I posted a new video to Facebook  כל עוד אני בחיים הפוליטיים לאויב הפלשתיני לא תהיה מדינה  כדאי לכם לצפות בראיון המלא הערב בערוץ הכנסת 99  מה לא תראו הערב בחדשות   אז תצפו כאן שתפו והפיצו  גאווה ישראלית אמיתית בפתחו של השבוע  תגליות ופיתוחים ישראלים שהשפיעו על העולם  האלבום החדש שהשקתי בשבוע שעבר  שבוע טוב יקיריי וחג שמח  הסיפור האמיתי מאחורי הסרטון שמסעיר את הרשת עד כדי כך שגם חכ יאיר לפיד משתף אותו  בשמש שלפני הסערה                 לכולכם מאיתנו חנוכה שמח שבת שלום וחודש טוב מאוד  Shabbat Shalom and Happy  מירושלים שלום לך ג׳ון קרי ישראל לעולם לא תיסוג לקוי 1967 לעולם  Dear John Kerry from Jerusalem Before  בחג הזה אנחנו מרוויחים פעמיים משרד המדע מזמין את כל ילדי ישראל  בחינם  למוזיאון המדע ע״ש בלומפילד  אין עם כובש בארצו נקודה  ואחרי שנשאלתי מה יקרה אם יהיה מו״מ לשלום אז הרי נצטרך לוותר אמרתי אולי הם  לכם יקיריי לבני ביתכם לחיילנו האהובים בכל הגזרות ולכל אזרחי ישראל              שבוע מצוין וחג חנוכה שמח  בגאווה ובהתרגשות השקתי היום את הספר ״תגליות ופיתוחים ישראליים שהשפיעו על העולם״ שמבוסס על התערוכה הנהדרת בנמל  בעוד עיר שלמה בסוריה על אזרחיה וילדיה נמחקת                 בעוד באירופה הטרור שוב מרים את ראשו  בינתיים במליאה שרת המשפטים עושה קרניים לשרת התרבותאנחנו ממשיכים להצביע על התקציב אז שיהיה לכם לילה טוב  עם יד על הלב כמה מכם ידעו הכירו או שמעו על פעילות משרד המדע ואולי אפילו שאלתם את עצמכם למה הוא קיים  אני  ההחלטה עכשיו על הסרת החסינות של חכ באסל ראטס  הישג ענק לדמוקרטיה הישראלית הישג ענק למאבק הצודק שלנו נגד אלה  ח״כ באסל ראטס נשבע לשמור אמונים למדינת ישראל  ולחוקיה שיתוף הפעולה שלו עם מחבלים הוא לא פחות מבגידה    הצטרפו אלי למסיבת עיתונאים מיוחדת עכשיו במשרד המדע לחשיפת מסקנות הועדה המיוחדת בעקבות התפוצצות עמוס 6  50000 תודות  על 50000 לייקים   יקיריי לכולכם שבוע מעולה שיהיה אנחנו הולכים יחד כבר כברת דרך ועוד נכונה  לכולכם ממני שבת שלום שבת חמימה ושקטה וסופ״ש מצוין  From me to all of you Shabbat Shalom  טיבי דיבר במליאה על ״שותפות גורל״                                    אז הוא קיבל את התשובה הכי פשוטה והכי  את פרופ׳ עמנואל טרכטנברג אני מעריך ומכבד מאוד למרות חילוקי הדעות הפוליטיים ועל אף אי ההסכמות במגוון נושאים  עוד תקציבים לפריפריה עוד פעולה של הנגשת המדע והטכנולוגיה לילדינו האהובים  שלום לכם מירושלים שמח להודיע  שבוע מעולה שיהיה לנו                                זאת התמונה שהכי אהבתי ושהכי שמחה אותי מביקורי בהודו בכל  כמה טוב שבאתי הביתהכמה טוב לראות אתכם שוב                                                      אני תמיד גאה מאוד להיות ישראלי  השבוע אפילו עוד יותר  הסתיים ביקור העבודה בהודו עם קבלת פנים חמה מאוד  אני תמיד גאה מאוד להיות ישראלי השבוע אפילו עוד יותר  הסתיים ביקור העבודה בהודו עם קבלת פנים חמה מאוד לבבית  אני תמיד גאה מאוד להיות ישראלי השבוע אפילו עוד יותר  הסתיים ביקור העבודה בהודו עם קבלת פנים חמה מאוד לבבית  בוקר אור יקיריי בזמן שישנתם נמשך במלוא העוצמה ביקור העבודה בהודו עכשיו רק תביטו בתמונה הזאת ותבינו באיזו אהדה  עוד הסכם עוד מדינה מהדקת יחסים עם ישראל הערב במשרד המדע ההודי בניו דלהי חתמתי על הסכם נוסף לשיתוף פעולה  בהתרגשות ובגאווה אדירה חנכתי עכשיו עם שר המדע של הודו את תערוכת הישגי המדע והטכנולוגיה הישראליים במוזיאון  מניו דלהי בוקר טוב ישראל אני מתחיל יום עמוס וגדוש בפגישות וחתימה על הסכמים להעמקת שיתופי הפעולה בין ישראל לבין  ירושלים של זהב בכל מקום גם בהונג קונג  בזמן שישנתם פגישה לבבית וטובה עם שר החדשנות והמדע של הונג קונג  יְהִי רָצוֹן מִלְפָנֶיךָ יְהֹוָה אֱלֹהֵינוּ וֵאלֹהֵי אֲבוֹתֵינוּ שֶׁתּוֹלִיכֵנוּ לְשָׁלוֹם וְתַצְעִידֵנוּ  גם בחיים הפוליטיים תמיד כדאי לשמור על קור רוח                                           לכולכם יקיריי  תלמידי ״גימנסיה הרצליה״ בתל אביב לא רוצים את ״ההרצאה״ של אנשי ״שוברים שתיקה״ אצלם  כבוגר ״הגימנסיה״ אני אומר  המסע להודו מתחיל בירושלים  את ביקור העבודה על פי הזמנתו החמה של שר המדע ההודי אני אקיים בשבוע הבא  המציתים הם טרוריסטים            כשנמצא אותם  ותהיו בטוחים שנמצא  צריך למצות איתם את הדין במלוא החומרה  נס  לוחמי האש  תודה רבה לכם   ערב השבת העם כולו מודה מצדיע ומחבק את לוחמי האש שעומדים בחזית בימים אלה מול  אין לנו ארץ אחרת גם אם אדמתנו בוערת  מצדיעים ללוחמי האש משטרת ישראל פיקוד העורף וכוחות הביטחון שנאבקים בגל  תגיד לנו אתה תומך בשתי מדינות לשני עמים תגיד  אז מה אתם חושבים שלא אמרתי לחבריי האופוזיציה שאתגרו אותי היום  מקדם בברכה ובשמחה את מר לי מנג סגן שר המדע של סין שמבקר בישראל  ועידת החדשנות ישראלסין תתכנס בתחילת 2017  שבוע טוב מאוד יקיריי  אני רוצה לשתף אתכם בסרטון מיוחד ומרגש במיוחד שהכין ושלח לי יוני ברק שלא הכרתי עד  יקיריי לכולכם ממני שבת שלום וסופ״ש מצוין  Shabbat Shalom from Israel  כשפגשתי את בני הנוער הנפלאים בנצרת עילית  ראיתי את העתיד המזהיר של ישראל  מיטב הנוער מיטב המוחות  כדי  הדמוקרטיה לפי האופוזיציה שלנו היא טובה רק כשהם מנצחים כשאנחנו מנצחים אז תמיד תשמעו שהדמוקרטיה בסכנה   הבטחות צריך לקיים עמדות צריך לבטא בהצבעות ותמיד אבל תמיד לדבוק באמת שלך ולהיאבק עליה  היום לפני שאאחל לכם שבת שלום אני מבקש להגיד לכם מילה אחת תודה                  תודה על התמיכה על המילים  Congratulations Mr President Elect The American people have spoken The alliance between Israel and the United  עוד ביקור חשוב עוד שיתוף פעולה מדעי ומדיני עוד הערכה והשתאות להישגי ישראל  נפגשתי הערב בירושלים עם שר  יקיריי שבוע טוב מירושלים  ממשיכים לעבוד בשבילכם  יקיריי לכולכם שבת שלום וסופ״ש מצוין  Shabbat Shalom  מה יהיה כבר עם הבידוד המדיני הנוראי שהממשלה הזאת הביאה אותנו אליו   במשרד ראש הממשלה בירושלים חתמתי עכשיו  מסיים ביקור עבודה בקרית מלאכי כתמיד השמחה הכי גדולה היא לראות את הילדות והילדים שלנו נהנים מפעילויות משרד  מתחילים את מושב החורף    ברגל ימין כמובן   לכולכם מאיתנו שבת שלום וסופ״ש מצוין  Shabbat Shalom from Israel  הסתיים ביקור עבודה מוצלח מאוד ברוסיה ואני יוצא בחזרה הביתה לארצנו היפה והטובה שאין כמותה בכל העולם  ירושלים היא בירת ישראל לנצח כמו שמוסקבה היא בירת רוסיה  ואין על זה ויכוח  כך התחלתי את פגישתי  עם סגן ראש  ברכות מישראל אומת ההיי טק והחדשנות  התחלנו ועידת החדשנות במוסקבה  בדרכי לועידת החדשנות הבינ״ל במוסקבה  זאת הזדמנות מצוינת להציג בפני מאות יזמים מדענים אנשי היי טק וטכנולוגיה  שישו ושמחו  בשמחת תורה  לכולכם מאיתנו חג שמח  עוד יש מפרש לבן באופק      כל שתבקשו  לו יהי  יקיריי לכולכם לבני ביתכם לחיילנו הגיבורים והאמיצים בכל  תודה לך צ׳כיה                        שוחחתי עם איוו שוורץ שגריר צ׳כיה בישראל והודיתי לו על החלטת הפרלמנט </t>
+    <t xml:space="preserve">michaeldvorin aviadglickman הייתי שמח לראות את התצהיר של הגב בן ארי כשקיבלה טופס 4 גליקמן אתה יכול לעזור לי להשיג אותו סעיף 239 ל… Roadrun86259229 michaeldvorin ErelSegal aviadglickman ״פיצול לשעתו״ mosheifargan זהו כרגע ברור לחלוטין שליאת בן ארי לא יכולה להיות אוכפת חוק בכלל ובטח לא לכהן בצמרת של אוכפי החוק אין לה שום תוקף מוס… aviadglickman הייתי שמח לראות את התצהיר של הגב בן ארי כשקיבלה טופס 4 גליקמן אתה יכול לעזור לי להשיג אותו סעיף 2…  rothmar וזה ממשיך  האירוניה הוסיפה ארבע קומות לא חוקיותפרגולה לבית שלה פיצלה לעשרים דירות עלתה למעלה וקפצה אל מותה  אומר  ועושה לה הנחה  rothmar ואז ליאת בן ארי טענה שמדובר באכיפה בררנית  וזהו דוקטור יותר אני לא זוכר כלום  dwwido AmirHaskel האיש מאיים על מפקד משטרת ירושלים יש מאחריו פרקליטות יועץ משפטי בג״ץ YanivTurgi אני מתנגד להפגנות בבלפור ולכל התקהלות המונית בעת הזאת הכל כולל הכל מי שרואה את הסרטון הזה מבני ברק ושותק כשהתחלואה בישראל… michaeldvorin ערימת חדלי אישים  היא קוראת לנו הגברת הזו giladzw בהמשך לציוץ הקודם מצורף שרשור מאיר עיניים המספק הסבר מקיף אודות הפשע של מדליפי פרטיו האישיים של טראמפ כמו גם העובדה כי הסיפו… michaeldvorin גמר חתימה טובה גידולי פרא שלי emilm313 כמה חבל שגם היא הודתה כבר שכשלה בלשונה תתעדכן גמר חתימה טובה גידולי פרא שלי giladzw והיום בפינת שמאלפלורליסטיאוהב אדם  גו ביידן בהשוואה מחליאה בין טראמפ לשר התעמולה הנאצי הוא סוג של גבלס   אין ספק שגב… Irisleal15 כתבת חברי ליכוד יקרים אני ועוד 120000 חברי ליכוד אם התכוונת לשרי ליכוד יקרים היית כותבת את זה אני…  JackPosobiec Democrats in panic mode ערימת חדלי אישים  היא קוראת לנו הגברת הזו  michaeldvorin הבנתם הם העלו למדגרת קורונה גם בת 88 אוכלוסיית סיכון אא בואו נזרום איתם ונניח לרגע שמפגיני בלפור חסינים לגמרי מהמגיפ… MidaWebsite אחרי הסערה הגדולה בימין mosheifargan מפרק בשקט את המשנה הפשטנית והטהרנית של קלמן ליבסקינד gtgt  YaaraZered לקחתי על עצמי החל מהשבוע לראיין בכל שידור שלי אנשים שאיבדו את היקר להם מכל בגלל הקורונה מוזמנים להפנות בפרטי מרואיינים שיר… michaeldvorin רק שתבינו מה זה שמאל אנרכיסטי navedromi פתאום נפל לי האסימון שזה שדובר צהל לשעבר משווה את המחאה הזאת לסוג של מלחמת שחרור יכול להסביר חלק מהדברים שעברו על הצבא בע… MidaWebsite המחאה נגד המנותקים הפכה בעצמה למפגן מפונק של ניתוק והפקרות gtgt  noamfathi כתבתי את התיקון הכללי   נסיון לתקן את מה שנשבר בין קלמן לגידולי הפרא שהם לא עיתונאים ברמה של קלמן ערב יום הכיפורים… רק שתבינו מה זה שמאל אנרכיסטי  הבנתם הם העלו למדגרת קורונה גם בת 88 אוכלוסיית סיכון אא בואו נזרום איתם ונניח לרגע שמפגיני בלפור חסינים לגמרי מה…  tadmorerez48 האמת היא שאני מתבאס להתעסק עם הרפש הזה דקה לפני כיפור אבל מכיוון שכדברי מארק טווין השקר מספיק לעשות את דרכו סביב חצי עול… amirivgi הסיבה לקורונה האזינו  liyaomer עוד נצחון כזה ואבדנו כשראש המפלגה שלך קורא למרד בפועל לא פלא שאתה כחרפה שאתה מתנהג כמו שאתה מתנהג fischlerpini תת ניצב גיא ניר שהצביע על שחיתות במשטרה ובין השאר הביא לפרישתו של ניצב רוני ריטמן מבקש לבטל את הסכם הפרישה שלו שלפיו… YanivTurgi היות ואני חסום אצל מייסדת הפקולטה להנדסת התודעה אשמח אם מישהו ימסור לה שהמשטרה קבעה שהנהג שנעצר אינו התכוון לדרוס דבר ש… arielschnabel מסתכל על התמונות מבלפור ומרחם על השוטרים ובני משפחותיהם המפגינים מכניסים את עצמם לסכנה במודע ובלב שלם אבל למה לשוטרים… SteveGuest Joe Biden says he got to the Senate 180 years ago    MiriBarbi ראשוני  אל תצאו החוצה   תראו מה קרה לאלי אבידר  ivgiz זו אותה מדינה כאילו  michaeldvorin BarakRavid KalmanLiebskind וואו יש עוד הרבה כמותם מה תעשו מר רביד Mcohen1234 hadarse הוא חסם אותי הדר סגל תני פה צילומסך שנראה מה כתב michaeldvorin shu3809 tadmorerez48 2 אי פעם יוכל מנהיג המחנה הלאומי להיות בשלטון בלי להיות משועבד לצד השני נתניהו עשה טעה רבות בנ… michaeldvorin shu3809 tadmorerez48 1 לא חושב שיש מישהו רציני שעוסק במאבק המורכב מאז 2016 שנקרא פרשות נתניהו שהמחשבה אם הוא צריך… dovikco iairLevy  iairLevy כעת בבלפור צפיפות מטורפת תוך כדי שהמפגינים רודפים אחרי השוטרים ודוחיפים אותם  amitsegal אבי בבקשה תמחוק את הציוץ המופקר הזה היית תת אלוף בצבא שדיבר על ממלכתיות וציות  bardugojacob אשכנזי תראה מה כותב היועץ שלך בצבא תא״ל בניהו בנוגע למפגינים ״ושמים את טובת המדינה לפני טובתם נוחיותם ובריאותם זוהי… YinonMagal טוב הגיעה התוצאה יש לי קורונה🤦‍ המזל הוא שהחום כבר ירד כמעט לגמרי ואני מרגיש טוב בהרבה ומקווה שזה מאחורי הבאסה היא שא… michaeldvorin noamfathi תוסיף בוויקיפדיה michaeldvorin מרד  הכל בסדר איתו michaeldvorin סגר rafiperlshtein עזוב בוא  אי אפשר להבין אחרת את מה שאמר bnyiroz עצוב ומזעזע אין מילה אחרת  RubiYona פחות מ24 שעות לכניסת כיפור   1 הכותל ריק 2 אלפי אנרכיסטים מתפרעים בעיר הקודש noamfathi לפני עוד יום שידורים מיוחד ופריצות מהפגנת הפריבילגים תזכרו 1196 מנדטים של ישראלים מצביעי ליכוד לא ליכוד ביבי לא ביבי… bnyiroz אתם רואים כאן שמירה על ההנחיות ריחוק מסכות כי אני לא וניסנקורן אומר שהקרונה לא קשורה לבלפור  anatnh שר המשפטים במדינת ישראל 2020 החרדים והערבים הם מחוללי הקורונה  MidaWebsite הנאום של שר המשפטים האמריקני ביל בר לא קל הוא לא עושה הנחות והוא לא מתנחמד אבל הוא כן מדגים מהי מנהיגות משפטית ואיך צרי… סגר  shlomokarhi כספית לא מגלה שהמפגש הזה היה ביוני כאשר בבית קפה מותר היה לשבת ולאכול ללא מסכה ושאם הייתי צריך לומר בסוף בבת צחוק גייס… BarashiKinneret ראש הממשלה ניהל את המשבר לבד בממשלת מעבר היום הוא תקוע עם יור ועד מפגינים חומה בצורה למנדלבליט והנחיותיו ההזויות שתפ… noamfathi תוסיף בוויקיפדיה noamfathi גם ברק רביד הצבוע יחטוף כשצריך michaeldvorin tadmorerez48 אגב למרות ביקורתי על מאמרו האחרון של קלמן להבדיל ממאמרו הקודם חייב להבהיר שקלמן יצא פעמיים נגד מעסיקיו… arisade94 קראתי תכתובת וואטסאפ של מפגינים היום והפסקתי להתעצבן אנחנו נישאר ספונים בבתים לא נפגוש את סבא וסבתא נצא רק לקנות אוכל תר… מרד  הכל בסדר איתו  IlanAharon שים לב ותבדוק אותי אני לא אמרתי מילה על המאמר שלו משבוע שעבר זו דעתו וזה לגיטימי אף שאיני מסכים איתה…  MatiHBL לא הבנת ביזו קלמן זלזל באחוזי המיקרופונים שהם היחידים שמהדהדים את הסיפורים שלו ומה אמור לקרות עכשיו ברק רביד יהדהד אותם ElkyBergstein אז שאבין כל המדינה בסגר וחבורת הפריבילגים הזאת יוצאת מתי שבא לה ועושה מה שבא לה MotTal נועם פתחי חושף את הצביעות של ברק רביד באולפן וכמובן ברק רביד לא מסוגל להשתלט על עצמו ומקלל את נועם פתחי  אלה הפנים האמיתיות… ivgiz פייסבוק בדק ומצא  ItsikSaban חובת צפייה  המפגינים רוצים אלימות הם רוצים להתפרע הם רוצים לשרוף את המדינה קדימה עיתונאים קדימה תעשו לזה יחסי ציבו… michaeldvorin לא יודע אם עתונאי או סדרן הפגנות michaeldvorin YotYotam שמע פתחי ניגב איתו את הרצפה זה היה מרהיב לוינסון תמיד תחמם את פתחי לפני שידורים YotYotam שמע פתחי ניגב איתו את הרצפה זה היה מרהיב לוינסון תמיד תחמם את פתחי לפני שידורים ivgiz נראה שהם לא שומרים על מתווה הקפסולות YotYotam אין דבר יותר מצחיק מלראות שמאל רדיקלי ישראלי מנסה לשכנע שמאל רדיקלי אמריקאי לא להחרים את האזכרה של רבין  לא יודע אם עתונאי או סדרן הפגנות  DrEliDavid OshryAlk geektimecoil נהדר בדיוק קראתי על זה אלי mclbgn ובינתיים בפיד שמאל דיון סוער האם רבין מחבל כמו ערפאת או סתם מיליטנט קולוניאליסט כובש ואלים אללה ירחמו איזה ממשיכי מורשת השאי… YotYotam חחח מה זה יש להם מחולל גנרלים  hkim14050017 אכן עסקו בכך והיו היחידות שעשו כן אבל הן עסקו רק בזווית של ההתנכלות לצ והנושא לא קיבל את התהודה המג…  hkim14050017 ציפורי הוא בוודאי עיתונאי עם רקורד מרשים של עשרות שנים שמעטים העיתונאים בוודאי בעיתונות הכלכלית שאוחז…  hkim14050017 כן מאז גלנט לפני עשר שנים היו לו עוד כמה תחקירים לא זכור לי שאפילו אחד מאלה האחרונים והמדוברים שלו…  Forever21Israel chaimlevinson יש כל מיני מדדים בעולם הפרסום בסוף אם ניקח את הפרסומת של 9 מליון או של אסי כהן עם…  hkim14050017 הם לא עיתונאים הם אנשי תקשורת מגישי תוכניות אקטואליה פובליציסטים וכיוב כשהוא פרסם סיפור הם קידמו…  shu3809 tadmorerez48 2 אי פעם יוכל מנהיג המחנה הלאומי להיות בשלטון בלי להיות משועבד לצד השני נתניהו עשה טעה רבו…  shu3809 tadmorerez48 1 לא חושב שיש מישהו רציני שעוסק במאבק המורכב מאז 2016 שנקרא פרשות נתניהו שהמחשבה אם הוא צ…  tadmorerez48 אגב למרות ביקורתי על מאמרו האחרון של קלמן להבדיל ממאמרו הקודם חייב להבהיר שקלמן יצא פעמיים נגד מעסי…  michaeldvorin מה שקלמן עשה מזכיר לי את פרק החתונה האדומה במשחקי הכס אלא שקלמן שכח שאלה שעליהם התגולל הם אלה שנשאו את הסיפורים שלו… giladzw חשיפות מטלטלות בארהב  1 חוקר לשעבר בצוות מולר מאשר לראשונה לא היה כל בסיס לחקירת הקנוניה בין טראמפ לרוסיה  עד לרמה שהחוק… oferdann chaimlevinson אבל לוינסון כתב הוא קופירייטר כושל דבר שאיננו נכון לכן לוינסון צריך למחוק את הציוץ הזה ו…  מה שקלמן עשה מזכיר לי את פרק החתונה האדומה במשחקי הכס אלא שקלמן שכח שאלה שעליהם התגולל הם אלה שנשאו את הסיפורים…  chaimlevinson חיימקה תבדוק את עצמך כשאתה אומר קופירייטר כושל ותריד את הציוץ הזה הקריירה של פתחי בתחום הקופיריטריו…  michaeldvorin סוף מעשה במחשבה תחילה  נכון תמיד ביתר שאת כעת  בעולם המשפט אומרים מעולם לא הצטערתי על תיק שלא לקחתי  על אותו משקל א… YotYotam זה לא נגמש אחי זה בימבה hofitsh מה השורה הזאת למטה זה ציטוט של מישהו הוא גחמה של העורך  michaeldvorin מעניין מה ליאורה גלאט ברקוביץ חושבת על ההערות האלה של קרא על איכות המקצוע מעניין מה ליאורה גלאט ברקוביץ חושבת על ההערות האלה של קרא על איכות המקצוע  michaeldvorin זה נהדר כמה שזה מכוער YotYotam רואה את דני קושמרו הדרמטי עם השקף של מחדל יום הכיפורים בפתיחת אולפן שישי ונזכר בדני קושמרו הפחות דרמטי שעמד בסוף הגל הראשון… MeirRubin זה לא משנה אם הממשלה נכשלה או לא ומה עושים אחרים  אל תכנסו למקומות סגורים כרגע עם מישהו שאיננו ממשק הבית שלכם אלא אם זה ה… yairkraus חכ אלי אבידר קורא למרד המונים ומספק הצצה מדאיגה למאחורי הקלעים של ההפגנות תגיעו לבלפור במוצש בשיירות שכל המדינה תהיה חס… Machlufb BarakRavid KalmanLiebskind דיבה BarakRavid KalmanLiebskind וואו יש עוד הרבה כמותם מה תעשו מר רביד סוף מעשה במחשבה תחילה  נכון תמיד ביתר שאת כעת  בעולם המשפט אומרים מעולם לא הצטערתי על תיק שלא לקחתי  על אותו מש…  dovikco מהדורות חדשות שהביאו את יורם לס שאמר שזאת ״רק שפעת״ ואת עידית מטות שסיפרה לנו שבכלל אין גל שני ואת אירה דולפין כדי לקדם אנר… mclbgn וואו נשמות אם תקשורת המיינסטרים ושאר שופרות הדיפסטייט היו עושים פולואפים לקלמן על החשיפות שלו של מערכת המשפט כמו שהם מהדהדים… liyaomer חחחחחחח רק אחרי שקלמן כתב ביושר עיתונאי את מה שבניהו מצפה ממנו לכתוב  יקרא כעת האדון בניהו את טוריו של קלמן על מערכת המשפט… זה נהדר כמה שזה מכוער  ErelSegal אמנם אני חמור זקן שראה הכל אבל הוא איתי שם תמיד הילד שהוריו התגרשו  גירושין מכוערים מאוד  קרוע בין אמא לאבא ואחרי שהצטער… JoeS15128922 rothmar Riklin10 tadmorerez48 bardugojacob YaaraZered שמחה הבין היטב מה כתבתי rothmar Riklin10 tadmorerez48 bardugojacob YaaraZered תבין  כשאתה אומר שאתה אוהב את האמת יותר אתה מאשים את כ…  rothmar Riklin10 tadmorerez48 bardugojacob YaaraZered במילה אחת אכזבה בשתי מילים חוסר תבונה RonelAdani rothmar Riklin10 tadmorerez48 bardugojacob YaaraZered כשאני רוצה לדעת מה זו אשפה אני הולך לפיד שמ…  rothmar Riklin10 tadmorerez48 bardugojacob YaaraZered שמחה יקירי כל האנשים המנויים ברשימתו של ליבסקינד הם הם ה…  YoavBlum דיבה tadmorerez48 לפני שבוע הציוץ הזה היה נראה לרבים מוגזם דומני שעכשיו רבים יותר מבינים את כוונתי תגובה מנומקת לגידופי קלמן תפורסם בשבוע… michaeldvorin מתי אתה יודע שהלכת צעד רחוק מדי כשהצד השני משתמש במה שאתה כותב כדי לקדם את האגנדה שלו קלמן ראה איך הפכת לכלי משחק בי… michaeldvorin שישאל את קרן ווקסנר michaeldvorin RavivDrucker amitsegal רביב יא עיתונאי דגול שכמוך כבר למדת את החומר על התאגידים שלא הואשמו בתיק 4000 או שאתה זקוק ל… שישאל את קרן ווקסנר  RavivDrucker amitsegal רביב יא עיתונאי דגול שכמוך כבר למדת את החומר על התאגידים שלא הואשמו בתיק 4000 או שאתה זקוק לעוד כמה חודשים mosheifargan תגידו לי רק באיזו רפובליקת בורקס דובר משרד המשפטים כותב דבר כזה בפומבי והוא נותר בתפקידו איזה כשל מערכתי צריך לקרות כדי… מתי אתה יודע שהלכת צעד רחוק מדי כשהצד השני משתמש במה שאתה כותב כדי לקדם את האגנדה שלו קלמן ראה איך הפכת לכלי משח…  NoamUrbach אני לא בטוח שאתה רוצה את מה שקורה בארהב בתחום הקורונה YinonMagal שלום קלמן הבנתי שמפריע לך שגדלו בימין גידולי פרא לא עיתונאיים תגיד  מה לגבי דוברי הפרקליטות דוברי כחול לבן דוברי מרץ שממ… YanivTurgi זכותך לחשוב שאתה העיתונאי הכי טוב בישראל קלמן העובדה שבחרת לחלק ציונים לאנשי תקשורת ממחנה הימין וללגלג עליהם היא לא לזכו… michaeldvorin טראמפ בדרך לפרק את ביידן smadarshmueli איך פרופ גמזו לא רוצה סגר עם 59 הלוויות ביממה לאן הוא רוצה להגיע טראמפ בדרך לפרק את ביידן  yoavgallant כך נראה עולם הפוך בשעה ש25 מיליון תלמידים בישראל נאלצים להסתגר בבתיהם בשל הנגיף  מאשר היועמ״ש לממשלה בלחץ כחול לבן ה… bardugojacob במהלך ממשלת הרוטציה נאלץ ב1986 שר האוצר יצחק מודעי מהליכוד שכינה את שמעון פרס ראש ממשלה מעופף להתפטר  ניסנקורן מפגין… ronitlev12 רק לחשוב על זה שבני גנץהצבי של הדואר היה רמטכל יאיר גולן כמעט וכרמי גילון ראש השבכ ועוד והמדינה עדיין עומדת על תילהחו… dovikco סיכום ההצהרות בערב הזה  נתניהו אנחנו במשבר חירום לאומי   לפיד רק לא ביבי  גנץ אני יכול ללכת להשתין רגע michaeldvorin natitucker טוקר מה אתה יודע אני מוכן אפילו לשקול לייצג אותך אם יש לך מספיק כסף לשלם לי igalmalka לגמרי natitucker טוקר מה אתה יודע אני מוכן אפילו לשקול לייצג אותך אם יש לך מספיק כסף לשלם לי moris1hakimi קרוב משפחה שלי חולה קורונה במצב קשה שתי ריאותיו קרסו אנא מכם תפיצו ותבקשו רפואה שלמה עבור יצחק בן טאג׳י תבורכו giladzw שמעתם שהבן של טראמפ קיבל 35 מיליון דולר ממיליארדרית רוסיה המקורבת לפוטין  אה בעצם מדובר בהאנטר ביידן הבן של גו ביידן הא… ErezZadok1 אכתוב את זה ברור כל מי שטוען שאין הדבקות במסיבות הקורונה המופקרות בבלפור הוא  או מטומטם או שרלטן YinonMagal ומה שהכי מקומם במאבק של כחול לבן להשאיר את ההפגנות ולא תשמעו על כך הוא שמדובר פשוט בשיקולים פוליטיים לבייס מדומיין שאגב ב… ivgiz תסמיני הקורונה חום בלבול קשיי נשימה ולהצהיר בסקר שאתה מצביע לשאשאביטון YoavNews1 מה ניתן ללמוד מהתייצבות בכירי כחול לבן לצד המפגינים בבלפור למרות הסיכונים הרפואיים השנאה לנתניהו וכמיהתם לסילוקו גדולים מר… arielschnabel אז עכשיו ניכנס לסגר חונק במיוחד רק כי זו הדרך היחידה להגביל הפגנות הקנאות המטורפת של קיצוני בלפור בסיוע דחלילי כחל״ב ב… YanivTurgi שתול ביביסט    Shiritc פרופ ברבש לחכ שאשא ביטון בחדשות 12 הוויכוחים שאתם מנהלים בוועדה אני לא רוצה להגיד נוגעים בהכחשת קורונה מערערים את אמון הצ… GadiTaub1 כדור הארץ לדגלים השחורים האם שומעים עבור elicoh1 ההתאבדות של חברי כחול לבן על קיום ההפגנות היא פשוט בלתי נתפסת המגיפה מתפשטת בכל העולם אנשים מאבדים במקרה הטוב את מקום עבודתם… YinonMagal כמו שטענתי השיקולים של כחול לבן בשעה קשה זו הם פוליטיים בושה amitsegal טרופר איך קרה שכחול לבן נותנת גיבוי לקולות הקצה אנחנו אמורים להיות הקול הממלכתי  nadavabeksis הרגע דיברתי עם קובי יעקובי מפקד תחנת מוריה חבר מהצבא אח נדבק בקורונה סליחה לא נדבק חולה חום חולשה כאבים כל התס… ShelleyWallach הישג אדיר כלכלי וגאו פוליטי לישראל נחתמה חוקת פורום הגז האיזורי החתימה גם מאפשרת את הקמת הארגון שבמסגרתו יקודם פרוייק… YossiFuchs שאלה לי ליועץ מנדלבליט אותה ממשלה בראשות נתניהו וישראל תחת מתקפת טילים משולבת מצפון ומדרום וכל תושבי המדינה במקלטים או בממ… Yossieli אין נתונים על הדבקות בהפגנות בבלפור אז קבלו פרסום ראשון מפקד תחנת מוריה בים ניצב משנה קובי יעקובי האחראי בשטח על אירועי… akibigman אגב השאלה אם איילת שקד מתווכת לעיתונאים פגישות או מסרים ממנדלבליט בנוגע לפרישה של נתניהו הרבה יותר מעניינת וקריטית מהשאלה א… yitzhak55 שלא תדע צער YinonMagal ראש הממשלה הולך הכי חזק נגד הבייס שלו וסוגר את בתי הכנסיות ביום הקדוש ביותר בשנה וכחול לבן כחול לבן כהרגלם במין פיינשמייק… omeryankelevitc עם 6700 נדבקים ביממה הגיע הזמן לומר די לדמוגוגיה למפגינים בדיוק כמו למתפללים  אין שום חסינות מהדבקות אותם כללי… moxypen500 אבא שלי נפטר כשפרש לגמלאות תיכנן לטרוף את העולם באה הקורונה וטרפה אותו אבא שלי לא הלך להפגנות לא הלך לים לא הלך למסעדו… liyaomer תקשיבו רגע כל מטורללי השמאל בראשות פקיד ההסתדרות  אתם באמת חושבים שההפגנות רעות לנתניהו ולכן הוא רוצה לאסור אותן בחיי שאתם… RanBaratz כחוללבן דבקה במשימת ההגנה על ההפגנות באופן מרשים מאוד לא זכור לי מפגן כזה של אווילות בו מפלגה שטוענת למרכזיות וממלכתיות… YanivTurgi עכשיו זה רשמי אביחי מנדלבליט מכהן גם כיועץ המשפטי למחאה filbers מדינה שלמה הולכת לסגר מלא מלא בגלל שניסנקורן התעקש 3 חודשים על ההפגנות מלא מלא טוב בהסתדרות רגילים שכל יור חדש שנבחר… itzikbam אני לא מבין למה התפקיד שממלא דר מנדלבליט נקרא היועץ המשפטי לממשלה לדעתי יותר פשוט ויותר מדויק לקרוא לתפקיד הזה ברוח הימי… hbsela ErelSegal  שומע את השיחה המרתקת עם itzikbam  יש לי הצעה ל michaeldvorin  אולי תנצ ניר ורפק צ יעברו  יושאלו לשרת במחש… avribloch המדליף לכאורה אל תוכנית המקור נחשף במזכר סודי  עד המדינה ניר חפץ מספר לחוקריו כי אילנה דיין אמרה לו שעד התביעה בתיק 4000… dovikco אז מנדלבליט עוד פעם נתפס משקר  לא הופתעתי ככה מאז הפעם הקודמת שמנדלבליט נתפס משקר liyaomer איך שגלגל מסתובב לו פעמיים במסמך אחד והמבין יבין  mosheifargan לימור לבנת הקשיבי הכל משתנה העולם בני אדם מוסדות וגם  מפלגות הכל בתנועה מתמדת לא מתאים לך הליכוד של היום מצאי מפל… tzvitessler עמוס גלזר זל נהג דן היקר שהיה כולו חסד ונתינה  בזכות הנסיעות איתו הפכנו לסוג של משפחה כל חייו התגעגע לבנו תמיר זל שנ… fischlerpini  amitsegal רק דת אחת בעולם כולו דורשת את המשך הפולחן גם במחיר חיי אדם הדת היא רק לא ביבי ופולחנה  הפגנה שבועית בבלפור GadiTaub1 אני אתרגם לכם לעברית את הצעתו של קלמן ליבסקינד שנתניהו יפרוש תמורת ביטול ההליך הפלילי נגדו המלצה להיכנע לרעיון שהפקידות יכו… LiberalRiWo בריטניה נוקטת בהגבלות שיהיו בתוקף עד חצי שנה עוד צעד של נתניהו לדחות את משפטו liyaomer כל עוד יהיו הפגנות לא יהיה כאן סגר חברי הכנסת האנרכיסטים שממשיכים לדחוף את ההפגנות שרי כחול לבן שנראה שזו כל מטרתם עלי אדמו… BarashiKinneret דובר משרד המשפטים מוציא תגובה שיקרית  ל natitucker ואומר שמנדלבליט מעולם לא ביקש להיפגש עם Riklin10 ובכן להלן גרסת… fischlerpini תת ניצב גיא ניר עושה להם בית ספר חשבו מתעסקים עם פראייר ומקבלים פייט מהסרטים haskioren michaeldvorin MatanKahana הלך להתייעץ עם בנט michaeldvorin MatanKahana צרצרים ממר כהנא MatanKahana צרצרים ממר כהנא GuyBechor דבר כזה עוד לא ראיתי חשוב להפיץ נגד כל שונאינו  GadiTaub1 הם רוצים עוד קורונה אין שום הסבר אחר אם לא הם היו נוהגים באחריות ודוחים את ההפגנות לאחרי הסגר שום דמוקרטיה לא נפלה בגלל… BarashiKinneret YanivTurgi TopazLuk איזה פיצלה תתקן בנתה דירה בניגוד לדין שהשיגה במרמה ולא שלמה עליה מס שמחתי לעזור YotYotam כתבה שלמה ומוצדקת על אוטובוסים של חרדים שחזרו אתמול מהפגנות באוטובוסים ומה עם החברה האלה אוקיי בהפגנות אין הדבקה כי… yotameyal הרבה בריאות dogly1900 בוא נראה כמה מסיכות אתם יכולים לספור בוידאו הזה   yossidavidov10 ובכן ברדוגו מטמטם את זהבה גלאון  bardugojacob בכירי מפלגת העבודה פרץ ושמולי פותרים את מגיפת האבטלה בקלות  בנט פותר את מגיפת הקורונה והאבטלה בקלות  שאשא ביטון לועגת ל… mosheifargan אם אנשים שהציעו את ראשו של נתניהו ורמיסת בחירתנו תמורת עסקה קיבלו לפניכן תדרוך ממנדלבליט הרי שלכאורה מדובר באחד האירו… michaeldvorin ReutBitton מוסר תשלומים לעורכי דין חייבים לכבד את זה ReutBitton מאיזו מבחינה לא יכול מאיפה לו לדעת מה מקור הכסף YaaraZered מוזר על המחאות הם לא דיברו רק בתי הכנסת מפריעים להם כמעט מפתיע  ReutBitton מוסר תשלומים לעורכי דין חייבים לכבד את זה YanivTurgi עלינו על מוקש צעק אז הפצוע עזוב מוקשים עכשיו לך לעסקת טיעון השיבו לו עיתונאים מהציונות הדתית liyaomer ארבעה עיתונאים בכירים קמו בוקר אחד והחליטו לכתוב בשינויים קלים את אותו הטור כולם מצאו את אותה התרופה לקורונה כולם החליטו… michaeldvorin MatanKahana לא הבנתי מתן אתה לא מכיר את הפעילות של הקרן לישראל חדשה לא מכיר שוברים שתיקה לא מכיר שלום עכשיו אתה לא… mosheifargan מה מה קורה כאן מי עוד נפגשו עם מנדלבליט מי פנה למי חייבים את כל הפרטים בלתי נסבל מה שקורה כאן mosheifargan תגידו לא מוזר שנושאים עיניים אל המנדלבליט בעניין חקירת ההדלפות כשסימן השאלה שעולה אצל רבים הוא שהוא עצמו נטל בזה חלק ל… mosheifargan שמרתי את זה כדוגמאות לכך שמדובר במידע שלא יכול להגיע מגורמים מחוץ למערכת מה אומרים  MatanKahana לא הבנתי מתן אתה לא מכיר את הפעילות של הקרן לישראל חדשה לא מכיר שוברים שתיקה לא מכיר שלום עכשיו את…  michaeldvorin נראה שמתווה ההפגנה בקפסולות שעשו כדי לאפשר את מימוש הזכות להפגין במדינה דמוקרטית עובד נהדר ואתם אמרתם שפקידות משפטית מ… iairLevy האנרכיסטים מהשמאל הקימו אוהלים במרכז הכביש בבלפור בכוונה להקשות על השוטרים את הפינוי </t>
+  </si>
+  <si>
+    <t xml:space="preserve">הנה פילוח התחלואה בקורונה לפי נתוני הצבעה מצביעי יהדות התורה ש״ס והליכוד מובילים בגאון את רשימת הנדבקים החדשים בק…  נשיא שלא שילם מס הכנסה 20 שנה וראש ממשלה שלא מסתובב עם ארנק 20 שנה מובילים את המדינות שלהם לאסון  מקריות מדהימה hadarse תודה הדר ניפגש מחר בירושלים תהליכים 2020   כמו במדינות הכי אפלות נתניהו יהפוך את מצב החירום לקבוע   הערב בראש העין מחר בירושלים  אל תאמינו לרגע לאומרים ש״חוק ההפגנות״ יהיה זמני כמו בכל משטר אפל מה שמתחיל כזמני נמשך לנצח  תגיעו מחר בהמוניכם ל…  razshlomo חתן פרס נובל פרופ ישראל אומן בראיון לנחום ברנע  שיקוף המציאות כפי שהיא ולא הדהוד מסרים מסיתים ושקריים של שלטון מושחת בשנה החדשה הזו ישראל חייבת לחזור לבסיס  אמת…  במקום לדבר על העלות הכלכלית המטורפת של הסגר תקפו את המפגינים  במקום לעשות את תפקידה ולדבר על מה שחשוב התקשורת ת…  אתמול ערוץ 12 נהג כמנהג מיקי זוהר והילה אסנת מארק ותקף אותם במקום לדבר על הסגר המופרע שאנחנו נכנסים אליו תקפו את…  וחדשות 12 משתפים איתו משום מה פעולה תבינו בשבועות האחרונים כל התותחים הכבדים של בלפור הופנו נגד המפגינים ונעשה כ…  אתמול ערוץ 12 עשה אתמול מעשה שלא יעשה  הצגת תמונת המפגינים מול תמונת רחבת הכותל הריקה היא חזרה נוספת על הספין השקר…  17 כשל הזנחת מערכת הבריאות  כל השאר ספינים שקרים ותקשורת שמשתפת איתם פעולה  חושבים על עוד כשלים תכתבו בתגובות 10 כשל העברת הטיפול לפיקוד העורף ולצה״ל 11 כשל יציאה לא מבוקרת מהסגר הראשון 12 כשל אי מינוי גורם מקצועי בשלב מ…  כשלי הממשלה 1 כשל הפעלת מערכת החינוך 2 כשל הטיפול בעסקים קטנים 3כשל הטיפול בעולם התרבות 4 כשל הטיפול בעולם…  בצלאל בני איש אחד  אנחנו והערבים מאותו מקור אברהם אבינו הוליד שתי אומות אם אתה קורא לפיוס הזה  אני איתך לצידך…  תפגינו אל תוותרו אל תשתקו המדינה היא שלנו ולא של נתניהו  תהליכים 2020   הליכוד  וימינה חוברים יחדיו כדי לשלול את זכותנו להפגין גם אחרי הסגר כלומר לתמיד   הברית הלא קדושה…  עוסק באובססביות רק במחאה נגדו ומתעקש על עוד כח וסמכות בלעדית כדי לדכא ביקורת עליו  עלינו לזכור בימים רעים אלה שע…  אם אתם חושבים שעכשיו משפחת נתניהו עוברת כל גבול דמיינו מה יקרה כשהם יקבלו סמכויות החלטה אבסולוטיות בתקנות שעת חירו…  ידרוש את ביטול זכות המחאה נגדו בתקנות חירום תוך שימוש בעלילות דם על המתנגדים לו ותיוג אנשים כמפיצי מחלות  אם את…  חברים ברוח יום הכיפורים רציתי לומר לכם שטעיתי אני מתנצל  טעיתי שכאשר הזהרתי מפני תהליכים רעים של ריסוק הדמוקטיה…  חירום תוך שימוש בעלילות דם על המתנגדים לו ותיוג אנשים כמפיצי מחלות  אם אתם חושבים שעכשיו הממשלה לא מתפקדת דמיי…  מדינת ישראל סובלת מארבע מגיפות  מגיפת הקורונה מגיפת השקרים מגיפת השחיתות ומגיפת הבריחה מאחריות של נתניהו ומפלגתו…  גמזו על התנהלות נתניהו ״ההחלטה על סגר אומללה הייתי צריך כדורים נגד בחילה״ האם יש צורך להוסיף מילה  האם ההפגנות…  הח״כים מהליכוד מדקלמים מסרי שנאה והסתה כאיש אחד בדיוק כנתניהו משעמם שוב בתי המשפט שוב הפריבילגים שוב היועמ״ש ו…  כדי שהרוע ינצח צריך שאנשים טובים ישבו בשקט אדמונד ברק  בממשלה הזאת יושבת קבוצה של אנשים שהבטיחו הבטחות גדולות ל…  אנחנו דואגים למשפחה נתניהו דואג להעליל על מפגינים אנחנו דואגים לפרנסה נתניהו דואג לסמן בוגדים אנחנו דואגים לברי…  גל תחלואה השני באשמת נתניהו 6000 נדבקים ביום באשמת נתניהו מערכת הבריאות קורסת באשמת נתניהו מיליון מובטלים באשמת…  הציבור מסכים עם ביבי  ״לראש ממשלה בחקירות אין מנדט ציבורי להכריע קיים חשש שהוא יכריע הכרעות על בסיס האינטרס האישי…  ההפגנות לא ייעצרו המחאה תימשך כללי הריחוק והמיגון יישמרו וכפי שאמר חברי avidareli אם נתניהו רוצה לעצור את ההפגנות שיתפטר השיסוי הכי ישן בספר של ביבי יהודית מול דמוקרטית תפילות מול הפגנות  אם יוצגו נתונים אמינים על הדבקה בהפגנות ובאוו…  ״טופזגייט״   פרשה בה נתפס ראש הממשלה הנאשם בפלילים משתמש בכספי ציבור כדי להפיץ פייק ניוז  נתניהו נבוא איתך בחשב…  למה להחליף את עמדת היועמש לממשלה בעמדת פורום קהלת לא יותר פשוט למנות את שפטל כיועמש את בן גביר כשופט עליון וכל השאר יסתדר מעצמו דקה אחת בלבד לקחה למזכירות הכנסת לדחות את דרישתי לשאילתה דחופה לבחינת פרטי ההסכמים עם איחוד האמירויות ובחריין במקב…  יש כאן הפעלת שופרות שמדקלמים דפי מסרים ולחץ בלתי נתפס על ערוצי התקשורת לצורך קיום תעמולת הסתה שקרית ושיטתית תיקי 2…  הדיפ סטייט האמיתי זה מערך ההכפשה וההסתה שבנה נתניהו במשך שנים זה לא רק אוריך עמית סגל ריקלין לוק ועופר גולן זה…  אקדח מעשן לוק טוען שהוא ״קיבל הנחיות״ לעבור עבירה פלילית כדי להפיק פייק ניוז על מפגינים תוך הפרת בידוד ברור שמי ש…  6 נתניהו מנהל יחסי ציבור ולא את המשבר כחלק מיחסי הציבור הוא לא מהסס להסית נגד מפגינים ולהכפיש אותם המפגינים יכו…  4 את טופז לוק וראובן עזר יש לפטר מתפקידם באופן מיידי עובדי מדינה אינו יכולים לסכן חיי אזרחים 5 שוב ושוב ושוב אנ…  2 צביעותו של נתניהו מתגלה במלוא העוז אילו הסגר היה בריאותי ולא פוליטי רה״מ ועוזריו לא היו מפרים את הסגר כמעט כל…  1 לכאורה ראש הממשלה ניסה לזייף אירוע בהפגנה אתמול בבלפור תוך שהוא שולח את דוברו המחויב בבידוד לצלם מפגינים נתנ…  ״אני יודע שרבים מכם יודעים בליבם ומסרבים להודות בלא החילונים והליברליות למדינת היהודים אין עתיד ישראל תהיה דמוקר…  שבוע לאחר החתימה ואף אחד לא יודע פרט לראש הממשלה הנאשם בפלילים על מה ישראל התחייבה בהסכם יש לי חשש כבד ולא בלתי…  הגשתי שאילתא דחופה לבחינת ההסכמים עם מדינות המפרץ  ההסכמים טרם פורסמו והשלכותיהם הביטחוניות לא נדונו בממשלה ובכנסת…  כרגיל מרגש להיות פה שומרים גם על הדמוקרטיה וגם על הבריאות  חייבים לצאת להפגין מחר   נתניהו מוביל את ישראל לקטסטרופה כלכלית ובריאותית כי זה הדבר היחיד שיאפשר לו לדחות את משפט…  צאו לרחובות ולכיכרות וראו כמה אזרחי ישראל ממושמעים הרחובות ריקים והמעט שמסתובב חבוש במסיכות אזרחי ישראל נושאים בע…    בראשון בערב מוצאי החג נתראה בבלפור  לא נעצור עד שננצח לקראת הימים הנוראים שאלה לעמית סגל  כשאתה אומר שאתה שונא מחבלים איזה מחבלים אתה שונא יהודים או ערבים  כי אני נלחמתי במחבלים כל חיי טוב עשה ביה״ד הצבאי שעמד מול ניסיון הפוליטיזציה של צה״ל כשרה״מ מטפטף שנאה ובונה קריירה שלמה על שיסוי הסתה ותיוג…  למה ביבי היה צריך לטוס למה שר החוץ לא נשלח לטקס החתימה למה ראשי מערכת הביטחון ממודרים מההסכם למה הוא רצה לטוס במ…  מברך על הסכם שלום עם כל מדינה ערבית  הסיפוח מת ההיפרדות מהפלסטינים ניצחה רק השמאל מבטיח את ביטחון ישראל את הרבנים שתומכים במחבל עמירם בן אוליאל יש לפטר מהשירות הציבורי ולהרחיק ממוסדות חינוך חשוב להזכיר הרבנים אלה ותומכיהם  כולם מצביעים בנט הטלת סגר בחגים  שערוריה נניח שרקטה אחת משוגרת מעזה לאשקלון האם הייתם מפעילים אזעקה בכל הארץ ומכניסים את כל ישראל למקלטים itayalmogbar סרט חובה בכוונתי ליזום דיון בועדת החינוך בנושא זה בעידן של פייק מערכת החינוך צריכה לעסוק בערכים…  את ההסכמים עם המפרציות יש לחשוף במלואם טרם חתימתם על פניו ישנו חשש ממשי לפגיעה בביטחון המדינה לאור מכירת נשק אסטר…  המחתרת היהודית כבר לא פועלת במחשכים ינון מגל קורא לרסס עיתונאים ״כמו רמבו״ קובי ועירית קוראים לשנוא חברי כנסת אברו…  זה ברור שנתניהו מנסה להשתמש בקורונה כדי להשתיק את המחאה זה לא יצליח לו אנחנו גם נמלא אחר החוק ואחרי הנחיות היועמ״…  47 שנים אחרי המחדל חוזר  הפעם זה לא אמ״ן הדרג המדיני לא יוכל לברוח מאחריות  זה ראש הממשלה החליפי והממשלה המנותק…  יש לנו ראש ממשלה פחדן הוא בורח לארהב כי הוא פוחד מהקורונה מישיבות הממשלה ומהתקשורת מגיע לנו מנהיג אמיץ שלא בורח  שוב טרוף מוחלט ושוב קבלת החלטות לא הגיונית ולא צודקת מה ההיגיון בהטלת סגר מוחלט על ישובים שאין בהם כמעט תחלואה ל…  AyeletShaked את הקמפיין הזה את זוכרת איילת  לכבוד שר הביטחון חכ בני גנץ הרמטכ״ל אביב כוכבי  מפקד גל״צ שמעון אלקבץ  הנדון דרישה להפסקת העסקתם של המגישים קו…  מי שהאזין אתמול לשופרות הליכוד ולימין המשיחי מבין שישראל הולכת לכיוון ברור דיקטטורת נתניהו בנט סמוטריץ מתהווה לנ…  עוד חוג בית  עוד מפגש עם אנשים טובים  עוד מפגש עם אנשים שרוצים שינוי  לא מאבדים תקווה  די די פעם קודמת שהבטחתם לנו הפגנת ענק הגיעו בקושי 150 איש תפסיק לחפש תשומת לב ותן ליועמש לעבוד   אל תתבלבלו לגבי מי זה בנט במה הוא מאמין ומה הוא והאנשים הקיצוניים והמסוכנים שמקיפים אותו יעשו ברגע שיהיה להם שוב כ…   הדובר של נתניהו עמית סגל יכול להמשיך למחזר ידיעות ולקרוא להן חשיפות  זה לא יעזור אנחנו יודעים את האמת ישראל קו…  נתניהו אל תתנצל  תתפטר  אל תתנצל על הסתה ושיסוי  תתפטר  אל תתנצל על ספסור בביטחון ישראל  תתפטר  אל תתנצל על…  לשלט הזה יש פנים ויש שם והוא נפתלי בנט והימין הקיצוני ככה ארגונים הזויים כמו מרכז ליב״ה חדרו למיינסטרים הישראלי ה…  אנחנו לא מכבים טלפונים אנחנו לא מדביקים אנחנו לא מפחדים אנחנו לא משקרים אנחנו לא עושים קומבינות  אנחנו התקווה…  KnessetT בנאום במליאה בירך חכ YairGolan1 על הסכמי אוסלו הביאו לנו הרבה ברכה  האם מישהו פה יכול לחשוב על מציאות שאין בה את גדר הה… ישראל היום וערוץ 20 מפיצים עלילות דם כאילו הובלתי מפגינים לעצור אמבולנס בירושלים ומסבירים כמה שסמוטריץ נפלא וליברל…  הייתי אומר שנתניהו סחיט וחלש אבל מה שאנחנו רואים זה אפילו לא נתניהו אלא צל חיוור של אדם הבורח ממשפט נתניהו ימכור…  העסקה פשוטה ביבי נותן לחרדים כל מה שהם רוצים ובתמורה הם מוציאים אותו מהכלא ומה קורה כשבריאות הציבור מונחת על כף…  נתניהו לא מנהל את המשבר  נתניהו לא מנהיג את המאבק בקורונה במקום לשבת עם ראשי הערים ולמצוא דרכים להיאבק בהתפשטות…  אנחנו במערכה על גורל ישראל  העם בצד הנכון  כיף לפתוח את הסופ״ש בראיון אצל דני סידס ואודי סגל  נתניהו משקר לנו בענייני ביטחון נתניהו איבד את הבלמים  פגיעה בביטחון היא פגיעה בחיילים שלנו בילדים שלנו במשפחה ש…  YoazHendel1 לֹא תִשְׂנָא אֶת אָחִיךָ בִּלְבָבֶךָ הוֹכֵחַ תּוֹכִיחַ אֶת עֲמִיתֶךָ וְלֹא תִשָּׂא עָלָיו חֵטְא יועז…  איריס בוקר לא היתה צריכה להיחקר במשטרה הניסיון להלך אימים על אזרחים תמימים הוא פסול המשטרה היא של כולנו והיא חייבת להישאר כזו מהתוכנית ״המילה האחרונה״ הבוקר  אריאלי מה ביאיר גולן הורג אותי אני שונא בן אדם על לא דבר לינור אתה רשאי לשנוא…     הישג מדהים תוך 8 שנים בישוב ינוח ג׳ת עברו מ39 למעל 87 אחוזי זכאות לבגרות הכל בזכות הצוות המקצועי והמחוייב ובזכות…  ברכות לילדי כיתה א המתוקים בבית הספר היסודי בינוח ג׳ת שמתחילים את שנת הלימודים ״כל עוד שרים הילדים על השנה החדשה…  רבים מידי נפלו בפח של בנט שקד וסמוטריץ  אני אגיד לכם מי הם באמת צלם אריה סנדו  radio103fm אלוף במיל חכ יאיר גולן מרצ צריך להבהיר לנסראללה חד משמעית שאם יהרג חייל שלנו בגבול זה יגמר בביירות העם הלבנוני כולו… קובי ריכטר צודק בכל מילה בכל אות ובכל פסיק היזמים הישראלים שעל גבם נתניהו עושה לעצמו יחסי ציבור הם אלו שסוחבים…  בצלאל אתה באמת גנרל טוויטר מרשים יודע לצייץ באומץ ולחסל איומים בטוויטר כמו ענק תזכור שהסיבה היחידה שאתה יכול לשבת…  בצלאל אני מציע שתשתה כוס מים ותרגע ביטחון ישראל הוא עסק מורכב וחשוב שלך ידידי אין מושג ירוק בו אתה גיבור גדול בצי…  רק רב״ט מהקריה שמעולם לא התמודד עם הפרות סדר יכול לצאת בהצהרות מהסוג הזה  רק פאשיסט יכול לקרוא לירי ללא אבחנה באזר…  עוד שבוע בבלפור  עוד שבוע שהימין המושחת משחית את המדינה עוד שבוע שלא ברור איך תיפתח שנת הלימודים  עוד שבוע שאין מדי…  LikudParty זה מה שאתם יודעים ועושים שקרים והפצת שנאה הכפשה והסתה אתם בשלטון מ 1977 ועדיין מתנהגים כמי שדפקו או…  הפערים האדירים בין תלמידי החינוך הממלכתי דתי לתלמידים חילונים וערבים הם מתקפה על ישראל הדמוקרטית והליברליות שנות ד…  בג״צ פסק נגד גניבת קרקעות בשטחים וכצפוי הימין המשיחי משתלח נגדו בפראות בכל פעם שהימין המשיחי  לא מקבל את מבוקשו…  אסור שתלמידי ישראל ישלמו את המחיר של ממשלה חסרת אחריות והיסטרית הצעתי לשנת הלימודים עד כיתה ו פתיחת לימודים רגיל…  שר החוץ ממודר מהסכמים מדיניים  שר הביטחון לא יודע על הסכמי רכש ביטחוניים שר המשטרה מנסה לחסל את שלטון החוק שר הה…  אני לא מאמין למה שקורה במליאת הכנסת יוליה מלינובסקי מעלה הצעת חוק נגד השחתת מודעות כל רקע מגדר הקואליציה מתנגדת…  האם מיקי זוהר מתכוון לקחת אחריות על הקורבנות המיותרים שיגזרו מההילולה באומן איש לא רוצה לפגוע באמונתם של אזרחים א…  EmilieMoatti אורלי יודעת  ההגנה הטובה ביותר היא התקפה אלא שבמקרה שלה זו התקפה של אישה מניפולטיבית ולא אמינה אמי…  מתיחות גדולה בגבול הלבנון צהל הגיב בנחישות ובזהירות מתבקשת הזדמנות פז להגברת הלחץ הבינל על לבנון והחיזבאללה לח…  DayanUzi אני חוזר בי אמנם כתבתי ״איך התדרדרת״ אבל לאור דוח מבקר המדינה ניתן לקבוע שדיין מתאים לליכוד והליכוד מתאים לדיין DayanUzi עוזי אנחנו מכירים הרבה שנים עוד מהימים שאתה היית סגן vרמטכ״ל ואני רמ״ח מצבעים אני זוכר עוזי אחר הומאני…  נתניהו מוכר את ביטחון המדינה תמורת קמפיין  אתמול פומפאו אישר את שכבר ידענו f35 ימכרו לאמירויות מאחורי גבם של שר ה…  ליאור שליין יורד מהמסך  תהיו בטוחים שעמית סגל ישמור על מקום העבודה שלו  אקוניס עומד על הבמה ומאשים את בוגי ואותי בהידרדרות השיח הציבורי בישראל אילו הוא היה מוציא אפילו לרגע את ראשו ממק…  הקוסם הפך ללוזר  1400 חולי קורונה חדשים ביום 150 תומכים בהפגנת תמיכה בבלפור 21 אבטלה  18 אמון מהציבור 3 פרקליטים…  ביבי אף אחד לא מאמין לך יותר  לך הביתה  בין כחול לבן למשותפת צריכה להיות מפלגת שמאל ציונית אחת ואעשה כל שביכולתי כדי שזה יקרה הייתי שם אתמול מול השוטר שחבט בעוצמה במפגין לא הייתה שום התגרות או פרובוקציה מצד המפגין אני מגיע לכל הפגנה תמיד…  בקרב על הדמוקרטיה לאף אחד מאיתנו אין דרגות על הכתפיים אין כיבודים ואין מעמד כולנו צעירים ומבוגרים נשים וגברים…  תיכף תתחיל הצעדה מגשר המיתרים לבלפור אל מול העליבות של הפגנת הימין אנחנו נציג מפגן כוח מרשים אז תבואו לבד עם משפ…  מה חדש בדרום אין חדש  מדיניות עלובה שמשמעה חוסר הכרעה או שמסירים את האיום מעזה או שמגיעים להסדרה מול חמאס כל ה…  הגעתי להפגנה בכיכר הבימה בעקבות המקרה הנורא באילת  הדרישות של המפגינות והמפגינים פשוטות לא לאונס לא להטרדות מיני…  אני חש כאב עמוק ממקרה האונס באילת לאף אחד אין רשות לצלק ככה את נשמתה של נערה צעירה אך אסור לנו שנדון רק באירוע לג…  HaleviAmit כמו כן אני מאמין שלמדינה יש מחויבות כלפי מאות אלפי ילדים חרדים שאותם היא מפקירה לחיים של עוני כל ילדי…  HaleviAmit עמית הלוי קבל את שתי ההתחייבויות הראשונות שלי לבחירות הבאות 1 הקמת זרם חינוך חילוני שבו יחונכו ילדים…  רבים שואלים אותי איך זה שגבי יושב בשקט ונותן לביבי להשפיל את בני ואני עונה גבי מרוצה מהמצב ובונה את כוחו לכיבוש…  צפיתי במסיבת העיתונאים של גנץ הדימוי שעלה בעיני רוחי הוא של ילד מוכה לאחר מפגש עם הבריון השכונתי שחוזר לאימו מוש…  נתניהו בחורף חייו הוא איש מסוכן אם השלום שקפץ עלינו כרוך במכירת F35 לאמירויות הרי זה המשך ישיר לאופן ההיסטרי ו…  הגיבורים שלנו מעולם לא היו ולא יהיו גזענים אבא מרשים ואמיץ אחד מול הסתה לאומנית קשה כשהייתי ילד צעקות ״אתבאח אל י…  לא שמעתם את זעקות השבר של הציבור ולא התפתחה מחאה עממית בשל ביטול הסיפוח הסיפוח הוא הזיה של הימין הקיצוני והיא לא מ…  נמצא בדיון של ועדת החוץ והביטחון בדבר המאבק על שטחי C לצערי למעט מרצ אף סיעת שמאל או מרכז לא שלחה נציג לדיון האם…  חוזר ומדגיש אלימות פוליטית בישראל באה מימין למרות האשמות השווא של נתניהו האירועים האחרונים ביצהר בהם נפצעה שוטרת…  מכתב ראש הממשלה למנדלבליט  עוד קוזאק שנגזל עוד ניצול ציני של הנורמות הציבוריות עוד שלב בעבודת מכונת השקר והתעמולה של נתניהו ניתוח קל והחלמה מהירה לבני גנץ הכי חשוב  הבריאות אני איש שמאל גאה 38 שנים שירתתי בצהל סיכנתי את חיי פיקדתי על מבצעים מורכבים ונפצעתי כדי להגן על המדינה  אף אחד…  sadibenshitrit מושחתיהו בוא אספר לך אני עובד במפעל מתכת 11שעות ביום מתקלח בעבודה לא הולך הביתה עולה לבלפור להפגין נגדךשלוש פעמים… כולנו חיזרים עזבו את נתניהו  התגובות שלו צפויות ושבלוניות תקשורת עוינת משטרה רופסת הפצת מחלות מה עם סער דיכטר קיש הנגבי…  רעיון מבריק של יואל מסתבר שגם הפגנות הענק אינן מדגרת קורונה פעילות נכונה באוויר הפתוח ולמען מטרה נעלה עושה לנו ר…  ההחלטות הן בממשלה החוקים הם בכנסת השינוי הוא ברחוב הערב חובת התייצבות בהפגנות  בכיכרות ברחובות בצמתים בגשרי…  ע׳דיר כמאל מריח דרוזית גאה ואשת ציבור מרשימה הביאה לכנסת הצעת חוק לאום מתוקן שוויוני הגיוני צודק ונכון אבל חב…   אלימות הימין לא תרתיע את המפגינים ככל שהמאבק יהיה קשה יותר הנחישות תגבר בואו בהמוניכם לכל הפגנה הרב רפי היקר  אתה איש של מילים תחזור ותקרא את נאום יום השואה ותגיד לי עם מה אתה לא מזדהה הדים לדברי תמצא גם אצל…  תודה בן  הצהרת ראה״מ ובמיוחד הצהרת ראה״מ החלופי לקו בפומפוזיות מיותרת עוד שלב באובדן אמות המידה הציבוריות טוב שצה״ל שומר עלינו ושומר על שקט TsahiDabush צחי בקצה יש לוחמים שישלמו בחייהם נכים משפחות שכולות הרס וסבל עצום מלחמה היא אף פעם לא הזדמנות נהד…  היום זה חוק ההמרה מחר יריבו על תחבורה ציבורית בשבת מחרתיים על הזכות לנישואים ובשבוע הבא זה יהיה סיפוח שטחים הכות…  ברכות לחברי ניצן הורוביץ על העברת חוק מניעת טיפולי במרה בקריאה ראשונה הישג חשוב ועקרוני ונקודת אור בחיים הציבוריי…  בית איל צובר גרעון ענק זו תהיה תרומה שתעזור להפעלה מצומצמת עד שהממשלה תקיים הבטחתה ותעניק לנו את המובטח תודה לכ…  אני כאן עם המפגינים האמיצים והנחושים צעדנו מבלפור לכנסת הגיע הזמן שהמשלה המושחתת והמנותקת זו תגיע לסופה מגיע לכו…  לא מחאה של אנרכיסטים ולא של בלגניסטים זו מחאה של אזרחים שאכפת להם מהמדינה שלהם מההורים שלהם מהילדים שלהם צוות ג…  האם יש באמת הדבקה בחדרי הכושר ובחופי הים למה אין לאזרחי ישראל גישה חופשית לנתוני הקורונה נתניהו וגנץ זו לא תקיפה…  חוץ מזה כל אגורה שאקבל כתוצאה מההיסטריה הזו תיתרם לחיזוק הדמוקרטיה האיש שהפך הסתה ביזוי ושיסוי למקצועו הפוליטי נלחץ ממחאה הולכת ומתרחבת זה סימן שהמחאה עובדת להמשיך הלאה במלוא העוצמה ועד לניצחון התקשרתי לחזק את פרופ רובין על המהלך האמיץ של התפטרותו כיור ורה השר אלקין ממשיך בניסיונותיו לחרב את מערכת ההשכלה…  הפוסט המלא  לא חוזרים על הטעות של 2011 כאשר המחאה צעקה שזה לא פוליטי וקיבלה בתמורה עוד עשור של התעלמות מנתניהו ישראל זקוקה לש…  בעלת בית קפה ממודיעין פונה ואומרת עסק של 500 מ״ר ורק לחמישים איש זה גזר דין מוות אכן טפשות במיטבה היה אפשר להכש…  2 הצעות לועדות חקירה פרלמנטריות הצעתי לחקור את תפקוד הממשלה באיבוד השליטה על משבר הקורונה והצעת סמוטריץ לחקור את…  YuvalKarni יובל אמנם התרגלנו למציאות שבה הכל דילים פוליטיים אבל אני מחוייב לייצר מציאות אחרת ופוליטיקה אחרת לא ר…  נדהם למשמע אוזניי כשאני שומע את צחי הנגבי אומר ״השטויות האלה שאין לאנשים מה לאכול זה חארטה״  החארטה האמיתית פה הי…  במקום שהמשטרה תחלק דוחות על אי חבישת מסיכה היא פשוט תחלק מסיכות ברחובות לכל מי שאין לו זה יהיה הרבה יותר אפקטיבי…  ראיון בטלוויזיה ומייד לירושלים גם אני כמו אלפי אזרחים שוחרי תקווה וטוב נגיע לבלפור כדי להביא לישראל שינוי כדי ל…  אמיר השכל נעצר ההפגנות ימשכו ישראל תמשיך את מסעה לתהום נדרשת מחאה עממית רחבה לא אלף אלא מאה אלף מגיע לכולנו מנ…  ממשלת חירום שקמה לכאורה בגלל משבר כלכלי אבל בפועל מתנגדת לדמי אבטלה לעצמאים בזמן שהיא מאשרת לראש ממשלה מיליונר הט…  אברמוביץ שרוף הוא שרוף כי כשהטנק שבו נהג כשנלחם במלחמת יום כיפור נשרף הוא נכווה בכל גופו אבל למפגיני הימין שטופי…  היום נסעתי דרומה לפגוש מנהיגים מקומיים מהקהילה הבדואית בנגב  הגעתי למסקנה בלתי נמנעת  יש בישראל פצצה מתקתקת פצצת…  מי שמקבל גובים ממושחתים סופו שיצטרף לשחיתות וישחית בעצמו  היום כחול לבן סידרו לראש ממשלה מליונר הקלות מס בזמן שיש…  אני מתנגד לסיפוח החד צדדי הסיפוח שיכניס מליוני פלסטנים לישראל הוא אסון מהכרותי העמוקה עם השטח אני יודע שרק היפרדו…  מנהיגיזם בימים אלה נכון לעיין במה אמר ז׳בוטינסקי ״בזה אחר זה בזו אחר זו נדבקים עמים וארצות באותה מחלה ממארת ומגלים בקרבם…  עיתונאים לכלאאמרתי לכם התנגדות הימין הקיצוני לתכנית הסיפוח של נתניהו מדגימה את שאיפותיהם בכל הנוגע לפלסטינים הם רוצים כאן מדינה חציחצי…  לא משנה כמה אנסה אני לא מבין איך המהלך שעלול להביא לתוכנו בין 25 ל45 מיליון פלסטינים יעשה את ישראל חזקה או טובה…  BenAnthony1948 YairGolan1 gives a fascinating insight into his political strategic amp religious beliefs in this interview exclusive… איני מקנא במי שתפקידו לעשות משפט צדק בזמן שמתנהל כנגדו מסע הסתה במטרה מובהקת להטות את עמדתו המקצועית אבל עודני סו…  אני שומע יותר מדי אנשים שאומרים אתם בשמאל אתם מחנה קיצוני וקטן אז לא היום אנחנו אולי קטנים אבל קיצוניים אנחנו…  2gt ושזה לא הופך אותם לכובשים מרושעים ונקלים מי שרוצה לבנות עתיד טוב יותר לכלל אזרחי ישראל ראוי שיאמץ קו מכבד הנות…  1gt צפיתי בסרטון שהוציאו הסטודנטים של חדש בו מצולמים חיילי צהל במטרה להפחיד מפניהם ולהשניא אותם אם חבריי בחדש ו…  שמחתי להצביע נגד ממשלת נתניהו החמישית או בשמה המכובס ממשלת החילופים בזמן ששריה מתחייבים לשרת את אדונם לא משנה כמה…  haggaisegal תמכתי בסגירת גל״צ כבר בראשית 2015 כסגן רמטכ״ל שיקולי אז לא היו פוליטיים וגם היום הם לא פוליטיים עצ…  הבעיה עם גל״צ אינה הטייתה הפוליטית אלא שצה״ל אמור לעסוק בשמירה על ביטחון ישראל לא בשידור ברדיו לציבור הרחב אולי…  ברכות לאורלי לוי על תפקידה כשרה לקידום קהילתי תחומי העיסוק הנרחבים של משרדה החדש בוודאי יהיו שונים בתכלית ממשרד הר…  חצי שנה הספיקה לתקשורת המגוייסת של בנט כדי להכתיר אותו כגדול מכולם מייקל גורדן של עולם הביטחון מייקל פלפס של מכס…  לצערי בני גנץ לא ניהל את ישיבת המליאה היום אבל אלה הדברים שהייתי אומר לו  חבריי מהציונות הדתית חלום הסיפוח לא יתגשם נתניהו יחזיק בו לפני חוטמכם ויוליך אתכם בכחש פעם אחר פעם בתירוצים שונים…  עוד לא החל הדיון בבגץ ושופרי הימין יחד עם הפוליטיקאים המכורים לביבי ממהרים להלך אימים על בגץ בגין אמר יש שופטי…  גדעון ככה נראה אובדן החלופה לנתניהו בתוך הליכוד אם היה נשאר לך עוד קצת כוח ועמוד שדרה לא היית משתף פעולה עם הD9…  VilnaiMatan מתן ברוך הבא לזירת הציוצים מקווה שנצליח לתרגם ציוצים לשירה אדירה  שירת העם הרוצה בטוב ברגעים כאלה צריך להסתכל גם על נקודות האור MeravMichaeli נלחמה על יושרתה של מפלגת העבודה עד טיפת הדם האחרונה וכנג…  למרות זחילת העבודה לממשלה  השמאל הציוני חי ובועט אסור שרוחנו תיפול זה הזמן להדק את השורות לאסוף אנשים טובים ולצ…  לרגל תחילת חודש רמדאן המבורך וחג הנביא שועייב עליו השלום אני רוצה לאחל לצמים ומשפחותיהם צום קל וארוחה מפסקת הפסק…  بمناسبة حلول شهر رمضان المبارك، وعيد النبي شعيب عليه السلام أتمنى للصائمين ولعائلاتهم، صوما مقبولا وإفطارا شهيا…  ivri99 אבישי ידידי אני במקומך לא הייתי מתייחס להתנהגות ראויה בבתי קברות יום הזיכרון מתקרב וזה לא מוציא אותך טוב ההחלטה למנוע ביקורי משפחות חללי צה״ל בבתי הקברות היא שערורייה מה הבעיה לייצר ביקורים במשמרות להגביל את הביקורים ל…  חבריי במפלגת העבודה ישנה תקומה לשמאל הציוני אך זו לא תבוא מחבירה לנתניהו כניסה לממשלה המנופחת לא תציל את ישראל א…  המיטו כמובן מספיק מילים נשפכו על התקפלותם של בני גנץ וכחול לבן אנחנו ממשיכים הלאה נהיה אופוזיציה חזקה ויציבה נאבק ללא מורא ל…  אם בני גנץ רוצה את תמיכתנו בחבילת החוקים המדוברת שיתכבד ויפנה את תפקיד יו״ר הכנסת לטובת נציג וותיק ומנוסה מהגוש שא…  אם כחול לבן מסירים את חתימתם מחבילת החוקים גם אני מסיר את חתימתי לא ניתן להם ללכת עם ולהרגיש בלי לא נעשה בשבילם א…  במקום להתחיל להפעיל את מערכת החינוך במשמרות בפיזור תלמידים במקום לגבש תוכנית כוללת לשגרת חירום עם מענה לילדים… </t>
+  </si>
+  <si>
+    <t xml:space="preserve">eyaldatz eranlaor פחות עובד לי ברחוב אבל לגבי המשלוח  מסכים מושלם almogtamar  alonbeer1 אלון כל הסרטון הזה הוא פייק ניוז אחד גדול הוצאה אחת גדולה שלו מהקשר חבל ליפול לשם asaflib בוא הבנאדם כתב ימים כלילות ILParliament MatanAlcalay מזמין משלוח כמובן TomerShlapnik וואוו זה פוטנציאל לארוחות שישי מטורפות KeDmE תוכן חשוב פלוס טיפ סטיילינג חשוב הכל במקום אחד  piniyellow  piniyellow אני פהההההה מעניין למה אין חריימה ומפרום בסעודת ההפגנה מול בלפור 🤔🧐 לא מאמין שרות ביידר גינזבורג מתה בת 87  ארורה תהיי 1933 NoamOxman נראה לי שיצא לי בכלל אלון בן דוד  netanyahu מוזמן לשיעורים אונליין בזמן הסגר  לראשונה לא קיבלתי שנה טובה ממפלגת העבודה בsms  המפלגה הזאת באמת מתה arielapi ברגע שמקפידים לקצוץ כל כמה ימים זה הופך להרבה יותר פשוט עדיין מזועזע מהמאמר של קלמן על נתניהו ביום שקלמן יגיד שאחרי כשלון הבחירות ב2019 בנט היה צריך להניח את המפתחות ביו…  shiraum איפה ומה המסקנות PascalLoop מעניין למה לא משולבת uricovagerev נו מעולה אני תומך בעבודה עברית gobuttercup1 למה איזו מכונת כביסה לקנות תזכרו שאני קמצן ItayBlumental והספר שהוא קורא זה ספר טלפונים וואוו ניצחת  YHepstein יש יותר שקוף מהאכזבה ששלמה פילבר הולך לדפוק לפיד רק לא ביבי כנראה לפרקליטות גם בעדות שלו במשפט נתניהו lielkyzer ruthlessrousso  UriahCanaff רצופות אולי עם איזה חור קטן באמצע  RoyIddan כמות הדברים שאתה יודע לעשות נמאסה עליי RoyIddan אם אתה נותן להם לאפר אותך אני אעלב באופן אישי eyaldatz ביבי ״שתבין כמה זה דפוק היא ובעלה התחייבו שהנכס בראש העין ישמש למטרת ׳מגורי חברי העמותה ומגורי קרוביהן בלבד ולא למטרה אחרת׳… ללכת לפאב  אסור לחבוש שטריימל  מותר ללכת לכנס של רם פרומן  אסור לאכול כשר  מותר  שיקולים מקצועיים עאלק AvishayBSG Arspoeti TomerNaor shacharbm sfardm LVertzhaizer CarmitSoliman הגבלתי חברותי בלשכת עורכי הדין naamuli84 אהבת זה היה מבנה באוהאוס dovieichler אין אפילו דיפלומה נהדר לצערי  יסלח לי איוב קרא אבל ככל שאני מבין לא הוא ולא המרכז הכלכלי לשלום עומדים בקריטריונים להגשת מועמדים לפרס נובל לשלום  GaliGnt בדקה הקרובה חשיפה רותחת בנושא העובדה שהיינו צריכים שחבר פרלמנט איטלקי יגיש את נתניהו לפרס נובל לשלום היא בושה וחרפה איפה שלמה קרעי איפה מיקי זו…  כל הכבוד לדתיים שמסכימים בזמן הסגר שלא להתפלל בהר הבית itayr2 כי אחרת לא ברור למה הציוץ הזה מענייןשונה משתף כי מדובר במעצב השיער של שרה לשעבר  iatzmon guyshamai מה קורה אחרי החגים guyshamai ילדים טובים וחמודים guyshamai וואוו איזה פספוס של החיים קצת פרספקטיבה  קונספט שלא תפס בישראל תור אחד לשלוש קופות realadamgold הרס את מצבנו עם יהדות ארצות הברית והפך את ישראל לסוגייה מפלגתית הרווחים הם מידיים בתקופת טראמפ אבל המחיר יגיע בהמשך therealnirs היועץ של טראמפ למזהת שהחליף את גייסון גרינבלט ילד בן 12 חבר של גארד סירי מה זה ריקליימינג  ליאיר נתניהו מגיעה התנצלות ביבי דיייייייייייייייייייייייייייייייייי לא להאמין בזמן שנתניהו חותם על הסכם שלום היסטורי עם איחוד הבחרייניות יונית לוי מקריאה את מספר המתים והנדבקים מקורונ…  דעה לא פופולרית במדינה היהודית היחידה בעולם צריך להחריג מסגר תפילות בבתי כנסת לחגי תשרי דעה פופולרית זו גם המדינה עם סגר היחידה בעולם MBlumenblat יש לי זקט פוטבול שמוכיח אחרת מעצבן אותי שאנשים ישר משליכים עליי שאני לולב ולא אני גם לא אתרוג מדובר בספקטרום שנע בין ערבה להדס וכל מה שבאמצע ברוך הבא UriahCanaff הcancel culture מגיעה לפריפריה היה היום סטטוס בפייסבוק לא של יאיר גולן בדיוק עם האמירה הזאת  הרבנים שתומכים בעמירם אוליאל  מצביעים בנט זמן קצ…  מצודת זאב ומוזיאון האצל יוחרגו תותר התקהלות של 80 אנשים בכל הדירות שיאיר שטרן שנצ בהן YHepstein לא הבנתם שהלוק החדש של נתניהו עם הזקט והטי שרט זאת התשובה למוב של יוסי כהן אתמול adispr חחחחח דעה לא פופולרית סגנון הבאוהאוס הוא למעשה השלכה של כמיהתנו לגרמניה של לפני עליית הנאצים אנחנו לא חוגגים את העיר הע…  odedkramer מוזר אני חושב שהיום נציג המשטרה בקלמןליברמן אמר שאסור לרחוץ גם אין מציל לא akivanovick לציין את עמדת הנחיתות בה אני נמצא מדובר בביטוי של ענווה דעה לא פופולרית ציוצי המלצרית של ריקלין כבר מזמן עברו לשלב הפארודיה המודעת לעצמה זה מצחיק והתגובות הרציניות שלא…  דעה לא פופולרית בניגוד לשוק מחנה יהודה בשוק הכרמל יש אשכנזים מתל אביב ולכן צריך לסגור אותו דעה לא פופולרית למרות שאיציק ורותי כבר סגרו צריך לקנוס אותם על אי קיום כללי התו הסגול TomerPersico עמיר פרץ רימה את השמאל אחרי הרמאות של גנץ אתה צריך לספור גם אותו בפנים דעה לא פופולרית טייק אוואי יוצר התקהלות  בסגר הקודם גם היווה פירצה לאכילה של הלקוחות בבית העסק עצמו אנחנו מפסיקים לרגע את הדיווחים על המגפה העולמית שהתפרצה בסין כדי לספר לכם על עדויות לחיים על כוכב הלכת נגה LermanRon guyzo שמחנו להיעזר PolarTash חשבתי שזה ברור AvishayBSG לגמרי דעה לא פופולרית ספציפית ההסכם עם בחריין הוא האירוע ההיסטורי הכי גדול מאז המלחמה של חמורבי בתותנחמון aryeyoeli האמת אהבתי בטירוף natitucker אוף 60 מליון בהכנסות עתידיות גם אני יכול לשלם dvirluger אשכרה זה טירוף brdvd ומזל טוב כמובן brdvd זה גבינה או בלונדי אני היחיד שבסדר עם כשלון של הממשלה כל עוד היא ממש משתדלת כמה כיפות בקצינים החדשים חוקרים גילו חיים על כוכב הלכת נוגה מיטב המוחות במכון הביולוגי עובדים על דרכים להרוג אותם porgcupinetree freyisrael1 זה טרם התפזרותה בגלל זה לא נכון לדעתי להשתמש בה בתור הבטחה לבחירות הנוכחיות freyisrael1 ישראל זה מלפני הבחירות האחרונות לכל אלו שצוחקים שזו רק סאטירה ראש הממשלה נתניהו בכבודו ובעצמו נכנס עכשיו למשרד וריסס את כולנו עם מכונת ירייה נו  באמתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתתת…  עתידות ההסכם יכלול הכרה במדינה פלסטינית עצירת הסיפוח הקפאת התרחבות בבנייה ולכן שרים מהליכוד יצביעו נגד וכחול לב…  Izikiel2517 בסדר גמור אבל לא צריך ללכת סחור סחור עם דוגמאות לתיאום ציוצים כדי להגיד את זה דעתם לא מעניינת אותך וזהו Izikiel2517 מה ההבדל הם אומרים בדיוק אותו דבר רק שהם מהמחנה השני זה אשכרה הגיבוי הכי גרוע שאפשר היה לתת למהלך במקום לצייר את המהלך כמהלך של אחריות וסולידריות שלח מצייר אותו כמהלך…  filbers 1 פרופ לס מדגיש כל פעם שהוא נשאל שהוא קורא לקיים את הנחיות הממשלה וחוקי המדינה הוא מבקר את ההגיון מאחו…  Izikiel2517 כל האנשים שמתנגדים לקיום הפגנות בזמן סגר אכן מתמקדים בתופעה של הפגנות בזמן סגר Izikiel2517 לקחת שלושה ציוצים שכותבים נגד הפגנות כאילו מדובר במזימה מתוכננת זה מוזר אני יכול לעשות בדיוק אותו דבר…  asaflib nitayp כן ואתה מגלה את זה עכשיו לראשונה בטח ברור נראה למי יהיו יותר לייקים Firkushim asaflib מאמין ולכן שווה נפש asaflib nitayp קיצר תתייג אותם אני כבר אחרי שיחה עם 4 נציגי שירות שונים מרגע שצייצתי asaflib nitayp למדתי לפני כשעה שיש משהו שנקרא פועלים קונקט תנסה 036530700 asaflib לא מאמין עליך RimonRan חחחח אז מה אם הוא נחת החלפתי כרטיס אשראי רוצה לקבוע פגישה בבנק כדי לקבל אותו poalim באפליקציה אי אפשר להזמין תור מתקשר לטלפון צריך קוד…  Sachback זוכה במיליון והולך לדפוק נאפיס אני שרוף על המדינה הזאת  אם אסי בוזגלו עובר לידי ברחוב  אני לא מזהה אותו eransinger שופר של בלפור ISudri ״הופך פתאום להיות הוגה דעות״  מצייץ בטוויטר אני מבין שאתה קורא לסגור את הרשתות החברתיות לסוגיהן למה יש לי תחושה שהסיבה שנתניהו לא משתף במסמכי ההסכם עם האמירויות היא לא בגלל השמאל אלא דווקא בגלל סעיפים שנוגעים לע…  rolbishaul תודה חבר arnavonet בלי לחשוב פעמיים נותן לעצמי את הראסיה של החיים ivri99 SaraHaetzniCohe החוק עוצב על ידי הבריטים ולוטש על ידי ייקים eyaldatz חחחחח YHepstein למה דווקא הערב מה מיוחד הערב הוא נראה חלומי כמו בכל יום שמאל תראו את נתניהו איך הוא לא יודע להתאים חליפות נראה כמו שלוך גם שמאל תראו את יוסי כהן מתלבש יפה מדי רואים לכם דקל וקנין YHepstein למה הייתי מת להראות כמוהו כמובן יוסי כהן מתלבש יפה מדי זה נרקסיסטי ולא שפוי זו היתה שאלה מאוד לא טובה ואין שום סיבה להפוך אותה עכשיו לדגל סגר ראשון חחחח לא צריך ללכת לבקר את ההורים איזה ״באסה״ 🤣 סגר שני אני אוהב את הוריי ומעריך כל דקה במחיצתם הריחו…  מה רוני גמזו עושה כדי לנצח את הקורונה לפתוח פייק נועם כץ אלקסה שני קילו קרפיון טחון ליום רביעי חבל שזה לא אני שמנהל את המשבר איזה פצצה היה יכול להיות פה akivanovick קקיבא נוביק GaliGnt עוצמה רעב רצח talialin מעולה מעולה ממש נהנינו אתגר הסכום בעין זו צלחת ריקה כדי שזה יהיה אתגר צלחת ריקה אתם צריכים לשבור אותה על הראש הסגר זה בגללי RTsipris אני קולו של דור שבעתי זה לא אומר שסוף סוף הממשלה הפכה להיות דה פקטו פריטטית אני נכנס לגוגל דרך מחשב חדש גוגל מזכיר לי את זה לנצח נצחים 100 שקל שכן יוחרגו  שמעתי שיש סקר שמוכיח מדעית שכל השמאלנים בוגדים אשמח להפניה  elirazsade מאוהב בך KeidarKesten לא ככה מדבר מנהיג שמאל סולידריות ואחריות חברתית הם הבסיס לחברה מתוקנת עדיף שתדבר על ההכרח בפיצויים מעבר לכך שמה שהוא… אז  ליצמן ליונה ״אם יהיה סגר אני אשתה יין״ YairJacobi  אז איפה היית באסון התאומים  בדיוק צפיתי בקרוקודייל דנדי  אחי זה רצח רבין  אתה לא תגיד לי כמה פעמים לצפות בקרוקודייל ד… therealnirs אני לא יודע איך אני לא יודע מתי אבל אני הולך לעקוץ אותך איכשהו naamuli84 יופי באת להסגביר לי ובכל זאת יצאתי מסגבירן בא לי למות naamuli84 זו הייתה עודדדדדד בדיחהההההההה naamuli84 כיף איתך במסיבות שיש מלא רעש והשכנים מתקשרים למשטרה זה לא להאמין שלא משנה כמה כסף יש לך תמיד תוכל להקלע למצב של רעש מהשכנים Itamarsassover למעשה זומן לחקירה considerthefish אבחנה considerthefish אתה סוטה ברמה גבוהה ביותר NoaHakim Muchas gracias estimada ministra es un placer estar en su maravilloso país   וזה כנראה הציוץ המתנשא שלי אי פעם אבל הוא למטרה טובה להגן על רני רהב מהביקורת לרני רהב אין את המאפיינים הנפשיים והתודעתיים המאפשרים התנשאות ברייקינג מהסטוריז של אח של זהבי עולה שהם לא שמעו רק מזרחית אני גומרת  mayarachlin kannnews דווח גם בזמן אמת בוושינגטון פוסט nynynyos התרשמותך בעוד שבוע תודה talwasser פיצה DenisVi amsterdamski2 horowitzb זהו בגלל זה אני לא מבין איך שני צירי וואי פותרים את זה amsterdamski2 horowitzb ואז מה הפרופורציות של ציר הy במתים זה לא היה פותר את הביקורת של בן להבנתי horowitzb למה לא איך אפשר כן להראות את שתי המגמות יחד AvishayBSG יש לך אחלה קליעות נגה ניר נאמן עכשיו בטריווגו בחריין  המשטרה מסרבת לנקות את שמו של זהבי רק כדי לפגוע בנתניהו zviashkenazi אוףףףףףףףף בדיוק כתבתי ציוץ בנושאאאאאאאאאא אתגר חדש באיזו תמונה ציפורי היה משתמש אם היה כותב עליי פוסט תמונהשלציפורי  janjosephcohen איזה שם משפחה יותר חזק כהן או נתניהו  רק שנבין את הסבטקסט שהפך לטקסט שי ניצן קבע שסובייקטיבית השוטרים בארוע חשו סכנת חיים ולכן פעלו כפי שפעלו בגדול ב…  זה באמת יפה מאוד שסוף סוף מזכים את שמו של אבו אלקיעאן אבל אוסנת מארק וזנדברג כמובן לא רק חושבת שהוא נהרג אלא שה…  galileoosh מיייייייייייייייייייייייייייייייייייייייייייייי אוף אני לא מאמין שהולכים לייבא לפה מודל שוודי זה יהפוך אותי לאפילו יותר מכוער באופן יחסי  מישהו יכול להסביר למה נתניהו החליט לבטל את המטוס הפרטי ולהקפיץ את מחיר הטיסה  רואה את הפרצופים באולפנים בזמן הטקס הם כמעט כועסים שיש שלום כמה כואב להם שזה נתניהו שם על המדשאה ועוד בלי שהוא פ…  EliHaviv אז קבעתי הופעה לאחרי העוד סגר כדי שנוכל לצאת מהבית ולגלות שכולם לא שפויים לא רק אנחנו זה יהיה בחוץ אז בלי קורונה ואם י… לעזאזל איתך מנדלבליט למה אתה מכריח את ראש הממשלה לטוס במטוס נפרד מכולם  רואה את יפעת שאשא מנסה להסביר על קורונה לרופא פרופ׳ גבי ברבש ופשוט משתגע מזה שאשה מרשה לעצמה לדבר ככה לגבר אני מבקש לספור אותו בתור ימני בפאנל  לדני קושמארו יש דעות ElkyBergstein היה סגר א׳ לגבי ברבש יש כיפה ErelSegal AvishayBenHaim אתה לא תחזיק שם יום אחד itayr2 טוב אדחה את הציוץ עם התמונה הלא מחמיאה שלך פלוס כינויים מעליבים לפעם אחרת itayr2 אבל גם אין סיבה לעשות לשי ניצן הנחות בהודעה הרשמית הוא פירסם שיש אינדיקציות לכאן או לכאן איזו מין קביעה…  עוד מעט הולך לסופר  mendygruzman התארחתי שוב בפודקאסט האלמותי של yoavr ושוחחנו על חשיפות הטיוחים במשטרה ובשאלה האם אלו טיוחים בפרשות נתניהו והאם אלו… YHepstein ruthelbaz DorDugy איזה שקרן יצאתי חבל על הזמן הארץ עשו ביקורת קטלנית על מסעדה מבלי לציין את שמה הגון לפי הביקורת מדובר בזוג מבוגר ונחמד שאין סיבה לפגוע בפרנסתו…  eranlaor DorDugy ruthelbaz YHepstein לגמרי אני לקחתי את הציליציזפרייז גם גבינה וגם בשר זו היתה חגיגה של פלסטיק וצרבת DorDugy ruthelbaz YHepstein אתה צודק לחלוטין אני מאוד נהניתי שם אבל אין צורך בתחליף גבינה DorDugy YHepstein בודגה קרליבך פינת הארבעה yuvalgeiger YHepstein פייקון הוא לא באמת תחליף לדעתי זה אכן בטן של טלה גבינה מזוייפת לעומת זאת היא תחליף YHepstein הגבינה מיותרת ShakkedRiver יש לי גם חתולה אבל אני מתכנן לטחון אותה לקציצות קרות אני צריך לדעת אם יש סגר בראש השנה לפני שאני קונה קרפיון משילות  שיקולים פוליטים אני קורא לכולם לשמור על ההנחיות hananamiur אורי משגב תוקף את עמוד הדעות של הארץ שנתן במה לנתן אשל ויונתן אוריך ואתה תוקף את עמוד הדעות של הארץ שנ…  arielapi יצאתי בומר DdongISR למה שירצה למנוע את הסכם השלום RoyIddan תתרחץ איתי פעם תבין arielapi תתעלם לחלוטין מעניין המבטא tamarlask Rereshef ביום שתפרקי עוף חזירים יעופו ויתפרקו TomerNaor תומר לפי מה שאתה אומר פה גם הכתבה בהארץ היא חסרת משמעות זה מה שאתה חושב bhovav amsterdamski2 זה חוב בגלל הלוואה שהמדינה לקחה מקרנות הפנסיה ואם כן  מתי גם לפני יותר מ40 שנה נכון הקטע הזה שגם הנינים שלנו ישלמו את ההלוואות שמדינת ישראל לוקחת יש משהו שאנחנו משלמים היום שהסבים שלנו לוו amsterdamski2 לא יודע אם בנימין נתניהו או אורי פינק </t>
+  </si>
+  <si>
+    <t xml:space="preserve">גמר חתימה טובה  odedshalev robertrabin ככה זה כשאין סבלנותסוף טוב הכל טוב גמר חתימה טובה עת לחשבון נפש ולבלימת השנאה המשתוללת בתוכנו ובינינו  haskioren רפואה שלמה DuduErez1 מאשר שנה טובה  Israelcohen911 ח״כ גדעון סער בניחום אבלים אצל הגאון רבי שמעון בעדני חבר מועצת חכמי התורה על פטירת רעייתו הרבנית שולמית ע״ה הרב ברך… כתבתי ואמרתי את זה אין ספור פעמים  לפני ואחרי החזרה ללימודים לצערי בשום שלב לא בוצעה האבחנה הפשוטה והמתבקשת הן מ…  קיצור הליכים מנוסח תקנות סדר הדין האזרחי החדשות דווקא התאיידו הסעיפים המחייבים את השופטים לתת פסק דין תוך 30 יום…  rothmar אני יודע שקורונה והכל אבל אחד הדיונים החשובים ביותר באמת שישפיעו על כל אזרח ואזרחית מתנהל כעת בוועדת חוקה  תקנות סדר הדין… היקפי התחלואה וההדבקה מחייבים שיקולדעת מחודש ודחוף בהמשך קיום הלימודים בבתי הספר התיכוניים  חטיבות הבינים והחטיבות העליונות elidukorski יישר כח אלי ortalshmueli בהצלחה לבנות ונחת להורים ״אל ביתהספר הולכים הילדים״ עם דוד בדרך לכיתה א׳ ושירה לגן החדש שתהיה להם ולכל ילדי ישראל שנה טובה  ofirbar yoavgallant תודה אופיר יקירי לפתוח שנת לימודים זו תמיד משימה מורכבת השנה היא קשה ומורכבת בהרבה אני מאחל הצלחה לשר החינוך yoavgallant איחולי…  מאחל הצלחה רבה למשלחת הישראלית לאבו דאבי ישראל היא מדינה שוחרת שלום ונקווה שמדינות נוספות במרחב יבחרו בדרך הנורמלי…  orenhelman מזל טוב  התוצאה אליה הגיעו שופטי הרוב בענין ״מצפה כרמים״ אינה הגיונית ואינה צודקת על המדינה להמשיך ולהאבק להסדרת מעמדו של ה…  pninatamanosh רפואה שלמה פנינה הפרת חוק על ידי רשות המופקדת על אכיפת החוק  בראש חוצות  קשה לתפוס את מה שעבר על נערה בת 16 שהיתה קורבן לפשע כה אכזרי וזוועתי קשה לחשוב על כך ששלושים גברים בזה אחר זה בי…  יש הבדל משמעותי בהשלכות הכלכליות על עבודת הורים ועל המשק  בין הגנים ובתי הספר היסודיים לבין חטיבות הבינים והחטיבות…  את חברהכנסת לשעבר גרשון שפט זכיתי להכיר בנעורי בפעילותי בתנועת ״התחיה״  החיוך ומאור הפנים לא משו מפניו ממייסדי ק…  פרופ׳ רות גביזון היתה אינטלקטואלית אמיתית מקורית המצויידת בפתיחות מחשבתית היא הבינה לעומק את חשיבות הפשרה כדי לא…  מברך על ההסכם עם איחוד האמירויות       מה שירגש אותי זה כשנזכה להחיל את החוק הישראלי על ההתיישבות היהודית ביהודה שומרון ובקעת הירדן giladerdan1 בהצלחה גלעד הלילה נפטר האדמור מסדיגורה הרב ישראל משה פרידמן הרב שימש כחבר במועצת גדולי התורה של ״אגודת ישראל״ מאיר פנים לכל…  מתקשה להבין את התוחלת שבאולטימטום של גנץ בשעה שבה ניתן לפתוח בדיאלוג למציאת פתרון מוסכם לסוגית התקציב  הוא מעדיף…  netanyahu זאת החלטה אומללה של בג״צ שסירב לבקשתנו להרוס את בית המחבל שרצח את חייל צה״ל עמית בן יגאל ז״ל שהיה בן יחיד להוריו   אני דור… תיקון הדיון יתקיים ביום חמישי זה לא רק ביתו זה המקום ממנו פעל ובצע את הרצח ועדת החוץ והבטחון של הכנסת תדון בנושא לבקשתי ביום רביעי החלטה אומללה של בג״צ לבטל את צו ההריסה על בית המחבל שרצח את חייל צה״ל עמית בןיגאל הי״ד  על המדינה לבקש דיון נוסף…  ללכת עכשיו לבחירות זה טירוףהדעת בראיון ל״יומן הבוקר״ בגל״צ הצגתי פתרון אפשרי למשבר התקציב מוזמנות ומוזמנים להאזי…  יחד עם תלמידיו הרבים וכל בית ישראל כואב את לכתו של חתן פרס ישראל הרב עדין אבן ישראל שטיינזלץ ז״ל  הרב היווה בחייו…  זה טירוף מערכות לשלוח הביתה את מורי פרוייקט היל״ה העושים עבודת קודש עם ילדים שזקוקים להם אני שב וקורא לראש הממשלה…  שנת הלימודים אני קורא לרה״מ נתניהו להתערב כרגע לא יפעלו עם תחילת שת הלימודים בין היתר תוכניות ההעשרה של קרן ״קרב״ פרוייקט ״היל…  מברך את המל״ג ואת חברי השר zeevelkin על הבחירה החשובה בפרופ׳ שירי נבוןונציה מarieluniversity לחברה בות״ת כשר…  פניתי היום למפקח על הביטוח כדי שיעצור אפליה גילאית ע״י חברות ביטוח  dandayan IsraelNitzan תודה לך דני על עבודתך המצויינת למען המדינה ובהצלחה בהמשך הדרך חג שמח לאזרחי ישראל המוסלמים והדרוזים לרגל חג הקורבן אלאדחה בריאות איתנה ואושר לכם ולבני משפחותיכם للمحتفلين بع…  בואו נעצור את שינאת החינם מספר מלים לפני תשעה באב   MyIsraelorgil חהכ gidonsaar במילים נחרצות מאד היום בדיון על שטחי c בכל ההיסטוריה של התנועה הציונית מה שקרה בשטח היה הדבר הכי משמ… הכנסת ציינה היום 15 שנים ל״התנתקות״ בזמן אמת נשאלו כל השאלות האם היא תקדם את סיכויי השלום האם המצב הבטחוני ישתפר…  YoavBlum 80 לפטירתו  מהו ז ז׳בוטינסקי בעבורי המצפן הערכי והמצפון הפנימי שלי וזאתמיום שעמדתי על דעתי עול ימים הייתי כשנפגשנואני וכ… SharrenHaskel בהצלחה שרן ״לעולם לא אעבוד יחד עם אנשים המוכנים לשעבד את דיעותיהם לדיעותי״                   80 שנה לפטירתו של זאב ז׳בוטינסקי  אנחנו במשבר ארוך וקשה ואמון הציבור חיוני להצלחה במערכה הזו פיקוח פרלמנטרי אמיתי אינו ״אינטרס״ של הכנסת הוא נדרש ל…  השינויים בעמדות הממשלה חופי הים הבריכות מסעדות בחוץ היו מחוייבי המציאות וההגיון וזוהי המחשה חיה נוספת לחשיבות הפיקוח הפרלמנטרי האיומים על ח״כ שאשאביטון מיותרים היא אינה שואלת את השאלות לבדה יש ויכוח עקרוני וחשוב האם נתוני התחלואה מצדיקים א…  realmadrid  ¡Buenos días CAMPEONES 34Ligas  RealFootball  YanivTzudik כן בין הדברים המוזרים בערב הזה נתונים על הדבקה בחופים מקום פתוח לא הוצגו בציבור מומחי הבריאות לא מצליחים להבין את…  אני מתקשה למצוא רעיון מסדר הגיוני בהחלטות שיובאו לממשלה הערב הן יביאו בוודאות להחרפת הפגיעה בכלכלה אך ספק אם ישיגו…  אסור לעבור את הגבול של גלישה לאנרכיה  אני קורא ליו״ר האופוזיציה yairlapid להתנער מדברי ח״כ רול  אתראיין עוד מספר דקות ב״יומן הבוקר״ של ReshetBet מוזמנות ומוזמנים להאזין ללא קשר לתוכן ההחלטות שקיבלה היום ועדת הקורונה  1 הכנסת אינה חותמת גומי של הממשלה  2 נכון יותר לשכנע את ועדות ה…  רק אמש צייץ גנץ ״הבשורות הערב חשובות מאוד״ עכשיו מתדרך ״הגורם הבכיר״ בכחול לבן ש״מפזרים כסף על האזרחים״ עמדה חלופית של החלופי XJVuTorl7xke5gr אשריך אריה על הליכה בדרך אביך שהיא דרך האמת ברכות להוצאת הספר וברוך הבא לטוויטר YonatanJaku המדיניות שgidonsaar קידם כשר הפנים הביאה לעזיבה הגדולה ביותר של מסתננים בקרב מדינות ה OECD בחצי מאה אחרונה הקמת חולות… Happy July4th to all the American people May our friendship and close bond go from strength to strength   realmadrid  ¡SergioRamos anotó el gol de la victoria en su partido 450 de LaLiga con el realmadrid  RMLiga  HalaMadrid YuvalRotem IsraelMFA AlonUshpiz Thank you for your service שמח שועדת החוקה חוק ומשפט של הכנסת בה אני חבר  אימצה היום את עמדתי לפיה לא יוטל סגר מקומי על עיר בטרם תינתן לרשו…  arutz7heb הסגר על טבריה חייב להדליק אור אדום  kannnews חכ גדעון סער לנציגת משרד הבריאות בדיון בוועדת חוקה אין שום דבר בהתנהלות שלכם שמצביע על מומחיות לסגור עיר זו לא שיטת עבוד… KnessetT עוזרת ראש שירותי בריאות הציבור דר ענת צוראל פרבר הודתה בדיון בוועדת החוקה הייתה טעות בנתונים שהובילה להחלטה על סגר בטברי… KnessetT בדיון בוועדת חוקה חוק ומשפט בנושא הצעת חוק להארכת תוקפן של תקנות שעת חירום אמר חכ gidonsaar השלטון המקומי הוא יחידה הרב… michaldiament השבוע נציין שמונה שנים לפטירתו של סבא שלי ראש הממשלה השביעי של מדינת ישראל יצחק שמיר   סבא שלי היה אדם של כתיבה תמי… 10elilevi מטורף פה  רות׳ס עכו   יש לחדש את המו״מ לצירוף סיעת ״ימינה״ לקואליציה ״ימינה״ היא חלק מהמחנה הלאומי וקרובה אידיאולוגית לליכוד אין סיבה ש…  yaarashapira הצעת חוק לצמצום התערבות בגצ בפסילת מועמדים לכנסת ביהמש העליון יוכל להפוך את החלטות ועדת הבחירות על פסילה רק בהרכב מיני… DaniCarvajal92 3⃣ y líderes  ¡¡¡Vamosrealmadrid  halamadrid realmadrid hastaelfinalvamosreal realfootball laliga dc2… עת תיקון על חובתה של הכנסת לעגן בחקיקה את דוקטרינת ״פירות העץ המורעל״ מאמרי בglobesnews  DFNnewsIL ״זאת זכות לשרת את עם ישראל כחבר כנסת״ ח״כ גדעון סער בראיון מיוחד לחדשות  DFN Drormandel    על הכלכלה במשבר הקורונה ועל זו שתהיה כאן לכשיסתיים הראיון שלי בתוכנית הכלכלית של ארז צדוק בarutz20  arutz20 גדעון סער מציע לממשלה להעביר כסף מהמגזר הממשלתי למגזר הפרטי שזקוק כעת לתמיכה צפו    gidonsaar  IsraelHayomHeb הצעת חוק ביהמש יפסול ראיות שהושגו באמצעים פסולים • gidonsaar ההצעה תשמור על זכויות הנחקרים gideonallon   GLZRadio פסילת חוק ההסדרה  חכ gidonsaar אצל efitriger התוצאה לא הגיונית וגם בעיתוי תמוה  מה הדחיפות לתת פסק דין על חוק שחוקק לפ… פסיקת בג״צ רק מחדדת ומחזקת את הצורך בהחלת החוק הישראלי על שטחי ההתישבות היהודית ביהודה שומרון ובקעת הירדן זה ישנה…  מברך את צה״ל והשב״כ על מעצר רוצחו של עמית בן יגאל הי״ד יש להרוס את ביתו ללא דיחוי arutz7heb החלטת בגץ פוגעת בהרתעה  על החלת הריבונות ו״עסקת המאה״ הראיון שלי לErelSegal וRoyIddan הבוקר בradio103fm  KnessetT חכ גדעון סער על החוק הנורבגי בוועדת החוקה חוק ומשפט אי אפשר להתעלם מההיבטים הפוליטיים שביסוד ההצעה בנוסף הציע לאמץ… YakiAdamker משתתף בצערכם בכאבכם ובאבלכם ושוב בתחתית הרשימה של מה שראוי להגנה האינטרסים של המדינה ואזרחיה  ״בליבנו בליבנו רק שיר אחד קיים לך ירושלים בין ירדן וים״  יום ירושלים שמח  israelconnect naftalibennett giladerdan1 בהחלט למיטב זכרוני היטיב להנציח זאביקו הגדול  ZSonenzon מדיניות של העלאת היטלים והטלת מכסי מגן על חמאה או על מלט  עלולה להעלות את יוקר המחיה ולפגוע באזרחי ישראל הליכוד…  אסור להדהד ולשרת את התעמולה הפלסטינית לשרת את האינטרסים של הרשות הפלסטינית ואת האיומים שלה לרבות איומיסרק  ״אי שם בתוך הלב עיר שלום״ זאב ז׳בוטינסקי     cohenmeirav מזל טוב DayanUzi נשב על זה עוד השבוע DayanUzi מזל טוב עוזי ברוך הבא למועדון עקב פניות עיתונאים וכדי למנוע פרסומים שגויים ההצעה היחידה לה סרבתי בנימוס היא לכהן כשגריר באו״ם ובוושינגטון וזאת…  זאת זכות גדולה לשרת את עםישראל ומדינת ישראל כחבר כנסת אני קורא לראש הממשלה נתניהו לנצל את הדחיה בהשבעת הממשלה כדי לחדש  את המו״מ עם ״ימינה״ להצטרפותה לקואליציה הפערים נ…  miriamperetz יישר כח מרים arutz7heb גיבור ובנם של גיבורים גדעון סער ניחם את משפחתו של עמית בן יגאל gidonsaar  על גיבור ישראל סמ״ר עמית בן יגאל הי״ד  idfonline דובר צהל מוסר את שמו של לוחם צהל סמלראשון עמית בן יגאל זל לוחם בסיירת גולני בן 21 מרמת גן סמלראשון עמית בן יגאל ז… giladerdan1 בהצלחה alizalavie המהפכה הציונית  המהפכה המצליחה ביותר של המאה העשרים הרצל הגדול מכולם  דחייתה פה אחד של העתירה בסוגית הטלת הרכבת הממשלה על נתניהו והנמקתה רק מעידה שלא היתה כאן שאלה משפטית כמו שלא היתה…  idomaor זה לא נכון הפנומן שהיטה את זרם ההסטוריה דברי במליאת הכנסת ב״יום הרצל״    Israelcohen911 מזל טוב ישראל High Court is drunk on power    בגץ מציג שבוע של שיכרון כוח  כך נראה אקטיביזם שיפוטי על סטרואידים בפחות משבוע ביטול חוק הפקדון למסתננים ביטול איכוני שב״כ  קורונה צו בינים…  zeevelkin מזל טוב זאב ברוך הבא למועדון לארץישראל עולים בבגדי חג אבי שמואל ציוני מובהק לפני 55 שנים על האוניה ״תיאודור הרצל״ בדרך לארץ עצמאות שמח…  nbjovsr88 שלא תדעו עוד צער AvishayBenHaim יאיר הונחה על שולחן הכנסת הצעת החוק שלי לשימוע למועמדים לשיפוט בביתהמשפט העליון  את ההצעה שאותה הגשתי לראשונה בכנסת ה…  gidonsaar החייםבזכותם אומרים אורי צבי גרינברג  amichaig מזל טוב GabriellaBerzin רפואה שלמה גבריאלה הרב אברהם ישעיהו הבר פורץ דרך בתחום עידוד התרומות להשתלת כליה הותיר אחריו בפטירתו הערב חלל עצום הקדיש את חייו…  החלטת בג״צ בנושא חוק הפקדון של המסתננים היא שגיאה חמורההיא פוגעת באחד הכלים האפקטיביים האחרונים שנותרו לעידוד יציא…  orbach131 שלא תדעו עוד צער ברכתי את נשיא איחוד הצלה ידידי היקר אלי ביר שהחלים מנגיף הקורונה ונחת בארץ לאחר שבועות ארוכים בהם היה מאושפז במיאמ…  YVider מזל טוב יעקב zalmanwolff מזל טוב זלמן היום לפני 77 שנה פרץ מרד גטו וארשה לוחמי האצ״י והאי״ל הדהימו את מכונת החיסול הנאצית בגבורה ובתעוזה שכמותה לא נראתה…  davidibension מזל טוב דוידי ה״מענקים״ לא יספיקו כדי להציל את העצמאים כל יום שעובר עסקים נוספים קורסים חוזר יש לפצות את העסקים בזיקה לירידה ב…  olgawaknin מזל טוב אולגה בריאות איתנה ונחת ok125125 תודה רבה ובעיקר תודה ל״רפואה ושמחה״ העושים למען הקשישים והבודדים פסח כשר ושמח geulaeven מה נשתנה הלילה הזה מכל הלילות שגם אמא של גדעון לא איתנו בסדר והכנתי את האושפלו במקומה על פי הוראותיה המדוקדקותפסח כשרשמח… droreydar פסח כשר ושמח אמבשטורה emmanuelnavon אני מודה ל gidonsaar על מאבקו עבור העצמאים ומבקש להמחיש את דבריו אני גם שכיר וגם עצמאי ואשתי עצמאית בלבד הכנסתנו נפ… RonHuldai יישר כח אהבת כלל ישראל במקום שינאת חינם  ממתק לשבת שירו הענק של אורי צבי גרינברג ״אחי יהודיהפאות״ שבת הגדול שלום  geulaeven זאת חברתי הטובה חיה אישה מושלמתאמא לשמונה ילדים בבני ברק מקפידה על כל ההוראות ולא מעיזה לצאת מבית לכל מי שקורא לה ולאחר… Israelcohen911 משתתף בצערך ישראל שלא תדעו עוד צער צעדים נדרשים לסיוע לעצמאים ועסקים קטנים ובינוניים  אתראיין עוד מספר דקות בתוכנית ״נכון להבוקר״ בGLZRadio מוזמנות ומוזמנים להאזין כנבחרי ציבור עלינו לתת דוגמה אישית  הראיון המלא הערב בערוץ 12 בערוץ הטלגרם שלי  notkin1985 זה לקח שבועיים וחצי ולא מעט כעסים ותסכולים אבל העובדה הברורה שבמשרד החינוך הקשיבו לבסוף אני מודה למשרד בראשות realrafipe… אתראיין במהדורה המוקדמת של חדשות 12 בשעה 1930 לערך מוזמנות ומוזמנים לצפות מי שיכול וצריך לפתור את בעית  ״גודל הממשלה״ הוא  gantzbe  15 תפקידי שר ל58 של גוש הימין זה מפתח סביר ואפילו צנו…  TomerAvital1 כן  לא צריך להמתין לחקיקה או לתוכנית ממשלתית כל אחד מחברי הכנסת יכול  כבר היום לעשות את זה  כל שקל שנחסך במגזר הציבורי צריך להיות מושקע במגזר הפרטי בתמריצים וסיוע לעצמאים למשל כדי שהכסף לא ייצא מהמשק בזמן האטה בנוסף לערך הכלכלי  הערבות ההדדית והדוגמא האישית הם יסודות חשובים בהתמודדות עם משבר הקורונה 2  קיצוץ משמעותי בשכר לתקופה שתוגדר לבעלי משכורות גבוהות במגזר הציבורי ובכלל זה שרים חבריכנסת שופטים מנכ״לים ו…  בימים בהם עיקר נטל המשבר הוא על המגזר הפרטי חשוב שביסוד התוכניות להקמת הממשלה ינקטו הצעדים הבאים     1 ״ממשלה רזה…  ErezZadok1 משתתף בצערכם  שלא תדעו צער nbjovsr88 NehemiaGA רפואה שלמה IsaacHerzog יש לי חבר יקר נתן שרנסקי קודמי בתפקיד אסיר ציון שישב בצינוק ובבידוד נתן נענה לבקשתי והסכים לתת 5 עצות לאלה שבבידוד ל… notkin1985 זו מטרתי  לדחוף למתן המענים אם אתה חושב שאני יכול לסייע במשהו  תעלה מולי בפרטי notkin1985 רון שלום אני מניח שיש דיפרנציאליות במענה לפי סוג לקות אבל מאנשי מקצוע אני מבין שיש מענים הוראה משימות הדרכה להורים YairOrbach הבדל בסיכומים הקיימים בין ארגון המורים להסתדרות המורים הערב בישיבה אצל מנכ״ל משרד האוצר שי באבד צריכה להתקבל החלטה על החזרה לאלתר של הלמידה מרחוק לתלמידי ישראל תשומתל…  sheffipaz hamakom סבבה גדעון סער לא היה שר פנים שגירש מסתננים יותר ממנו emmanuelnavon מול אובדן הבושה השתוללות הצייצנים וחנופת הצייתנים יש אחד בליכוד שמפגין אומץ שומר על קור רוח ומציל את כבוד התנועה של… יושב ראש הכנסת YuliEdelstein רשאי ואף צריך לעמוד על עמדתו בהליך המתקיים עתה בבג״צ דבר אחד אינו בא בחשבון קריאות…  שוחחתי עם שר הפנים ariyederi בעקבות הפרסומים בענין הארכת שעון החורף הכוונה להאריך נקודתית בחודש את שעון החורףכך…  gMnukAg0bYx3jAY תודה אורנה gMnukAg0bYx3jAY גדעון  סער   זה הזמן להגיד שהרבה בזכותך למידה מרחוק זה סיפור הצלחה  תכנית התקשוב הלאומית  שהובלת עכשיו מוכחת כצעד…  לצוותים הרפואיים המופלאים על העבודה המסורה שהם עושים ועושות בימים אלה ועל הבחירה בדרך חיים ובמקצוע של שליחות הצטרפו כעת לערוץ הטלגרם שלי  וקבלו עדכונים היישר לנייד שלכם gtgt   בכל משבר גלומות גם הזדמנויות במשבר הנוכחי לפי מאפייניו יש פוטנציאל לקפיצת מדרגה במעבר הרשויות למתן שרותים דיגיטל…  odedrevivi gidonsaar צודק הבוקר יוצאת קריאה של מרבית ראשי הרשויות נגד המהלך הזוי שבכל התרגילים ביקשו לבחון את הלמידה מרחוק וכאשר יש… ההסכם הכולל למעשה ויתור על שיגרת הלמידה מרחוק הוא טעות חמורה לא רק בגלל הצורך לשמור על שגרת למודים וקשר בתקופה זו…  GermanYael1 רפואה שלמה יעל Italia A country is made up of people but its their union that makes it great Yesterday afternoon thousands of people with a sing… geulaeven יומיים  בלי גןאני בתיה עוזיאלמציירים בפנדה על ארגז  geulaeven ״החופש הגדול״ של מרץ משחקות ב״חוף הים״  kannnews חכ gidonsaar מהליכוד לrbinyamini על ממשלת חירום אנחנו בעיצומו של משבר ענק הנזקים למשק עצומים ברור לחלוטין שצריך הפסק… אתראיין בשעה 0715 לערך ב״יומן הבוקר״ של ReshetBet  מוזמנות ומוזמנים להאזין הקמתה בהקדם של ממשלת אחדות  ולו לתקופה קצובה  היא צו השעה כדי להתמודד עם משבר הקורונה שהשלכותיו מוחשיות ומרחיקות…  ״והימים האלה נזכרים ונעשים בכל דור ודורוימי הפורים האלה לא יעברו מתוך היהודים וזכרם לא יסוף מזרעם״ אסתר ט כח…  geulaeven אוקיי היא אלזהבעיניה נחשבת יותר אני לוהקתי לאנה פורים שמח   dandayan מִנִּי דָן עַד בְּאֵר שֶׁבַע מִגִּלְעָד לַיָּם אֵין אַף שַׁעַל אַדְמָתֵנוּ לֹא כֻפַּר בְּדָם  דָּם עִבְרִי רָווּ לָשֹׂבַע… realmadrid1191 ״טוב אשר תאחז בזה וגם מזה אל תנח את ידך״ freyisrael1 קרית מלאכי גדעון סער וגדי יברקן משלבים ידיים לפי סער אחוזי ההצבעה גבוהים יותר משני הסבבים הקודמים לא זוכר אף פעם שעמד… מחל  realmadrid  FP RealMadrid 20 FCBarcelonaes  viniciusjr 71 marianodiaz7 902 RealFootball  Emirates  28 שנים ללכתו של מנחם בגין מפקד האצ״ל וראש הממשלה השישי של ישראל האדם והמנהיג ששבה את לבנו בנעורינו ושם נותר יהי…  amichaig צילמתי סרטון תעמולה ותמרוץ צפו עד הסוף מה אנחנו הליכודניקים עושים יום לפני בחירות ומחר גשם פתקי מחל  אתראיין בתוכנית ״נכון לעכשיו״ בGLZRadio בשעה 0805 מוזמנות ומוזמנים להאזין אתראיין הערב בתוכנית ״לפני החדשות״ בערוץ 13 Reshettv בשעה 1900 ובמהדורת החדשות של arutz20 בשעה 2000 מוזמנות ומוזמנים לצפות ערב טוב תלאביב  עוד 8 ימים לנצחון  HaimJelin משתתף בצערך חיים הצטרפו כעת לערוץ הטלגרם שלי  וקבלו עדכונים היישר לנייד שלכם gtgt   הראיון המלא ב״פגוש את העתונות״  pgoshMTP 9 ימים לבחירות gidonsaar מגיע לאולפן לריאיון ראשון ובלעדי ״פגוש את העיתונות״ מחר ב 1900 ערוץ 12   RMatsliah  N12New… kannnews חכ gidonsaar בוועידת הנשיאים של הארגונים היהודיים בארהב על תוכנית טראמפ אני מקווה שאחרי הבחירות תהיה ממשלת ימין כדי ש… OstrovA MK gidonsaar at COP2020 acknowledging tremendous support and friendship of US Trump Administration to Israel adds “A P… ״מסר של אחדות מסר של התגייסות״  הערב בנשר  voiceofajew הערב בת״א  יום הולדת 90 וערב הוקרה לזמרתshula557 שולמית לבנת ״זמרת המחתרות״  לדעתי אוחזת בשיא ישראלי לזמרת פעילה  לאורך… amichaig היכנסו לקישור תימכו באהבה זה מפעל חיי ודבר אדיר וחשוב באהבת אדם עם ארץ ומסורת תבורכו בכפליים שפע וטוב ת ו ד ה   ״כולנו ביחד למען נצחון הליכוד״ הערב בבתים  ב2003 שגה בית המשפט העליון כשהפך ברוב דיעות את ההחלטה על פסילת בל״ד  היום טעה כשהפךברוב דיעות את ההחלטה על פס…  עו״ד דן אלדד הוא מועמד ראוי ומתאים לתפקיד מ״מ פרקליט המדינה משפטן מנוסה רציני שקול ונבון realmadrid  ¡21 partidos invictos  RealMadridAtleti  HalaMadrid </t>
+  </si>
+  <si>
+    <t xml:space="preserve">מפגינות ומפגינים אלף מטר מהבית  וכמובן חבריי לסיעה YairGolan1 NitzanHorowitz מסתכנת שאפספס מישהוי אבל osamasaadi63 YSegalovitz KElharrar ofercass eliavidar odedforer בלתי נתפס היה לצפות בלילה באובססייה הליכודית בכנסת לא חולים לא מערכת הבריאות ולא מובטלים עניינו אותם רק חיסול המ…  אלפי חולים עשרות מתים ומאות אלפי מובטלים חדשים למי אכפת מה צעקו לו  רק שתבינו הכנסת מתכנסת עכשיו ערב יום כיפור ובאמצע משבר לא בשביל מתווה פיצויים לא בשביל בריאות הציבור אך ורק לש…  שר האוצר שר הכלכלה כל שרי כחול לבן שראו במו עיניהם את אירועי הלילה ויודעים שהחלטות מונעות משיקוליו של נאשם בשוחד…  לנתניהו אין מנדט לנהל את ענייני המדינה אי אפשר לסמוך על שום החלטה שלו במשבר הגדול בתולדותנו אזרחי ישראל מופקים לג…  הממשלה מתכנסת בשעה זו להחליט על סגר שמשמעותו עוד מאות אלפי מובטלים חצי מה100000 של השבוע האחרון הם מוצאים לחל״ת…  הבוקר בוועדה לזכויות הילד על ״מחשב לכל ילד״ אותה הבטחה נושנה היא עכשיו צורך אקוטי כשעתידה של מערכת החינוך לא ברור…  עשרים ושמונה אלף מובטלים חדשים רק ביממה האחרונה אבל ההפגנות ובכן מסתבר שחוות הדעת המהוללת של מומחה ה״משילות״ מציעה לממשלה להשתמש בתקנות שעת חירום כדי לעקוף חוק שחוקקה הכנסת רק…  הזוי ומפחיד שבזמן משבר בריאותי וכלכלי חסר תקדים ממשלה מתעסקת באובססיביות בהשתקת המחאה נגד עצמה ואגב מי שחושב שחוו…  והנה הסיבה למה בממשלה הזו אין וגם לא תהיה אחריות לא דוגמה אישית ולא טיפת מוסר או הגינות בסיסית כי בראשה עומד נאשם…  ״הילדים לא שמרו״  רק ממשלה שהמילה אחריות זרה לה לגמרי תשלח ילדים להחליף בין חמש קפסולות שונות ואז להאשים אותם בזה  MeravMichaeli חיבוק משתתפת בצער קודם אקלל חצי מהעם שאני שר בממשלה שלו ואחכ נריב  מדכא ומקומם שזה הדיווח הראשון של השנה הסגר קצת עצוב ובודד עבור כולנו יש כאלה שעבורן זו סכנת חיים יש מה לעשות ויש…  SherriPizza liliLongstockin יום הולדת שמח ושנה טובה נזכרת שעזבתי בית חולים ליולדות עם בת יומיים בפברואר 2020 וזה היה נראה מוזר שהופסקו הטיסות לסין אחרי חודש העולם נעצ…  בתי חולים בפריפריה התחילו להעביר חולים ומונשמים למרכז ומש׳ הבריאות כבר הוציא הנחיות לביטול ניתוחים לא דחופים ולסגי…  כל הכבוד לעיריית תל אביב יפו מהיום גופן של נשים הוא לא סחורה  נזכרת שהייתי חברת מועצה וביקשתי לסגור את מועדוני הח…  urizaki סבבה אבל איך לעסוק באובססיביות בנסיון לעגל כלפי מטה את מספר הנפטרים וכלפי מעלה את גילם ובאופן כללי להסביר…  הייאוש המוצדק מהטיפול הכושל בקורונה ומהמצב הכלכלי מביא יותר מדי אנשים להמעיט בחומרת המחלה המאבק שלנו צריך להיות על…  EmilieMoatti חיבוק אמילי אהובה אין ספק שהגענו למצב הזה בגלל כשלון לטפל בקורונה בזמן ובצורה נכונה אין ספק שראוי להשקיע במערכת הבריאות אחרת כל צעד…  לצערי הדיון היום בוועדת הקורונה גבל בחלקיו בהכחשת קורונה לדוגמה הוצג נתון חשאי על פיו באחד מבתי החולים 23 לא נפט…  היבט בכלל לא מדובר לגבי הסגר הקרוב כשכולנו נסתגר בבתים עם המשפחות יש כאלה שעבורן הבית הוא מקום אלים ומסוכן בתקו…  בעולם שבו את ההחלטות מקבלים גברים ועם הילדים נשארות נשים הרי ידוע שגבר זה 50 מכל משפחה  ההפגנות לא יכולות להמתין לסיום המשבר כי ההפגנות הן נגד ניהול המשבר ובפרט נגד ניהולו ע״י ראש ממשלה נאשם בשוחד אין כ…  NitzanHorowitz YairGolan1 Ahmadtibi AidaTuma AyOdeh idanroll MKMickeyLevy KElharrar MeravMichaeli HVazan…  פניתי עם קבוצת חברי כנסת משמונה סיעות לוועדת הכספים בדרישה לקיים עוד השבוע דיון והחלטה על חבילת פיצוי כחלק מההחלטה…  במקום להילחם כל אחד על המגזר שלו על שרי הממשלה להתאחד ולהחליט על רשת בטחון נדיבה ופיצוי הולם לעובדים לעסקים ולענפ…  JaljuliMaisam בהצלחה ישראל נכנסת לסגר בגלל דגל אדום שמרימה מערכת הבריאות לא מיותר להזכיר שוב את ההרעבה השיטתית שהביאה אותנו להיות המדינ…  השבוע נחקר פעיל חברתי על שלט אנס בגשר רחבעם זאבי וצייצנית נוספת על ששיתפה קללות שהופנו כלפיה ברגעים אלה ממש מחוץ…  אין דבר כזה או בריאות או כלכלה בדיוק בשביל זה יש ממשלה כל הגבלה של המשק כדי להוריד תחלואה חייבת להיות מלווה ברשת…  michaelzil מה זה לא רזולוציה זו ארכיטקטורה בחיים לא נגעתי בקונסולה ואני יכולה לצפות בזה שעות OECD פרסם היום מסמך שקורא למדינות הארגון ״לחשוב מחדש״ על הכלכלות שלהן לאמץ מדיניות שמתעדפת מדדים כמו קיימות רווחה…  Ayeletnnv חיבוק RamiHod זה פשוט לא ייאמן במה מתעסק ראש ממשלת ישראל בזמן המשבר הבריאותי והכלכלי החמור בתולדות המדינה מעל 3500 חולים מאומתים ביום מעל… RamiHod זה מה שצריך לעשות   RamiHod 17 הפיילוט כדי לבדוק אם יש ביקוש הוא נרמול זוחל של תופעה פסולה נפרד זה לא שווה נקודה גם במסלולים האקדמים הנפרדי…  לקראת ראש השנה תרמתי לאגודה לזכויות האזרח  ארגון זכויות האדם החשוב בישראל תודה שאתם עומדים על הזכויות של כולנו כ…  zionnenko צפיתי בדמעות קורה לא פעם שהצדק ברור וזועק לשמיים ומכל מקום ובעיקר מהממשלה נתקלים בעולם הפוך גם קורה אם כי פחות שהצדק יוצא לאו…  peretzsami הועלה לדרגת חף מפשע עאידה שהיא בדרך כלל חברת כנסת נחושה ונוקבת מחייכת פה חיוך נמס ואני שמחה שאחראית עליו הבת שלי שמחתי להפקיד אותה היו…  אישור תקציב המדינה נדחה ב100 יום אבל מדברי נציג האוצר בו׳ לביקורת המדינה עולה שאין עבודה על הכנת תקציב מכיוון שלא…  בשולי החדשות הבוקר ידיעה קטנה על שריפה בבית הספר ביישוב נווה שלום שריפה שניה בשבוע הערכת המשטרה הצתה אסור לזה ל…  המשותף בין מנדלבליט וגמזו שניהם נפלו קורבן לקמפיין האנטי מקצוענים בשירות השחיתות והפופוליזם של ביבי ככה נבעטים של…  hadarse מזל טוב היום 6 בספטמבר הוא יום השכר השווה היום הגבר הממוצע סיים להרוויח את מה שייקח לאישה הממוצעת עד סוף השנה להרוויח פארסת הטיפול בקורונה היא הוכחה ברורה מדוע נאשם בשוחד פשוט לא מסוגל למלא תפקידו נאמנה הכניעה של נתניהו לחרדים היא ה…  המעצר של אמן בתחפושת היתולית הוא פארסה שיכולה היתה להיות סתם מגוחכת אם לא היינו נזכרים במופע האימים של אשת ראש הממש…  מנהיגות מקומית אחראית יש כמה שרים בממשלה שצריכים לקחת דוגמה  גאה במיקי גיצין מנכ״ל הקרן החדשה שקם כל בוקר לעשות את ישראל טובה יותר הוא גם אדם מסור וחרוץ באופן יוצא דופן שלא…  NadavPerez kereneubach kannnews RotemPV גאווה בישראל אין מפכ״ל אין פרקליט מדינה אין תקציב ואין ישיבות ממשלה פספסתי משהו  מסתכנת בלהישמע הזקנה שאני אבל כשהייתי עוזרת פרלמנטרית הייתי עוברת בספרית הכנסת בשביל עיתונים שלא הגיעו הביתה וקטעי…  האובססיה של הליכוד ונתניהו לרבין היא כבר מזמן עניין לפסיכואנליטיקאים  AyOdeh מזל טוב אבו שאם השבוע העליתי בכנסת הצעה נגד תרבות האונס דיברתי שם על הפמיניסטיות הצעירות שמובילות מאבק חדש ונחוש היום תרמתי לעמות…  Shiritc בהצלחה את עיתונאית מצוינת mikiros1 מזל טוב סבא׳לה  ריחוק חברתי  הכנסת מצביעה על הסתייגות של אחמד טיבי לפיה הרוטציה תקוים הליכוד וכחול לבן נגד נתניהו וגנץ יצאו מהאולם  אנרכיסטים פרוגרסיבים פריבילגים נדמה לי או שהטוקבקים מימין לקוחים מסמינר תיאוריה וביקורת בחוג לסוציולוגיה ניצב דורון ידיד הודיע כרגע בוועדת הפנים שסנ״צ גואטה שתועד מכה מפגינים יחזור לשטח במוצ״ש הקרוב זה מתן היתר לאלימות…  המדינה זה אנחנו  המפגינים לא באו ״משולהבים לעימות״ כן הם נלהבים וזועמים כי בראש המדינה עומד נוכל נאשם בשוחד שללפחות חצי מהציבור א…  השר דרעי ישתתף בדיון אצל רה״מ בנושא נסיעה בראש השנה לאומן ראש השנה יחול ב18 בספטמבר אותו שר דרעי אחראי על כניסת…  מישהו יודע למה כחול לבן יושבים עכשיו לעוד מו״מ עם מושחת ונוכל במקום לשבת למו״מ עם סיעות האופוזיציה על הקמת ממשלה חלופית מחר תודה  ״פשרת האוזר״ במקום להציע להתפשר עם נוכל עדיף שהאוזר יפסיק את הפסילה הגזענית של נציגי הציבור הערבי ויתן את האצבע ה…  LimorYoav Ayeletnnv אם אין טורטית הסקר לא תקף יש ממשלה אחרת כבר בכנסת הזאת ללא בחירות לגוש המרכזשמאל יש רוב 61 בכנסת הנוכחית כל מה שצריך לעשות זה שכחול לבן י…  מוסי עם המשפט שלו כמזכ״ל שלום עכשיו שנכנס להסטוריה   חוזרת מההפגנה דרך זה לאיזה עולם רעיל ומסוכן הבאתי את שתי הבנות שלי אין ברירה אלא לתקן אותו  הילדה של כולנו את לא לבד  עכשיו נגד תרבות האונס  radio103fm דיון בכנסת על בלוני ההטרדה נגד אשת רהמ  חכ תמר זנדברג tamarzandberg מרצ לא כל מה ששרה נתניהו אומרת זה נכון זה הפך… אני רק שאלה במסגרת זה שהכנסת היא הריבון ויש הפרדת רשויות האם רק לבית המשפט אסור לבטל חוק אבל לשר מותר עמדתו האיש…  בוועדת קורונה המשך הסאגה הקפקאית של משפחות קרועות שרוצות להתאחד מש׳ הפנים מתייחס אליהן כאל משפחות שמבקשות מעמד הת…  האמת היא שהנתון שרוב מוחץ ציבור הישראלי לא מתעניין בסיפוח הוא עקבי וחוזר על עצמו עוד כש״ריבונות״ היה הדבר החם בעיני…  למה מגן המושחתים הוא גם מגן הזנאים  בלפור הערב ביבי הביתה  מתברר שהיום זה יום הולדת 110 לנתן אלתרמן בעברית יש המון שירים על העמק וההר הקיבוץ והכפר אבל מעטים הם שירי האהבה…  IsaacHerzog מזל טוב חמודים איש ימין בכיר מודה הגדה המערבית לא שלנו  הנרטיב שמנסים למכור כאילו נשברה הפרדיגמה שטחים תמורת שלום פשוט לא נכון הנה עובדה כדי להגיע לנורמליזציה פומבית יש…  GLZRadio יור סיעת מרצ tamarzandberg הסיפוח הוא אסון לישראל וביטולו היא ההחלטה הנכונה כעת יש לעשות את הדבר החשוב ביותר  הסכם שלום… האנרכיסטים החוליגנים שמפעילים אלימות נגד כוחות הביטחון אמר אף שר בממשלה אף פעם לא שמאל לא מגנים  אשה מוכה  GLZRadio אשת רהמ שרה נתניהו מרגישה שעברתי הטרדה מינית אני כמו אישה מוכה חכ tamarzandberg לירון וילנסקי וbardugojacob זה ג… karineb הכי פשוט לנסות להשתיק פוליטקאיות דרך המשקפת המינית והמשפילה שרמוטה זונה כלבה ועוד שאר ירקות  בעידן המידע זה כבר לא מרתיע… YinonMagal AvishayBenHaim מנסים שבית משפט יכריע אבל ביבי מפחד AvishayBenHaim חבר אני נולדתי ב 76 ולמי שרוצה להשאיר על כנו את המהפך של 77 יש לי עצה לא לקחת שוחד אירועי השבועות האחרונים הם ב ד י ו ק ההוכחה למה נאשם בשוחד לא יכול לתפקד כראש ממשלה צהריים ואין תגובה לטרור המתנחלים ביצהר אפשר לדבר על ״קומץ״ ועל תושבי יצהר ה״חלוקים״ אבל האלימות שמקבלת גיבוי בשתי…  NadavPerez idanlandau למפלגות אסור לגייס כסף מבעלי הון מעבר לתרומה של 2000 שקל בשנה למשק בית בשנת בחירות ו1000 ב…  אין כוח בעולם שיעצור מאבק צודק של אימהות כואבות  האימהות השכולות בחברה הערבית יצאו למאבק על הדבר הכי בסיסי שיש הח…  בעקבות פניה שלי מח״ש תבדוק את התנהלות השוטרים בהפגנה בתל אביב בה הוכו מפגינים  urizaki noalandau ואם אצטרך פתאום מטריה באוגוסט noalandau שומרת לפעם הבאה ש urizaki יתלונן שיש לי יותר מדי דברים בתיק זה באמת גזל שאין לתאר לא רק שעבר חוק שהמעסיקים צריכים להפקיד 20 ממשכורת עלובה גם ככה מסתבר שהם לא הפקידו ועכשיו…  LinoyBarGeffen מרגש מזל טוב פשוט לא ייאמן שכל הדברים שהיו ברורים כשמש בצהרי היום מדווחים עכשיו כחדשות מפתיעות מה ביבי נוכל ועבד על כחול לבן…  akivanovick לפעמים האופוזיציה יודעת לנהוג בממלכתיות להלן שאילתא דחופה שהוגשה בשעה האחרונה לנתניהו ע״י חברת הכנסת tamarzandberg  kannnews חכ tamarzandberg לקלמןליברמן אם כחול לבן לא היו נכנסים לממשלת נתניהו הוא היה כבר מחוץ למשחק זה הזמן לחזור ליוזמה של… אז מה עם קבינט הפיוס אדירים  מוצ״ש בגשרים דמוקרטיה  הערב בפינתנו ״קיצונים משני הצדדים״ סימטריה בין צד שרוצה לקיים הסכם ובין צד שרוצה להפר אותו ביבי גנץ כתבה מבהילה באולפן שישי מתחקה בדיוק מצמרר אחר המסלול הסתה —gtgt אלימות נתניהו מאשים את המפגינים בהפצת מחלות ועשיית צ…  lironmatalon בסרטון שערכתי עבור tamarzandberg קשה לפספס את ההסגברה לא רק שנתניהו לא היה אומר את זה לח״כ גבר אלא גם שלח״כ תמר זנדב… gershuni שזה מצחיק כי בכתבה מצוטט מחקר לפיו הפניה בלשון נקבה הורידה את הישגי הגברים משמע עד היום היה נהוג פקטור …  adibenhur2 אני מניחה שאדוני יודע לקרוא בכתבה מצוטט מחקר לפיו הפניה בלשון נקבה מורידה את הישגי הגברים מכיוון שאינ…  חוזרת לכתבה הזו מהבוקר בגוף הכתבה מצוטט מחקר לפיו הפניה בלשון נקבה העלתה את הישגי הנשים ופגעה בהישגי הגברים צ…  כל הכבוד  eyaleyal564537 tamarzandberg תמר שמעתי אותך צועקת לו  מהיציע שוחד  שהוא שאל מה המילה שאביו אמר לו צחקתי בקול ⁦⁩⁦⁩ מה שמצחיק זה שהייתי היחידה שתמכה במענק שלו  שומעת את נתניהו מסית ומשתלח ומתקשה לתפוס כמה שנאה יש לראש הממשלה כלפי האזרחים של המדינה שלו LinoyBarGeffen ברור שתמוז הגיוני סה״כ ששרת התפוצות תסייר מחוץ לישראל  ״החרדים נתנו ערבות לממשלת אחדות״  אם גנץ קונה את הבלוף הזה זו תהיה בדיחת הבדיחות תקציב מאושר בכנסת הוא חוק לאשר תקציב ״דו שנתי בממשלה וחד שנתי בכנ…  מהתיעוד המצולם ומהעדות זה נראה כמו פשע שנאה מהסוג הגרוע ביותר יש לטפל בו במלוא החומרה כמו כן הגיע הזמן להתיר את ק…  למי שצפה אתמול בחדשות ותהה איך ולמה מדברים שוב על סגר ולמה למרות ההתייצבות בנתונים נתניהו שוב במוד הפחדה הוא מפח…  ה״סטודנטים״ הזרים שיגיעו בחגים בתנאים משופרים  סבבה אבל מה עם משפחות של ישראלים ישראלים שלא ראו את הילדים שלהם…  תתחיל מ״חייזרים״ ״מקבלים כסף״ וכמובן ״מפיצי מחלות״  רק ליהודים שהתחתנו ברבנות  האפליה פשוט זועקת לשמים 12000 בחורי ישיבות זרים ייכנסו לישראל בזמן שאלפי משפחות של ישראלים חלקם הורים לילדים עד…  IssDean AGvaryahu אז מסתבר שיש לו אח בגלל הבחורילות  לפי מה שכתוב פה ההפגנות זה המקום הבטוח ביותר מפני קורונה והדבר היחיד שמסכן בהן זה ובכן השימוש במכתזית כי מרטיב…  איזה מזל שכחול לבן ״מנעו בחירות רביעיות״  יש עכשיו דרישה מהתקשורת לסקר פחות את המחאה ואני שואלת מה עם דרישה מהמרואיינים לומר אמת דרישה פשוטה כזאת לא לשקר…  מבחינת נתניהו הקורונה באה לעולם כדי למנוע את ההפגנות נגדו בינתיים ממשלת ישראל היא מדגרת קורונה יותר מכל ההפגנות יחד תוספת משובחת לעמוד הדעות של הארץ מעניין ומקורי akivanovick  תומכי ביבי מתחלקים עכשיו ל2 1 פליז פליז תפסיקו להפגין 2 טוב אולי אם נעצום את העיניים ממש חזק אולי זה ייעלם  הם מ פ ח ד י ם YinonMagal באמת שלא הבנתי מי שואל אותך YinonMagal מה אתם רועדים רוצים להפגין זו דמוקרטיה ״על מה הם מפגינים״ זו השאלה החדשה תגידו מי שואל אתכם מפגינים שביבי יילך הביתה כן שמעתם נכון מושחת מנותק וכו…  בלפור עכשיו מנותקים נמאסתם  pgoshMTP עכשיו ב״פגוש את העיתונות״ בערוץ 12 סקר מיוחד  מי אשם בהליכה לבחירות ומה סיכויו של איזנקוט בפוליטיקה הפרשנים שלנו razibar… מזכירה שהסמכות להכריז על התארגנות כארגון טרור נמצאת בידי שר הביטחון ושפניתי אליו אתמול כדי שיעשה את זה על לה פמיליה…  אני שייכת לאלה שחושבות שנתניהו הרוויח ביושר את החשדנות כלפי כל צעד שעושה אבל בלי שום קשר כואב לי לראות אישה נאלצת…  LinoyBarGeffen מדהימים אה אז מסתבר שיש נשים עם כישורים ושלא מיותר להעיר ולהילחם כי אפשר לתקן מה אתן אומרות  dormimun משתתפת בצער השתתפתי הערב כמו כל שנה באירוע ״הלילה לא לומדים תודה״ שעורך כנס שדרות בט׳ באב בערים בכל הארץ לא כמו כל שנה השנה…  איפה בעולם קוראים היום ליהודים מפיצי מחלות בכנסת ישראל אמסלם עכשיו במליאה צריך לומר ברור מי שמגנה היום ״אלימות משני הצדדים״ מכשיר את האלימות שהיתה בלילה לא היו לה ״שני צדדים״ אלא תוקף וקו…  פניתי הבוקר לשר הביטחון כדי שיכריז על לה פמיליה ארגון טרור דפוס הפעולה השיטתי שזורע אימה ברחובות באלימות מחייב נקי…  הבוקר המשטרה מגדירה נסיון לרצח מול עיני השוטרים ״קטטה״ שרות בממשלה מגנות מיצג אמנותי ולא דקירה ברחוב חברי כנסת מ…  אחרי העדויות על אלימות נגד מפגינים מהלילה אי אפשר להתמשיך להתעלם המשטרה חייבת להגן על המפגינים והיועמ״ש לחקור את ה…  עד עכשיו היחידות בהנהגה ששילמו מחיר סיגל סדצקי ויפעת שאשאביטון עכשיו הבנתי למה אין נשים בקבינט הקורונה כדי שלא יהיה את מי לפטר מה שמוזר זה שברשימת הדרישות של נציג העצמאיים כביכול מתוך 9 דרישות רק 2 איכשהו נוגעות תכלס לעצמאיים כל השאר זה לקפ…  כל מילה  מה נשים לא חולות בקורונה לא רופאות לא אחיות לא מעניינות מה נסגר  moshe150160 אתמול חילקת לי ציון בבכיינות והיום ציונים על ענייניות נו טוב מכיוון שאנו לא נופלות בכישורים הייצוג…  moshe150160 אוי טפשונות שכמונו שוב פעם התבכיינו פשוט אין לנו כישורים טוב נסתום לאלה שאומרים ״אבל למה לבחור לפי מגדר״ ובכן אם יש רק גברים זה אומר שכבר בחרו לפי מגדר פשוט רק לפי מגדר אחד בוועדה לקידום מעמד האישה עליה של מאות אחוזים בדיווח על אלימות במשפחה בתקופת הקורונה אבל רק 15 בתלונות למשטרה עם…  מתי זה קרה שמלחמות ישראל הפכו ממלחמות אין ברירה למלחמות שמחפשים ״זמן טוב״ לצאת אליהן  עכשיו בוועדה לקידום מעמד האישה חשפה יו״ר הוועד ענבל חרמוני שההסכם עם האוצר אמנם נחגג והשביתה הסתיימה אבל הוא לא נח…  MkSondos 10 גברים יהודים 0 נשים 0 ערביות  תמרור אזהרה גדול קבינט קורונה ללא נשים לא חל על נשים  נגמר הזמן שתקבלו החלטות עלינו  בלעד… MCchuchem זה לא לפי מדינות אלא לפי סטטוס הזוגיות הוסיפו לנוהל ״ידועים בציבור״ אבל המון זוגות שעומדים בכל מבחן של…  אלפי ישראלים ובני הזוג שלהםן  חלקם עם ילדים משותפים  עדיין ממתינים להתאחד כבר חמישה חודשים אחרי שנקרעו זה מזרועו…  השר לבטחון נתניהו ממשיך לנסות לדכא מחאה בשירות אדונו ובניגוד לחוק ואיכשהו אפילו מחלץ מהממז הודאה באכיפה סלקטיבית…  בחדשות מפגינים בעוטף עזה מספרים על תוקפים שירדו מרכב והתחילו לירוק לקלל ואז אחד הרגיש דקירה של סכין הקריינות …  YinonMagal תוכל להגיד את זה עוד מאה פעם ולקרוא לי באיזה שמות שתרצה אין אלימות בשמאל אין עכשיו ומעולם לא היתה…  YinonMagal אין לנו כוונה לחכות לרצח הבא ואין לכם מונופול על היהדות תעצרו את האלימות במקום להמשיך להסית כשיהיה רצ…  YinonMagal אין מכות לשוטרים המפגין שהפיל את המיקרופון לאבישי בן חיים זכה לגינוי מקיר לקיר בשמאל הרפרנס היחיד שלנ…  YinonMagal אין אלימות בשמאל  כמו שכתבתי אני חושבת ששתיקתו של ביבי כהסכמה אבל אם אין לך משהו לומר על ערב אחד שבו…  moshe150160 תראה מה זה אנחנו עושות גם מה שלא ביקשת איזה עולם יום קסום moshe150160 התכוונת ״למה את לא מחייכת״ נפגעות מהקורונה יותר מנפגעים נשים עניות נפגעות אלימות עובדות סוציאליות אחיות אימהות היעדן של נשים מקבינט הקור…  urizaki אחד הטיעונים המרכזיים של צייצני הימין הוא איפה היו ארגוני השמאל כשהופעלה אלימות משטרתית בשרשור הבא אביא שורת דוגמאות לפעו… akivanovick בהצלחה ואגב אין פה אלימות משני הצדדים וגם לא הפגנות משני הצדדים אין פה ״בעד ונגד״ יש פה ישראלים שמפגינים בלהט נגד שלטון…  ביבי דיבר בפתח ישיבת הממשלה אבל לא הוציא מילה נגד האלימות ברחובות שתיקה כהסכמה יש שרים שהאשימו את המפגינים באלימ…  לצפות עד הסוף ולשמור את הקטע האחרון לפעם הבאה שמישהו חושב שאין סיכוי שהוא שוביניסט בגלל שיש לו אישה ובנות  זו האנרכיה האמיתית והמסוכנת לא ציצי אלא מיליציות אלימות ברחובות שנתקלות ברפיון חשוד מצד המשטרה אפנה ליועץ המשפטי…  נזכרת בכל אלה שהסבירו כמה ההסכם הקואליציוני יצוק בבטון סותם כל פרצה גאוני בניסוחו יהווה חיסון נגד נכלוליותו של ב…  עובדת סוציאלית מושכת תשומת לב למאבק ״בהמה״ ״אנרכיסטית״ ״״מבזה את סמלי המדינה״ לה פמיליה מזיינים את השמאל צרצרים  אבל למה לא התלוננתן  JoavLewy פונה אליו תיראו מופתעים השר כץ מיהר להודיע שישעה מענקים לארגונים שמסייעים לפליטים אלא שהדבר בכלל לא בסמכותו  נגד חוק צמצום הדמוקרטיה בחסות הקורונה  אפרופו ביזוי סמלי המדינה אז אדם שנפסל מלהתמודד לכנסת בגלל גזענות ירצה בלילה המוקדש לשנאת חינם בחסות משרד ממשלתי  ברוכים הבאים הלוואי שתובילו את כולנו להניח את הנשק ולשנות כיוון לשלום  עוד משהו על הצבעת טיפולי ההמרה היום זו היתה אחת ההזדמנויות הנדירות בכנסת שבה כל ח״כ הצביעה נטו לפי המצפון שום מש…  אולי באמת שגוש כחול לבן יצטרפו לאופוזיציה ואז האופוזיציה תהיה קואליציה של 62 שזה רוב וזה בעצם מה שהיה אמור להיות מל…  העברת חוק איסור טיפולי המרה הוא אירוע הסטורי ודרמטי בתולדות הקהילה הגאה בישראל עוד הוכחה ששווה להיאבק על הדברים הצ…  כרגע מתחיל הדיון בהצעה לאיסור טיפולי המרה של חברי ניצן הורוביץ עוד כמה דקות ההצבעה מדובר בהצלת חיים פשוטו כמשמעו…  ברכות לענבל חרמוני יו״ר הוועד ולעובדות הסוציאליות שהנהיגה על מאבק הירואי ומעורר השראה שהתחיל עם ״לא יהיו תוספות שכר…  לא רק קורונה הורגת  הורדת שכר המינימום זה לא רק אחד הדברים האכזריים אלא גם אחד המטופשים נניח רק נניח שעסקים ישכרו יותר עובדים למי… </t>
+  </si>
+  <si>
+    <t>NiflaPo נמסתי Paranoi98696546 זה נכון תוך כדי שיצעקו שהכל אנטישמיות החרדים הכי חכמים והכי צודקים והכי מבינים יותר מכולם ולכן למרבה הצער יזכו בפרס של לקבור הכי הרבה מתים nitayp קשה מאד להתחיל להבין אפילו את הקלאסטרפאק הקולואסלי הבין גלאקטי אליו מתגלגל עולם הישיבות מול עינינו ממה שאני מצליח להבין היה… RealMrKav ״וחוזרים בריאים לבין הזמנים״ rebellien משתתפת בצערך מילא אם היו מסכנים רק את חייהם אבל כאופי המגיפה הם מסכנים את כולם סביבם שמור על עצמך RealMrKav קשקוש כולם יוצאים הביתה בבת אחת להדביק את המשפחות במלון קורונה בפיקוח הם מחוייבים קודם בבדיקות קורונה יחידניות וזה לא המצב כפי שכתבתי בעבר הקהילה החרדית נמצאת בעמדת נחיתות שלא באשמתה מבחינת תנאי ההתמודדות עם הקורונה צפיפות אורח חיים…  ISudri בוא תנקד לי את זה  ISudri לא צריכים שיסבירו לנו מה זו קפסולה צריכים שיסבירו להם שכל התחכומים האומללים שלהם לא פוטרים אותם מאיסור התק…  Nadav1Levy moshenayes קראת מה שכתבתי Nadav1Levy moshenayes למה נראה לך שנבדקו הוחלט שכולם בריאים אז למה להיבדק moshenayes מעניין שכל הרוקדים תמיד בריאים בקפסולות אבל איכשהו כל נבדק חרדי רביעי מאומת לקורונה FrauDoc למה לחכות  TPKcJLOj7ROho5Q חח  nachmankan נהדר גם הקבורה אחר כך בקפסולות  מי שרוקד במוצאי יום כיפור יבכה במוצאי שמחת תורה ElkanaShor NadavEyal הו וואו ככה נלחמים בהתקהלויות לא חוקיות בעל חווה נקנס ב£10000 על שאפשר בשטחו קיום חתונה המונית המגבלה לחתונה באנגליה 1…  SettyYael אם נהיה כנות שני המאפים חסרי טעם אם הם לא אקסטרה טריים נאלץ לבקר פיזית בישראללונדון בשביל החוויה המלאה SettyYael במקומך לא הייתי יוצאת מהבית odaskal בינתיים באנגליה  moshenayes רפואה שלמה SettyYael דיל Galileo89507087 myartkids תמונה כשמוכן בבקשה כי אני מזוכיסטית myartkids חח אמג את לא מכירה את ההיסטוריה האסונית שלי במטבח עדיף שאתמקד במה שאני פחות גרועה בו myartkids Galileo89507087 התעללות SettyYael לפרט אין עוגיות עבאדי michalnsharoni האמת שיש מצב שיודעת איפה להשיג אולי מחר myartkids אני כל כך חסרת יכולת או רצון לאפות שאין לי תנור myartkids ומי יכין michalnsharoni מה שלא במרחק הליכה מהבית שלי לא קיים swedishkeren אני בתקופה לחוצה וכשאני בלחץ אני לא מסוגלת לאכול ShaiAvraham1 נשמע לי הוגן אתם אמנם בסגר וזה מבאס אבל בניגוד אליי יש לכם גישה לעוגיות עבאדי yoni416 RanBalicer ClalitResearch זה לא לדעתך זה ממצאי המחקר צפה בסרטון שהגבתי אליו RanBalicer ClalitResearch דקה לפני שדיברת קושמרו הציג אותם כ״מתים מקורונה או מתים עם קורונה״ כל עוד זו האג׳נדה…  DavidNevo3 זה לא נכון בהחלט אפשר להקפיד ועדיין להידבק moshenayes מי המיוחסים Arspoeti מצטערת שעברת את זה חיבוק  erancherpak אולי כולם נוסעים לחדר המיון כדי לפנות את הילד שדרסו shaulig הסתר פנים זה הכי 2020 השנה אלוהים צריך לבקש ממנו סליחה ronkat1 עדיין בין אדם לחברו שיום כיפור לא מכפר NeumanAdi בטח כמו בארץ שכביכול לא אבל כולם בטוויטר AltabenElad אני לא יכולה לדבר בשם כל הממלכה כי לא יצאתי מהשכונה שלי מאז מרץ מההתרשמות שלי כאן הרוב מקפידים על מס…  Idollete לי היה מוזר לקלוט שאני מבינה גרמנית אחרי שאני יודעת קצת יידיש Jenny666Beans ברובם נראה שהרשויות בבריטניה עושות מאמץ גדול יותר לעודד את הקהילות החרדיות להיענות להנחיות הקורונה מאשר הרשויות בישראל  zdanielz כן yoni416 NiflaPo יש עוד יותר משלושה חודשים לשנה הזו נסה להיזכר בהבדלים בין ינואר למרץ NiflaPo עד סוף 2020 גם זה לא יהיה SchibyAmir הוא יכול להרים הוא לא יכול ליצור אותה מקווה מאוד שאלו שמתפללים כעת בצפיפות בבתי כנסת סגורים מכים היטב על חטא ומביעים חרטה מראש כלפי אלו שלא יראו את יום הכיפורים הבא בגללם TheknighwhoSaid לא ברור למה אבל קר לי היום במיוחד מכל העולם מתקשרים להתייעץ  yokkyg GadiAleks כן כבר הסבירו לי טעות שלי מכורבלת עם שתי שמיכות חמצוואר ובקבוק חם בזמן שבישראל 30 מעלות מעולם לא הרגשתי מנותקת יותר מהארץ Eranw44 תודה רבה גם לך razshlomo ביבי קלאסי שקרן פתולוגי PhysicsRocks3 גם לך אם בחרתם להגיב כאן תגובות מפלגות ברכותיי אתם חלק מהמקהלה הסיבה שהעם מפולג ומוסת אלו נגד אלו אינה מקרית הכל בעידודה של מקהלת השנאה ובניצוחו של הנאחז בקרנות המזבח כוחו של ה…  אני חולקת עליכם המציאות הפכה למגמת ביולוגיה שיצאה משליטה בוג׳ו קורא לעולם להתאחד מול הקורונה ו״להפסיק להשוות שיעורי תמותה״ זו כנראה הדרך הכי פחות אלגנטית שראיתי להתמודד עם…  יצאה שבת נכון  מיקי זוהר נובח שהשמאל רוצה להחריב את המדינה כדי להשיג את השלטון ומיד אחר כך מתלונן שהשמאל לא מראה סולידריות המידה…  אולי בעצם מגיע לאנושות להיכחד  EladSi JohnBishop100 הם צודקים תכלס אתה יכול לשבת לארוחה בבית כל יום מחדש עם 5 אנשים ממשקי בית שונים SherriPizza avivyashar כן ראי תגובות כאן amitm123 לא הבנתי למה לא מוכנים amitm123 מה הכוונה לא מוכנים abubizuna הבחירה שלהם מנותקת מהמגיפה היתה זמן רב לפניה והיא חלק מאורח החיים שלהם כיום האתגרים שלהם להתגונן מפני…  ReutBitton הפרסומת עם החתול על הפח הכתום יותר מעצבנת מאסי עזר doronziv MichaelKarmon 1 chaimlevinson אולי זו מעריצה אלמונית שהתאהבה בו בגלל כל הקמפיינים המצליחים abubizuna זכותם לבחור באורח החיים הזה אין אשמה בלבחור באורח חיים דתי קהילות לא אמורות לבחור אורח חיים שמותאם מראש למגיפה אם תגיע atoneveret michalbgigi במקום שמתים בו פחות ההגבלות גדולות יותר אין פה משחקים naglistal זה לא כל הסיפור הם חיים במשקי בית מרובי ילדים בקהילות מאוד צפופות עם אורח חיים קהילתי מאוד אלו אתגרי…  michalbgigi שלא יעבדו עליך חרא בכל העולם yoni416 ממש נורא וזה עוד לא נגמר NiflaPo חתול בלתי נסבל על פח כתום זו סוגה עילית תתנצל stwiess זה לא הוא pandool אין כאן חכמה רק אטימות לב AviMo6 אל תדאג נדאג שגם התמונה שלו תיחרט היטב AviMo6 אוי לא שם טוב לחלוק chaimlevinson זה על כנרת assafma צודק הקריירה והמוניטין של אביעד משה כל כך לא משמעותיים שכבר שבוע גוגל קורס מחיפושי השם שלו ועדיין אף אחד לא פענח במה הו…  FarberRonit געגוע chaimlevinson  undisabled28 אז מה המיסטייק בדיוק undisabled28 רגע הוא ייצא מהאסלה zdanielz MemeR התחלתי ללמוד ולא נראה לי שאראה את הפקולטה עצמה בשנה הקרובה zdanielz MemeR הגיע חשמלאי לתקן אצלי בדירה משהו לפני בערך חודש והיה מרגש לדבר עם מישהו לא דרך זום MemeR עדיין מוזר לי שכולם עם מסיכות על הפנים MemeR בעצמי לא יודעת איך המקומות המוכרים לי בלונדון נראים כיום לא יצאתי מהשכונה שלי מאז אמצע מרץ eyalweinberger כשכולנו כבר נהיה מחוסנים אולי בסוף 2021 לא מצליחה להיפטר מהמחשבה שבפעם הבאה שאוכל לבקר בארץ הכל יהיה שונה האנשים והמקומות שישרדו את המגיפה לא יהיו כפי שהכרתי אותם לפניה Dcatlady1 זה המקסימום המוחלט eman70y אני חושבת שהם אוכלים עכבישים קטנים יותר eman70y אני באנגליה לחרקים אחרים קר מדי להסתובב פה יש רק עכבישים eman70y שלי כן טווים קורים בכל מקום nestor36925 Eranw44 יש חסינות שר הבריאות יולי אדלשטיין שבמשמרתו המגיפה בארץ הגיעה למימדים קטסטרופאליים יושב בטלויזיה ומטיף לציבור לקחת אחריות…  Tooj29683434 chaimlevinson מה בקצב הזה הקורונה בישראל תדרוש בקרוב זכות להגדרה עצמית כעם chaimlevinson ״קול חשוב״ dorzach מה קורה שם בגיל 23 nirizhaki ronityamin zoharm7 כמה שטויות כולם כאן עם מסיכות במקומות סגורים ובמקומות שאי אפשר לשמור על ריחוק ReutBitton לא פופולארית אבל נכונה ״דמוקרטיה״  zoharm7 התפשטות הנגיף היא כבר חסרת תקדים והאשמה היא על הממשלה לא על האופוזיציה תמשיך להאשים את כל העולם אבל האח…  michalkoriat אני הומו מצד האמא erancherpak למסגר NadavEyal ״מרבית מדינות אירופה״ I wish idokius רגע הגילוי  ColmanRosenfeld MitMaHa תהרוג את ההורים שלך לא את ההורים שלי שלום וביי ColmanRosenfeld MitMaHa מה אתה מציע ReutBitton ניצלנו ReutBitton שמחה שהממשלה תישאר יציבה התפטרות שלו היתה מרעידה את כל היציבות RevaMandat עכשיו יש לך עוד זמן לחשוב על זה החל ממחר תשבו בבית ותחשבו על מה שעשיתם לביבי codswallop שירה בימי כולרה thistle8blower הוא אחראי על גורל ההורים שלי והיקרים לי אז כן חייבת לקחת ברצינות קרן מרציאנו תמצתה את הנאום של ביבי במדויק ״זה נאום אני מאשים  אתכם״   ביבי עם עניבת האיומים האדומה לא מסוגלת להזכיר שם של אף אחד שלומד איתי בלי שאמא שלי תשאל אם הוא יהודי einatovadia yairy גם אני חסום כבר נצח במקרה נתקלתי MichaelKornB מעולה giladgaron ובכן  לכם ולכל עם ישראל  גמר חתימה טובה  Tylerdu57494124 efsharibari כן זה מיולי NiflaPo סיים סיים באט דיפרנט NiflaPo גוד פור מי גוד פור יו Idanyo yaelsr barzik אני באמת לא יודעת אני חיה בלונדון yaelsr barzik לקחתי את זה כמובן מאליו שכולם על סיבים אופטיים כמו פה אני די בשוק shaynotkin talchaim barzik לא ידעתי את זה זה די מזעזע talchaim barzik כן ברור משרד החינוך יממן להם תשתית אינטרנט בבית שניה אחרי שישלמו להם שכר נורמאלי barzik אולי זה בגלל שעם המשכורת של המורה היא יכולה לקנות רוחב פס של עט כדורי העברתי את היום למתכונת קפסולות אצרוך חדשות בקפסולות קטנות עם ריחוק חברתי אחת מהשניה MitMaHa זה לגיטימי לגמרי MitMaHa לא טענתי שזה ריאלי טענתי שזה מה שהמערך האפידימיולוגי מסוגל להתמודד איתו כרגע לא רק בארץ להבנתי אף מערך…  MitMaHa זה לא מסובך הדרך היחידה להשתלט על המגיפה היא קטיעת שרשראות ההדבקה לפי כל הגורמים הרשמיים מערך איתור ובי…  ivgiz chaimlevinson אז למה בעצם היא עברה בדיקה לפני שבוע MitMaHa אני בוחרת בקפידה למי אני מקשיבה לא להוא שהנפיץ את ה7 Giddonbd adindan באמת היה לי מוזר שאיבדתי היום בבת אחת עשרות עוקבים וניסיתי לחשוב אם עצבנתי היום באופן חריג יותר מכרגיל adindan גם אני מתנצלת כולנו על הקצה  adindan כן הכל נשאר אותו הדבר זה יתעדכן אצלך אוטומטית קרה לי אותו הדבר כשמחקתי את החשבון והחזרתי תוך יום הכל חוזר לבד adindan היה היום באג בטוויטר להרבה מאוד חשבונות זה יסתדר בתוך 24 שעות yudash למה אני מתה עליך כל הציוץ שגיאות הקלדה חוץ מהמילה הכי מסובכת ״חלמאות״ haakshan באה ממשפחה של מתנחלים לא מפספסת כלום GadiAleks רגע נחסמת haakshan מתנחליםבליחושהומור haakshan וואי איזה מקורי אתה LiatNadel מצטערת שומרת כאן על אנונימיות zdanielz לולז zdanielz לא לגעת לי בפיצה עם התוספות הלא קשורות שלך zdanielz צנצנת אחת בשבילי אני מבינה מחר מתחילה ללמוד הסמסטר נפתח אונליין מנסים לשחזר איזו חוויה סטודנטיאלית אז בין הרצאות הפתיחה השחילו שעתיים של מן…  awwwpi כמוך כמוני אני ככה מאז מרץ חיה בזום awwwpi אילו היתה דרך לטוס בבטחה כבר הייתי מעלה את אמא שלי על מטוס לכאן awwwpi מה פתאום כולכם נגועים awwwpi לא לא ברמת תחלואה גבוהה גם היכולת של בתי החולים לטפל במקרי תחלואה אחרים תיפגם משמעותית ימותו על ימין ועל שמאל מהרבה גורמים awwwpi אין מצב עם הגופות תגיע ההתעוררות אנשים יאבדו את היקרים להם ויהיו בהלם ShavitR תיזהרי מלהגיע לבריטניה יש כאן שרת פנים נאצית ששולחת פליטים שמגיעים בסירות לטיזנאמו ומפקירה אותם לגורלם LiatNadel למה לחכות Daniela28289133 וואלה יש שלום עם בחריין לא במקומכם הייתי בודקת אופציה לטיסות חילוץ מישראל maayanef לא נעים לי לומר אבל מי לעזאזל ירצה לטוס למדינה עם כמות הדבקה מטורפת כזאת NiflaPo באמת קראתי שזה ויראלי אחי ShaiNaamat ברור הבנאדם עובד שעה בשבוע ואז יוצא לנופש ShaiNaamat אבל היותר עצלן ShaiNaamat התאום הצהוב הדמוקרטיה הכי שכונה במזרח התיכון  merutsa כתבות פח אהבתי את זה שבעצם כבר הכריזו על סגר בשבוע שעבר אבל עכשיו מכריזים על סגרעלאמת בשבוע הבא יוכרז סגר אבל הפעם ממש ו…  isaacs צחקתי בקול yaelsr הכל במחשב אבל עדיין וידאתי מרקרים לקראת פתיחת השנה  yaelsr זה אשכרה שכנע אותי לחזור למאמרים ששעממו אותי yaelsr I can’t Lolavanhorn הכי ישראלי שלך TheKingSlayer11 למה בשרשור הזה האסקפיזם בארץ הוא תרנגול מרקד עזבו תנו לקורונה לנצח ErellitaA אני Eranw44 לסירוגין arikmashraki Natichuulloo arielschnabel עדיין אחוז החיוביים בארץ הוא 117 יותר מפי 4 מבבריטניה גם אם כל המדינה תמות מקורונה חדשות 12 ימשיכו עם הכתבות היומיות על מצב הצימרים בארץ  ShaiNaamat shireuven קדימה עוד מאמץ קטן וחמש ספרות  MosheRecanati זה יעיל עם מאות בודדות של נדבקים כרגע הדרך היחידה להגיע לשם זה סגר מוחלט עד שההדבקות יירדו מוזמן להמשיך להטריל מושתק MosheRecanati יש 117 חיוביים לבדוק מי נחשף אליהם ולבצע בדיקות לכולם מי מהם שייצא חיובי יבדקו גם את המגעים שלה…  NoaZamsky ממש לא בבריטניה נדרשו 10 שבועות MosheRecanati בדיקות מסיביות לכל מי שנחשף לחולה מאומת וקטיעת שרשרת ההדבקה TheKingSlayer11 לציין שלאחר 10 שבועות עדיין הפתיחה היתה הדרגתית ובצד הכי מתיר שלה התאפשר לעד שני משקי בית להיפגש…  TheKingSlayer11 בבריטניה לקח 10 שבועות</t>
+  </si>
+  <si>
+    <t>Nowa המדקרת לא מרשה לי יאללה מתי שרה מזמינה חשמלאי MetachGavoah גמר חתימה טובה עידן Noamkatz7 שנה טובה ילדון yankihebrew Noamkatz7 גמר חתימה טובה יענקי  Noamkatz7 במי אתה יכול לפגוע נועם כץ אתה כולך צוף וארגמן AvinoamKutscher חחחחחח RonelAdani אלוהים גדול מלקק ידיות רוצה להתנצל בפני האיש שניסה לרצוח את אשתו לא רצינו לפגוע במוניטין שלך YinonMagal אני רוצה סליחה שקראתם לי משרתת EliBitan חזק ואמץ ביתאן  asaffzamir מאמו אומרת שכל צום אוכלים חרירה כי הוא מאד משביע dahanmicha בגלל זה מכינים יום קודם שיהיה יותר טעים מחר Avner01553626 שאלתי אם עש איזו ברכה או משהו מעבר אבל אמרה שאין אולי ISudri סודרי ידע וכמובן חרירה   במרוקו היה מסורת El hada לאכול בערב יום כיפור סוג של קישוא Krah sallouya המנהג היה לאכול כמה מנות קטנות לאורך…  Rereshef אל תשכח שאני הייתי בקפסולות הראשונות שלך Rereshef יש לך עלייה אקספוננציאלית בעוקבים מה האחים שלי שולחים בוואטסאפ המשפחתי  תמונות וסרטונים חמודים של הנכדים מה אני שולחת  צימצורי שהכנתי YehudahGlick כל יום הוא יום הדין בשבילי oranmikel נראית שחזרה מאומן MetachGavoah לופ שלא נגמר YHepstein זה נכון כל תשומת הלב התמקדה במשהו מבהיל אחר kobimiz100 זה אני ואתה itayalmogbar תודה וגמר חתימה טובה  ילדה מקפצת באלנבי הרחובות שוממים ואין אף אדם ברחוב מחר יום הדין האימתני שתמיד חששה ממנו שתמיד פחדה לעבור מול אלו…  YehudahGlick יהודה בוא נביא את השלום יחד לא להאמין שבזמן שמחנה הימין נמצא תחת משבר ענקי של פיצול ביבי מתעסק בקורונה YotYotam אנחנו צריכים ללמד אתכם לסבול בשקט YotYotam אתם מכורים למייק אפ סקס GoelPinto וואו מהמם מי היה מאמין שהימין יתפרק קודם לפני השמאל וואלה אין לנו מנהיג ואיך דרך אבל כוח סיבולת קטן עלינו  GoelPinto קרם פטיסייר בתחתית DaliaEdelstein אוי תרגיש טוב  horowitzb לראש התורן NirACohen77 איזה אחד אתה לא מכיר barzik ותראה לאן הוא הגיע ואיפה אתה יש לך על הרבה על מה לעשות חושבים DaliaEdelstein דליה את כל הזמן מרגשת אותי יו amsterdamski2 שאול המצאתי את זה הרגע אני מודה amsterdamski2 כל חלק שווה יום כלומר 1000 ימים almogbenzikri קברנו אותו עכשיו אגב השופט שאסר על פרסום שמו של האיש שניסה לרצוח את אשתו ממש פגע במוניטין שלו מעורהההההההה  miriambaram נכון  למי שלא מאורע בביטויים תזכורת סגר טוב אומרים עד יום כיפור ומיום כיפור עד הושענא רבה אומרים גמר סגר טוב shaquedmorag מגדילה לך על קנבס orikol מדהים אותי כמה כסף יש לפעמים לאנשים די נמאס מכל הגברים האלו שקיבלו השראה מלוליטה  TomerKariv  TomerKariv אבל תומר חירפנת אותי תעלה הכל בבת אחת ריפרשתי שעה אני ככ אוהבת שתומר כותב על אלבומים  LVertzhaizer תפתחי את הדלת אני למטה LVertzhaizer לא יודעת איך אתאושש ליעד saragershuni מזל טוב שרה mohsaud08 מזל שיום כיפורים מוחמד יש לך מלא על מה לכפר ItayBlumental הלב שלי רצה נסיך אחד בסוף קיבלתי צפרדע הו כמה העולם אכזר הגם אתה מוחמד את מכירה בחור הוא מקדיש לך שיר את חושבת שהוא שלך וזה לנצח ואז הבחור מקדיש שירים לכל בחורה שנייה כאילו זה מזומן במפר…  YoniSaadon פי אלף יותר סגר איזה יופי שכל מי שלא הבין בתחילת הקורונה מה הפירוש של עלייה אקספוננציאלית  עכשיו ממש מבין  Obar06485129 כפפות שחורות זה בשרים מעושנים אה ועשינו מוקסות גם   RonelAdani רונאל אתה הכי רזה שיש בעולם איזה בטן RonelAdani חייך ישתנו RonelAdani הלו לא לרדת על המדקרת שלי רק לי מותררררר chaimlevinson תייגתי בלב דברים שהמדקרת אומרת לי גם היום הבטן שלך נפוחה אכלת גלוטן אני אסנת את כל מפגש אומרת את זה אני חושבת שאנחנו צריכות להפנים שזו הבטן שלי OferHadad עופר תבקש סליחה בשבילי גם YehudahGlick BenShush אין על אבא YehudahGlick יהודה בוא נלך מכות משעמם לי itayr2 תעף יגידו שהוא לא מבקר את בגצ iketzef חחחחחח iketzef קצף את יודעת כבר שאני קומת קרקע  IdanDorfman אה כנראה לא שמתי לב לזה והסכמי אוסלו זה משהו אחר לא שאני רוצה להתערב יותר מידי אבל עד עכשיו אף אחד מגידולי הפרא שקלמן הגדיר לא הגיב לטור שלו באופן ענייני כל מה ש…  yairtar לפעמים גם לאכול אותו ruthlessrousso NaorMeningher בואי ניקח גם את שגית yairtar הזעזוע שרק עכשיו הבנתי חרדל או שאני מבינה חרדל NaorMeningher ruthlessrousso בואי נעשה שתפ כמו כן מחר משיקה את ספרי איך הפסקתי לפחד מחרדל והתחלתי לתקוע אותו בכל דבר וואי מה זה לא נעים לי אבל הכנתי את סלט הביצים הכי טעים שהאנושות ידעה ורק אני אכלתי ממנו עדיין אומרים לא נגעתי זה מאד בומרי מה דעתכם לא נגעתי  yosefhacohen אורח כזה לא פוגשים כל יום חברים קלמן חתם על עצומה הקוראת להתפטרות ראש הממשלה ksoko123 הן הביאו לו שמרים שוקולד על חשבון הבית לא להאמין הוא למד לצקצק ולשתות אספרסו מדהים ראיתי את קלמן יושב בנחמה וחצי כותב תסריט לסדרה arielplaksin1 KalmanLiebskind הוא גרם לי להתבלבל ולשים מלח במקום סוכר בקפה החרגה נוספת מלחמות הימין הפנימיות יועברו לקפסולות מוחמד מה דעתך שנקדיש שיר לקלמן mohsaud08 amitsegal נו אבל מה זה המתח הזה מה אתה חושב על זה YanivTurgi נו בחייאת יש מהכל בקטעים האלה את מי זה מרגש כבר eyaldatz מסכימה מאד YanivTurgi ושבת שלום וגמר חתימה טובה  YanivTurgi אבל אבל יש מצב ששבוע שעבר לא אהבתי משהו שיניב תורגמן כתב אבל היום אני אוהב זה הופך אותי לצבועה למה ה…  YanivTurgi יש לי סברה אחרת שבה העולם לפעמים קצת יותר צבעוני עם אינספור חבלים ולא רק חד מימדי yaircherki נתון שמוכיח לי כל פעם מחדש כמה קשה זה לגדול תאומה chaimlevinson חיים לוינסון yodfatyoni מה chaimlevinson לא שמעתי אף פעם תלונות מהדייטים שלי זו הייתה אישה אגב  אחד הדברים הכי מצחיקים בלהיות ביסקסואלית לספר לחברות שהיה לי דייט והן מנחשות אם זה היה עם גבר או אישה mohsaud08 BarashiKinneret וואי אתה ממש מכיר את נקודות התורפה שלי mohsaud08 BarashiKinneret אני בחורה קנאית חבל mohsaud08 BarashiKinneret מה קורה פה מוחמד לפחות תחכה שההקדשה שלי תתקרר noalandau לכמה זמן litigilad צחקתי בקול arielplaksin1 מה היא לא שמה לב yonipi0 אבא שלי לימד אותי להיות כזו  BarashiKinneret mohsaud08 עד מחר הכל אצלך avihaihaddad mohsaud08 זה פיפי ברמות mohsaud08 ItayBlumental מוחמד בסוף אני ואתה נביא את השלום almogbenzikri אלמוג אל תתחיל איתי אתה הכי גבוה שיש בפירמידת מאסלו NirACohen77 talialin אתה בבידוד והזמנו כרטיס למחר misscorina2 מאזינה לזה בלופ  BarashiKinneret mohsaud08 את רוצה על חולצה או על בלון  talialin טליה בואי נטוס לאבו דאבי gilgu אני רוצה כסףףףףףף ItayBlumental mohsaud08 מה עוד יכולתי לבקש mohsaud08 איזה מלך כלומר שייח אני מתההההההההההההה  arielplaksin1 פלקסין היא קצת צודקת בהלצה שלה פה מיקי זוהר נותן וואחד עלילת דם יפה פה AvishayBenHaim יאללה למה אתה מחכה AvishayBenHaim טוב מתייחסת להתחלה מה יש בישראל המסורתית המזרחית שאתה חושב שהיא המקשרת בין ישראל המודרנית לתורה וה…  AvishayBenHaim אני בהלם שמישהו ביקש ממך שם להסביר מה זו ישראל הראשונה והשנייה ויש לי המון להגיד אסיים לצפות בהכל ואשוב omerbabai logreisas YehudaGizbar תקרת הזכוכית של להסתכל מלמעלה logreisas YehudaGizbar omerbabai אין דבר כזה סתם דתלש יש דתלש שסתם לו omerbabai YehudaGizbar משכתבת את ההיסטוריה מחדש or5708 omerbabai alizalavie אין סיכוייייי YehudaGizbar omerbabai חחחחח omerbabai לא באתי מעולם חרדי דתי רגיל  avihaihaddad אני מקווה  Ayeletnnv אמסור  omerbabai מה זה הנושא הכי שחוק בעולם omerbabai מצאתי את זה במייל alizalavie וואו אני מבינה למה הציון הנמוך omerbabai הקורס היה תקשורת ומגדר הסמינריון סטריאוטיפים באתרי שידוכים  CarmitSoliman תני כמה ציטוטים nadavabeksis לדעתי הברזתי מלא למה אני נהנית פה 3324281  mohsaud08 Noamkatz7 רק אם תקדיש לי שיר כמעט שכחתי להרים ליומולדת של מאמו מזל טוב אהבת נפשי אני מודה לך שאת רוקמת לי זכרונות על הילדות שלך כאילו היו שלי ו…  oranmikel אני באמת מקור לגאווה אחרי אתגר המטאטא קבלו אתגר הקורונה  מייצבים חולים קשים oranmikel מי זה alizalavie zviashkenazi למדתי לסלוח עם השנים  ביבי מיקי אתה מיום חמישי עד יום שבת אסנת את יום ראשון אסנת אבל זה כיפור אדוני ראש הממשלה ביבי הגנה עליי זה פיקוח…  המתווה אושר שרי הליכוד יתחלקו לקפסולות בהסתה נגד המפגינים alizalavie zviashkenazi מזל טוב עליזה למרות שנתת לי ציון ממש גרוע בסמינריון שלי אני דווקא שמחה שיהיה סגר כללי לכולם ולא יפלה בין המפגינים המתפללים וטופז לוק מסתמן כי שבוע הבא יהיה סגר  הקובץ הסופי סופי YehudahGlick אבא אני חוזרת הביתה omerbabai טיפ תמיד לתמצת מסתבר שזה רעיון שהיה בארץ נהדרת אתמול ולא צפיתי אז אני חולקת את הלייקים שלי איתם irisbaz אה סעמק Leemalach רפרנס שאני לא מכירההההה Leemalach אני בעד להקים ממשלה שדואגת לאזרחים  omerbabai מדהים  רעיון הפגנות בבית כנסת oranmikel נו בשביל זה יש הפגנה  Obar06485129 תעשה את זה הנעוץ שלך תאמינו לי אנשים השתגעו מהסגר מזמינים חופשה בסרביה arielapi תראה גם בטיסות כתוב Tel Aviv כשבפועל זה לוד Ayeletnnv AnatNir יפה שלי זותי Ayeletnnv ענת ניר Riklin10 judash0 איך בודקים moranynet יש חיים במאדים EfratFinkel זה אומר שאנחנו שלישייה עכשיו sagitderi מה עושות judash0 אני אוכלת מלא בשר מלא וגם בשר אדום בחיי אני לא מבינה תוצאות בדיקות הדם שלי הגיעו והרופאה התקשרה להגיד לי שאני אנמית אני חושבת שאני המרוקאית הראשונה בהיסטוריה שהיא אנמית kobimiz100 אתה  כזה אוקיי כן זה או בן או בת יאפ זה ממש נכון בהתחלה חשבתי שהם מתכוונים שיש אופציה שלישית  schaingarte yaelshevach זה יפה במרוקאית  currlygirll למדתי משהו israzohar קצת מתגעגעת currlygirll מה זה בייסטיק ביצ מהאינסטגרם razsf אה לא קראתי טוב razsf סוף סוף אנחנו ביחד  yonipi0 ונאוה בנות ירושלים  NiflaPo המדינה בחרא אני די בסדר  NewProfilePic  MayaZivWolf אני לא מבינה איך יש לך ילדה בת 9 YanivTurgi בחורה סקרנית מה יביא יום APersiko CarmitSoliman talshalev1 אני אבוא לאיזו לשכה שאסתר תרצה beni5342 EfratFinkel פה EfratFinkel beni5342 היא לחלוטין האהבה הנשית לא הראשונה שלי gilicohen10 עוד שלוםםםםםםםםם beni5342 EfratFinkel אשמח לשמוע גם omerbabai בוא נהיה שותפים בחיים לא עשו לי כזה פאסיב אגרסיב הסגברה התנשאות בחיי על כל הקטגוריות הוא סימן וי אתה מתחיל הכי חזק שלך ולאט לאט מגביר   arielapi אני שולחת לו הודעההההההההה ללא קשר רגע לכלום המלצת צפייה חובה הכרחית אתם תעופו על זה ותתרגשו ותבכו ותאהבו  my octopus teacher בנטפליקס זה יפה ככ באמת amitlvr חיימשלי את misscorina2 רק שאנחנו בוכים  טופז לוק הערב בהפגנה של השמאל  oranmikel ישראלי תמיד יהיה ישראלי oranmikel הם התבלבלו בין 1000 מטר ל1000 אנשים yaakovmatan Lahman00 הראה לי משהו שכתבתו עליי אז חשבתי שלא עשיתי את זה כמה חודשים</t>
+  </si>
+  <si>
+    <t>השימוש הציני של הימין בהובלת משפחת נתניהו מראה על ניתוק וחוסר הבנה לתופעת הפדופיליה הקשה והמחריבת חיים shiramakin…  ifatglick וואי איך בא לי  EstyS מזל טוב ושנהנטובה ואופטימית IsaacHerzog שנההטובה לך ולמיכל ולכל אהוביך EmilieMoatti אמילי אהובה תנחומי הכנים וחיבוק גדול לך ולבנות itamars מזל טוב🥳 origivati המשטרה מספרת שמצאו טביעות אצבע שלי על השלט סבבה אני בטוח שאם היו משקיעים פה בתפיסת עברייני מין כמו שמשקיעים ברדיפת פעילים… chaimlevinson hadover1 אנא מסור לו איחולי החלמה מלאה  shireuven 1982 אי טי בקולנוע שכנתי הצעירה ממני בשנתיים ואני מיבבות מתישהוא בילדות צפיתי ב Love story ובכיתי את נ…  HALOBYSSVAG עשינו את זה  לקח שלושה ימים מהפגישה עם לשכת השר YuliEdelstein ויום אחרי הדיון בכנסת והבוקר התבשרנו בלובי למלחמה באלימות… מחכה כבר לקרוא בהצלחה חברYossiYonah  MeravMichaeli מה אתם מְגַנִּים  Syechimovich היכן ישנם עוד שרים כמו שר התרבות והספורט הזה שלא מתבלבל הולך להפגש עם הקטינה שנוצלה בערלות לב בידי הכדורגלנים  ומביע ע… shaquedmorag נירמול יחסים עם איחוד האמירויות כשישראל בסכסוך מדמם היא כמו מענק של 750 שקל כשיש מיליון מובטלים IsaacHerzog מזל טוב זוג מקסים תמשיכו להנות מהחברות האהבה והנחת מהילדים שילוב של רוע וטיפשות היא המסוכנת ביותר   einatovadia לפי סקר של פיקוד העורף רק 17 מהציבור מבינים את ההנחיות של הממשלה לציבור בטיפול בקורונה ורק 19 מאמינים למוסדות הממשלה דב… YoavYoavkrak אין לי ספק שתצליח bezalelsm חובת ההוכחה עליך נראה אותך ואם תצליח מבטיחה לקיים את מודה ועוזב ירוחם צום קל dormimun תנחומי הכנים מסמך מעולה של רכז המדיניות eyallurie של ZulatEquality שקובעי המדיניות יקראו ויישמו  הציוצים של gantzbe ושריו מכעיסים ומחרפנים לא פחות מההתעלמות של רוהמ ושרי הליכוד אתם לא באופ׳ אתם בשלטון אל תצי…  noalandau RonenManelis התבלבלת מנליס השיח יצר עליה בדלגיטימציה לכיבוש לשליטה הישראלית על העם הפלסטיני וטוב שכך תודה ⁦zehavagalon⁩ בזכותך כותבים על בר מגניב בפתח תקווה  noalandau מקומות שבהם גברים מתירים לחשוף ציצים פורנו זנות חשפנות פרסומות ריאליטי מקומות שלא הנקה מחאה או כל מה שאינו מיני וא… כמה עליבות גועל   gilicohen10 ובכל זאת יום הולדת שמח   YaelSherer איך זה נראה כשבתי חולים לא מקיימים את הנהלים בקשר לבדיקת סמי אונס ככה קטינה מגיעה במצב הזה לא בודקים לא מבררים לא דוגמ… zehavagalon ב 2008 הגשתי לראשונה את הצעת החוק להפללת לקוחות הזנות גאה בשותפתי ShuliMR ובכל השותפות במערכת הפוליטית התקשורתית ובחב… noalandau לכל המוחים אתמול היום ומחר אין דבר כזה מחאה ״לא פוליטית״ פשוט תגידו ״לא מפלגתית״ orikol urizaki tamarzandberg היא פשוט מהמממת ⁦⁦panievsky⁩ ״איך מבחינים בין שיקולים מסחריים שיקולי רייטינג או סתם התחנפות לבין שחיתות בין אם מדוברת או שמוסכ…  ZulatEquality גנץ ואשכנזי בלמו את הסיפוח בדיוק להפך הם שותפים מלאים במסיבת הקצף ובועות הסבון במכבסת המילים של נתניהו  עינת עובדיה… EretzNehederet 1 ביולי שמח  לעוד מערכונים של ארץ נהדרת לחצוgt   ZulatEquality איך נתניהו כיבס לכם את השיח ושכנע אתכם שזה לא אפרטהייד אלא החלת ריבונות עינת עובדיה מנכלית מכון זולת חושפת א… PeaceNowIL הפלסטינים קוראים לחדש את המשא ומתן בלי תנאים מקדימים אסור לנו לפספס את ההזדמנות ולהיגרר לסיפוח חד צדדי מנותק שיפגע בסיכוי… ZulatEquality כך נראה האפרטהייד המקורי עוד sfardm מתוך סרטון מעולה של NIFIsrael בשיתוף פעולה מהמם עם ברק היימן וליאור אשכנזי ש… ZulatEquality שתפו כדי שכולם ידעו את האמת דוח המכבסה חושף ככה שוטפים לנו את השיח ב7 שלבים פשוטים איך הם עושים את זה קראו את הדוח… yarivop שונא מתנות יחיה YozmatGeneva  Meravbenari עד כאן אל תתעסקי לי עם תוכניות האוכל  AGvaryahu תודה לכל מי שעזר לקבוצה הזו לקום למי שהיה איתנו הערב ובעיקר למי שהסכים להצטרף אלינו בראשם פרופ שטרנהל שהערב הוקדש לזיכרו… LinoyBarGeffen מחזיקה אצבעות בהצלחה יהי זכרו ברוך  KarenLHaber חיבוק zviashkenazi netacheha ishmuli DotzMR מזל טוב נטע יקרה zviashkenazi בדיוק היום כיבדתי את המסורת ואכלתי צהרים אצל בכור את שושי תענוג יום שלישי פעמיים כי טוב זכיתי לגדול על ספריה וכך גם ילדי שארון הספרים שלנו גדוש בספרים מימי ילדותי וחדשים יותר מילדותם ילדי גם זכו לבקר…  ״זהו מאבק של הפריבילגיה הגברית לקבל הסכמה לתקוע את הזין ולחמוק ממשפט פלילי״ כבוד ⁦chaimlevinson⁩   sfardm ישנה גזענות לטנטית ועקיפה יש גזענות מודעת אך מנומסת ומתחפשת ויש גזענות גאה מתפרצת וחסרת עכבות עלינו להפנים שגזענות עירומה… כשקלמן ליבסקינד מדבר על אונס – צריך להפוך שולחן ״לדיון תרבותי יש סטנדרטים והם לא כוללים מיזוגיניה הומפוביה וגזענו…  KseniaSvetlova הסיפוח מסוכן לישראלים לפלסטינים לאזור כולו וגם למעמדה של ארהב במזהת הוא יצור מציאות מסויטת של אפרטהיד וישנה לעד את… בגץ הורה על ביטול חוק ההסדרה החוק לגזילת קרקעות כל היועצים המשפטיים והמדיניים היו נגדו והזהירו מהחקיקה רק הימין…  meretzparty זה הזמן להתעורר ולהצטרף למאבק הכי חשוב שהיה כאן חייבים לעצור את אסון הסיפוח  ranyakir בתצפית על יריחו כחלק מסיור של נבחרות ונבחרי מרצ בהדרכת ד״ר שאול אריאלי מבינים את המשמעויות האיומות של הסיפוח שמתכנן נתניהו… meretzparty זהבה גלאון הסיפוח לא מעניין את נתניהו גם לא שפיכות הדמים שתבוא אחריו הוא הולך למהלך הזה מסיבה אחת להסיח את הדעת מהמשפ… NitzanHorowitz עכשיו עם ראשי מרצ בבקעה במאבק נגד הסיפוח כשעומדים כאן רואים את הטירוף מאות ק״מ של גבולות חדשים מובלעות הפקעות גיר… meretzparty עוצרים את אסון הסיפוח  במוצש הקרוב כולם בהפגנה בכיכר רבין בום כשסמולנים מפוחדים מפרסמים ריבועים שחורים באינסטה  זה עצוב ⁦shiramakin⁩    FarkashOrit RonenManelis מינוי ראוי בהצלחה ל RonenManelis eitanrom בהצלחה MeravMichaeli הזוועה הזאת לא תקרה יותר כשייושמו מסקנות דוח ברלינר לפי הצעת החוק שלי ושל MichalRozin ויוקמו מחלקות מיוחדות לעבירות… YakiAdamker אין מילים שיצליחו לנחם ואין אחר שיוכל לחוש את כאבכם כמוכם שולחת לך ולמשפחתך חיבוק גדול ותנחומים מכל הלב עבור הנערה שלי בבית הנערה שבי וכולנו   ילדות נערות ונשים  אנא חתמו על העצומה TogetherKulan  yairlapid גנץ ואשכנזי שומרים על זכות השתיקה תראו את השמאלנים האלה איך הם שמחים אה לא  כמה זלזול עצמי ועליבות צריך להיות לכםן כדי שתתיצבו באופן הזה לפוטואופ הבושה מתה  peacenowisrael  EsawiFr חג שמח בריאות אושר ונחת מהמשפחה zehavagalon  AmirKochavi מבאס ככ shiramakin כל מילה של שירה אמת shiramakin ושמי ששלח את אלפי מבקשי המקלט לשם היתה המדינה ועכשיו אשב פה ואחכה לצבא האמת של שפי אנשי העליונות הלבנה שיתקפו כמו שהם יו… shiramakin מאז יצא לי להכיר ולעבוד עם פעילים משכונות הדרום אקטיביסטים ואקטיביסטיות שבאמת היו מחוייבים לתושבים ולא רק טענו שהם כאלה כ… shiramakin gtgtgt יום אחרי אחת הפגישות הללו שפי עלתה להתראיין איפשהו וצעקה כהרגלה שהמנותקים ממרצ מתעלמים ממצוקת השכונות שאכפת להם רק מה… shiramakin וזה הסיפור שלי על שפי פז הBFFית החדשה של אוחנה כשעבדתי כיועצת פרלמנטרית למיכל רוזין שהיתה אז יור ועדת העובדים הזרים קי… asafzamir אלוף bezalelsm תפורה עליך האופוזיציה chaimlevinson לציוץ כזה חובה לצרף מתכון או יותר טוב  טעימות ShaniAshkenazi את באיסלנד ISudri אדם יקר ישר דרך צנוע והגון זכיתי בחברות עימו zulat4 gantzbe  הציבור לא מטומטם כולם רואים שבהסכם הקואליציוני נתת לנתניהו אישור להרים יד על הדמוקרטיה הישראלית לקריעת מגילת העצמאו… zehavagalon  IsaacHerzog מרגש כל הכבוד למיכל  zulat4 תהיו בטוחים שמיד לאחר השבעת הממשלה נתניהו הנאשם בפלילים ישוב לעיסוק הכי חשוב מבחינתו וזה סיכול העמדתו לדין הוא ימשיך בקמפיין… meretzparty שחיתות  זה מדבק  שבענו מהפרת הבטחות ברמה הארצית גם ברמה המקומית ראוי שמרצ תקיים את הבטחותיה לבוחרת eyallurie  KarenLHaber מדויק תודה eyallurie וואו מהמם ReutMor חחח קורע המהממם הקטן BenCaspit radio103fm מזל טוב  AbuKedem להקת פיקוד מרכז  NirACohen77 משלימים פערים MichalRozin  חתמתי  eyallurie על זה אומרים Be careful what u wish 4 yudash בנזין לבן מאז הקורונה שמתי לב שתחזית מזג האוויר מעניינת אותי משתי סיבות בלבד הכביסה שתלויה בחוץ והאם מתאים להכין חמין לשבת חוץ מזה לא רלבנטי לי Ayeletnnv אני גאה בך עכשיו נראה אותך שולחת גם את עברי אליהם  roysharon11 הבן  בבסיס בדרום הצליח לראות אנחנו בפתח תקווה נכשלנו במשימה  שמי bezalelsm  אולי אתה חושב כמו האליל שלך טראמפ שיש עובדות אלטרנטיביות אבל גזילת אדמות ושלטון צבאי על עם אחר אינ…  בצר לי דווקא היום שלחתי בקשה באתר histadruthadash לביטול חברותי וחברות האיש שלי בהסתדרות העובדים אם ראשי הארגון…  בגץ קבע לבתי חולים אין סמכות למנוע הכנסת חמץ לשטחם בפסח  hbyogev שני בניי נולדו בתקופה זו והם נקראים אביב ועומר ממליצה בחום  azariarachel וואו מרגש ביותר רחל ״אין לי ארץ אחרת גם אם אדמתי בוערת רק מילה בעברית חודרת אל עורקיי אל נשמתי בגוף כואב בלב רעב כאן הוא ביתי לא אשתו…  EstyS מזעזע ILParliament האיש שלי קורא לזה כוכבי מישלן hkim14050017  הלב נקרע zehavagalon דרדסבא וברמוח סיכמו הדרדסים ימליצו על גרגמל ולא ולא יקבלו חופש הצבעה בנושא אכילת דרדסים על ידי חתחתול אכן מרגש IsaacHerzog כל הכבוד על היוזמה היצירתית והחשובה נשבר הלב לראות את העיניים העצובות של דיירי בית האבות  Ayeletnnv נראה מאד כואב תרגישי טוב יקרה Syechimovich tasmc1 טוב שאת אחרי תרגישי טוב ותנוחי ביטול ״חוק הפיקדון שמחייב מבקשי מקלט להפריש 20 משכרם  הוא הצלחה אדירה של שוחרי זכויות האדם בישראל ואני גאה להיות…  החלטה נכונה חשובה וראויה ולא פחות מאמיצה באקלים הפוליטי הנוכחי leeyaron  ברייקינג אמש yairlapid הפך להיות אלטרנטיבה אמיתית ומשמעותית לשלטון המושחת המאוס והשערורייתי פה נחוש והחלטי כבו…  yairlapid אם הממשלה יכולה למצוא פתרונות להפגנות לג׳וגינג לקניות ולתפילות אז היא יכולה למצוא גם פתרונות למשפחות שכולות שרוצות לעמוד ל… revitalamiran מזל טוב Meravbenari מההתחלה נוצרה אפליה לא ראויה אפשר היה להעמיד שומרים בכניסות לשוק ולווסת כניסה של אנשים כפי שעשו בסופרים Syechimovich אמא חזקה ואמיצה שגידלה בת אמיצה וחזקה עדות מרגשת וכואבת noalandau אפשר כבר להפסיק עם המלים היפות אחדות וחירום ולאומית זו עוד ממשלת נתניהו בדיוק כמו קודמותיה זוכרים את האמירה של בנט ושקד שאם לא יהיו בממשלה יפעלו באופוזיציה להעברת חוקים נגד שחיתות אז זה מה שעושה עכשיו gantzbe בול IsaacHerzog סיפור מרגש ביותר הדמעות חונקות את הגרון TomerMichelzon התשואות שקיבל עודה אמש חשפו את ערוות המרכז שמאל הציוני זה שרק רוצה את ישראל הטובה והישנה ומתפלא בכל פעם מחדש שנתניהו… attaliami כתבה מרגשת ביותר ShovrimShtika המודעה הזו ש56 שרים וחכים לשעבר חתומים עליה אומרת אמת פשוטה – סיפוח השטחים יהפוך את ישראל למדינת אפרטהייד זה לא גר… zehavagalon לתשומת ליבכם תומכי תוכנית הסיפוח gantzbe GabiashkenaziMK אם עוד לא ראיתם הבוקר את המודעה שלנו ב Haaretz של 55 חכים ושר… mikiros1 פתק שנמצא בגופתה של דגללבן לא בגדנו התאבדנו zehavagalon מה זה אומר על רהמ נתניהו אם הוא מגיב על הדברים המחליאים האלו זה אומר שהוא בסדר עם כל הדברים המחרידים האחרים שהבן שלו כתב… הבן שלי וחבריו סוגרים השבוע שבת רביעית בבסיס כולל שני חגים קורונה וזה קשה לחיילים וקשה להורים רק אומרת roysharon11 זה לא רק צהל שמעניק מעטפת מפנקת לנערי הגבעות זה קודם משטרת ישראל כולם שם היו יכולים לחטוף לפחות קנס על הפרת בידוד ועל ני… כל הכבוד לחקלאים שתרמו את התוצרת שלהם עשרות טונות כתרומות לנזקקים חוצפה שהמדינה מאפשרת יבוא ירקות בזמן שהחקלאים מ…  ׳העשבים השוטים׳ התפשטו לכל עבר  Shiritc מזל טוב  ISudri יש משלוחים Mickeygitzin כזה  ILParliament תודה ששיתפת yanivkub אנשי קבע יוצאים באופן קבוע הביתה גם אם במשמרות מדוע חיילים צריכים לסגור למעלה מחודש בצבא אין בזה שום הגיון zehavagalon כמו שכתב בצילום אפסים כולם  Ayeletnnv מנתחות את המצב הפוליטי בזוםהייתם מתים להיות זבוב על המסך   zehavagalon ShuliMR KElharrar MichalRozin Meravbenari… YakiAdamker מרגש אז חיילים וקצינים הודחו ונשלחו למחבוש כי הפרו את הנחיות הממשלה אבל לIsraeliPMheb ו ruvirivlin  מותר לא להישמע ל…  BarakRavid moshebst זהו אפשר לסגור   BarakRavid moshebst רגעעעע עוד לא שלי עוד בדרך אמא אמרו בתקשורת שממחר עוצר עד שישי בבוקר מה אנחנו פלסטינים  עכשיו בפתח תקווה העירייה עושה שמח לשכנים  כבר מותר להשוות  AGvaryahu amirperetz I fix it  תקשיבו אם זו הממשלה שמתגבשת עדיף שנישאר בבידוד עד הבחירות הבאות PeaceNowIL גנץ קודם הם יספחו אותך ואחרי זה את השטחים עדיין לא מאוחר להתעשת  RanLior מזל טוב הפתענו את ההורים ליום הנישואין עם שלט בלונים עוגה ויין  הכל מרחוק  shiramakin מתחרפנת מצעירים שזורקים זין על ההגבלות וממשיכים להתגנב לפגוש חברים אפילו אלו שבשגרה מזדעקים על עוולות לצד האשטאג סולידריו… העובדה שהצבעתי ל amirperetz בבחירות משתווה להחזקת כרטיסי טיסה בתוקף לנופש בצפון איטליה תחושה של תבהלה גועל ואובדן דרך talschneider פלטפורמה חשובה ביותר למאבק הפמיניסטי עצוב ומבאס עכשיו בימי קורונה קיבלנו הזדמנות פז לעצור לשנייה את המרוץ המוטרף הסיזיפי בעקבות מודל היופי הבלתי אפשרי — ופשוט…  מלכה  לכל אורך שנות הקריירה הפוליטית שלי מגיל צעיר מעולם לא התאכזבתי והתביישתי במערכת הפוליטית כמו בשבוע האחרון noalandau כזו בדיחה עוד לא היתה בני גנץ האיש שקיבל מנדט להרכיב ממשלה והריץ את עצמו לתפקיד יו״ר הכנסת tamarzandberg גנץ לא קיבל את המנדט כדי לנהל מו״מ לאחדות אם תעלה מועמדותו כיו״ר כנסת כדי להיות גשר לאחדות  נצביע נגד akivanovick לא  GMMivs סבתא בישלה דיסה  נתנה לשלח ראשות הועדה למאבק בנגיף הקורונה  נתנה לפורר ראשות ועדת הכספים  נתנה לאשכנזי ראשות ועדת החוץ וביטח… zehavagalon הם לא יכבדו את החלטות בגץ אבל ברור שהם יכבדו את הסכם הרוטציה עם כחול לבן כנסו וחתמו על העצומה נגד הפיטורים של lucyaharish מ kann   ימים של השתקה ודגל שחור להצלת הדמוקרטיה  orikol תנחומי הכנים אורי זכיתי להכיר אותו בארוע שהפקת ולספר לו איך גידל בן נפלא חיבוק גדול alonschustermk רק בריאות origivati בזמן הטירוף שמתחולל סביבנו אסור לשכח את מבקשי ומבקשות המקלט אוכלוסיה שתלויה בענף המסעדנות והמלונאות הסגור כמעט לחלוטין ולא… זכיתי להכיר אשה מופלאה שותפה למאבקים על הדמוקרטיה שעות על גבי שעות בועדת החוקה ועל השוויון כשותפות בשדולה הגאה…  Meravbenari לא מבודדות  zehavagalon Ayeletnnv ShuliMR MichalRozin  shiramakin הארווי ויינשטיין קיבל 23 שנה על אונס בניו יורק האופרה של לא הודיעה היום שעשרות התלונות שהתקבלו נגד פלסידו דומינגו על הטרד… בסבב בחירות אפריל 2019 הופעתי עם YoazHendel1 ושאלתי אותו מדוע לא הצטרף לרשימה ימנית שתואמת את תפיסת עולמו הוא ענה…  nitzanzur zehavagalon  noalandau להכין לכם סיר לשבת zehavagalon בכל בחירות מצביעי שמאל מענישים את המפלגות שהיו נאמנות להם ומאמינים שוב להבטחה הבאה שתפיל את נתניהו ואז מקבלים את נתניהו… mossiraz מרצ תומכת בהחרמת מוצרים המיוצרים בהתחלויות שהם חלק מכלכלת הכיבוש זו עמדה מוסרית המבחינה בן ישראל הלגיטימית לשטחים הכבושים… YaelSherer  ברד בפתח תקווה  ישיבה משותפת ראשונה של רשימת העבודהגשר מרצ שיהיה לנו בהצלחה  tamarzandberg MeravMichaeli תודה רבה סומכת עליכן שתדאגו לדחוף ליישומו מבפנים 3 זו תהיה תחילתו של הליך ריפוי הנדרש כדי לפתור את משבר האמון בין נפגעות עבירות מין ובין מערכת אכיפת החוק המחלקות…  2בשנים האחרונות אנו עדות למהפכה של ממש עם תנועת מיטו ולמהלאהתלוננתי באופן שצועק למקבלי ההחלטות לשנות את המד…  1 אני נרגשת שהגענו ליום הזה לאחר שנים של מאבק בו מערכת אכיפת החוק החליטה להכיר בייחודיות של הטיפול הנדרש בעבירות…  ishmuli eranlevi81 וואו הוא פשוט מהמם חג שמח יקרים  ברייקינג הכישוף עדיין לא הפך את פתח תקווה לעיר אמיתית hamakom  YunaLeibzon אחלה שרשור אחלה טוויטגאם ושיחוק אמיתי תמשיכי לשתף לא לעיתים קרובות אני נתקלת בכותרת שגורמת לי נחת גדולה שינוי תפיסה מרגש שזה מכבר הגיע זמנו במשך עשור נאבקתי לחוקק…  eyallurie bezalelsm tomermeiri zehavagalon מה עם אמת בפרבום עד שלא אראה תמונה שלה על הקרח לא אאמין  אכן פאטה מורגנה zehavagalon מציבה מראה של מציאות מול כולנו  תעודת עניות למדינת ישראל פחדנים  shiramakin כשהקפיטליזם מנצח את הליברליזם הוליווד הליברלית לא מתביישת לשתף פעולה עם הרודנות הסינית שירה מייקין מעשירה את עולמ…  NitzanHorowitz משה יהודאי רב איש מרצ וגם מכר ותיק הותקף באלימות קשה כשהתנדב במסיק זיתים בשטחים אגב משה הוא בן 80 ומי שתקפו אותו… yaronavraham מזל טוב zehavagalon הרב משה יהודאי מרבנים לזכויות אדם שהתנדב למסיק הזיתים בבורין הותקף קשות זו אינה תופעה חדשה היא מסוכנת ומבהילה והסתיימה כ… ״אנחנו אשמים אשמה האדישות לנוכח הפיכת ערים ישראליות למעוזים של מצוקה ומשפחות פשע זה קורה שם לא אצלנו זה משהו שק…  האנטישמיות מרימה שוב ראש באירופה כמו במקומות נוספים בעולם תנחומים למשפחות והחלמה לפצועים   בדיוק  YaelCohenParan LiatBs LiliBenAmi אמסלם כיו״ר הקואליציה היה מי שמנע בנובמבר האחרון את הקמת ועדת החקירה בעניין רצח נשים שהצענו להקים… פתח תקווה מעולם לא היתה תוססת יותר 🤓  ״לא נטייה לפשע ולא התרבות שלנו אחראיות לגלי הרצח בחברה הערבית אלא הזנחה הדרה ואלימות במדים מזעזע כמה שזה לא מז…  zehavagalon צריך להפסיק להיגרר אחר סדר היום של הימין ולייצר סדר יום  של התנגדות בכנסת וברחוב מול האפרטהייד המדינה צריכה לעצור מלכת ח…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">בגלי ישראל ממשיכים גם היום לעסוק בנושא אחד ויחיד כמעט  קלמן ליבסקינד לפני שבוע העלילו עליו ועליי היום כועסים נ…  הרבנית לוינגר הייתה אחת הנשים המשפיעות ביותר בישראל שלאחר מלחמת ששת הימים סמל חלוציות מודרני תנועה אנושית אדירה…  arielschnabel גם אני כמו רבים מבני הדור השני של מתיישבי יו״ש בחרתי לגור מהצד האחר של הקו הירוק לא עברנו לשמאל שזה לגיטימי פשוט ב… טוב מאוחר מלעולם לא  FakeKogan לתהות בוודאי מותר אם כי לא חייבים לצייר את התהיות כעובדות  ממש לא SemelYair חד משמעית כמו שבגין אמר בעת פרשת לבון ״עוד לא נולד האדם שמותר להעיד נגדו עדות שקר״ ולסיכום מותר אפילו מצווה לכעוס על דעות שאתה קורא בעיתון אסור אפילו פשע לטפול שקרים וקונספירציות על מניעי הכותב avishaigrinzaig השבוע הפך קלמן ליבסקינד שתחקיריו על מערכת אכיפת החוק נישאו על גלי האהדה של הליכוד לשופרו של מנדלבליט והוא לא היחיד •… לאור גל השמועות הבה נעשה קצת סדר בעניין שיחות הרקע עם עיתונאי הימין היועמש חשש להתקשר ישירות אלינו ולכן פנה תחי…  הרב אבי גיסר רב היישוב עפרה החליט בחוכמתו ובאומץ לבו לקיים את תפילות השבועיים הקרובים כולל יוה״כ בחוץ זהו אין…  בחזרה ליום הכיפורים ההוא  MakorRishon  שטויות שמעון פשוט שטויות  אם שארית המשק תושבת רק כדי לרצות את שרי כחול לבן שמתעקשים לסגור הכול לא רק את מחאת בלפור או את דרעי שמתעקש לפת…  BarashiKinneret גם זאת הטעיה מה זאת אומרת ״חגי סגל הודה״ בעיתון שלנו בשבוע שעבר בטור של יפרח צוין במפורש שהיתה…  ציטוט שקרי שהפרקליטה שמה בפי תוך הולכת שולל של לקוחותיה ברשת היא הוסיפה מילה לא תמימה ״איתי״ למשפט כללי יותר שא…  1 שיחות רקע עם אחמים הן לחם חוקו של עיתונאי 2 הוא לא אמור לתת עליהן דוח לאיש 3 לפנים משורת הדין צוין אצלנו מפו…  אם המגפה תשאיר פה בסוף רק שני יהודים אחד יפגין בבלפור והשני יתפלל בבית כנסת ספר מצוין מעלה על נס את גבורת הלוחמים בחזית הדרום ואת יכולת ההתעשתות של המפקדים סוף סוף הבנתי מה קרה בין שרון לגו…  הטענה שמפומפמת בשעות האחרונות כאילו MakorRishon נחלץ לקדם איזשהו בלון ניסוי של היועמש או לשרת פתאום את הפרקליטו…  ממליץ לעקוב אחרי הסיפור הסבוך אך המרתק הזה שכתבנו לענייני תפוצות כבר עושה עליו דוקטורט  rothmar שמחה לא מכיר אותך כל כך טוב אבל אתה כנראה חזק בפלפולים אין לי כוח לזה במקרה נפלתי אמש בארכיון המצהיב שלי על הטור הזה שפרסמתי ב׳בשבע׳ באפריל 2004 אחרי שתוכנית ההתנתקות יצאה לדרך לענ״ד…  amitsegal את האבחנה הכי מעודדת על מצבנו סיפק רן ברץ במקור ראשון בחג בעיניו ההפקרות בנושא הקורונה לא מעידה על אובדן הלכידות כמו למשל… MakorRishon למה עשינו את מיזם החיבורים המוזיקליים דווקא עכשיו  YHepstein   עפרה רגע לפני תשפ״א הצטיידנו ברמזור ראשון וגם בבניינים בני שש קומות בשנה הבאה אי״ה נשב על המרפסת    דברים נכוחים של השר חילי טרופר על תפילות והפגנות ומה שביניהן  ביום הכיפורים תשלד 73 תפילת נעילה בבית הכנסת שלי בצפון עכו נקטעה בגלל פיצוץ פתאומי אדיר בחוץ כל המתפללים שטרם…  ShuliMR מצורפת קריאתו של חברי דר אלי רוזנברג רופא בחסד ואיש ירא שמים לקיום תפילות החג במרחב הפתוח בלבד  haggaisegal  KalmanLie… גיליון דיוקן לערב חג אנשי השנה כותבים את הסיפור שלה שלהם בין השאר יולי אדלשטיין נפתלי בנט צבי האוזר שגריר יש…  יהודים אין מנוס תפילות הימים הנוראים  רק בחוץ bezalelsm ככה נראית אחריות מי שמכיר את ישיבת הר המור יודע שהדבר האחרון שאפשר לומר עליה זה שלימוד התורה הוא לא הדבר הכי חשוב בעולם אב… amitsegal טירוף קווים לדמותו או שסוגרים הכל או שפותחים  הטילים באשדוד ובאשקלון  תזכורת טקסית לשלום של ספטמבר 93׳ וגם הבעת תודה פלסטינית להשעיית הריבונות מיזם ייחודי של מקור ראשון לימי הסליחה והמחילה שבמסגרתו הפגשנו שורה של אמני צמרת לסיעור מוחות מוזיקלי אשר הוליד חיד…  הטענה מימין ש״גם בגין לא הביא לממשלה ולכנסת את ההסכם עם מצרים לפני החתימה״  חלשה בעיקר מנקודת מבט ימנית אילו…  MakorRishon אנחנו גאים להציג שיח סליחות מסוג חדש פרויקט זההזמןלסלוח מביא עיבודים מחודשים של המוזיקאי יעקב אסרף לשירי סליחה מוכרים מ… מה ששליחתנו לוושינגטון אומרת  ניצן הורוביץ אמר עכשיו בלהט בישיבת סיעת מרצ ידוע לי שניתנה הבטחה להקפאת בנייה בהתנחלויות תמורת הנורמליזציה עם מדי…  ISudri ההתנשאות האמיתית פה היא כמובן שלך מדבריך עולה שתפילות ראש השנה הן עניין היקר ללב החרדים בלבד  הציבור החר…  מתווה התפילות במבנה סגור הוא טרלול מושלם שמגחיך את כל הסגר כניעה נמהרת להנהגה החרדית ולגבאי הפגנות בלפור הרב חיים נבון כתב אצלנו לאחרונה ש״עולם התרבות הישראלי הוא ברובו בידור במיעוטו הפגנות בעיסת נייר וצבע״ נעם סמל נפג…  אם ההסכמים עם האמירויות ובחריין כה נפלאים אין סיבה להסתיר אותם מהממשלה מהכנסת ובעיקר מהציבור אל דאגה מחוץ לבית הכנסת יימשכו כסדרן התפילות ההמוניות של שושקה ושות׳  529648 בחסות הקורונה הוקלטו השנה תפילות נוסח בית אבא הכי יפות שבעולם בדוק ונקי אובייקטיבי ונטול פניות  צייצני עפרה רטווטו עד שעוף… yairkraus ¹לא אני אמרתי את זה פרופ גמזו אמר לי הפגנות בלפור מעניקות לגיטימציה להתקהלויות אסורות צאו מהפוזיציה למרות שאין נתוני… MakorRishon המסכה ירדה האופי הישראלי התגלה והוא לא משהו haggaisegal   Danmargalit זו כותרת שמאדירה את כבודו הוא אמור להגיד את אשר על לבו ולא לחשוש מציוצים כאלה אגב הוא גם צודק אפי…  אם אתם לא מנויים על ״יום ליום״ זה בשבילכם  אישית אני מעדיף ריבונות ביו״ש על יחסים דיפלומטיים עם האמירויות וגם מוזר לי שמקבילו האמירותי של נתניהו לא יבוא לטק…  MakorRishon ״הדברים שנאמרים נגד נתניהו גרועים בהרבה מאלה שנאמרו על רבין לפני הרצח״ הרב חיים נבון דעה  אם אכן הולכים להחלטה על סגר מלא  כולל חנויות ומסעדות  הוא חייב לכלול השבתה מלאה של בתי הכנסת תוך דחיית הלחץ הכבד…  מי משרטט את הקווים האדומים של צוות קו כחול יהודה יפרח מכה שוב MakorRishon  גם ח״כ קרעי משחק הערב באש  KalmanLiebskind חוזר מבית העלמין בקיבוץ נחשון מלוויה של יזהר חבר טוב איש משפחה לוחם שנפצע שלוש פעמים במהלך שירותו הצבאי ונכנע רק… מי ייתן והידיעה על העיון החדש של מנדלבליט בשאלת הנבצרות אינה נכונה אם כן בצלאח אדין מהמרים עכשיו על העתיד שלנו שלא לומר משחקים באש וזה הטור המלא אז  בין הראשונים שזיהה  יהודה יפרח שלנו אביב 2018  אכן יש משהו מביך בהתהפכות הכללית והפתאומית של הימין בפרשת אום אל חיראן מצד שני יש משהו מביך בעובדה שהשמאל נאחז רק…  בוגי שוב חוצה את הגבול שבין כסילות לזדון ובין דמיון לכזב  MakorRishon שייקספיר צדק משהו רקוב בממלכת דנמרק  ZvikaKlein   המוסד זקוק לסוכנים וליועץ לשוני ״איך זה מרגיש״  כניעה דוחה לנושאי נס העברית הקלוקלת  Riklin10 eitz1 מאבקם הצודק מה צודק בלסכן חיים אדם Riklin10 בקיצור שמעון ידידי אתה בעד המשך שריפת מחסני המזון ההדדיים בעיצומו של המצור Shlomogedalowis השוואה מטופשת הסגר על הערים האדומות לא נועד להרוס אותן הוא נועד להציל יכול להיות שזה מהלך מוטעה…  קיץ שלם מטיפים פה למרד ולאנרכיה אמנם מכיוון אחר הנה זה בא  מי שצריך לספק הסברים בפרשת ״מסיבת הטבע״ זה ההורים המחנכים ושאר מעצבי דעת הקהל הצעירה בישראל לא המשטרה ברוכים השבים דני התגעגענו  moryo19 משפט נוקב אמיתי וכואב של עמית סגל המוכשר לא צריך להיות דוס כדי לכבד את המורשת שלנו  מאז הסרת הסגר באביב ועד היום ביקרתי עשרות פעמים בקניון מלחה שוקק הלקוחות מעולם לא נתקלתי שם בשוטרים שפועלים נגד סרבני מסכות תפילות קורונה ירד אמש לדפוס כשמספר הנדבקים היה כאלפיים ״בלבד״ ⁦MakorRishon⁩  אני  מומחה קורונה קטן מאוד אבל שוב ושוב שמעתי שדיבור בקול במתחם סגור מגביר משמעותית את תפוצת הנגיף אם כך כדאי לה…  זה כמובן ניסוח של מדיניות בינוי שמאלנית ביו״ש כל עוד נתניהו לא מאפשר לכנס את מת״ע והוא הרי המחליט בנדון הוא בעצ…  MakorRishon תוכניות סאטירה מחליפים בשלט בטח אם מדובר בערוץ מסחרי שכל שיקוליו נתונים לפרסומת הבאה שנכנסת כך מצא את עצמו אביר המונולו… הקשר בין ההקפאה הנמשכת ביו״ש לרומן המתלהט עם האמירויות ברור כשמש בצהרי אבו דאבי זה בוודאי לא ״שלום תמורת שלום״  מכתב ההתפטרות של מרידור מכיל רכיבים פופוליסטיים ופוליטיים לא מבוטלים ובכלל זה האזכור העוקצני של ז׳בוטינסקי למה רק…  SharrenHaskel AntiquitiesIL  אני קוראת לכם להגיע למקום מחר בבוקר כדי לוודא שהמקום לא נפגע ושאין גניבת עתיקות במקום חוק העתיקות תקף ג… arnonsegal1 בור נפער בהר הבית לדעת הארכיאולוג צחי דבירה ייתכן שמדובר במחילה מימי הבית השני ככל שזה תלוי בשלטונות ישראל לעולם לא נדע Shiritc 70 שנה אחרי הקמתה ספריית הכנסת מרוקנת את מדפיה חלק יעבור למוזיאון הכנסת שנמצא בהקמה וההשאלה תיעשה בדלפק שיישאר במקום בשתפ עם… bennyteitel ועוד קצת מנציג הפרקליטות שי ניצן בועדת חוקה על ההפגנות בבלפור סליחה נגד ההתנתקות ב 17 במאי 2005 על מה שמותר למשטרה אם יש… It appears that Jared Kushner controls it all He foiled Israeli sovereignty in Judea and Samaria and also decided…  תסריט לא לגמרי היפותטי  shaimaymon את הבית שלי יהרסו בית שהמדינה הקימה בית שעבר פינוי ממקום אחר והמדינה החליטה איפה יקום מחדש בית של אזרח שומר חוק משלם… כשמדובר במתנחלים בגץ לא יכול להתגבר על יצרו פשוט לא יכול אם ישראל אכן מדינה יהודית ודמוקרטית איך זה שהיא מגבילה כעת בצדק מגבלות חמורות על תפילה בבתי כנסת ואפס מגבלות על…  ramonhaim הועד נגד צביעות ומוסר כפול שמח לבשר לנכים לחרדים  לערבים לאתיופים למתנחלים ולכל מי שמתכוון להפגין מהיום מותר לכם לחסום כב… חיפוש מהיר בגוגל חושף התפתחות מרתקת במדיניות הפרקליטות כלפי חסימת כבישים  במילים אחרות מחזיק תיק הדמוקרטיה בממשלה מבקש מצה״ל לפעול נגד עיתונאי שהכעיס אותו  מי הסטיריקן שכותב להם את הטקסטים המתוקים האלה  השעות הנכונות בגל״ץ אה 800 1100 1200 1400 1600 1700 ו׳ 800 1200 מוצ״ש 2200  לפי הזעם הנורא של הרב ליצמן על גמזו אפשר לחשוב שמצוות העלייה לרגל לאומן היא הלכה למשה מסיני או משהו בסדר גודל תורנ…  hodayakh ראשי ישע מאשימים נתניהו מונע אישורי בנייה  עפרה של ראש חודש אלול החצבים עדיין לא פורחים פה אבל הסברס הם פיצוי זמני נאות אגב בלי קוצים  חמישי בערב ראש חודש אלול גם המוסף הפוליטי בדפוס ⁦⁦MakorRishon⁩  בג״ץ התיר לשמש לזרוח מחר אמנם תוך הסתייגות מסוימת תופעת החל״ת המתרחבת במרכז החיזוי ⁦MakorRishon⁩ עיצוב אלישע נדב  ריבונות כבר לא תהיה השנה אבל גם יקב פסגות החדש בשער בנימין הוא סוג של ריבונות  גילוי נאות מעודי לא צפיתי בהיהודים באים הפרומו הספיק לי MakorRishon לא יכולים לדבר על זה יותר מדי אבל פרויקט מיוחד שלנו נמצא על האש בקרוב גם אצלכם   ומצד שלישי אנשי ימין שקידמו בתרועות יגון את בשורת הריבונות בסוף ינואר אינם רשאים להתעטף יגון גם עכשיו או או ארי שביט חוזר אל הריאיון המאלף שבלשון המעטה לא קירב את רות גביזון ז״ל אל ערכאת ברק  HaimJelin מסכים לגמרי חיים ועדיין אבו דאבי זה לא בית אל שארגה לא שילה והליכוד מחויב לריבונות  לא למזרח תיכון חדש למה עוד נשאר לצפות אחרי שער בעיתון הנפוץ במדינה  שבת שלום  לשווא נתכחשה כמו שכתב אלתרמן בהקשר אחר ההסכם עם איחוד האמירויות כן גובה מישראל מחיר משמעותי  ויתור על מימוש חזון…  חלום הדורות מתגשם יחסים דיפלומטיים עם איחוד האמירויות הרהור פילוסופי לקראת סיום שבוע ספיגה של אלפי גילויי שטנה ברשת שאני מכבב בהם ותגובות מרושעות שגרתיות אגב לשניים…  אם אין קמח מצוקות הפרנסה של רבני קהילות ולא רק בעיתות קורונה איור רועי קדם ⁦MakorRishon⁩  שרה נתניהו צודקת מיצג הבלונים מול בלפור היה המבחיל ביותר בתולדות ההפגנות הפוליטיות בישראל לו היה מדובר במישהי אחר…  משהו טוב בכל זאת קרה בזכות ממשלת האחדות גנץ ואשכנזי כבר לא תוקפים את מדיניות חוסר התגובה הישראלית בגזרת עזה goldman1007 דניאל אם אתה מתעקש לא לשמוע אז לא תשמע כבר פעמיים לפחות הקדשתי את הטור שלי בMakorRishon  לקריאה לנ…  אם כבר הולכים לבחירות ואין רוטציה אז מתבקש שגנץ יודיע שאמנם נתניהו הפר את ההסכם עם כחול לבן אבל למען טובת האומה…  טוב מתקנים אותי המבשר והמודיע דיווחו על פטירת יעקב אבינו אחרי יומיים יתד נאמן  אפילו זה לא  בזכות הרב שטיינזלץ זצ״ל הבנתי סוף סוף את טענת הגמרא במסכת תענית דף ה ע״ב ש״יעקב אבינו לא מת״ העיתונות החרדית פשוט לא דיווחה על זה סבתי מלכה סגל ומנחם בגין בחנוכת גן בכרמל על שם דודי ידידיה סגל שנחטף אל מותו בידי יהודים ״רק לא מלחמת אחים״ זה…  קבלת שבת בעפרה  Ayeletnnv מעולם לא קלעה כותרת של ראיון כך לתחושותייעל הקרע בישראלהמערכת הפוליטית והחלטתי לצום ב9באב תודה ל Shiritc על דיוק ולב עד… ZvikaKlein עוד תמונה של אריק סולטן ראיינו את הרב בשעת לילה מאוחרת  הוא ישב בלשכתו המבולגנת והמשיך בכתיבה  רשי לא זכה להשלים את מפעל הפרשנות שלו לתלמוד הרב שטיינזלץ זכה הוא היה ארון הספרים היהודי תפוצת כותריו עקפה כנרא…  ZvikaKlein ברוך דיין האמת נפטר הרב עדין אבן ישראל שטיינזלץ ראיינתי אותו לפני 6 שנים זה היה ככל הנראה הראיון הקשה בחיי אך אחד המעני… רק לא בחירות עכשיו  Riklin10 הנה הקטע המלא שמעון  עוד לא נמצא חיסון להפרעות קשב אבל ZvikaKlein שלנו כבר על זה בסדרה חדשה MakorRishon  כשהספרייה הלאומית של עם הספר נסגרת הדבר האחרון שעושים זה ללכת לבחירות  ויכוח לוהט על מקום מרענן למדי בעיצומו של קיץ MakorRishon  הערת אגב לטקסט המופלא הזה ממשלת בגין דווקא חתמה על הסכם שלום עם לבנון ב1983 אחרי שנה הלבנונים ביטלו  kariela את חלשה אריאלה משטרת ישראל מתעקשת להוכיח הקיץ שהיא גיבורה על חלשים ומפוחדת מול חזקים  noamamir74 בזמן שבתל אביב מתרגשים מהקשקוש הזה של להאיר את בניין העירייה בצבעי דגל לבנון הלבנונים חושבים שישראל מביכה מתחנפת ומריצים ה… MakorRishon מבטיחים לבדוק את העניין בינתיים אתם מוזמנים להצטרף למקור ראשון ולקבל חודש ראשון מתנה gtgt  MakorRishon אם זה כתוב על שלט בהפגנה זה כנראה נכון מקור ראשון לחודש מתנה למצטרפים חדשים gtgt   גיהנום קיץ 2020 מצד אחד אופוזיציה שלא מכירה בתוצאות הבחירות באביב מצד שני קואליציה שגוררת אותנו לבחירות  נוספות בסתיו באמת תודה על רענון הזיכרון והעמדת הנרטיב על כנו איך שכחנו רוב המפגינים הובאו לכפר מימון על ידי אלדד יניב סיעות מ…  משהו קונצנזואלי להירגע איתו שקיעה בעפרה העץ במרכז  ארז הלבנון  MakorRishon מן המפורסמות הוא שגדולי הקנאים הדתיים הם ליברלים גלויי ראש עובדה חובשי הכיפות נכנעו לצו שמונע מהם להתקהל בהמוניהם בבתי ה… MakorRishon היבוא המשמעותי ביותר בכוורת של בנימין נתניהו  עכשיו הריאיון   פסקת ההתגברות היא עניין רציני מכדי להפוך אותו לטענת אליבי לפירוק הקואליציה ולהקדמת הבחירות בעיצומם של מגפה ושל שבר…  הביקורת מימין שמתמקדת בפינוק שערוצי 12 ו13 מרעיפים על מחאת בלפור מקפחת קשות את כאן 11 MakorRishon חדש במקור ראשון מצטרפים דרך הצאטבוט ומקבלים חודש ראשון מתנה צוטטו עכשיו gtgt   roysharon11 ״מי שלא שמע את תפילת הנערות לא שמע תפילה מימיו לא ראה תום ותמימות וגם לא ראה איך התום הזה נחבט על הסלעים״ כותבת במקור רא…  yanircozin KnessetT הנה מברק משטרתי עם רשימת העצורים מאחת ההפגנות אז מול משרד רוהמ ירושלים רשימה ארוכה ומפוארת ש…  yanircozin KnessetT זאת ועוד כמעט כל ראשי הימין החוץ פרלמנטרי נעצרו לכמה ימים בעוון הפגנות בלב ירושלים נגד הסכם הנסיגה מסיני yanircozin KnessetT יניר הנוסטלגיה של מרידור סלקטיבית בגין לא רק מנע ממפגינים להגיע לימית ערב עקירתה במשך חודשי…  ShayCharka היום במקור ראשון  ZvikaKlein היום במקור ראשון הכירו את אהרון קליין היועץ היהודיאמריקני של ראש הממשלה נתניהו ששימש כאסטרטג המרכזי בבחירות 2020 עד לפנ… bezalelsm מוצאי ט באב חמש דקות לשמונה החדשות בתאגיד השידור הציבורי של המדינה היהודית פותחים בשידורים חיים מהפגנות השמאל אף מילה ע… סרטון כואב מרתק לקראת הכתבה מחר במהדורה המודפסת שלנו  מתפלל שמחאות השמאל יעברו בשלום בימים הקרובים בלי כל תגובה אלימה של מאן דהוא ושמח לגלות שטעיתי אתמול כשמיהרתי להאמ…  בוגרות תפילת הנערות התכנסו שוב ודיברו עם בתאל קולמן שלנו שגם היא הייתה שם ⁦MakorRishon⁩  כפי שאפשר לראות עמית לא חזק בכדורגל אבל נאום הפיוס והאחווה שלו בדקה ה90 הוא בהחלט פיצוי נאות  Shiritc הערב במקור ראשון משדר מיוחד לליל תשעה באב  השר alonschustermk שוסטר מכחול לבן חכ משה ארבל משס ואנוכי מדברים על הביחד האפ… NadavEyalDesk אל דאגה נדב אצלנו אין בעיה כזאת MakorRishon הכל או כלום מדברים מציאות לא פנטזיה הערב ט באב אנחנו בשידור מיוחד מהעיר שהיא מקרה הבוחן האפקטיבי ביותר להבנת עתיד מערכו… מקור ראשון השבוע לפני 15 שנה  שני דברים דחופים שמשטרת ישראל חייבת לעשות עוד היום 1 לפעול בתקיפות נגד בריוני ימין שתוקפים מפגיני שמאל 2 לחקור…  ramonhaim YinonMagal באביב 95 למשל היה פיגוע באוטובוס ליד כפר דרום 7 הרוגים ramonhaim YinonMagal חיים לצערי אתה טועה בין החתימה באוסלו לשנת 2000 נהרגו למעלה משלושים ישראלים באזור הרצועה גני טל קיץ 2005 מקום קסום בלי ספק  MakorRishon הכתבה הזאת של hodayakh על פינוי הישובים בצפון השומרון בהתנתקות היא בדיוק לכל מי שמנסה לשכנע את עצמו בסיפורים שההתנתקות קר… זאת ועוד השפה הרשמית בנווה דקלים הייתה יידיש משפחת חטואל הגיעה לגוש קטיף מביאליסטוק אבי פרחן כיהן כמזכ״ל בני עקי…  MakorRishon הי טוויטר שימו בצד את החיזבאללה הפגנות תורידו מסכות אם אתם בבית ושבו מול נושאים וצבעים קצת יותר אופטימיים  הערב השני… קורים גם דברים טובים הקיץ אגב יותר משקלמן וסג״ל זקוקים לתוכנית קובלנץ זקוק להם  LifeRivlin זה נכון LifeRivlin בסבסטיה היה מאוד שמח נא לקרוא בבקשה לפני שמגיבים שליחתנו לבלפור במוצש חזרה למערכת עם דוח רגיש מדויק  elishanadav 20 שעות אחרי אירועי אתמול התאגיד מעלה פתאום קליפ אמפתי  כאילו חדשותי  בעד המחאה ונגד נתניהו תעמולה פוליטית במסווה של ד… elishanadav אלישע נדב הוא לא רק מעצב בכיר של שערים רבים שגוררים פה תשואות הוא גם האיש שמאחורי המדור הייחודי אשר צץ לאחרונה במו…  מתוך ארכיון חדשות ערוץ 7  קיץ 95׳ הלוואי והיתה אז מכת״זית  נכון מאוד בואו ניזהר  וגם על כך כתבתי בטורי הצנוע הליכוד חתם עם גנץ על תקציב דושנתי הליכוד צריך לעמוד בדיבורו בחירות  חס ושלום  ZeevKam מעולם לא זכו כל כך מעט מפגינים לכל כך הרבה חיבוק וליווי תקשורתי כותרות ראשיות מעקב סביב השעון שידורים אין סופיים ובעיקר קר… נכתב בהשראת ימי החורבן של שנת 70 לספירה ובהשפעת הרטוריקה של ימינו אלה  15 שנים להתנתקות עם 20 אחוזי סימפטיה תקשורתית להפגנות הענק דאז ביחס להפגנות הבינוניות כעת  גוש קטיף לא היה נעקר  ArielZigler אוקיי הבנתי  שבת שלום  הפגנת הימין בבלפור הערב מיותרת ובעייתית עם ישראל כבר מבין היטב שההפגנות נגד ביבי הן לא בדיוק הפגנות עממיות ומי מפ…  עכשיו תורו לדבר ⁦MakorRishon⁩ צילם אריק סולטן דובב שמואל מוניץ  RonnieBaron1 MakorRishon אני כבר מתחיל לגשש רוני RonnieBaron1 MakorRishon המהלך הוכתר בהצלחה וכבר במהלך הלילה קיבלתי בקשות גישור נוספות רבות היום יום חמישי בדפוס שלנו עובדים קשה עיצוב רועי קדם⁦MakorRishon⁩  YairNetanyahu יאיר אני מוכן לתווך לקראת הסכם שלום כחול לבן התנהלה היום באופן מופקר כשהימרה על עתיד הקואליציה למען חוק בעל משמעות סמלית בעיקר אבל גרירת ישראל כעת לב…  נפלאות התבונה ללכת לבחירות בעיצומו של אסון טבע כבד ומשבר כלכלי איום בגלל חוק ההמרה arielschnabel בעיניי השלט המזעזע ביותר בערב הזה מדינה מחלה באמת  אחרי שצבר ניסיון רב בסיקור הפגנות פתח תקווה שליחנו המיוחד עלה ירושלימה  arielschnabel ראיון בלעדי ראשוני ומיוחד עם נושאת השלט ההשוואה לשניהם צפו כמו שאומרים  לפני שנתיים וחצי ביקרתי בבית שבו נולד זבוטינסקי באודסה בפתח נתקלתי בחתול ביתרי  Shiritc  אם ארצי דללה וקטונה היא שלי מראשה עד קיצה משתרעת מים ישימונה וירדן הירדן באמצע שתי גדות לירדן  זו שלנו זו גם כן…  MrRobotjew אני ממש נגד בחירות arikbender הפוך אריק הדוגמה החינוכית ניתנה במוצאי שבת קצת מגוחך להתנפל על המסיבה הקטנה בגמנסיה כשכמה עשרות מטרים משם בכיכר פאריז היתה רק יממה קודם מסיבה גדולה פי כמה שזכתה לקריאות הידד המוניות האחיות עובדות היום במתכונת שבת כי עקב המחסור הגואה בכוח אדם והקורונה הן עברו  לעבוד בשבת במתכונת חול גילוי נאות אחד שיודע מהבית לכל אלה שלא חיבבו בלשון המעטה את ציוציי אמש נגד הכותרות הטלוויזיוניות הכוזבות ״מדינה במחאה״  נוסבאום אישר הערב מפו…  כמה יפה שיש אצלנו חופש מחאה לכול  סיכום זמני העובדה שמאוד קשה פה עכשיו בלשון המעטה ושהממשלה מטפלת בגל השני באופן חלטוריסטי  לא מתירה לתקשורת הממו… </t>
+  </si>
+  <si>
+    <t>tamarzandberg עשרים ושמונה אלף מובטלים חדשים רק ביממה האחרונה אבל ההפגנות שמואל אליהו אינו ראוי להיקרא רב או בכלל לתת דוגמא למישהו בציבור אין מקום במגזר הציבורי לגזענים והומופובים לכהונה…  שנה טובה  talshalev1 ניצן הורוביץ נתניהו הסכים להקפאת בנייה בהתנחלויות תמורת הנורמליזציה עם מדינות ערב יודע את זה ממקורות מוסמכים נעמוד מול המושחת מבלפור תמיד בלי זגזוגים  האלימות קורעת את החברה הערבית ואת החברה בישראל בכלל הממשלה לא יכולה להמשיך להתעלם  יש להעביר תקציבים לפתוח בשיח…  attilus פרופ ירון זליכה ברדיו 90 מפציץ ומפתיע שאול מרידור מיצה את הפוטנציאל שלו לגרום נזק לכלכלה טוב שהתפטר בגללו משלמים 6 דולר ל… האלימות נגד נשים לא מספיק חשובה לממשלה כדי למנות ועדת שרים מיוחדת לטיפול בנושא אבל כשזה מגיע לסוגיה הקריטית של הנס…  tomereznik כמה מנותק יכול להיות שר האוצר Israelkatz שמציע קיצוצי שכר במגזר הציבורי בזמן מיתון השנאה לעבודה המאורגנת ולכל דבר שהוא צ… EilonTohar מחכות לך במרצ להתפקדות gtgt  לא יועז זה המשטרה שהופכת מפגינים לשק חבטות אי אפשר להתעלם מהאמת כשיש תיעוד ברור שלה  ביבי נמאסת לך הביתה  tomereznik YairNetanyahu אין דבר יותר פוליטי מזה שיש יותר ממיליון מובטלים ועוד מאות אלפים שפרנסתם נפגעה בגלל המדיניות הכושלת של הממשל… YairNetanyahu אצלכם זה כבר מזמן לא פוליטי  זה פלילי ילד צוחק מי שצוחק אחרון  ביבי מקשקש היום בתקשורת על הסתה כנגדו אין גבול לחוצפה  המסית הראשי הוא האחרון שיכול לדבר על מחירי השנאה  את בי…  talschneider לבקשת NitzanHorowitz עכשיו במליאה שר האוצר כ״ץ משיב שלא תהיה פגיעה בשכר המינימום כדי לממן את המענקים ואת הפריצות התקצי… שמחים להציג תכנית כלכלית חדשה להתמודדות עם המשבר לקריאת התכנית המלאה gtgtgt   עכשיו בבלפור ביבי הביתה  אנרכיסטים מסוכנים  סוגרים שבוע אופטימי ומלא הישגים למרצ  ניצחון הצעת החוק של ניצן הורוביץ לעצירת טיפולי ההמרה עברה עכשיו במליאה  מברכים את איגוד העובדים הסוציאלים על הגעה להסכם בסיומו של מאבק מרשים ומרגש הוכחתן שוב שביחד אנחנו חזקים ויכולים לכ…  tomereznik אפשר לקוות שהתנהלות הממשלה תזים לכל הפחות את הטענות המגוכחות שאין כסף  לקצבאות הנכים לעובדים הסוציאלים למיטות אשפוז… NitzanHorowitz עוד סקר שבו מרצ מתחזקת ל7 מנדטים הרבה יותר מהעבודה גשר ודרך ארץ ביחד  כי אנחנו לא בוגדים בבוחרינו לא גונבים קולות… נאבקים עם העובדות והעובדים הסוציאלים השירותים החברתיים צריכים הנשמה עכשיו  השטויות האלה שלאנשים אין מה לאכול זה חארטה  צחי הנגבי מצליח להעביר את כל הסיפור של הממשלה המנותקת הזאת במשפט אחד…  יור מרצ ניצן הורוביץ בתגובה ליוזמת שר האוצר הצעת שר האוצר לקיצוץ 45 מיליארד שח במגזר הציבורי בעיצומו של משבר הק…  kannnews חכ תמר זנדברג בישיבת סיעת מרצ ועדת הכספים במקום לשלם דמי אבטלה לעצמאיים תדון בפטור ממס לרהמ  הנאשם בשוחד אם זה היה… עוצרים את אסון הסיפוח  טיפולי המרה הם התעללות הם לא עובדים ולעולם לא יעבדו הגיע הזמן לשים להם סוף  הצטרפו אל יור מרצ ניצן הורוביץ לשיד…  את המבחן הזה כחוללבן חייבים לעבור  הזמן לקיים  בפרק הבא של הליכוד ביטול המענק לעצמאיים בגלל שהבן של גנץ לא עשה שיעורי בית  אצל קיצוניי הדת הביטוי ״עד שהמוות יפריד בנינו מקבל משמעות חדשה  YairGolan1 עיתונאים לכלאאמרתי לכם בפגישה עם יו״ר מרצ שגריר האיחוד האירופי מזהיר מסיפוח סכנה ליחסי המסחר והמחקר הורוביץ לזופרה חייבים לעשות הכול…  זה הזמן להתעורר ולהצטרף למאבק הכי חשוב שהיה כאן חייבים לעצור את אסון הסיפוח  זו הוועדה למעמד האישה זהו את היור  בוא שנתחיל לפנות על כל הסתה לרצח ברשת נגד אנשי מרצ לא שלוש ולא ארבע בחודש אצלינו סופרים בK חביבי   מצפים לתגו…  tamarzandberg הסיפוח הוא דיל מסוכן ומושחת שאין לו קשר למה שטוב לנו ישראלים ופלסטינים שגרים כאן במזרח התיכון זה דיל שיהפוך את ישראל ר… NitzanHorowitz הסיפוח הוא פשע מלחמה שיעלה לנו בדם  גנץ אשכנזי פרץ ניסנקורן  האחריות תהיה עליכם אין לכם מנדט תרתי משמע אין לכם… ח״כ תמר זנדברג בהפגנה נגד הסיפוח  ״עכשיו הזמן להגיד לא להיאבק בכל הכוח לא לשתוק יהודים וערבים ולהקים גם אלטרנ…  יור מרצ חכ ניצן הורוביץ בהפגנה נגד הסיפוח הסיפוח הוא פשע מלחמה  פשע נגד השלום פשע נגד הדמוקרטיה פשע שיעלה ל…  NitzanHorowitz עוצרים את אסון הסיפוח  כיכר רבין  בקרוב מתחילים בואו  מחר 1900 כיכר רבין  מחנה השלום משיב מלחמה  NadavEyalDesk בהודעת המשטרה בבופאלו נאמר שהוא החליק ונפל JacobMagid Meretz chairman ⁦NitzanHorowitz⁩ warns against Trump ‘apartheid’ plan in West Bank protest tour  זהבה גלאון הסיפוח לא מעניין את נתניהו גם לא שפיכות הדמים שתבוא אחריו הוא הולך למהלך הזה מסיבה אחת להסיח את הדע…  יור מרצ לשעבר יוסי ביילין בסיור מרצ בבקעת הירדן סיפוח בסדר גודל כזה יביא איתו סיפוח נוסף גדול יותר ואנחנו נמצא…  יור מרצ לשעבר זהבה גלאון בסיור מרצ בבקעת הירדן למהלך הזה יש מטרה אחת  להסיח את הדעת ממצבו המשפטי של נתניהו זה…  עוצרים את אסון הסיפוח  במוצש הקרוב כולם בהפגנה בכיכר רבין  דר שאול אריאלי בסיור מרצ בבקעת הירדן המשמעות של החלת הריבונות בבקעת הירדן היא שנצטרך להקיף את יריחו בגדר את ירי…  יור מרצ ניצן הורוביץ בסיור מרצ בבקעת הירדן הגענו לשטח כדי לעמוד מקרוב על ההשלכות של הסיפוח סיפוח שהוא אסון מדיני…  כל יום צפרדע חדשה  האזנה חובה ראש השבכ לשעבר מזהיר מתוכנית הסיפוח נצטרך להשקיע ים של כסף בביטחון נידרדר למדינה אחת דה פקטו  אסון…  מחר תעלה במליאה הצעתה של tamarzandberg לוועדת חקירה פרלמנטרית בנושא רצח נשים בואו לדרוש מהממשלה החדשה להתחיל עם צ…  לעצור את הסיפוח הצטרפו אלינו לרב שיח בפייסבוק לייב ביום חמישי  בטוחים שOrlylevy תעשה עבודה לא פחות טובה מקודמה במשרד  אקורד הסיום של ⁦naftalibennett⁩ במשרד הביטחון  השוואה מקוממת ומסיתה של ארגון העובדים הגדול במשק לחמאס הזוי לחשוב…  סיפוח אינו תרופה לקורונה PeaceNowIL  PeaceNowIL יישר כח לחכים שבאו למחות איתנו NitzanHorowitz tamarzandberg  ישיבת סיעת מרצ  שחיתות  זה מדבק  לתשומת לב Kachollavan19 HavodaParty פסיקת בגץ היא לא הכשר לשחיתות ולא הופכת שיתוף פעולה עם נאשם בשוחד ללגיטימית…  KnessetT בנאום במליאה פנה חכ YairGolan1 מmeretzparty לאנשי הציונות הדתית חלום הסיפוח לא יתגשם הנאשם מבלפור יוליך אתכם בכחש פע… מושחתים נמאסתם איתכם עכשיו בכיכר רבין לא ניתן להם לסגור את הדמוקרטיה  כחול לבן או ארדואן למה לבחור כשאפשר גם וגם  משטרת החמץ  הסוף קביעת בגץ מסמנת את  הסוף למשטרת החמץ בבתי החולים ומהווה ניצחון חשוב נוסף במאבק בכפייה הדתית ובדר…   מזל טוב למדינה וגם לחכית הלוחמת המצטיינת שלנו tamarzandberg אוהבים אותך תמי   יום עצמאות שמח לכל הישראלים והישראליות  מרצ כאן כדי להיאבק על מדינת ישראל דמוקרטית שוויונית חופשית ושוחרת שלום…  זוכרים את הנופלים נאבקים על החיים  מפלגת העבודה ביצעה היום חריקירי אידיאולוגי ופוליטי ונכנעה לשחיתות ולסיפוח סיבוב של 180 מעלות מדרך רבין  אנשי שמאל…  שמאלנים הביתה  עשרות מצטרפים חדשים למרצ מאז הבוקר להתפקדותgtgt   מפלגת העבודה חדלה להיות בית עבור רבים עמיר מתעקש לקבור את מפלגת העבודה בעבור גוב בממשלת סיפוח בראשות נאשם   חברי…  NitzanHorowitz כבוד לפעילי מרצ הרבים בהפגנות הדגלים השחורים המאבק הזה של השמאל ההפגנות בכל הארץ הוא שלב חשוב במאמץ לחיזוק השמאל לאח… תרגום לא יכולתי לעמוד בפיתוי העדפתי לבגוד בבוחרים להפר כל הבטחה ולשים את המסמר האחרון בארון הקבורה של מפלגת העבו…  איזה יום מעניין בחר לו סמוטריץ לקרוא לשינוי חקיקה שיאפשר אפליה על רקע נטיה מינית  אמונה ותפיסות עולם הן לא תירוץ ל…  די נו הוא לא באמת עשה את הקישור הזה עכשיו  הגנרלים הפכו שכפץ משפטי לנאשם בפלילים מה שיקרה לכחול לבן זה בדיוק מה שקרה לכל מי שנכנס תחת נתניהו  הם ימחקו וישא…  זאת לא ממשלת אחדות זאת לא ממשלת חירום זאת ממשלת שחיתות  KnessetT מצאו קורבן חדש במדינה  המורים בשלב נאומים בני דקה במליאת הכנסת דיבר יור meretzparty חכ NitzanHorowitz על סוגיית המור… KnessetT יור meretzparty ניצן הורוביץ התארח בבוקר טוב כנסת עם YuvalKarni ותקף את ראשי Kachollavan19 וLikudParty כשאמר גנץ נ… עכשיו  הילד הזה צריך לשטוף את הפה עם הרבה אלכוגל לא להאמין שזה האיש שמנהל את ראש הממשלה  מדיניות המעקב של הממשלה ושתי הצעות החוק שהונחו היום בנושא הן פגיעה בלתי מידתית בחירויות היסוד משטרה לא צריכה לנטר…  NitzanHorowitz מביך ועגום שגנץ בחר לתקוף לא את נתניהו שמעביר אותו זובור משפיל אלא את בוחריו ושותפיו שזועמים שהפר את הבטחתו להם  על נ… tomereznik הפתכם את פתק אמת לפתק שקר tamarzandberg המשפט של ימינה ״אם נהיה באופוזיציה נילחם בשחיתות״ פסיכי ברמות ועדיין עובר בשקט יחסי וכדחקה משעשעת במקרה הטוב בשמאל זה… יפוטר ליצמן  TomerPersico אז בסוף מסתבר שמכל קונגלומרט אמת רק היאפים הפרוגרסיבים המתנשאים האשכנזים הסחים המזויפים הקרים האליטיסטים המנותקים האנטי… hamakom היום היום היום  קוראים המפגינים לחכ NitzanHorowitz שמבהיר כי לפי פסיקת בגץ אדלשטיין חייב להביא להצבעה את בחירת יור…  newsisrael13 מליאת הכנסת אישרה את הקמתה של ועדת החינוך שבראשה יעמוד יור מרצ NitzanHorowitz הוועדה תטפל במצב מערכת החינוך לנוכח התפ… התחלנו  אלפי מפגינים הגיעו היום לכנסת להפגנת הדגל השחור יחד עם חברי הכנסת של מרצ  נמשיך להיאבק כנגד ניסיון ההפיכה השלטונית…  הם סגרו את בתי המשפט בשביל רהמ הנאשם סגרו את הכנסת כי אין להם רוב דרסו את חוב והפעילו מעקב אחרי אזרחים ללא פיקו…  tamarzandberg רק שתבינו את גודל הבזיון לליכוד אין שום בעיה לפתוח ועדות בתנאי שיחסי הכוחות בהם יהיו חצי חצי ולא יבטאו את היחס 6158 ש… NitzanHorowitz שאלה לח״כים הנדל האוזר לוי אתם מצהירים על רצונכם באחדות גנץ פנה לכל ראשי הימין  הם מסרבים אפילו להיפגש אתו אז הימ… ממליצים על גנץ לנשיא נשמרים מהקורונה  לא ניתן לנתניהו לנצל את הקורונה כדי לברוח מאימת הדין הצטרפו למשמרת מחאה מול בית ראש הממשלה gtgt  התרענו מראש כבר בבחירות 2020  אנחנו קוראים לבני גנץ לקחת את המנדט מהנשיא ולהקים ממשלה חדשה שתביא תקווה לישראל  NitzanHorowitz המון אנשים אמרו לנו בבחירות שהם נקרעים בין התמיכה בשמאל לבין הכמיהה העזה להעיף את ביבי הזהרנו אותם שכחוללבן לא סגורים… NitzanHorowitz גם דנה אינטרנשיונל הצביעה לאמת שלה  שעות אחרונות וקריטיות נלחמים על כל קול עד הסוף לא משאירים אף שמאלני בבית  לא נוטשים את דרך השלום מצביעים אמת  דרך רבין בסכנה צאו להצביע אמת  mkgilon אנחנו נכנסים לשעות המכריעות חייבים שתצאו להצביע זה הכל תלוי בכם תבחרו באמת שלכם  Syechimovich בפעם הראשונה השנה באתי להצביע מאופרת ובג׳קט בפעם השניה יותר קז׳ואל והפעם בכפכפים ובתחושה מסתורית שאני טום קרוז שקם שוב… שעות אחרונות להצבעה כל קול חשוב לכו עם האמת שלכם  עכשיו  הגענו לרגע האמת זה הזמן להלחם על כל קול תלחמו על האמת שלכם על העתיד של הילדים שלכם תלחמו על המדינה תלחמו על הש…  בשביל שותפות אמיתית  יוצאים ומצביעים אמת  תקשיבו לתמי  mkgilon עכשיו בבאר שבע לא מוותרים על אף קול תבחרו באמת שלכם  ראשי העבודהגשרמרצ בהצהרה מיוחדת NitzanHorowitz אנחנו קוראים לציבור המצביעים שלנו לא להתחשב בהודעות הכזב שמופצו…  22 הגשנו כבר 3 עתירות מהבוקר לועדת הבחירות המרכזית על זיופים השחתות פתקים והבטחות שווא שאם מישהו יחזיק קמע הוא י…  12 ראשי העבודהגשרמרצ בהצהרה מיוחדת מתחילת יום הבחירות אנחנו מתמודדים עם אי סדרים של הליכוד וש״ס בקלפיות בכל האר…  עמר בר לב רוויטל סויד ואילן גילאון מתנדנדים  הפיצו את הסרטון עכשיו ושכנעו חברים להצביע אמת  את מי אתם רוצים באמת  אנחנו כבר בחרנו באמת שלנו עכשיו תורכם  רק פתק אמת הוא פתק בטוח לממשלה של שינוי בישראל  עוד פתק אמת ומחנה השינו…  מסתערים על תאיפו  עתרנו הבוקר לועדת הבחירות נגד חלוקת חפצים אסורים על ידי שס בקלפיות במרכז ושלחנו אליהן את חניכי תנועות הנוער   החו…  גם יור מרצ ניצן הורוביץ בחר באמת שלו היום אסור להשאר בבית צאו לבחור ושימו אמת בקלפי עוד פתק אמת ומחנה השינוי מנ…  חייבים להכניס את אילן לכנסת  הקלפיות פתוחות והפעילים שלנו כבר מחכים לכם שם היום כולם בוחרים באמת שלהם עוד פתק אמת ומחנה השינוי מנצח  NitzanHorowitz כדי שנתניהו יילך סוףסוף  וגם ולא פחות חשוב באותו פתק    למען השיוויון      למען החופש           למען השלום… עוד פתק אמת ומחנה השינוי ינצח  משמרת נעימה אילנה רק אמת  NitzanHorowitz בתוך כל הרפש ההקלטות וההשמצות הנה משהו ברוח אחרת חוק חדשני שאני הולך לקדם בכנסת הקרובה שייתן לכל אחד את הכוח להיאבק… לא מוותרים על אף קול ממריצים את כל הבוחרים לקלפי  עוד פתק אמת בקלפי  ומחנה השינוי מנצח  אצלנו אין עריקים ואין פקפוקים פתק אמת שלך ומחנה השינוי מנצח  NitzanHorowitz רם פרומן יו״ר הפורום החילוני ״הצלת מערכת החינוך הממלכתי מידי שרי ההדתה היא המשימה החשובה ביותר העומדת לפתחה של ממשלה… מי שרוצה שינוי בישראל מי שרוצה חלופה רעיונית לדרכו של נתניהו  צריך לבחור באמת שלו  סופ״ש אחרון לפני הבחירות פוגשים אתכם עכשיו בכל רחבי המדינה  רק פתק אמת הוא פתק גם להחלפת נתניהו וגם לקידום כל מה…  יש שופטים בירושלים  משהו רע ועצוב קורה בכחוללבן  NitzanHorowitz ״הלהטבים הערבים נעים בכמויות אדירות לקלפי״ תקראו את חאדר אבו סייף  גם הוא בוחר באמת שלו   tamarzandberg רויטל סויד 10 עיסאוי פריג׳ 11 וחגי רזניק 12 הם חברים שלי ח״כים מצטיינים ושליחי ציבור מעולים חשוב שיהיו בכנסת לא… גם נעמי בוחרת באמת שלה  נסגר המפעל שעבדת בו כל חייך הליכוד מציע לך ללכת להיות שוטף כלים הגיע הזמן להעיף אותם הביתה ולהקים ממשלה חדשה עם ל…  גם אתם בוחרים באמת שלכם  גם רן יקיר בוחר באמת שלו  ממשלה ישנה או ממשלה חדשה הבחירה בידכם   גם רויטל בוחרת באמת שלה  ממשלה ישנה או ממשלה חדשה אתם תבחרו  ממשלה חדשה או ממשלה ישנה רק אתם תבחרו   גם יסמין ורויטל בוחרות באמת שלהן  גם גיא בוחר באמת שלו  צלמו גם את עצמכם מסבירים מה האמת שלכם ותייגו אותנו  IsraelHayomHeb אפשר להקים ממשלת מיעוט עם הימנעות הערבים שרי החינוך שבאו מהציונות הדתית הרסו את החינוך הממלכתי NitzanHorowitz ברא… ישראל מחכה לממשלה חדשה ממשלה שתביא שינוי ותקווה ממשלה שתחזור לתהליך השלום ותקדם מדיניות חברתית באמת  tomereznik אני מעדיף כלכלת הסתדרות על כלכלת מסודרים גם בyeminaparty מבינים שתקום פה ממשלה חדשה  לב חברתי או קפיטליזם חזירי במה תבחרו  מזל טוב לחכ תמר זנדברג וחבר הנהלת מרצ אורי זכי על הולדת בתם בריאות ואושר tamarzandberg urizaki YuvalKarni הקמפיין של העבודהגשרמרצ הערב על בניין מצודת זאב בתל אביב  הגיע הזמן להחליף yeminaparty realrafiperets  NitzanHorowitz אנחנו מתחייבים היום שהעבודה גשר מרצ תבקש את תיק החינוך והתרבות בממשלה הבאה  ראש בראש הורוביץ מול שקד מדינה יהודית ודמוקרטית מול סיפוח ומדינה דו לאומית  תאמת אמת היא הבחירה שלכם למה כי זה לבחור במי שאתם תבחרו באמת שלכם העבודהגשרמרצ  newsisrael13 חכ tamarzandberg התייחסה במליאה למשיכת החסינות של נתניהו הניסיון להפוך את הכנסת לעיר מקלט למושחת  קרס מאוד מקווה שנ… חכ tamarzandberg נותנת בראש בפאנל באוניברסיטה העברית  תאמת  אמת היא הבחירה שלכם  הנבחרת שלנו יוצאת לשטח יצאנו הערב לפגוש אתכם בברים ברחבי תאיפו בחודש הקרוב נחרוש את השטח בכל רחבי הארץ ונאבק על…  הגשנו הערב את רשימת העבודהגשרמרצ לכנסת ה23  יוצאים לדרך ביחד  NitzanHorowitz שר ״החינוך״ קיבל היום חינוך אמיתי דווקא מהתלמידים   תכלס שיעור באזרחות בערכים ובאהבת אדם  רפי פרץ לא ראוי לנוער המד… ועידת מרצ אישרה הערב ברוב גורף את הסכמי החיבור עם העבודהגשר ועם חכ יאיר גולן  יוצאים לדרך ביחד לשותפות של תקוו…  אויש השריון להומופוב מוצהר  בשורה גדולה לגוש המרכזשמאל חדשות רעות לגוש החסינותגזענות  מאוחדים  mkgilon מרגיש טבעי  שותפות של שינוי ותקווה  NitzanHorowitz שר הביטחון הזמני ממפלגת שלושת המנדטים משתולל מינה את קובי אלירז יקיר המתנחלים  להיות אחראי על שטח סי נותן לחתול לשמ… תיקנו לכם   NitzanHorowitz היה נכון בפברואר ואפילו יותר נכון עכשיו  הוסרו המסיכות כחול לבן פונים ימינה ושואפים להיות ליכוד ב׳ אין לנו צורך בעוד בעוד ממשלת ימין לא שינוי אמיתי מבטיח…  tamarzandberg מי שלא רוצה לראות ראש ממשלה בכלא שינסה לדאוג לכך שראש הממשלה לא ייקח שוחד אפשר להפסיק עם המנטרה החלולה על אחדות אין אחדות עם נאשם בפלילים  הפעם הוכח מעל לכל ספק – רק גודל הגוש קובע רק שמ…  מהיום הרע הזה אנחנו מסתכלים על ההזדמנות שלפנינו בבחירות הבאות נגדיל את כוחנו ונחזק את גוש השמאל כולו ואז תהיה פה…  mkgilon פותחים את הכינוס בנושא קצבאות הנכות לא דורשים חמלה ולא דורשים רחמים דורשים את מה שעבר בחוק על ידי כל יושבי הבית הזה דורשים… mkgilon דוח העוני של לתת הוא כתב אישום חמור נגד רה״מ כתב אישום נוסף העובדה שילדים נאלצים לוותר על ארוחה וקשישים נאלצים לוותר על תרו… 4 שנים ללכתו של יקירינו יוסי שריד זל שר חינוך ראש אופוזיציה חבר כנסת מנהיג יהי זכרו ברוך  22 הוא אינו מתחשב בדבר  בוודאי לא בטובת המדינה  בשלטונו המופקר  לנוכח מהלכיו המופקרים של נתניהו והתקפותיו על של…  12 נתניהו אינו בוחל בשום קומבינה ובשום תרגיל בזוי כדי להיאחז בכסאו ולחמוק ממשפט מינוי שרים בממשלת מעבר הוא פסול ו…  כמו בכל שנה גם הערב הגענו לעצרת לזכרו של יצחק רבין זל כדי להגיד כן לשלום לא לכיבוש  EsawiFr זאת מציאות חיינו  עוד ועוד פיצוצים עוד ועוד נפגעים הפעם סמוך לפארק בו מבלות משפחות כשאתם קוראים על עוד פיצוץ בכפר קאסם אנ… להסתה נגד האוכלוסייה הערבית בישראל יש מחיר כבד וליד המקלה והמלטפת כלפי המתנחלים גם את התוקפים לא צריך ללטף ולחבק…  חילונים שקד ובנט מוותרים עליכם  לא תוכלו לנסוע באוטובוס לים בשבת לא תוכלו להתחתן בדרככם לא תוכלו לחיות ללא כפיי…  מיידי אבנים צריכים לשבת שנים ארוכות בכלא השר לביטחון פנים גלעד ארדן ספטמבר 2015  tamarzandberg תרמתי למשפחת חסדאי הרצח המזעזע והמיותר של אופיר לא יוצא לי מהראש חושבת על דקלה חולה בניוון שרירים ומטופלת בשתי ילדות ע… שוב אנחנו רואים שממשלת החיים עצמם מתעלמת מהחיים שלנו וועדת הכספים חייבת להיענות לדרישתו של חכ mkgilon ולהתכנס…  עכשיו אפשר להגיד רשמית  המחנה הדמוקרטי יוצא לדרך תודה רבה לחברי ועידת מרצ שאישרו ברוב גדול את האיחוד  חכ EsawiFr לא סתם נתניהו לא פנה למרצ בניסיון להקים ממשלה המחנה הדמוקרטי לא יהיה חלק מממשלת ימין אנחנו כאן כדי…  חכ tamarzandberg במשך יותר מידי שנים חבטו בשמאל היום השמאל הוא מקור לגאווה מצטרפים אליו לא מפחדים ממנו היום…  חתן פרס ישראל דויד גרוסמן הצירוף של סתיו שפיר ואהוד ברק בהנהגתו השקולה והמחושבת של ניצן הורוביץ מבורך בעיניי אנח…  ראש המחנה הדמוקרטי NitzanHorowitz להיות שמאלני זו גאווה  ראש המחנה הדמוקרטי NitzanHorowitz אנחנו לא מתחפשים למרכז  אנחנו שמאל ראש המחנה הדמוקרטי NitzanHorowitz לראשונה יש לנו הזדמנות להוביל ולעשות היסטוריה השמאל הישראלי לוקח את המפה הפוליטית שמאלה</t>
+  </si>
+  <si>
+    <t>bars10 GanganaMoshe talschneider תפילות עם התקהלות שלא במסגרת הכללים אסורה כולל הפגנות של מטורללים איך אפשר להאמין לליאת בן ארי שווקי כתובעת אמינה ישרה וצדיקה בתיק התקדימי נגד בנימין נתניהו כאשר השופט רוזן טוען שהי…  Arieliluz BarashiKinneret ולגבי הבן שלה elizipori ליאת בן ארי מודה אני עבריינית בנייה  ״מן הראוי שהשינויים המסויימים שנעשו בבית כמו גם הפיצול ל2 יחידות דיור ייעשו רק לאחר… InsteadofGame elizipori לא ניקח אותה למשפט כנתבעת elizipori אבל חתמה על חוזה בקניית הבית ובלקיחת המשכנתא חחח על מי היא עובדת esnet120 באמת קשה להיות בין פטיש לסדן BarashiKinneret 🤣🤣🤣🤣נוכחתי בטיפשותו בצפיה בפטריוטים rafi14412819 מקבל פנסיה תקציבית עושק ArielleBenO  UzanShoshi rothmar יתרה מזה היא מתלוננת על איש ליכוד שחיפש ומצא את החומר זה עוד יותר חמור כמו מנדלבליט והקלטת ArielleBenO חחחחח גדול rothmar פשוט לא יאומן האישה הזו חושבת שהיא מעל החוק עשתה מעשה עברייני וכועסת שחשפו אותה מפני שאלה שהיו אמורים לש…  ErezZadok1 אז היא עבריינית פריבילגית  כמו שחשבנו תושבי ראש העין שקיבלו קנסות ומשפטים בגלל חריגות בניה חייבים לתבוע את הרשויות על אפליה ErezZadok1 להבנתי השופט בעניין ליאת בן ארי קבע שהיא עברה עבירות בניה אבל היא לא עברה עבירות בניה או שהיא עברה עבירות בניה אבל זה לא ע… dogly1900 הבן של ליאת בן ארי N12News זה פייק ניוז של עיתון נוני הנאשם בפלילים BarashiKinneret בואי נראה אם זה מה שיקרה הלואי קשה לי להאמין  ומה זה אומר  galidalal talschneider במלחמת יום הכיפורים הורים לא ראו את ילדיהם חודשיים והילדים האלה נלחמו בשיניים בכדי שכולנו נחייה ונגיע עד הלום… BarashiKinneret בואי נראה אם זה מה שיקרה הלואי קשה לי להאמין KnessetT bezalelsm naftalibennett חחחחח התקלה לבנט KnessetT היור למה אנחנו יושבים פה בלי מסיכות חלל סגור הכל עובר חכ bezalelsm הזהיר בוועדת הכספים רהמ אמר ששני ההצדדים עם מס… בניהו חייב לעמוד לדין על הסתה להמרדה ביום כיפור אנחנו במלחמה אם הפנסיונר לא שם לב  BarashiKinneret מה זה אומרתביעה פלילית נגד ליאת בן ארי שווקי zahavabitton ייתכן ייתכן ייתכן Riklin10 קלמן עשה סיבוב על כל הימין בוחרי הליכוד בכדי לרצות את הפריץ בידרמן צוחק גם על קלמן הרי הם לא סובלים מתנח…  Sigalbz esnet120 Riklin10 בדיוק נמאס מהחסידים השוטים שמלקקים לשמאלנים רק בגלל שהם עובדים איתם קלמן ליבסקינד מבייש את עצמו Riklin10 tadmorerez48 אפרופו לשיחה ששוחת עם איפרגן ממש בדקות אלה השמאל עושה עלינו סיבוב ודחקות bars10 talschneider אתה מדקלם מבלי לדבוק סתומה מי שילדה יצור כמוך yon32440037 ChaimShore misscorina2 משתמשים בך ומהנדסים לך את המוח כמו שהצליחו להנדס אותי בזמן אוסלו וההתנתקות ה…  Eladingo זו אמירה של אנרכיסטים רדיקלים יש חוקים במדינה ואתם תאלצו לקיים אותם ההפגנות לא יעזרו לכם לדעתי הם רק מתסכלים אתכם מיום ליום ChaimShore misscorina2 בכל חברה יש דבילים שימושיים היא אחת מהם talschneider הכתבת טל מפיצה פייק ניוז תקראו שהיא משקרת תמחקי את הציוץ המסית  talschneider אתה מפיצה פייק ניוז כמעט ונפלתי בפח שטמנת YairNetanyahu ושאני פרסמתי את הכתובות שלהם קיבלתי צו הטרדה מאיימת מ״שופטת״ כנגד אנשים שקראו לרצוח אותי דרך אגב YanivTurgi נכון AmirHaskel על מי אתה מאיים עבריין שאוכל ושותה מהכיס של הציבור הישראלי איש אלים ופריביליג talschneider במלחמת יום הכיפורים הורים לא ראו את ילדיהם חודשיים והילדים האלה נלחמו בשיניים בכדי שכולנו נחייה ונגי…  dogly1900 מישהו מקשיב לתכנית שלו מפיץ קורונה AkerZeev כנראה מתוכננת להיום שיירת קורונה לדעתי עכשיו זה רשמי מיליון מתים מהקורונה בעולם מעט יותר מחצי שנה בקצב הזה 2 מיליון בשנה  יורם לססססססס מכר לציבור הי…  Riklin10 המשפט האחרון הכי חזק ומשמעותי בתזה הזו ההגמוניה משמידה כל מי שמאיים עליה זו עובדה מוגמרת לצערי חייבים לשנות את הנוסחה צפו שרשרת משאיות יצאה עבור ניצחון טראמפ בבחירות הבאות  NitzanHorowitz תפגינו בקפסולות מתחת לבית שלכם ותדביקו רק את הסביבה הקרובה אליכם GadiTaub1 OrenNahari בדיוק חחחח מעתיקים מעיתונאי שמאל רדיקליים מציאות מדומה ושקרים GadiTaub1 OrenNahari הדרך היחידה להמשיך לחשוב שהניו יורק טיימס הוא עיתון עיתון היא להתעלם מזה שהעיפו את גיימס בנט ממכתב ההתפטרות של… giladzw אורן מזמן איבד את אמינותו מצאתי אותו מסלף חופשי בכל הנוגע לטראמפ כתב פח IlanTsion משה נוסבאום מקשת 12 משתמש באולפן החדשות בכדי לעודד הגעה להפגנות האיש מתאר בהתלהבות מהיכן יצאו השיירות היכן ייפגשו משער… עומר עליאן משלמת כסף למצביעים בכדי להכנס שוב לקונגרס שחיתות הדמוקרטיים נחשפת  freyisrael1 זה חלק מהציבור שלך saragusti kann לא מכעיס בכלל תתמודדי את חיה במדינה יהודית לפני דמוקרטית וכל אזרחיה למה קשה לך להפנים AfifAbuMuch saragusti kann אתה חי במדינה יהודית תפנים מתי הגברת שאשא ביטון לוקחת אחריות ומתפטרת מהחידלון שיצרה  N12News KerenBNews וואלה לא רק בישראל אז למה המטורללים עדין ממשיכים לנסות להדביק את כל המדינה ולרצוח אנשים XQuiql5V6JZExCE ההגדרה נכונה רבנים אומרים בתי כנסיות וזו העברית הנכונה האיש מאיים על מפקד מחוז ירושלים ככה עובדים במאפייה איך לא עוצרים את האיש בגין הסתה פרועה  levimano lioratz yarivop אם נקבל בעוד 10 ימים 10000 נדבקים ביום עם 35 בדיקות חיוביות במגזר הפצצות הביולוגיות ועלייה בהתאם במספר ה… NoaSaar עכשיו מחוץ לבית של שר הבריאות יולי אדלשטיין אין מחילה ואין כפרה למפיצי מחלות  haskioren על מי הם עושים את הפסיכולוגי הזו אפשר לחשוב שיש לנו השפעה על הבחירות שם ערוצי התעמולה פתחו בחדשות השנאה עברו לטראמפ tsahi8 האמת נשלח בטעות מפגינים לי הבית של גנץ יצאנו מיום כיפור למציאות השנאה לא נרגעו levimano RubiYona הפקרות ומסיבות ההדבקה  ממשיכות בחסות מנדלבליט   DonaldJTrumpJr Him and everyone else in NYC DWHKHouSvgzitvz חתימה טובה שלומי ISudri תקשיב לזה  אולי לכבוד כיפור נזכה לראות את פניו של תומר שוויקי בן ארי וכך תכפר האמא על מעשיה yarivop אם כולם היו חושבים כמוך הוא היה מתפטר הבנת קוץ בגינה של שושנים BBWEWillWIN pL7D1FqaohiX3fh womanizer99 Riklin10 אמן גם לך randalal netanyahu המראה שלכם misscorina2 netanyahu את יודעת מה משמעות הקיר מתוך תפילה ליום הכיפורים תשמעו את הקול ואת הצלילים שהוא מפיק ובעיקר הניב הירושלמי צום קל ומועיל  netanyahu אָבִינוּ מַלְכֵּנוּ מְנַע מַגֵּפָה מִנַּחֲלָתֶךָ אָבִינוּ מַלְכֵּנוּ חַדֵּשׁ עָלֵינוּ שָׁנָה טוֹבָה  BBWEWillWIN womanizer99 Riklin10 חחחח כן  הייתי בשוק סוג של ילדותיות שלא מתאימה לו yarivop netanyahu yonikedem בתי כנסת הם הנשמה של העם היהודי netanyahu חתימה טובה לך ולמשפחתך היקרה שמע ישראל השם אלוהינו השם אחד BBWEWillWIN womanizer99 Riklin10 מסתבר שהוא חסם אותילא תייגתי אותו לא יודעת איך זה עובד אצלו 6hoidGvp7QTnmQs Bet4JsCdHAViBNM היא אישה רעה אין מה לצפות filbers attilus אטילה לא הבנת את הקונספט ביום כיפור כל אחד מתחרט על העוונות שלו לא מגיש רשימות לאחרים סולחים לך גמר חתימה טובה attilus עוד שקרן המעיד על עצמו שהוא כזה filbers attilus זה טוב אטילה לא יודע להבחין בין יום כיפור ליום חול הוא גדל ברומניה הקומוניסטית michaeldvorin רק שתבינו מה זה שמאל אנרכיסטי LeoraLev חתימה טובה צום קל ומועיל YinonMagal שלום תמורת אסד moxypen500 אמן יקירה Irisleal15 איזה פאתוס יצא לך מהמקלדת לכי להתקלח החג מגיח והסירחון רב avivgeffen השנה הקב״ה צריך לרחם ולחוס עליך החטאים של כולנו גדולים מאוד yanircozin מי זה הם ronitlev12 התקוה יום כיפור שנת 2020  segaleran MeirRubin אשכרה ישבת והכנת גרפים של ערבים חרדים וזהו PeretzMimi באירוניה יום כיפור בפתח  מבקשת אני סליחה ומחילה  אם פגעתי במישהו  צום קל ומועיל   galidalal תל אביב נגועה בקורונה חלוקה לפי אזורי מגורים זאת העיר של רון חולדאי זה שאמרו עליו מנהל עם יכולות של ספיידרמן   dogly1900 חחחחח חוסר נשיות עיתון השנאה כולל סופרים אומללים שמנסים לעשות הפיכה ומתרגמים אותה לאנגלית  haaretzcom זבלים כמוכם לא יהיה תחלמו על זה rankarmibuzaglo בני עמו של ריבלין בחרו בטרור מפיצי המחלות אתמול שומרים על הכללים כאשר המסיכה על הסנטר  dogly1900 חחחחח tadmorerez48 8000 נדבקים אומר שבעוד כמה שבועות אנו צפויים ל50 או 60 מתים מדי יום זו מלחמה על חיי אלפי ישראלים ככה פשוט במצב כזה י… N12News edho12345678 הוא שמאלני שהיה על סמים IdanOfgang RealDuduA ואיפה הרובריקה הראשונה נעלמה YossiFuchs ערב יום כיפור את חטאי אנוכי מזכיר היום טעיתי כאשר תמכתי בהקמת ממשלה עם כחל במקום ללכת לסיבוב רביעי לא האמנתי שכחל תהי… edipuskaplan rafiavizov SShpurer אמת zvisheena הרוצחים של מפגיני בלפור יותר גרועים מיגאל עמיר  הוא ירה כדור אחד אבל הם יורים מליוני כדורי וירוס הקורונה על כל עם ישראל Vitaliko למזלו של טראמפ 2 שופטים מתו במהלך כהונתו והוא יכל לעשות צעדים למען האומה האמריקאית הנורמטיבית והם ממונים לכל החיים א גרינצייג בדמו׳ הגדולה בעולם הנשיא הנבחר ממנה שופט עליון מינוי שלישי שלו על בסיס פוליטי מובהק  כדי להעמיק את…  בוקר קשה תמונת כותל ריקה  159 מתים בשבוע רק מקורונה והפקרות של מנדלבליט ניסנקורן ואנחנו בחרנו בחיים וישבנו בבית…  moxypen500 AvivBenderman AviNissenkorn אבא שלך הוא אחד מ 1000 נפטרים בגללו ביום הכיפורים האלה הוא חייב תפילה מיוחדת שתסלח על מעשיו jratosh טוב שגנץ גילה פרצופו והתיצב מאחורי אויבי המדינה המורדים נגדה ונגד הדמוקראטיה מהומות בלפור חילקו  סופית את העם בין נורמטיביפט… realadamgold הצעה לתקשורת הישראלית המופקרת על כל שלושה אייטמים ששוב מנסים לנרמל ולקדם אנרכיה כשמגפה משתוללת כאן תראיינו גם אמא – אחת… YinonMagal אמש התברר בסקר שרוב הציבור חושב שהוא עצמו אשם במשבר הערב אחרי הנאום המצויין של ראש הממשלה אמרה קרן מרציאנו שביבי וממשלתו… toomyko ההיפך הוא הנכון מי שהתעסק באובססיביות בשנאה לשרה ולנתניהו הם תקשורת עלובה ששלחה לגן הילדים עיתונאים הזויי…  UriMisgav חשיבה של קוגליק בעצמך filbers למה שקורה כעת בירושלים קוראים נאמנות  אנשים מבוגרים וצעירים עם מודעות לסכנת התחלואה שמים את טובת המדינה לפני טובתם  זוהי… cshlomit 🤣🤣🤣 amirisrael ronitlev12 Platypu12330753 תחבר את כל שכונות הצפון תגיע למספר גדול בהרבה משכונות דרומיות מצביעי הליכוד זו הטעייה מספרית  בשולי החדשות הנשיא טראמפ הציע מועמדת לשופטת בעליון   המועמדת החדשה קוני בארט הגיעה לאירוע מלווה בבעלה ובשבעת ילדי…  לחוצפה אין גבול ניסנקורן גזען  GLZRadio Sykocan חבל שהוא טועה הקורונה היא אחריות אישית לכל אחד ואחד bardugojacob אמת ויציב ניסנקורן מחבל בעשיית הממשלה bardugojacob ניסנקורן ממשיך להפגין בתוך הממשלה נגד ראש הממשלה כעת מבשר לציבור הצופה בטלויזיה שראש ממשלתו עוסק רק בהפגנות  שר לא יכול… GordieLachanc13 ronitlev12 עוד משהו אני גרה בצפון היא ומשלמת ימבה ארנונה לחודשיים GordieLachanc13 ronitlev12 העיר כרגע במקום רביעי בטבלה הכללית עוד משהו ראש העיר חולדאי משמן מערכות במליונים שה…  yuvalim123 ronitlev12 תחשוב לבד Tiranmi1 אלו נתונים של העיריה CDvir ronitlev12 ברחוב החילוני Platypu12330753 ronitlev12 המפגינים הפיצו בירושלים וחזרו להפיץ בתל אביב yohaico  galidalal אני עם ריקלין ואתם galidalal Riklin10 אוהבים אותך שמעון הלב שלך מפיץ אהבה לכולם ההצלחה שלך מטאורית MoriaTshuva השעה כמעט 12 בלילה לא מפזרים את הגועל הביתה EttiYaakov iairLevy ככה זה אנשים בלי אמונה מתחרפנים shlomokarhi מילים כדורבנות ASHER501 לדעתי הכל מהכל תל אביב נגועה בקורונה חלוקה לפי אזורי מגורים זאת העיר של רון חולדאי זה שאמרו עליו מנהל עם יכולות של ספיידרמן   netanyahu אנחנו בשעת חירום לאומי כולנו צריכים להתגייס יחד כדי לנצח את הקורונה עדכון חשוב ממני אליכם  ronitlev12 וכל הכבוד לשר זה מנהיג שאכפת לו מהקהילה שלו זה מנהיג שכואב לו על כל חולה או נפטר מעם ישראל ומהאנשים ששלחו אותו לכנסת כל… adibergman2 ronit1974 Riklin10 יחד עם זאת קלמן הלך צעד אחד רחוק מידי לומר על ריקלין עשב שוטה זו  אגרוף לבטן נתונים חדשים 1378 חולים חדשים בתל אביב תוך 7 ימים האחרונים ירושלים 4644  תשאלו איך  elikmargalit RMatsliah צודק ronit1974 adibergman2 Riklin10 בדיוק 2 הערמומים iairLevy חיות אדם כאשר נערי הגבעות זורקים אבנים ופוגעים בחפים מפשע כל הימין יוצא מגדרו בהצהרות וציוצים שמגנים זאת לא ראיתי שרחכלשע…  Riklin10 לפני מספר דקות עזבתי את קבוצת הווטסאפ של הפטריוטים לי אין את יכולת הצביעות של קלמן לצחקק איתי בפרטי ולטנף עלי בפומבי כמו כן… ארץ ציון צופיה  לא עוד adibergman2 Riklin10 קלמן ירה צרור אחד מיותר שגרם לפציעה קשה AviBenayahu judash0 פנסיונר הממריד ציבור שלם נגד חוקי המדינה תתבייש RonRonglog AviBenayahu תפסיק לצפות בערוצי התעמולה הם שונאים אותנו תראה את הציוץ של הפנסיונר מרד הם מדרבנים…  kannnews VeredPelman שקרנים adibergman2 Riklin10 מפני שקלמן הגזים smadarshmueli היו שמים אותנו במחנות מעצר XcaqzxAURqRA3Zc רפואה שלימה היום השמאל קבר את עצמו הציבור לא יסלח להם על הפגנות בתחילת סגר כאשר יום כיפור החשוב ביותר בחגי ישראל כמעט ולא יתקי…  Sigalbz egozim1 MotTal BarakRavid זבל מושתן BoazGolan השמאל האנרכיסטי שהפגין היום הוא הגיבנת של העם היהודי לדורותיו Esi52804020 זוכר בגל הראשון נתניהו אמר אם לא נשמור נגיע ל 10000 נדבקים ליום ועשרות מתים אם לא נשמור לא שמרו והוא…  Sigalbz נדבקו מההורים שהיו בהפגנות YinonMagal טוב הגיעה התוצאה יש לי קורונה🤦‍ המזל הוא שהחום כבר ירד כמעט לגמרי ואני מרגיש טוב בהרבה ומקווה שזה מאחורי הבאסה היא שא… Vitaliko YinonMagal בדיוק אולי נדבק באולפן חוסר מזל YinonMagal באסה באסה באסה החלמה מהירה תשמור על עצמך והשם איתך arutz20 זעם רב בציבור החרדי בעקבות דבריו של שר המשפטים שיצא להגנת המפגינים בבלפור – והאשים את החדרים והערבים gtgt  יוסי יהושוע בעקבות העלייה בהיקף התחלואה בצבא   1200 מאובחנים כחולי קורונה מתכוונים בצה״ל להגביל את היציאות החל מ…  מספר התגובות גדול ממספר המקבלים את ההתנצלות האיוולית שלך תתבייש גזען  avigrin10 AviNissenkorn בדיוק למען האמת החילוניים הדביקו את החרדים avigrin10 AviNissenkorn אדוני השר הציבור החרדי סיים להיות שטיח של פוליטיקאים כושלים תתנצל בפומבי באותה במה שהשמצת תבהיר שהקורונה… dwwido AviNissenkorn ממש קללה עונש לעם ישראל AviNissenkorn לא מעוותים אותך מניפולטור אמרת זאת במילים שלך חרדים וערבים פלטת את מה שאתה חושב לא נסלח גזען reuvenharel FogelEran shlomokarhi האיש ד״ר ומי אתה Sigalbz noamfathi מעניין מה הוא סוחב בשק החיים שלו mmotish avyklbo האיש אנטישמי RomanoHoring mazkirhakibutz Riklin10 מעתיקים משם לפה RubiYona השם ישמור אותנו אמן 8221 מאומתים חדשים אתמול 259 61101 תוצאות בדיקות שהתקבלו אתמול 259  היום 269 נכון לשעה זו 226586 מאומ…  michaeldvorin נראה שרק הקרחת בסדר nilitn1 Paris9316 AviBenayahu מהטוויטר זה נראה מפלצתי במציאות זה חלש מאוד אל תדאגי הם אספסוף וישארו כך לעולם barak56976102 FacuI29147752 BarashiKinneret אמן YanivTurgi dovikco חחחח בלי חשבון ניסנקורן גזען נגד החרדים והערבים גזען הביתה YinonMagal רק בריאות ינון ישועות השם כהרף עין arutz20 חלאה R431j האם ההורים של ההסתה והפילוג שונאי אדם חלאות מטונפים noamfathi בגלל זב נעלי התעמלות האדומות שלו חבר של פדו ILpolice צפוי שתעצרו רק ימני כי שמאלנים פריבילגים limorh6 🤣🤣🤣🤣🤣 הלל ביטון רוזן שר המשפטים ניסנקורן משקר בשידור חי ״הקורונה התחילה במגזר החרדי והערבי ועכשיו היא בעיה של כולם״ הק…  BoazGolan הבטחת תקיים  rankarmibuzaglo R431j ממש כואב לראותך מתייסר אל תרפה ותתבע את המטורלל הד״ר לפיסיקה שהיכה אותך רק זה יפגע בנשמתו החולה AviBenayahu אם זה נקרא מרד אז מצבנו מצויין חחח תקרא מלחמות היהודים של יוספוס תלמד מה זה מרד אתם אספסוף של 4000 איש כולל ילדים gal100sh Riklin10 כאשר ירדו לו אלפים הדכדוך יעמיק barak56976102 BarashiKinneret הוא ראש הממשלה ההפגנות הם נגד הימין לא נגדו זה הבלוף של השמאל שמאל שקרנים מאז ומעולם אני עם ריקלין ואתם  joseph45709596 boristhenice anatnh תורת גבלס אני לא צופה שנים צופה כאן בטוויטר וזה מספיק לי לא מכניסה למוח שלי הנדסת תודעה IlanTsion חנפנית dogly1900 🤮🤮🤮🤮🤮🤮🤮🤮🤮 SagiOrli עקבתי כדי לדעת ואז הבנתי שהוא בניסט להחרים את התכנית עם רינה מסריח אין לימנים מה לעשות לדבר ולהסביר הם מביאים אתכם לעשות להם אקשן לתכנית כלומר להרים את…  Riklin10 אוהבים אותך שמעון הלב שלך מפיץ אהבה לכולם ההצלחה שלך מטאורית YotYotam פתחי יצא תותח על bardugojacob ומה דעתך על האמירות של קלמן כלפיך היש יותר מביש מזה</t>
   </si>
   <si>
     <t xml:space="preserve">במחשבה שנייה הגרסה המלאה של מה שחוויתי ביום כיפור 73׳  ביום הכיפורים ההוא לפני 47 שנים חזיתי בסוד כוחו של עם ישראל אירוע שלא אשכח לעולם  שתפו הפיצו גמר חתימה טובה ל…  ישראל לא תצא מהמשבר עד שנתניהו יועבר מתפקידו אנחנו במלחמה עם הקורונה ועם האסון הכלכלי שהיא ממיטה על מיליונים ובמל…  נתניהו לא נלחם בקורונה כדי להבריא את ישראל הוא נלחם במפגינים כדי להימלט ממשפט לכן חייבים להמשיך להפגין  גמר חתימ…  נתניהו נחשף חדשים שמענו שההפגנות ׳לא מענינות ולא מטרידות׳ אותו כעת מסתבר שזה הדבר היחידי שמעסיק  אותו הנאשם הולך…  ׳תעשיית הכזבים׳ של ביבי נתפסה ׳על חם׳ כשדובר המשפחה עופר גולן והעבד ׳טופז לוק׳ יורטו מפברקים ׳הכחשת קורונה׳ בהפגנה…   הסגר הזה ייכשל לא בגלל האזרחים באשמת הנהגה תועה שהאזרחים איבדו בה אמון ויש גם פתרון אמיתי דברים שאפשר לעשות עו…  לנשיאת בית המשפט העליון אסתר חיות עוד יהיה זמן להרהר באמירתה שום מבצר אינו נופל המבצרים נופלים כאשר אלה שאמורי…  ׳צו 8׳ מאמיר השכל האיש שהחל בהפגנת יחיד זכרו הכשלון בקורונה הוא הדחוף ביותר האסון הכלכלי שזרק מיליונים לרחוב…  באופל השנה הזאת הבליחו ניצוצות של תקווה בזכותם השנה הבאה יכולה להיות טובה יותר צפו שתפו והפיצו חג שמח לכולם   הישג בוושינגטון לצד מחדל הקורונה והאסון הכלכלי   על כך ועל עוד נושאים  אחרים  הערב ב1800 בפאנל דיגיטלי עם אטיל…  ישראל מתנהלת כמדינה בהתפרקות החלטות מתהפכות פעמיים ביום אין ניהול משבר אין אסטרטגיית יציאה אין תקציב אין ישיבו…  גנץ ואשכנזי בשיא חדש של פשיטת רגל מוסרית אין גבול לזחילה הצביעו כנגד חוק  שנאשם בפלילים ושוחד לא יוכל  להיות נשיא…  הספינים כופפו את שרי הליכוד שלא פוצים פה הספינים כופפו את גנץ שנמס מול איומי סרק הספינים כופפו את מנדלבליט שלא ח…  מחיר העסקה מוטח בפנינו גם העובדה שבראשנו עומד נוכל והשאלה הנותרת האם לא היה ראוי לדון בכך טרם מעשה עם שר הבטחו…  מנדלבליט שוב נגלה בחולשתו הנבצרות של נתניהו נדרשת לא רק בגלל המשפט שמעסיק אותו אלא בגלל סירובו לחתום על הסדר ניגו…  יש באמת איומים על נתניהו ומשפחתו הנה ההסבר שלי  שאול מרידור ׳סיביל סרוונט׳ למופת מתעקש לשרת את הציבור ולא מתבלבל ולא נרתע מהשררה עדותו  מרתיחה גם אם לא מפתיעה…  אלימות משטרתית בוטה הלילה בבלפור בשליחות הנאשם רדוף החרדות ובהנחיית השר לבטחון בלפור והקרנפים בפיקוד העליון שוטר…  טירוף וסירחון בבלפור נאשם רדוף מכופף את  המשטרה  לפינוי פוליטי ואלים של מחאה חוקית הריקבון מתחיל ונגמר בצמרת א…  אפשר לברך על ההסכם מעליו עננה של חשש שאצל נתניהו אתה לא יודע באמת הכל אבל המחאה חייבת להימשך עד הנצחון   התרסקות מבהילה אדם אחד נכשל בניהול משבר הקורונה  נתניהו כי לנתניהו אכפת רק מהמשפט הוא הפקיר מיליוני ישראלים לסכ…  ההסכם עם  ה UAE צעד בכיוון הנכון נקווה שיתקיים ויצלח כן ירבו   אולם המחאה חייבת להימשך כי ראהמ מושחת שעסוק בה…  נתניהו בזמן שאתה מתפתל כדי להימלט מהמשפט שכחת את כשלונך המביש במאבק בקורונה מליון איש מתפרקים נטושים ברחובות …  אכן היו לאחרונה התבטאויות מיניות דוחות כלפי בני משפחת נתניהו כשם שהיו אינסוף התבטאויות מיניות דוחות של שלוחי נתניה…  לגנץ נותר רק מוצא אחד של כבוד נתניהו והליכוד מצביעים רק בטרומית בעד דחיית התקציב אז גנץ וכחל״ב מצביעים רק בטר…  שוב ׳תיראו מופתעים׳ נתניהו אוחנה אמנון יוסף ו׳דנה רון׳ ממשיכים לתעתע בציבור ולהכפיש מבקרים כשלונו המהדהד של נת…  שתי מילים בואו לבלפור  שתפו והפיצו  נתניהו בפאניקה ופולט ציוצים היסטריים לא מפתיע הוא מבין שהמשחק הולך להיגמר בתמונה אני עם נעה רוטמן נכדתו של יצחק…  תקציב ל3 חודשים יש הגיון  הנאשם רוצה בחירות כדי לחמוק מהמשפט כדי לנצח בבחירות הוא חייב לשחד את הציבור במיליארדי…  אני לא מכיר את הילד אבל מכיר את האבא יותר מ50 שנה הוא לא צוחק מהחייזרים הוא חרד ומזיע לא איש חזק אלא ׳איש חלש…  עמית סגל ׳נתניהו משוכנע שינסו לרצוח אותו ואת משפחתו׳ זה נכון שהוא פניקער אבל עד כדי כך  שתי אפשרויות או שהאיש…  טובי צעירי ישראל מפגינים נגדך ביבי כי מרגישים שאתה פוגע להם ׳בחיים עצמם׳ בכל מה שחשוב להם מטיל צל כבד על ישראל…  אלימות בנוכחות המשטרה אמש בת״א המשטרה בגיבוי היועמש חייבת לעצור מייד את המתפרעים ולהביאם לדין אין שום בעיה בזיהו…  מפגין שהותקף בת״א לפני שעה ע״י בריוני הימין הדם הוא על הידיים של המסית הגדול ולא בפעם הראשונה בפרוס תשעה באב לפנ…  פרופ׳ רוני גמזו  מינוי מעולה מוכשר מקצוען חף ממניפולציות  נתניהו כבר עוטה קלון טרמפיסט כושל מהמערכה הקודמת ב…  קראו כל מילה של הסופרת ליאת רוטנר לא אשת שמאל ולא אנרכיסטית אלא פטריוטית שמבינה שטובת ישראל חשובה מטובתו האישית ש…  הנאשם יורד מהפסים מאבד את בוחן המציאות הלחץ נותן אותותיו תנועת ׳קומי ישראל׳ ובעיקר צעיריה קמים בנחישות מרגשת…  על ההבדל בין פייק ניוז לאמת  תודה אור   פאניקער אמר שרון הוא יודע שמצוקת מיליוני הישראלים היא כשלונו האישי הפגנות הסופ״ש מבהירות לו שהחומות מתחילות להיס…  ביבי אתה מזיע רואים את הזיעה למרחקים כישלון מוחלט בטיפול בקורונה כישלון מוחלט בכלכלה עשרות אלפי מפגינים מלח ה…  ביבי מר כלכלה עוד פייק ניוז שמנפצים כספית ובייגה   נתניהו הוזה מבוהל ומבולבל פונה להסתה ופייק ניוז אלה לא הפלסטינים זה עם ישראל שיוצא לרחובות כי אין לחם אין כסף…  נתניהו בפאניקה ומנסה לשחד את כלל הציבור  6 מיליארד צריך לתת למי שבאמת שצריך 2 מיליון שעובדים בשירות הציבורי או בו…  עו״ד גונן בן יצחק איש השב״כ לשעבר במעצר שווא בעקבות הפגנה חשובה ומוצלחת בבלפור שקראה לנתניהו להתפטר  אין סיבה כ…  זעקתו המצמררת הזאת של אב שכול וזעקתם קורעת הלב של אזרחים נאמנים שמאבדים את מטה לחמם וכבודם  אל מול הניתוק המבאס של…  דברים כדרבנות כתבה רינה ענתי אינני מכיר אותה אבל ניכרים דברי אמת קריאה חובה  אכן מטלטל  צו 8 לכל אזרח החיים שלכם מתרסקים יום אחרי יום בגלל כשלונותיו והוא עסוק בעצמו ובפרזיטים מסביבו הדהיר…  אל תהיו מופתעים אם בחסות הקורונה ינסה הנאשם להשתמש בחוק הטרי כדי לדחות את המשך המשפט ככה נראית דיקטטורה זוחלת  הכשל הניהולי בעיצומו מדינות שהיו במצב חמור בהרבה התישרו ללא איכוני שבכ מופעי האדרה עצמית וחוקי חרום ללא ממשלת ק…  כל מילה שתפו והפיצו  נמחקו תיקיות במחשבי הפרקליטות ובמקרה הן מכילות פרטים חסויים על חקירות ותיקי נתניהו אם זה נכון  זה נורא  מאפיה…  האיש נוהג כמי שירד מהפסים לגמרי מסוכן למדינה ולעצמו חייב להכריז נבצרות או שהמדינה תמצא דרך לכפות זאת רק לפני 3 ח…  גיא זהר ומערכת מהצד השני מזימים את עלילת הפייק ניוז של שופרות נתניהו בישראל היום כן ירבו עיתונאים הגונים וישרי…  הכנסת משותקת בשת״פ משחית של נתניהו וכח״ל נמנעת חקירת מבקר המדינה את פרשת הצוללות וכלי השייט שהיא השחיתות הגדולה בת…  נתניהו בוזז מהקופה מיליון שקל בזמן שלמיליון מובטלים אין שקל  במילה אחת  זה מה שאמרתי לאופירה וברקוביץ׳ צפו שת…  בתמונה עציר פוליטי מהמפגינים אתמול אזוק בידיו וברגליו לא אמיר השכל לא ייאמן ׳עציר פוליטי׳ בישראל תא״ל מיל בחיל האוויר אמיר השכל אזוק בידיו וברגליו משטרת אוחנה נתניהו מועלת בתפק…  ׳מפי עוללים ויונקים ייסדת עוזלהשבית אויב ומתנקם׳ תהילים מ״ג האזנת חובה למבוגרים שאכפת להם…  ״זהו צו קריאה צו 8 לכל מי שעתיד המדינה הזאת יקר לו קומו עלו לבלפור והצטרפו אלינו״ נאומו האחרון של תאל מיל אמי…  חרפה טייס ומפקד תא״ל מיל אמיר השכל קורס 72 בחקירה לילית סמוך לחצות מפגין יחיד באומץ וקורא להתפטרות ראהמ שנאשם…  24 שעות אחרי טקס הסיום של קורס טייס נעצר תא״ל מיל בחיל האוויר אמיר השכל בוגר קורס 72 כשהוא מפגין נגד השחיתות ו…  הלך מאיתנו יהודה וקסמן הצטרף אל נחשון הי״ד בנו באתי אליו ואל האם אסתר למחרת אותו הלילה כמי שהיה אחראי לפעולה שבה…  האומץ והפטריוטיות של אמנון אברמוביץ  אינם דורשים הוכחה הם כבר הוכחו בשדה הקרב ואינספור פעמים מול המצלמה החרפה על…  החזירות קורנת מבלפור בעוד מיליוני אזרחים זועקים אני לא יכול לנשום השתגענו לגמרי נתניהו לא ישלם מיסים ואתם כן…  הלך מאיתנו פרופ׳ זאב שטרנהל חוקר מעמיק וזקוף קומה ופטריוט ישראלי אמיתי היכרתי אותו לפני כמעט 40 שנה במדי קצין מי…  רינה מצליח ניצבת אמיצה מגדלור של אמת והתרסה מול גל של התקרנפות בתקשורת  נתניהו ש׳שלח את דרוקר לכלא׳ עושה על מצליח…  מה שגנץ כתב היה ונותר נכון מסע״ת של שרגא אליעד היום היא צעד חשוב לאור היעלמות הלחץ הפוליטי לחקור פרשת הצוללות חיי…  גם אז בלבנון וגם היום בקנאביס המרוויח הגדול יהיה עם ישראל   קרבות שמסתבכים יוצרים מחלוקות כואבות שנמשכות שנים הגיבורים האמיתיים הם הלוחמים שלחמו באומץ בתנאים שלא הם יצרו אות…  ההסתה נגד השופטת העליונה ענת ברון מקורה בשלישיה המהוללת מבלפור זו רק ההתחלה ההמשך יהיה חמור בהרבה אם היועמ״ש לא י…  כעת ברשתות דוגמא אישית ירדן שוורצמן אזרח חושב מהנדס קצין  מיל בסיירת מטכל בן צעיר למשפחה לוחמת ׳כשנאשם בש…  נאשם בפלילים כממונה בלעדי על קיום חוקי חירום איפה ה׳חליפי׳ ואיפה השכל הישר מה כל כך חירום שאיננו מאפשר דיון בפורו…  בדיוק לפני 53 שנה 6 ביוני 67’ בבוקר אני מתדרך כח של סיירת מטכל למשימתו  צו 8 המחטף לחיסול הדמוקרטיה נמשך הנאשם בשוחד יהיה מוסמך להחליט על צעדי חירום והוא יקבע מה שם פלילי השתגענו הקו…  חוק הסמכויות  הזוי ולא יעבור מי שינסה להכניס שוטרים ללא צו אל בתי אזרחים יגמור עם מרי אזרחי מי שינסה למנוע הפגנ…  יסלחו לי שופטי העליון אך את הקביעה כי ׳הצבת נאשם בשוחד בראש המדינה זהו כשל מוסרי חמור׳ גם אם איננו נושא משפטי  ה…  תעלול פתטי של הנאשם׳אין כלום כי לא היה כלום׳  הפך לנסיון בוטה להפחיד את בית המשפט התנהגות מפיוזית אסור שזה יעבו…  לפני בדיוק 20 שנה הערב החלה יציאת צהל מלבנון ועד הבוקר  הושלמה ללא הרוג או פצוע אחד כך נסתיימה טרגדיה של 18 שנ…  מינוי ראשון מצויין של גנץ במשרד הבטחון  אלוף מיל אמיר אשל איש רציני שהגביה עוף ונותר עם ראש על הכתפיים ורגליים…  אנחנו לא פראיירים זו לא ממשלת חרום לא ממשלת קורונה לא אחדות לאומית ולא פיוס זו ממשלת ביזיון 52 שרים וסגנים ובז…  ׳ממשלת החרום׳ להתמודדות עם משבר הקורונה תושבע מחר יהיו בה יותר שרים 36 ממספר הנדבקים החדשים במחלה אתמול 23 תו…  חכ אלי אבידר בנאום הכי ממוקד של השנה האזנת חובה עד המשפטים האחרונים avidareli   איילה חסון היא קול אמיץ ועקבי בענין מנדלבליט ואשכנזי לאורך שנים גם כשתקפו אותה שוב ושוב כל פעם מכיוון אחר בענין ה…  אילה חסון חושפת ׳מנדלבליט שיבש חקירת אשכנזי׳  בעיני נתניהו זה מצא חן הוא מונה ליועמ״ש ומאז שיבש כעשר חקירות של נ…  20 שנה אחרי חזרתי לרגעים בהם יצאנו מלבנון סדרת ראיונות נרחבים עם הד״ר אורי מילשטיין על האומץ לקבל החלטות קשות ו…  אומץ ועצמה זה מה שמביאים איתם ותיקי הלוחמים שכבלו עצמם אל שערי בלפור בסיסמה ׳אין מצב׳ שנותן ונוטל שוחד יקים לנו מ…  החלטה מאכזבת של הבגצ על בסיס הבטחה בעייתית של היועמ״ש ׳לנתניהו יהיה הסדר ניגוד ענינים׳ איך הוא לא יכול לגעת במשר…  דיון מרשים ומעורר כבוד בעליון טוב ששודר חדות שליטה בפרטים תבונה עמוקה נקיון דעת ויד בוטחת על הגה הדיון הכבוד…  שחר של גורל אלו ימים שייחרתו על לוח לדיראון עולם או ל׳לידה מחדש׳ של ישראל דורות המחר לא יבינו איך הוכה בסנוורים ח…  וואו אילה חסון שוב מוכיחה שכשהיא רוצה אין עליה כל מילה בין העיניים  AyalaHasson  הנאשם בשוחד מאיים על הבגצ סחיטה באיומים מאפיה כבר אמרנו הדילמה בפני בגצ אכן מתחדדת אם יפגעו רק בהסכם הקואליציונ…  מנדלבליט מגלה שוב חולשת דעת ורצון 2 הערות על ׳הרוב של 78 חכים׳ שרוצה לדבריו לראות את נתניהו ראש ממשלה 1 19 מהם נ…  כתב לי חבר רוני כהן חמר למחשבה במוצאי יום העצמאות לכל ישראלי שהמדינה יקרה לו אינני יודע מה יקבע הבגצ אם לא יכר…  אני חושב היום על החייל האחרון שנפל בכל אחת ממערכות ישראל כאשר הנצחון או חוסר התוחלת כבר היה ידוע עם חפץ חיים חי…  על קורונה ומנהיגות מרקל מול נתניהו אינני יודע מי כתב אך מדויק להפליא  קריאת חובה שבת שלום…  מאפיה כבר אמרנו ׳המרצע יוצא מהשק׳ ההנחיה מבלפור הפעם היעד הוא מנדלבליט חייבים להיפטר ממנו לפני הכרעת הבגצ ולפנ…  בני גנץ תתעורר הקורונה מחלה קשה אבל השיא שלה ממש ממש מאחורינו  אני מאמין לך שאתה חושב שאתה פועל לטובת האזרחים א…  הסכם פוליטי רקוב הסרחון והחשד לסחיטה עולים לשמיים הנאשם ימנה את היועמש ופרקליט המדינה ויבלום כך את משפטו ואת החקי…  רגע הכניעה של גנץשכנזי בערב יום הזכרון לשואה ולגבורה אירוניה היסטורית קריסה אישית פוליטית ומוסרית של גנץ בפני סח…  חדשות טובות לשבת המספרים מדברים שיא המגיפה במובהק מאחורינו עכשיו לעצור מהר את המפולת הכלכליתחברתית ואנושית  נ…  גנץשכנזי עורו הרי לא תתנו לו למנות את חוקריו ושופטיו ולדרוס את בגצ גם לשכנע את חבריכם ל61 שאינכם משתמשים בהם כד…  גנצשכנזי  אין רע מאשליה עצמית כולם כבר רואים שהמלך עירום מישהו מאמין שזה קורונה זו ממשלת חירום לא וגם לא היתה…  חג באמת שמח שיא המגיפה ממש מאחורינו מספר החולים הקשים המצטבר מאז תחילת המגפה עלה ביממה האחרונה ב8  מספר המונשמי…  גם זכות ההפגנה נרמסת 200 איש הבוקר בהפגנה בכפר סבא המשטרה מטילה קנסות מ 5005000 ש״ח את מי אתם מפחידים עומדים ש…  שיא המחלה באופן מובהק מאחורינו הדרך פתוחה להסרה הדרגתית של הסגר קבוצות בסיכון יישארו בבידוד בגיבוי של המדינה תי…  ׳ראשונים בעולם׳ עוד כזב מה׳מושיע׳ שהפחיד אותנו עם מיליון חולים ועשרת אלפים מתים עובדים עלינו בעיניים עצוב…  אפשר לחייך הבוקר שיא המגיפה מאחורינו פוסט מס 8 החזרה ל׳נורמליות חדשה׳ דורשת מנהיגות אחרת  אם המגמה תימשך עד יום…  3 הערות  א טרגדיה בבתי האבות  מחדל חודש של התעלמות מהקשישים ואחריו שבועיים של הוראות נכונות שאיש לא מוודא את ב…  עדכון מחזית הקורונה  פוסט מס 7 על קורונה ומנהיגות  אמלק השיפור נמשך אם לא נעשה שטויות אפשר יהיה אחרי החג לה…  בחזית הקורונה  שיפור מוחשי וחשוב פוסט מספר 6 לראשונה מאז פרצה המגיפה מספר הנדבקים והחולים הקשים החדשים קטן מיום…  Good News Bad News מחזית הקורונה פוסט מס 5 Bad נדרש מבצע חירום בסופש להטסת ריאגנטים והעמקת הפעולה בבני ברק וב…  ביבי תתעורר כוכבי תתכונן בבני ברק זו טרגדיה לפי 35 יש שם 70 אלף שנדבקו גם לפי 1 של מתים זה 700 מתים והחרמש עו…  מצב חזית הקורונה 142020 פוסט רביעי בסדרה  אמלק  עת לפעול לבלום את הנסיגה בציבור החרדי למגן את צוותי הרפואה…  מצב הקורונה כיוון טוב מאוד אבל עדיין מסובך  פוסט שלישי בסדרה מוזמנים לקרוא ולשתף   אופטימיות זהירה מצבנו היום בחזית הקורונה   די להפקרת החיים של האנשים שאנו חייבים להם את לידתנו ואת הקמת המדינה בתי האבות בסכנה חייבים לבדוק ב72 השעות הקרוב…  כדאי לשים לב לא רק הגידול במספר החולים הקשים משתטחלאט גם במספר הנדבקיםכשהיה צריך דוקא לגדול עם עלית היקף הבדיק…  רס״ן מיל טל טייס קרב מלח הארץ כתיבת מופת ביטוי מושלם למה שחש היום הרוב שהלך אחרי גנץ עם גוש ה 61 כל מילה…  יום אחד כתום ימי המבחן האלה נביט אחורה ונתהה איפה היתה התקשורת הישראלית איך זה שבערוץ מוביל הוקדש יותר זמן לתוכי…  ׳להצביע היום׳ היא אמירה אמיצה של יועמ״ש הכנסת אייל ינון הכדור עובר אל ׳העליון׳ שמפגין שוב ושוב אומץ וחיות ׳בית ה…  בעיצומה של הפיכה שלטונית שמוביל אדלשטיין נשואות עיני כולנו אל ׳העליון׳ המגן האחרון של הדמוקרטיה רגע לפני הכאוס המו…  ההפיכה השלטונית נמשכת אסור לאבד אף דקה חיוני לפנות מייד לבגצ ולדרוש כינוס המליאה היום בראשות אחד הסגנים ׳צו עשה…  חיוני לבלום את ההפיכה השלטונית של ביבי היו״ר המתפטר איננו חדל מלהיות יו״ר ל 48 ש׳ ולהפר ׳צו עשה׳ של העליון אדלשט…  יש שופטים בירושלים סוף סוף צו עשה  מצדיע לבית המשפט המגן האחרון של עיקרון הדמוקרטיה הכול כעת על כתפי גנץ וכחול…  החכים של בלוק הימין מנסים להמשיך את ההפיכה השלטונית חרף קביעת הבגצ טירוף מערכות אנחנו האזרחים לא ניתן לזה לקרות…  הנאשם שלנו מאחז העיניים הגדול מנווט את הטיטניק זוכרים מה היה הסוף נכון  למה אסור לגנץ האיש שניצח בבחירות שהמנדט בידיו לחתום על הסכם כניעה בפני הנאשם בפלילים צפו שתפו והפיצו  מרי הדגלהשחור יצא לדרך הכנסת נמחקה בית המשפט ננעל מפגינים נעצרים  יש רגעים בחיי עם בהם אזרחים מתווים בפעולה…  ותודה לנועה ולכל מי שלא התקרנף בתקשורת  ורואה עם כולנו שהקרבן הראשון של הקורונה בישראל הוא הדמוקרטיה אנחנו לא פרא…  כן דגלשחור  כשיהיו מיליון כאלה על כל חלון ומרפסת  הנאשם ילך הביתה לא ייסגר בית המשפט ולא תיסגר הכנסת אנחנו…  שקמה בסרטון וירדן כותב הטקסט שוורצמן אחות ואח משפחה לוחמת פטריוטים ישראלים צפיית וקריאת חובה עת לפעול …  כל מילה עיתונות אמיצה בימי קורונה  המאמר הטוב ביותר על הקורונה קריאת חובה  אמלק 1 ניתן להתמודד צעדים מיידיים כמו טייואן לא איטליה 2 כעת נדרש…  10 יידחו כל תשלומי מס לשלטונות ל 1 במאי 2020 11 יינתן מענק לעסקים בתחום המלונאות תיירות וענף ההסעדה 12 יחולק…  5 יוכשרו לאלתר תלמידי ישיבות לעבודה ככוח עזר רפואי 6 יוקצו חללים בישיבות ובמוסדות להשכלה גבוהה לחולים בבידוד 7…  חבר שהוא יועץ כלכליאסטרטגי העביר אלי עיקרי תכנית פעולה לטיפול במשבר הקורונה משתף אתכם  1 יקוצצו לאלתר כל הפנסיו…  6258 נגד נתניהו ולטובת המתנגדים להיתכנות של ׳נאשם בשוחד מקים ממשלה׳ זה הזמן לחשבון נפש גם בתקשורת כמעט כווולם נ…  אחוזי ההצבעה גבוהים מאבק צמוד בין גנץ לנתניהו  הקרב על עתיד ישראל יוכרע בקולות בודדים  צאו להצביע אם כבר יצאת…  נתניהו נחשף הערב שוב בשפל עליבותו לא איראן ולא ׳תכנית המאה׳ אלא פוליטיקת ביבים הוא עוסק אישית בהשמעת הקלטת סתר ש…  מזעזע צפיית חובה  פרופ׳ עוזי ארד מי שהיה ראש המל״ל של נתניהו ובכיר במוסד על ׳שבעת פשעי נתניהו בבטחון הלאומי׳…  קריאת חובה עוד היום עד השורה האחרונה  זעקת ׳עורו׳ מיוסי לוי איש מוכשר שהיה מעוזריו הקרובים של נתניהו גם הוא ו…  נתן אשל בגילוי מלא הקלטה מרתקת כל מילה חשוב לכל מי שמתכוון להצביע לנתניהו האיש שבז לבוחריו מתעב אותם ומשתמש בה…  קריאת חרום לבוחרים בשום מקום בעולם נאשם בשוחד לא יכול לפטר את היועמ״ש שהחליט על העמדתו לדין אחרי שכבר מינה שר משפ…  הסרטון המלא  מצמרר ששה ראשי מוסד ושבכ קובעים כל אחד במילותיו שנתניהו מסוכן לביטחונה ועתידה של המדינה זה היה אמור לזעזע מוסדי…  אני מכיר היטב לאורך עשרות שנים את שני המועמדים מול אויב בחפ״קים ובדיונים לקראת מבצעים כולל בהקשר האיראני יש לג…  ואם ביבי ינצח ב23 זה מה שיקרה    זה בידיים שלנו צאו להצביע  שתפו והפיצו מייד ובכל הכוח עם חברים בנ…  פרשת הצוללות גם אבריאל ושי ברוש יועמדו לדין כך גם מנור ושימרון אבל איפה הקברניט של השחיתות הזאת שעל סף בגידה הפ…  זה לא חוקי מגניהו אנגלמן מנסה להעניק לנתניהו היתר לממן את משפט השוחד שלו בכספי אנשים כמו פרטרידג׳ שהיו חשודים בשי…  נתניהו שיורד על הברכיים בפני החמאס יורד על הברכיים גם בפני הרב ליאור למי שלא יודע הרב ליאור היה מקור ההשראה לרוצח…  אבחנה מכוננת מדויקת של אחד מהבולטים בראשי אמ״ן בעבר אלוף מיל עמוס מלכא  ואני אומר באחריות מלאה משהו לא טוב מעוות קורה שם בין הקירות של ׳קן הקוקיה׳ בבלפור ואסור להמר על זה זה הגורל של…  על מי אתה מתגולל כגולם שמבוהל מדמותו המבועתת הנשקפת אליו במראה הרי מפיך שמענו ש׳ראש ממשלה שעסוק במשפטו איננו יכול…  איננו יכולים להמר על עתידנו רואים את זה בכל ראיון והופעה מאחז עיניים על סטרואידים אשף הבירבור החלול קומפרסור של…  ברור שמשהו לא טוב קורה אצל ביבי נתניהו זה מעבר לחילוקי דעות משהו קורה אולי זה המשפט שייפתח בעוד שבועיים סיוט בג…  חוסני מוברק איננו מנהיג של יציבות ואחריות לעמו הובלה ומנהיגות בעולם הערבי ודבקות בהסכמי השלום עם ישראל אדם מיוחד…  אם הנאשם נתניהו ייבחר לראש הממשלה בעוד שבוע הוא יאיים על היועמש יעביר פסקת התגברות מורחבת ויחוקק חוק צרפתי שיאפש…  קריאתם של 540 אנשי צוות אוויר מיל תומכי כל המפלגות לא לאפשר לנאשם בשוחד להקים ממשלה חייבת לטלטל כל אזרח ולהול…  חברים להתעורר  לא ׳ידיד השם׳ ולא בטיח עבריין נואש בדרך אל המעמד של ׳מדינת ישראל נגד בנימין בן בנציון נתניהו׳ ׳ה…  על מה הוא מדבר מאחז העיניים הזה עבריין שמשפטו יחל בעוד 3 שבועות מנסה לבצע רצח אופי לאדם ישר בגין ארועים שאין בהם…  ׳פרשת׳ המימד החמישי היא קשקוש מקושקש שתיגמר בנזיפה משמעתית לשוטר אין לה שום קשר אל בני גנץ בקיצור  עוד ספין והס…  לרבים שפנו אליי ושאלו מדוע צייצתי אתמול על פרשת הרפז הנשכחת להלן התשובה אמש במקום לתקוף את נתניהו בחר גבי אשכנז…  ב האדם שאחראי להשמדת הקלטות בלשכת השר הוא בכיר במשהבט מקורב לאשכנזי שפעל מטעמו ובידיעתו לאנשי לשכת השר לא היתה…  האמת אשכנזי שיקר אז שוב ושוב לחוקרי משטרה לחברי המטכל ולציבור והוא משקר גם הערב   אהצא״פ כולל כ 15 שיחות שנוגע…  לא אתן לשקרים להרוס את הסיכוי להחליף את השלטון לא לשקרים של נתניהו ולא לשקרים של גבי אשכנזי נאשם בשוחד מרמה והפרת אמונים לא יכול להקים ממשלה בישראל נקודה  שתפו והפיצו  פשע שנאה מעורר גועל בגוש חלב האחריות המיידית היא של מבצעי הפשע אבל מקור ההשראה שלהם יושב בבלפור ומסית בלי חשבון…  נתניהו בפאניקה וההפקרות שוקעת לשפל חדש ראש ממשלה ש׳רומז׳ הערב בכנס בחירות על מעורבות אפשרית של ישראל בכשלון שיגור…  נתניהו ממשיך ב׳קרקס המעופף׳ קודם מוסקבה והיום אוגנדה ׳הפקות׳ של האדרה עצמית עם פמליה שמגחיכה את הארוע וניחוח של ה…  קצ׳ה שמעון כהנר  איננו יחיד ומיוחד בין המעטים לצד חבר הילדות מאיר הר ציון שבעוז רוחם ובצלקות שעל גופם עיצבו א…  נתניהו פועל להכשלת התכנית בסיפוח מבוהל גנץ פועל למיצוי הסיכוי לאחר הבחירות בתאום עם טראמפ והכוחות המתונים באזור  הופעה מצוינת של גנץ  אהשג דיפלומטי מול טראמפ שמבין כנראה שסופו של נתניהו קרוב  בעמדה מהותית בהירה בטחון קודם ל…  ארועים מרגשים בבית הנשיא ו׳יד ושם׳ חבל שלא נמצא מקום בולט יותר לניצולים עצמם לצערנו איש מהם לא יהיה עימנו כאשר נ…  נתניהו נגרר אחרי סמוטריץ׳ להפקרות בטחונית כולנו מסכימים שהירדן הוא הגבול הבטחוני של ישראל אבל האויב העיקרי הוא אי…  חשיפה מפי אנשינו של פרטים ממבצעי מודיעין חיסול מבחוח הערב ב12 חן יונס לפני חודש  הם מתנת חינם לאויב וסופה שתעלה…  החלטה חשובה אחראית ובוגרת של סתיו שפיר אסור לאבד אף קול טובת המחנה והמדינה לפני כל שיקול אישי משוכנע שעוד נראה א…  קריאת חובה בני בגין בקריאת אזהרה מדויקת ובוטה על נתניהו והשחתת ישראל  השג וטעם מר בצידו  ברכות לעמיר פרץ וניצן הורוביץ על החלטה נכונה שילוב הידיים הוא חיוני  ׳בלי איחוד הקול אבוד׳…  מה שמבזה את הכנסת ואת כולנו היא בריחת הנאשם בשוחד מאימת הדין ואפילו מהדיון על חסינות שהוא עצמו ביקש לקבל הוא מקור…  קודם הוא הסית נגד המפכל אחר כך נגד פרקליט המדינה ניצן אחר כך מנדלבליט בשימוע כעת שליחיו עותרים נגד ינון  הכנסת לא…  מאמר מעולה מעמיק מדויק אמיץ ובוגר של איציק שמולי היום ב׳הארץ׳ קריאת חובה לבוחרי ומנהיגי המחנה כולו  איך זה שבמ…  חיוני למצוא לסתיו מקום ראוי מסביב לשולחן המשותף זמן לפעול  דברים נכונים של איש שאומר את האמת מצרף את קולי זמן לפעול  מברך את יאיר גולן ומרצ על השגת ההסכם כעת יש להמשיך בחיבורים קודם כל עם התנועה הירוקה בראשות סתיו שפיר פרלמנטרית…  הבאתי לארץ 250 קילו קנאביס במטוס מפורטוגל רוצים לראות  את המחנה הדמוקרטי צריך לשמור לא לשבור לרסיסים ולסכן מחנה שלם במחיקה תחת אחוז החסימה  סתיו שפיר ויאיר גולן הם נכס…  החלטה דרמטית ואמיצה של אייל ינון יועמ״ש הכנסת ניתן להקים את וועדת הכנסת ולדון בחסינות נתניהו אם יו״ר הכנסת אדלשט…  מאמר מעולה של חברי לדרך אלוף במיל׳ יאיר גולן אכן זו הברירה העומדת בפנינו סיפוח שבסופו אלימות וסוף החזון הציוני…  מה דעתה של אופירה על חיסולו של סולימאני מהי התחזית של ברקוביץ׳ לבחירות הקרובות ומה דעתי על החיקוי של זרחוביץ׳ קפ…  חסינות לנתניהו או חוסן לישראל זו השאלה נאשם בשוחד  מתעתע בציבור הוא יודע שהוא אשם הוא יודע שפרשיות המניות…  adindan מבקשי החסינות בתולדות ישראל  • באסל גאטס — הברחת טלפונים לאסירים בטחוניים  • סעיד נפאע — מגע עם סוכן זר  • בנימין נתניהו — ש… קבלו עצה ממי שראה כמה הצהרות דרמטיות לתקשורת לפני ומאחורי הקלעים  אל תעצרו את נשימתכם גם אם הנאשם מבלפור יחליט…  ימים יגידו האם אנו בדרך לפשיטת רגל מוסרית היועמש מפחד להכריע הבגצ נרתע מלהתערב הנשיא יתקשה להפעיל סמכותו לאחר הב…  ביבי לא כולנו מטומטמים החסינות נועדה להגן על ח״כ במעשים שנעשו לצורך מילוי תפקידו אף אחד מהאישומים לא קשור למילוי…  שבוע טוב הערב ב1935 אתראיין אצל איילה חסון בתכנית המטה המרכזי ברשת 13 מוזמנים להצטרף ולצייץ לאורך השידור המטההמרכזי ביום שלישי הקרוב היועמ״ש או בג״ץ חייבים להכריע הכרעה מוסרית נאשם בשוחד אינו יכול להקים ממשלה  שתפו והפיצו חג חנ…  ההתחמקות של מנדלבליט ממתן חוות דעת בעניין נתניהו מזכירה תובע איטלקי שחרד ממשפחת פשע   השתגענו האם היועמש מנסה להכתיב לעליון את גדר הדיון ופסיקתו למה לא לקבוע באומץ שנאשם בשוחד איננו ראוי לכונן ממשלה… </t>
   </si>
   <si>
-    <t xml:space="preserve"> עוד התבטאות חסרת רגישות מחברי כחול לבן הפעם זה שר המשפטים אבי ניסנקורן שנלחם למען קיום ההפגנות על אף העיקרון הפשוט…  אזרחים יקרים ממחר יחל סגר הרמטי מהודק לאור מספר החולים העולה ושובר השיאים הממשלה החזקה שלנו בראשות בנימין נתניהו…  אמש חגגו בסעודיה את היום הלאומי ה90 בממלכה אני מאחל להם ולנו שלום וביטחון במיוחד כשהסכם השלום עם ישראל קרוב מתמיד…  סגר הרמטי זה מה שמדינתנו האהובה זקוקה לו כעת בשעה קשה שמספר החולים מזנק ושובר שיאים עברנו את ה 7000 חולים וזה חמ…  לאור מקרי הרצח ביממה האחרונה במגזר הערבי פניתי לשר לביטחון פנים ח״כ אמיר אוחנה לזרז יישום תכניות מיגור האלימות וה…  GLZRadio הרצח בירכא  סגן השר FateenMulla אומר לamirivgi מדובר באדם נכה בן כיתה שלי שנסע בקלנועית ברחוב ומצא את מותו אין תחושת… נפל דבר בישראל שאט אט האמת שדיבר עליה ראש הממשלה בנימין נתניהו כל הזמן שמתרחש משהו לא תקין בין כותלי מערכת אכיפת הח…  לחקור את החוקרים הפרשה שחשף אמש עמית סגל היא בגדר רעידת אדמה לכל מערכת המשפט אני בעד הקמת ועדת חקירה פרלמנטרית שת…  כיתה א׳ בבית ספר יובלי הנגב בדרום מדהים חוויה אחת גדולה   ביקור בית ספר יובלי הנגב  ראש מועצת בני שמעון מר׳ ניר סמיר מנהלת בית הספר גב׳ מרים אלי גרברי  וכל תלמידי בית הספר ה…  אני שולח תנחומים למשפחת אוחיון על רצח אב המשפחה הרב שי בפיגוע דקירה היום בפתח תקווה עצוב מאד לשמוע על נסיבות הפיגו…  לשכת שר הבריאות שר הבריאות יולי אדלשטיין מודה לסגן השר פטין מולא על העבודה החשובה שעשה בטיפול בקורונה בירכא עבוד…  אני מברך את ראש הממשלה שלנו שעושה עבודת קודש אין ספק שהמהלך של ההכרזה על הסכם שלום האמירויות הערביות הוא מהלך היסט…  התראיינתי אתמול בכתבה ששודרה בחדשות 12 על התחלואה בנגיף הקורונה בישוב ירכא ועל הפגיעה הקשה בעסקים בעקבות התפשטות הנ…  ההסטוריה מתהווה לנגד עינינו הנה הגיע היום שבו מדינת ישראל תחתום הסכם שלום עם איחוד האמירויות הערביות זה הוא הסכ…  ישיבת עבודה מקצועית בה הציג ראש הוועדה הקרואה אלי רגב את אתגרי הרשות המקומית ואתגרי מערכת החינוך השר בירך את יור…  כסגן שר במשרד רהמ האחראי על המיעוטים אני מייחס חשיבות רבה לנושא קידום החינוך השבוע הזמנתי את שר החינוך חכ יואב ג…  לאור התפתחויות הביטחוניות האחרונות בגבול הצפוני אני שולח הרבה חיזוקים לחיילי צהל ולתושבי הצפון אני סמוך ובטוח שמ…   בפגישת עבודה שקיימתי היום עם שר התקשורת ח״כ יועז הנדל אשר התחיל לבצע את מתווה פריסת הסיבים האופטיים בכל הארץ קיבלת…  היום ביקרתי בישוב בית גאן כידוע ביום שני האחרון חולקו צווי הריסה למבנים אירעיים שמשמשים את התושבים כסוכות חקלאיים…  נסגר בפני הציבור בכלל  חלקם נמכר לציבור בתשלום אני בעד השמירה על כל השטחים הירוקים בארץ אך אני בעד גם החיבור בין…  הבוקר נסעתי לגן לאומי אכזיב על מנת לתמוך במחאת העמותה לקידום הדייג הספורטיבי ושמירת הסביבה הימית שמטרתה למחות על מד…  כמו כן אני שולח את ברכותיי לחבריי חברי הכנסת חכ אסנת הילה מארק מהליכוד וחכ צבי האוזר מדרך ארץ על בחירתם לוועדה…  בחירת חברים לוועדות שופטים  תחילה אני שמח לבשר לכם שהממשלה אישרה את בחירתי כסגן שר לחבר בוועדה למינוי קאדים מדהב…  במגזר הדרוזי קראתי לשר לחדול מכל צווי ההריסה בעת הזו במיוחד שבקרוב תוקם ועדה לבחינת חוק התכנון והבנייה קמיניץ ואנ…  השני של התפרצות נגיף הקורונה הדבר החמור בעיניי הוא שהוועדה לתכנון ובניה ואו כל גורם אחר המוציא צווי הריסה הינם חסר…  הוצאתי ב1372020 מכתב חריף לשר הפנים חכ אריה דרעי ובו התייחסתי לחלוקת צווי הריסה לרפתות ובתים פרטיים בישובים הדר…  אני מגנה בתוקף את הסרטון שבו אב ומשפחתו מאכילים ילדים בדואים זה מעליב ומקומם להתייחס לבני אנוש בצורה מבזה כזו ומח…  אני מברך את ראש הממשלה בנימין נתניהו ושר האוצר ישראל כץ על הצגת התכנית הכלכלית החדשה בצל הקורונה מדובר ברשת ביטחון…  אני מברך על מינויו של אלמ עמית אדרי לתפקיד מנכל משרד החינוך אני מכיר את אדרי באופן אישי ואני סבור ובטוח שימלא…  אני רואה לאחרונה ששר הביטחון לשעבר נפתלי בנט לא חוסך בראיונות ותוקף בחריפות את רהמ ומדיניותו ואני שואל איפה היית ע…  שר הכלכלה עמיר פרץ רוצה לשמר מונופול לחברת המלט נשר שלחתי היום מכתב לשר האוצר שבו התנגדתי למהלך של פרץ וביקשתי לא…  מחאת הרשויות הדרוזיות והצרקסיות הגיעה לסיומה  אתמול נחתם הסכם הבנות המסדיר את עניין תוכנית החומש לשנים 2020  20…  ברגעים אלה ממש מתגבש הסכם לסיום מחאת הרשויות הדרוזיות והצרקסיות במשרד רהמ ביוזמתי  פגשתי היום את שר האנרגיה יובל שטייניץ לפגישת עבודה חשובה הצגתי בפניו את כל הבעיות והמצוקות הזועקות הקשורות במשרד…  היום קיימתי פגישה עם השרה לאיכות הסביבה גילה גמליאל בנושא משבר הרשויות הדרוזיות והצרקסיות בנוכחות ראשי רשויות הש…  הגעתי היום לבקר במאהל עובדי תעשיית התרבות והאירועים מול משרד האוצר בירושלים הקוראים לממשלה לסייע לענף מפני קריסה נ…  את השבוע הזה פתחתי בביקור מבורך של השיח מוופאק טריף המנהיג הרוחני של העדה הדרוזית בישראל אין זה סוד שהשיח  טריף…  אני מאחל בריאות שלמה לחברי מהרשימה המשותפת חכ סמי אבו שחאדה מדובר בפיגוע פוליטי מאחר ובית הנבחרים השתתק כמעט מפ…  roiberenshtein rtelem FatenMolla זה יו״ר פורום ראשי ראשיות yanircozin קבלו את המינויים החדשים והישנים בפגישה מקרית בכנסת יברקן  סגן שר לביטחון פנים פטין מולא  סגן שר במשרד רהמ ענייני צר… shitritketi אני רוצה לברך את חבריי ח״כ zoharm7 שאושר היום מינויו ליו״ר סיעת הליכוד ואת חברי הכנסת GYevarkan FatenMolla ו Yoav… המשפט של ראש הממשלה נתניהו הוא המשפט שלי ושלך ושלה ושלנו ושל מדינתינו היקרה לנו מפז משפט נתניהו הוא משפט השמאל וש…  גם אני מצטרף לחבריי השרים סגני השרים וחברי הכנסת מהממשלה ביום ראשון הקרוב במפגן נוכחות שתומך ומחזק את ראש הממשלה…  عيد فطر سعيد لجميع المحتفلين كل عام وانتم بالف خير  עיד פיטר סעיד חג שמח  AobVlbOKRDzKsyM תודה רבה חברי היקר מאוד מעריך  cohenmeirav מזל טוב מירב יקרה  AmnonHarari BarakRavid BismuthBoaz  AmirOhana ידידי שר המשפטים היוצא ברכות רבות למינוי החדש השר לביטחון פנים אתה איש עשייה ומאמין שתעה רבות במשרד החשוב זה לעם ישראל netanyahu zoharm7 בהצלחה רבה לידידי מיקי ראוי בהחלט ברכות לח״כ יריב לוין על בחירותו בסיעת הליכוד ליו״ר הכנסת  ה  23 מאחל לו הצלחה רבה ח״כ פטין מולא מהליכוד להמיטב אני מבקש שתיק המיעוטים יופקד בידי אין בקיא ממני בבעיותיהם של בני המיעוטים במדינה…  אסור שבג״צ יתערב ברצון הבוחר שבחר ברוב מוחלט בראש הממשלה בנימין נתניהו כמו כן אני אשעה את כל פעילותי בכנסת ולא אשתתף בדיוני הוועדות עד שהתקציבים יועברו לרשויות אני מצטרף ביום ראשון למחאת ראשי הרשויות הדרוזית והצרקסיות מול בית ראש הממשלה במחאתם הצודקת נגד מדיניות האוצר  שעד…  SamerBarhamS שבת שלום סאמר היקר אחרי הזיכרון והשכול מגיע יום העצמאות שבזכות חללינו הקמנו מדינה חזקה ומובילה  חג עצמאות שמח  אני מאחל לכל אזרחי…  אחרי הזיכרון והשכול מגיע יום העצמאות שבזכות חללינו הקמנו מדינה חזקה ומובילה  חג עצמאות שמח  אני מאחל לכל אזרחי…  יום הזיכרון לחללי מערכות ישראל ופעולות האיבה נזכור ולא נשכח  liyaomer הוא כנראה לא יודיע איך עובדת הכנסת שלח את חברי הסיעה המובטלים להתנגד אבל לא יעזור לו החוק יעבור הלילה בוועדה ובסוף השבוע במליאה MKMickeyLevy אתם תמשיכו לעשות הצגות לתקשורת ואנחנו נמשיך לפעול למען אזרחי ישראל gtgt תושבי המקום ותושבי הגליל בכלל עם התפשטות הנגיף באזור  כולי תקווה שבקשותיי ייענו בהקדם האפשרי למען בריאות הציבור שתי בקשות שוגרו היום  מלשכתי לשר הבריאות הרב יעקב ליצמן  האחת לפתוח באופן מיידי מוקדי בדיקה לנגיף הקורונה בכפרים ה…  gtgt משמשים אותם לתשלומים חיוניים לכן אני מתנגד לקצץ בשכרם או לשנות את תנאי תעסוקתם של עובדי ציבור זוטרים  לפיכך א…  לאחר פניות רבות שהגיעו ללשכתי של עובדים מהמגזר הציבורי המוחים על ההצעה שהוגשה על ידי השר בצלאל סמוטירץ המבטלת א…  بمناسبة حلول شهر رمضان الكريم اتقدم باجمل التهاني للامة الاسلامية وكل عام وانتم جميعًا بالف خير سائلًا المولى ان يج…  بمناسبة زيارة مقام نبينا شعيبعليه السلام في حطين أتقدم لطائفتي المعروفية في كل مكان بخالص التهاني وأسمى التبريك…  לרגל חג הנביא שועייב עליו השלום אני מברך את עדתי הדרוזית בשפע ברכות מאחל לכולם בריאות וחג שמח למרות שהשנה לא יערכו…  היום ביקרתי בתחנת היבדק וסע לבדיקות קורונה ביאנוח גת אני שמח שיש היענות מצד התושבים של יאנוח גת שלוקחים אחריות…  האתגר התקבל לכל לובשי המדים בעבר ובהווה הצטרפו לאתגר ופרסמו תמונה שלכם במדים לחזק את כלל כוחות הבטחון בימים ק…  יום השואה והגבורה תשפ 75 שנה לסיום מלחמת העולם השנייה   יום שבו זוכרים את ששת מיליוני היהודים שנרצחו במהלך השואה…  KahanaMatan DayanUzi אני מצטרף לחבריי חברי הכנסת מתן כהנא ועוזי דיין שמקדמים הצעת חוק לקיצוץ מיידי בשכרם של הבכירים במגזר הציבורי ומקבלי…  عيد فصح مجيد  אל״מ הישאם אברהים מפקד חטיבה 460 בביהס לשריון ברכות לבביות חמות על בחירתך ובצדק להשיא את משואת צה״ל לכבוד יום ה…  חג פסח שמח וכשר לכל עם ישראל  YosephHaddad ח״כ פטין מועמד לשר מיעוטים בממשלה GizelleZ   samiaah10 יותר מ3000 דגימות לבדיקת נגיף הקורונה צפויות להילקח היום במתחמי היבדק וסע ברחבי הארץ ועוד אלפי דגימות יילקחו בבתיםהחל… gantzbe כל הכבוד לך בני גנץ רק כך מתנהג מנהיג שרוצה לשרת את אזרחי ישראל ישר כוח בהמשך לשיחתי עם שר הבריאות ליצמן על נקודות בידוק לקורונה במגזר הערבי והדרוזי  בקשתי התקבלה בחיובי בכך אושרו שתי נק…  התארחתי באולפני הכנסת בתוכנית כיכר הכנסת בתוכנית נשאלתי על המצב הבריאותי במדינת תחת מגיפה נגיף הקורונה כמה הממש…  RamBenBarak Kachollavan19 gantzbe netanyahu רם בן ברק זה חוקים לא דמוקרטים ופרסונלים נגד ראש ממשלת ישראל ונגד…  כמו שאמר מנחם בגין ז״ל  ת ת ר ג ל ו  hebayazbak היבא אתם לא מייצגים את המגזר הערבי אם אתם רוצים באמת לייצג את המגזר הערבי והדרוזי תפסיקו לתמוך בטרור ות…  כל הכבוד gantzbe לא יעלה על הדעת כי בגץ יהפוך למנהלה בפועל של הכנסת העם הוא שבחר את נבחריו  אני תקווה כי הדרך החכמה בה נקט אדלשטי…  אדלשטיין אשר שמירת החוק  וטובת אזרחי ישראל לנגד עיניו נאלץ לנקוט בדרך ביניים זו כדי לכבד את בגץ ולהוות דוגמא איש…  barakehud אהוד ברק אנחנו נתלה דגל אחד וזה דגל מדינת ישראל איך בעיצומו של משבר עולמי  כחול לבן עדיין עסוקים בפוליטיקה קטנה  Kachollavan19 יחד נעבור את המשבר ונצא ממנו מחוזקים ומאוחדים  שלכם חבר הכנסת פטין מולא אני נציגכם בכנסת מבקש מכל אחד ואחת מכם להתגייס בימים טרופים אלו ולהקפיד למלא אחר הנחיות ראש הממשלה ומשרד הבריאות…  ראש הממשלה מר בנימין נתניהו השר ליצמן משרד הבריאות והצוותים הרפואיים עמלים יומם וליל לספק פתרונות לבעיה ולאפשר הת…  חברים יקרים  כידוע אנו עומדים בפני אחד המשברים המאתגרים של העת הזונגיף הקורונה ההולך ומתפשט ברחבי העולם  זהו אינ…  נוכח ההתמודדות הנדרשת עם מצב שהעולם כולו ובכלל זה מדינת ישראל טרם הורגלו בו חובתנו לפעול יחדיו כדי שנעבור בהצלחה…  ראשי רשויות יקרים אני כאן לעמוד לרשותכם בכל בקשה או פנייה או סיוע שיידרשו מול גורמי הממשלה בעת הזו   כולנו רתומים…  זוהי אינה תקופה פשוטה עבורו של התמודדות עם ביקורת מחוץ  אני משוכנע כי יושב ראש הכנסת אדלשטיין ימשיך לפעול במסירות…  אני מוצא לנכון  לחזק בימים אלו את ידיו של יושב ראש הכנסת יולי אדלשטיין אשר מתמודד כמו כולנו בסיטואציה מורכבת של ניה…  SagiOrli אחינו הדרוזים חוגגים את הנצחון בראשות בנימין נתניהו   netanyahu עוד שני מנדטים ואנחנו מנצחים ומוציאים את ישראל מהפלונטר  SamerBarhamS إصحوا يا عرب إسرائيل ערביי ישראל התעוררו  ב23 נוצריםמוסלמיםדרוזים וצרקסים מצביעים מחל   רק ליכוד גדול ידאג למגזר… עשור של עשייה    בכלל התחומים והשפעה ישירה על הכיס שלכם  קבלו סיכום קצר שלי לחלק ממה היה כאן בעשר שנים האחרונות …  doko2015 תודה רבה ממשיכים בעשיה למען הצלחת הליכוד ולמען ראש הממשלה היום בגני הגליל ראש הממשלה מגיע מחכים לכם  ב23 מצביעים מחל דרוזי…  netanyahu שמעתי שגבי אשכנזי אמר בהקלטות שלו אמירות מזעזעות על אחינו הדרוזים שקשרו את גורלם לחיילינו אני חיייב את חיי להם לא אשכח זאת… rabeabader netanyahu   GabiashkenaziMK   סוגיית גבי אשכנזי והעדה הדרוזית מעלה הרבה תהיות והשאלה שנשאלת כאן    אם אין בשר בדברים למה עד עכשיו לא יצא גבי א…  היום מכנס נשים מהמגזר הדרוזי שהתקיים בו השתתפו מעל 100 נשים שרת הבינוי השיכון דר sbyifat  חכל OsnathilaMark…  فطين ملا، الممثل الحقيقي لكل قضايا الطائفة الدرزية والوسط العربي   نشارك ونصوت وننتخب ليكود محل   פאטין מולה ה…  ביקרתי בעיר הבדואית הגדולה ביותר בדרום בבית חבר מרכז הליכוד ידידי עאטף אלגרנאוי בפגש השתתפו נכבדים רבים מהעיר בפג…  SamerBarhamS תודה סאמר היקר פתחתי את השבת בסיור בנגב  לעמוד מקרוב על הבעיות והנושאים המציקים לאוכלוסיה לבדואיים בדרום תודה רבה לכל מי שנכח וה…  ביום שני בשעה 1900 נפגש במסעדת ג׳יראף  בהשתתפות חכ״ל OsnathilaMark ושרת השיכון והבינוי sbyifat מחכים לכם  Yossi31026569 netanyahu 30 מליון שח הושקעו בישובים דאלית אלכרמל להקמת אודיטוריום   202 מליון שח תוכנית חומש לישוב…  Yossi31026569 netanyahu שר המדע והטכנולוגיה ושר העבודה והרווחה אופיר אקוניס חנך כיתות מדעיות בכפרים הערבים  מימון…  Yossi31026569 netanyahu שר האוצר משה כחלון חתם על צו חיבורי חשמל לבתים שנבנו לא חוקי מחוץ לתוכנית המתאר לסעיף 157…  Yossi31026569 netanyahu זה רק בשנה האחרונה מה שממשלת הליכוד בראשות בנימין נתניהו   10000 מליון ש״ח לקידום תוכנית…  SamerBarhamS מזל טוב סאמר היקר חבריי תומכיי ועוקבים אחר הפעילות שליאני שמח לפרסם כאן סרטון  תקציר של ביקור ראש הממשלה במגזר הלא יהודי והחיבו…  ביקרתי יחד עם ראש הממשלה ושרת התרבות והספורט  regevmiri ושר החוץ Israelkatz  ושר הכלכלה elicoh1 אצל השיח אבו ח…  כנס המגזר הערבי הגדול ביותר במעמד ראש הממשלה netanyahu   ב23 הדרוזיםנוצריםמוסלמים ו צרקסים מצביעים מחל  netanyahu שידור חי מגוליס רק ליכוד גדול יקים ממשלה וימנע בחירות רביעיות וממשלה של אחמד טיבי עם גנץgtgt  מחכים לכם מחר   כנס המגזר הגדול במעמד ראש הממשלה netanyahu  W7NhCPUdxmOvtIh תודה רבה הכנס הגדול במגזר  והפעם בנוכחות ראש ממשלת ישראל מר בנימין נתניהו זמן  יום רביעי  תאריך  190220 שעה  1800   מ…  SamerBarhamS רק ליכוד ישמור על המגזר הערבי   במפגש מרתק במסגרת הערכות לבחירות ב 2320 עם השר yoavgallant בהשתתפות קצינים בכירים במיל מבני העדה הדרוזית   השר…  עקב צווי הריסה שמרחפים מעל ביתם של תושבי הכרמל במיוחד בעוספיא ולאור פניות רבות של התושבים אלי בנושא זה  יזמתי ישיב…  השתתפתי היום בחוג בית בישוב ביר אלמקסור אצל חבירנו חסין עדיר בראשותו של שר הכלכלה חכ elicoh1  חברי מרכז ומכובד…  matanco999 תודה רבה 2346479Orna תודה רבה אורנה SamerBarhamS netanyahu כל הכבוד סאמר העבודה הקשה והמאמצים הכבירים שאני עושה למען העידה בפרט והמגזר בכלל מניבים פירות היום הממשלה אישרה את הצעת השר לשת…  EliVaknin12 תודה רבה לך אליהו אני עובד למען כל המגזר הערבי דרוזינוצרימוסלמיצ’רקסי gantzbe ואני רוצה לשאול אותך ח״כ בני גנץ איך אתה תטפל בעוטף עזה שאתה תלוי ברשימה המשותפת shahar300 netanyahu המון תודה רבה ב23 מצביעים מחל התארחתי במפגש פוליטי בביתו של חברי אבו מוחמד אחמד גאנם מישוב שעב בהשתתפות ראש מועצת זרזיר אמיר מזאריב ראש מועצת ב…  עוד מפגש מוצלח לפתיחת הקמפיין ולאיחוד כוחות ליום הבחירות בישוב מגאר בביתו של חברי אבו כרם פאיק סרחאן בהשתתפות חברי…  הנאום שלי היום בכנס בחירות עם ראש הממשלה netanyahu בנהריה  יוצאים לדרך בכל הכוח    ראש המטה במגזר הלא יהודי חכ לשעבר פטין מולא יחד יור מטה ראשי השר ישראל כץ יור מטה קל…  כנס ראשי המטות של הליכוד במגזר הדרוזי המוסלמי הבדוי הנוצרי והצרקסי  אווירה חיובית נוכחות מסיבית ורוח ניצחון ריח… </t>
-  </si>
-  <si>
-    <t>AryehHasfari על הרודנות טימותי סניידר  מדינה מס 1 feeling blessed 🥰  כיפור יצא לפני שעה טוב עדיין אתקע בשופר בשמונה ורבע שזה פחות לפתוח את שערי שמים ויותר לצלצל להם באינטרקום ולברוח HaishVeHaagada איש מושלם אני כל שבוע 🤔 פאנסקסואליות זה כשלא נמשכים למגדר או למין רק לנפש לא משנה איפה היא נמצאת 🤔🤔 אז אני פאנסקסואלית 🤔🤔🤔 אם הנפש נמצאת בגוף של בת irmyshikblum תכניסו אותי בחזרה לבורגנות mgenelevi נשמע מקסים הדייסון שלי מקולקל בסגר אנד דיס איז ג׳קאס בשמונה ורבע אני תוקעת בשופר מביתי שבקישון פינת פלורנטין מוזמנים לבוא לבקש משאלה אפשר לשכור קורקינט עכשיו gititfisher עינב בובליל באינסטה בפוסט נגד ההפגנות כשהכותל ריק והתגובות  ממי ההפגנות לא מדבקות צום קל תחנקו כל השמאלנים צום קל וגמר… Syechimovich אמסור  noamsch נשבעת באלוהים שאין לי מושג איך אני עושה את זה אולי אהבה Zeshe לפי העין עד שאת איטלקיה הכנתי את הבולונז המפחיד ביותר שהכנתי אי פעם אני חוזרת המפחיד ביותר מפחיד כמו הודעה מאמא בשלוש בלילה תתקשר דחוף לא ישנתי דקה ואמא של שרון פרסמה תמונה שלה עם אבא שלה שנפטר הלילה ובאתי להגיב לה ״מהממתתתתתת״ לא הצלחתי לישון כל הלילה אז אני אמשוך עד שבע וחצי ואלך לקצב לילה שכבה עליי ושתיתי מים אז היא קמה לשתות מים גן חזרה לספה אמרה גררפ גררפ ונשכבה עליי שוב במה זכיתי הקשר שלי ושל לילה  סרט של פיקסר אנשים שאומרים ״כן חיחיחיכיף איתי במסיבות חיחיחי״ שידחפו אתכם בשלמותכם לתחת של דינוזאור eyaldatz למה אי נוחות OmriAsher בנסיבות משמחות למסירה מאפרת זין בלב העיר  באיזה קטע אין דוקו קצר על טרנס בן 35 שגדל לו זקן פעם ראשונה ואבא שלו בן 70 שמלמד אותו להתגלח וכל הסרט זה הם מדברים…  lt לא להתמסטל ולקרוא ספר במיטה כי את בטיפול מדי יושבת עם ג׳וינט ביד וחושבת מה אני צריכה למחוק את עצמי כשאני יכולה לחבק את עצמי להתמסטל בטבע lt להתמסטל אחרי מקלחת בבית מבריק עם מקרר מפורק אני בשנה האחרונה השתכנעתי סופית שדתבולשיט 100 נגמר הסיפור לא צמה בכיפור לא שומרת בפסח אוכלת בשר וחלב ביחד מה…  הקו הדק בין רעב טוב של יאללה תביאו אוכל לרעב רע של לשכב בתנוחה עוברית על הרצפה ולבכות מה קודם כל לאכול אמבונגר עם בצה או להחליף מצעים ולעשות כביסה עזבו אל תענו לי המבורגר יותר טעים עם רעש רקע של מכונת כביסה טוק טוק ינון מגל בבית כן מי שם הפסיכיאטר המחוזי באתי לאשפז אותך על שימוש פסיכוטי באימוג׳ים מה אשתו של ינ…  Elzavered נו תגידי 17 חיוביים יאללה חברה אנחנו יכולים יותר אם על הרגליים אהלון  למה הגוף מבין רק כח למה אני לא יכולה לבקש ממנו יפה מסת שריר שיניים ישרות ועור חלק והוא פשוט יבצע למה הוא מאלץ אותי…  אוי לא פגע בי ברק בצורת מאמר מערכת על השימוש במילה שלום כמילה ביטחון במערכות בחירות בישראל עד ביבי ובחלחול של סמנטיקה לתודעה איזה השפלה אם אני באה להפעיל את האחריות על הדייסון ואומרים לי לא ממי האחריות לא מכסה שיער ברמת קווקזיות הזאת ועוד שתי חתולות תקני חדש למה למה סגר דווקא כשאני צריכה להפעיל את האחריות על הדייסון ולעשות קניה גדולה באיקאה מושחתיהו תתפטר נכון יש אבא שהוא סבבה והכל אבל פעם בשבוע מפרק אותך במכות מעניין אם ככה החתולות תופסות אותי שסבבה והכל אבל פעם בשבו…  זה רק אני שופר ודממה טוב אני במרפסת אבל לא אשרוק ראשונה באמת יוצאים למרפסת לשרוק בוז להוציא שופר LeahLev אם הכל בסדר אצלך למה את נשמעת ככה MmandraA מרי ביבי פאק יאיר קיל שרה סורי סורי סורי בפני עצמי ביבי אמר קשקוש בלבוש על הקשקוש בלבוש  יאללה ממי תפרוש מראשות הממשלה ותקליט קלטת ילדים מלאה מסרים סמויים על למה יוב…  בני גנץ איך זה נראה על הקרטון ראש הממשלה הבא של ישראל רמטכל לארד צריך לעשות אחרת נעשה אחרת איך זה נראה באמת אני…  ישראלים אנחנו ממש אבל ממש לא היהודי הגלותי ממש לא חלשים ממש לא אכפת לנו רק מכסף ממש לא מפיצי מחלות הכל שקרים ב…  Jacoberesheet מינון בצה גחנון מושלם ItaGaz הסתדרתי תודה רבה  זה באמת מאד נח הן יודעות מה הן עושות רבים שואלים אותי שיראל מהו אוריינטליזם ותשובתי היא סחבתי שישיית מים מהאמפם על הראש כמו הודית samanio וואי כמה נמשכתי mtklng זהו לוקחים את שניהם אוקיי ראיתי לבד מה ההבדל בין מענק עסק קטן למענק סיוע אני אמורה לבחור רק אחד מהם או את שניהם מתי אייל דץ קם אמרו משהו על מענק נוסף לעצמאיים בגלל סגר 2 אני אקטיביסטית א עושה ק לייקים ט לתגובות י רעות ב פוסטים י של ס ביבי ט באינסטגרם י  ת SharonDisk חברים בטוויטר הלפ אם יש כאן מישהו שיכול לתת לי כללי אצבע לגבי איך יודעים מה להוכיח בהוכחת נכונות באלגוריתמים בעיקר של גרפ… Sachback כן והיא מובילה למקרר RBilova כן לצערי רעיון לספר שירה סמסים שלא שלחתי לאקסיות בזמן שליצור אמנות אומר בואי נמיין את הערימת חרא המגעילה הזאת ונמחזר אותה יכול להיות שיצא לנו חנוכיה מגלילי נייר ו…  מה עצוב בוויד שיש כזה גודש של רגשות שהוזנחו במשך כל כך הרבה שנים שלפעמים פשוט נהיה בלתי אפשרי להרגיש אותם א…  foolforlove69 הסתדרתי תודה חיים שלנו 3333333gtgtgtgtgtgtgtgtgt זה עצוב גם היתה לה הפרעת אכילה והיא ניהלה יומן שמתעד כל דבר שהיא אכלה באותו יום ובסוף מכרה אותו באיביי כשהיא יצאה…  Cusamano תודה אהוב שנים רבות תהיתי איך למירה גונזלס נשארו תאי מח עם כמות הוויד המשוגעת שהיא עשתה והיום הבנתי שהיא הוציאה ספר שירה מדהי…  האם יתכן שאין למצוא את הפרק של בואו לאכול איתי עם פנינה רמון והבחורה הדתיה ששרה שמן שמן שמן שמן מישהו כותב רשימת קניות למכולת טוקבקיסט בהארץ כתיבה שמזכירה את אתגר קרת סרט שראיתי בכיתה ה וחשבתי יה ככה אני אהיה כשאני אהיה מבוגרת אמנית ופרוגרסיבית וכזהשרלילה מה נשים רוצות לינק לצפיה ישירה לסרט צריך שלושה לטנגו אני חיה בבניין עם הבנות הכי חמודות בתל אביב שחולקות עוגיות וויד ועציצים כל היום למה אני לא אמריקאית יש לי את כל הרגשות הנכונים  איילת שקד היא הילדה שחוזרת מהחופש הגדול ומספרת שבן דוד שלה שכן של יהודה לוי והם הסתובבו אצלו בבית כל הקיץ  VxvI8jA9y62ez94 לא  תמלול חקירות נתניהו בליווי עשרה נגנים אז יש בלפור מחר קניתי אייפד כי קינאתי בשרון השתמשתי ל א ללמוד לבגרות במתמטיקה חד מש לא הייתי מקבלת מאה בלי האפשרות לתרגל בלי מחי…  נקודת אור מישהו מאמין לנאום של ביבי מאתמול פעם היתה לו כריזמה שהצליחה להחזיק את הנרטיב שהוא ניסה למכור אבל היא פש…  החלק הכי קשה ביישור שיניים זה התפוררות הדמוקרטיה איך בסגר הראשון היתה באינטרנט אווירה של ״כולנו בזה ביחד״ ועכשיו יש אווירה של ״אנחנו מסתכלים עליכם מחלון מסורג ששם ע…  למישהו קרה שהדייסון כל הזמן אמר שצריך לנקות את הפילטר למרות שהפילטר נוקה אתמול אני פוחדת לישון כי כל פעם שאני קמה יש חדשות מפחידות יותר איך מה שקורה עכשיו חוקי אני משתגעת אנחנו בני ערובה של אדם שאיבד את זה noamsch פחממה יאללה טלפון מכובה עד הערב זמן להשקיע את המח במה שחשוב ממליצה לכם לעשות כמוני אוהבת בודהה לילה גדלה מגור רזה מהפחים לחתול מטופח שעושה שימוש היפסטרי בואכה אוריינטליסטי במוצא שלו כדי לחרמן כמו אמא שלה לפני כמה שנים  כאשר הבית מדיום מלוכלך אז את מטנפת אותו עם לאכול בסלון ולהוריד נעליים בכניסה שיהיה וול דאן ובערב תתעצבני ותדפקי נקי…  SharonDisk אני Nefolet ShaiNaamat זה מהראשי של הארץ  ShaiNaamat הארץ בראשי תחת מעקב קורונה JewMoleman ביי ממוש רגע מה  ping93  ping93  פסיכופת לא היה רואה את האחר ככה נמשכת לאסף גרניט לא מתביישת בזה יותר תוקעת בוז בשופר בואו  Rebbetzin אשכנזי ואתיופית מה נשים רוצות לחיות מחדש את שנת 2019 בלופ HaishVeHaagada Rutshapira אלא מההההה zelokova מה זה Rutshapira אחת לי השאר יחולקו שמאלנים אנלא מבינה  אם אין נתונים על הדבקות בהפגנות למה להפסיק אותן מה לאפות shaipct2019 That teeth tho שבוע בלי חדכ לראות אפל ווטץ׳ מטרגר אותי DorDugy וואווווון aaddams האכלתי אותו כל הזמן והוא הסתובב בדירה חופשי אבל החיים שלי היו בקריסה ולא היה לי משאבים רגשיים לדאוג לעוד ח…  tomereznik זה טיפול של שישה עד שמונה חודשים מה כפת לי aaddams כן זה היה ממש עצוב  noamsch אסמר פיפי אני עושה יישור שיניים כדי לחייך יפה כשביבי יתפטר aaddams כן נזכרתי בבעלי דירה הכי גרועים שהיו לי א השאירו בדירה ארון שלהם שאסור היה לי לזרוק ב השאירו חתול שאמרו שיקחו תוך ש…  תקוע לי בראש השיר מהפרסומת הפרובוקטיבית של פוקס 2002 LilacBL לחץ חברתי שנתקלתי בו בסדרות תבריזי משיעור תעשי סמים תשכבי עם שחקן פוטבול לחץ חברתי שנתקלתי בו במציאות תרשמי לצופים תרשמי… Cusamano מנטור לאסיד וכאכי שיניים mtklng אוקיי הבנתי Cusamano כאב מסוג ״לחץ״ בשיניים וקצת בחלל הפה שנחתך כואב כל הזמן אבל אני עם זה פחות מ24 שעות mtklng מה קשור פעולת יניקה וויד שעד כה היה הדבר היחיד שעוזר לי עם המגרנות הכי חמורות מחמיר את הכאבי שיניים מהיישור eliranlevy1 אינוויזיליין זה ההכי קל  sliced0range הזמנתי וקיבלתי תוך שבועיים עם טראקינג ומיילים DorDugy יאללה נוסע למילואים א ב ל  יש פרק חדש בהסכת שאין חומר את שמו בואו להעביר נסיעה או את הסגר בבית עם shireuven ואיתי   ShaharTaiber HaishVeHaagada על האש Cusamano  Cusamano חצי שנה עד שמונה חודשים Cusamano סיוט אלוהים ישמור אבל הדד ליין של השבוע לסיוט הכי קשה מרגיע Cusamano  כמה זמן נשאר לך sliced0range מדהים שלא רואים וזה מציק בטירוף sliced0range  shanisaggy אני משלימה איתי הילדה עזבי כדי לנעוץ את הרגרסיה אני לא רק עושה יישור שיניים אלא גם מתכוונת להתקשר לאמא שלי ולבכות לה שמציק לי בפה לא הבנתי למה נקטע לפני שהוא מתחיל לזיין אותם  למישהו יש ספק שאם הייתי גבר הייתי עושה השתלת שיער אפילו בלי להקריח אני לא מאמינה שעושים כתבה על חבילןת נופש בסרביה ולא על זה שהתחלתי יישור שיניים אלוהים ישמור מציק לי בפה dOyWeUOloMUH79R מליון שחלים התחלתי יישור שיניים אינוויזיליין מתי זה יפסיק להציק לי בפה היי וולט לא הזמנתי מגיפה עולמית הזמנתי להיות חודש בניו יורק לאכול עוף להתמסטל ולראות כנר על הגג בברודווי iftachh תייגו את השכונה בנפולי ושכונת עמידר בקרית מלאכי ואל תגלו להן מי זו מי  MaiBarzilay חיבוק ענק  LilacBL ההההההההה SharonDisk צמדים דבק בישראל סטטיק  בנאל ג’חנון  רסק מחפשים שותפה לדירה  חיחי סליחה בנים  BaradBracha כמובן   להגיד שם של מישהו זה כזה כישוף mtklng חחחחחח עלק mtklng קטלוג איקאה זה ספרות mtklng שיגיע כבר קלינג 2027 שידבר איתי על רהיטים מאיקאה lbiadgo  הטרלת השנה  nynynyos חחחחחחחחחחחחחח mtklng גהי זוכרים שראיתי את הפסיכולוגית שלי בהופעה של רונה קינן אני לא נרגעת מזה עברו שנתיים אח חתול הרהיט ההיי מיינטננס מה שמבאס במשבר הקורונה זה שהוא גורם לי לשנוא את ביבי אישית והוא היה הדמות האהובה עליי בישראל עד עכשיו עבדתי מה ביבי עשה הפעם פאן פקט הקלדתי באינסטינקט וולדמורט ורק בחצי הדרך קלטתי שזה לא השם שלא רק הכריזמה klarago מבחינתי כל דבר שלא אדום או לבן  יש ריב על האש מה הלב הכי מסריט במה נפלתם בקורונה nynynyos בשביל תירוץ להתלונן שלח אצלי קלללל למה אין מוצר בדארקנט שירצחו את האשה הזאת ואותי באותה שניה בדיוק כדי שאני אתגלגל לגוף שלה ואאכיל חבר שלי דב בתותים  eyaldatz kann נראה פצצה מתה לראות limormoyal אז היה ערב סוער ומרגש בבלפור וקשה להירדם אחרי כל מה שחווינו לכן החלטתי להתחיל לחקור קצת את חבורת מכחישי הקורונה ההזויים… ShiraDavidson14 עודדת מאד דווקא  ShiraDavidson14 lt3 אז מה עושים  טוב של רוגל אלפר שמתאר בול בול את הרגשות שלי בנושא הגירה netah מה חשבת עליו אני מדברת ברבים לא בקטע קווירי אלא בקטע אולד סקול משוגע שיר יפה לדעתנו  nynynyos מאד אבל הייתי בתקופה שחוויתי פחד אלוהים nynynyos סרט פחד אלוהים artistsofcolour MIDNIGHT AURA Billie Zangewa 2012  nynynyos חחחחחחחלללחח nynynyos או אאו אותי סם  שרתי ללילה את מסיבה בחיפה והיא תקפה אותי נעמה הכינה לי תה עם מלח בביתי לא אכפת לי מהטעם נעלבת שחשבה שבבית ככ לסבי יש סוכר לבן Jacoberesheet כן זה מה שעושה כעת  Jacoberesheet נכנסתי לסרטון בשם ״זה צא נראה כמוך״ ותוך כדי שהעמוד נטען הבנתי שהכתובת זה משהו בסגנון virusvirusvrsbad מה עושים אם אני מפגרת ונכנסתי לווירוס shirdecker DorDugy ItsAaronKlar לזייף תני להם לזייף DorDugy shirdecker כן אבל זה לא מאד נדיר שאנשים שגרים בתל אביב לא משנים כתובת shirdecker מה תוציא להם חוזה דירה shirdecker שהם גרים ביחד kafkafel לא נורא תפסיקו לקרוא לשנים במספר ברצינות זה מביך אותי התפיסת זמן שלכם נמאס לי מזה שאחרי כמה שנות שימוש הגוף פשוט קורס כמו אייפון ישן אף אחד הנפש שלי תעשי סיר פירה ותאכלי לבד בתחתון שנה טובה הסגר יפתח ב11 באוקטובר קחי אותי קנדה  ריאלטי שבו עשרים ישראלים מתחרים במשימות שונות על הזכות להגר למדינת עולם ראשון מתפקדת ומשעממת הכנתי מם  איך יודעים מתי יש איקאה סייל ולמה זה לא כשמחזור הירח מסתנכרן עם המחזור שלי רבו מכות כאילו הן יריבו על פוליטיקה החתולות רבו מכות ונתקעה ללילה הציפורן בחלוק שלי היא השמיעה משהו שהוא בין יללה לקריאת קרב ולא נתנה להתקרב אליה בלי…  LucyFord יש כבר מישהי על הכוונת אני ושרון שוקלות להביא חתול נוסף וחושבות על שמות אני צריך על שם דמות מיצירה שאנחנו אוהבות כמו מופי ולילה שרון שמש אחותי נמאס מהשנה הזאת חשבתי שיהיה לי טוב אם אני אעשה כל מני דברים ואז עשיתי אותם והיה לי חרא אני אושר לא מגיע מלה…  Duduoppe די יד צאי מהתחתון כאשר מישהו מסתכל עליי ליותר מחמש שניות ממי אני לסבית ל ס ב י ת אין מה לגשת אין מה לפנות אביא לי הטלפון של אחותך הג…  ככה זה עונה 2  ללקק תאצבעות דודה שלי תראי איזה חזה ענק נהיה לי 70b netah אהה וואי הייתי מזיינת את זה netah מה זה מבחן המרשמלו</t>
-  </si>
-  <si>
-    <t>sagic AronRabino1 תהיה מקורי לפחות AzoulayHana זה לא האמיתי זה בגלל שליחות של תן ביס ShefDoron manuelbaz לא כי וייל סמית AronRabino1 מניח שנתניהו יודיע היום על חקיקה מזורזת כדי למנוע מקרים כאלה  אה לא ChasmanShachar כבר חתומה לשלוש עונות אני אחרי ששליח של וולט מנסה לפצות אותי על איחור עם הפיצה  gershuni filbers דהיינו מתקפל manuelbaz זכות ובקיצור מזל טוב GuyLouzon filbers עיתון manuelbaz את קולטת איזו זכות זו שנולדת באותו חודש בו נולדו ירדנה ארזי ו׳יל סמית ונדב אבוקסיס filbers אבא שלי בשבתו כמזכיר המפד״ל בחצור יותר מ30 שנה קיבל כל בוקר הביתה עיתון הצופה כשהוא מגולגל בצורת בגט gershuni filbers רוצים לעשות עליי שידברו איתי בדולרים filbers תסגור את עיתון הארץ ולימניים לא יהיה מה לקרוא gershuni filbers נכון אבל גם נגד לעשות עליי פיילוט filbers הלו שלמה אני קורא הארץ למה ככה DoriaLampel נגנב ממוזיאון הלובר RonelAdani נבלים ברשות התורה RonelAdani IritLf למה להדליק סתם אני כבר חצי שנה לא מתפרנס מכלום RonelAdani IritLf היא בטוחה שהיא באינסטגרם RonelAdani בדוק זה בבלפור matanamirr כל הארץ ככה וזה מרגש עד כדי שהלוואי שכל שנה תפילות כיפור יהיו בחוץ mohammadkabiya MohamedBinZayed עזוב זה מנהיג זה לא עוקב אחרי אף אחד זה עוד יגרום לסכסוך עולמי  shimonliberty הוא ככה תמיד לפני הצום בסוף הוא מתרכך סתם עצבני עד סוף הצום הוא מתרכך עליי  deanarielmd הכי אהבתי שלא שכחת את ההאסי  omrifeinstein אתה לא שוכח אותי בדיוטי של דובאי לא הבדיחה של נתב״ג כן omrifeinstein יש מצב שזה נסיך מדובאי לך על זה nnnnaa deanarielmd עכשיו שם את השיר באפל מיוזיק nnnnaa deanarielmd איזה deanarielmd מקסים ויפהפה  כל צילומי הרחפן עושים חשק לגור בשמיים  הכי כואב על המשפחות של השוטרים שלא יחגגו את הסגר יחד השנה MottyFarangy אאוץ׳ amirayelet ששש אל תפריע להם DavidSaranga vladutv Digi24HD AdiHadean Peschetta שמע סחתיין על הרומנית לא יודע אם attilus אפילו מדבר ככה…  KalmanLiebskind אתה המצפן שלי DavidSaranga vladutv Digi24HD AdiHadean Peschetta נראה כמו ארטישוק ירושלמי אבל אצפה ב2100 זה בטח עדיף על חדשות vladutv DavidSaranga Digi24HD AdiHadean Peschetta איפה האוכל kaisos1987 zviashkenazi תודה יא חביבי DanaYarkechy zviashkenazi  lilacsigan kbeladev zviashkenazi תודה לילך alisaripel zviashkenazi לא לא איזה פוליטיקה איזה HaimJelin zviashkenazi אתה איש יקר תודה חיים איפה ימים שלא היתה קורונה והתעסקנו רק בקסאמים ואש בעוטף  talialin zviashkenazi תודה טליה Reut21918544 zviashkenazi העיקר שאתם אוהבים  EfratFinkel zviashkenazi תודה רבה kbeladev zviashkenazi תודה יא קובי זוכר אותך מההופעה אצל תומר  עוד נשוב  roeep86 תודה רבה אחי idanviezman תודה אח שלי מביאה אחלה חומרים רק מול מי נעשה אותם  NirKipnis zviashkenazi בדיוק AfekAlon zviashkenazi תודה אחי זה לא אני זה השנתון שלנו שאחראי לזה Meravbenari zviashkenazi  yosefyisrael25 zviashkenazi ממש לא אבל תודה אחי mohammadkabiya Hakufsah תודה יא עאמי moriamalka12 SharonaMazalian Hakufsah  issacharoff shnaiderman אתה אומר מברוכ ואני מחפש אנשי שב״כ סביבי תודה יא אחי moran56049995 zviashkenazi תודה תודה אחי SharonaMazalian Hakufsah אינשאללה תודה בשנה הבאה עונה חדשה של טהרן חוגגים בטהרן יחד perezesty Hakufsah תודה רבה חברה  RimonRan עד שהגיע גנץ ונהיה רמטכל במקומי shnaiderman וכן גם ברשת הקשה הזו יוצאים לא מעט סיפורי חברות shnaiderman תודה חיימייייי Hakufsah תודה לעמוד האהוב עליי ifatyakobsonpr Ayeletnnv zviashkenazi אחפש אותה היום mottyn תודה יא צ׳ארמר ifatyakobsonpr Ayeletnnv zviashkenazi חחח ifatyakobsonpr Ayeletnnv zviashkenazi תודה תודה לזו שעשתה עליי כתבה בפנאי פלוס לפני כמעט 20 שנה כשהיו לי בטוויטר בקושי 10 עוקבים Ariav השאלה מה ישאר Abutir omerbabai שתוק zviashkenazi תודה תודה ברכתך ברכתנו אבל למה לעזאזל התמונה הנוראית הזו למה antoineeliaroni יש אפילו גייז Abutir omerbabai איך אתה אוהב לקדם את הטור שלך אצל אנשים עם השפעה omerbabai בדיחות מתרומם זה התחום של Abutir GitelmanDima יש פה פתח תקוואים שפותחים עין לא לעניין avrimusic פיקוח נפש avmeridor asaflib אני מאוד לא אוהב את ההסתה שלך נגד אנשים שעושים את עבודתם בתקשורת htyaniv דקה לפני שאני בן 49 נתקפתי חמלה אנשים טובים חיפאי לפני סגר עם 25 עוקבים  תעשו מצווה ותנו לו עוקב תראו לחיפאים שאכפת לנו  YairNetanyahu ivgiz יופי לכם בסוף אתם תשכבו ואני אשב לבד בסגר noamfathi אם היה מתפטר לפני שבוע היה מספיק להיכנס למצעד השנתי avmeridor asaflib אתה לא רווק asaflib כמו איזה שני משוגעים michaelzil odaskal אבל להם אין שלום עם אבו דאבי amitsegal גנץ ביקש קצת זמן כדי להשתין ואז להיפגש EliPahima ivgiz YairNetanyahu כל עוד זה לא בבלפור זה מותר ivgiz YairNetanyahu איתך נראה לך יש לי כוח לעבור את כל מעגל האבטחה בבלפור ivgiz YairNetanyahu אבל הבטחת לי ivgiz לא זה פיפי GLZRadio gantzbe moriahasraf והתמונה של גנץ מה נסגר איתה מסוג התמונות שאתה אומר לצלם ״תיזהר להעלות״ shnaiderman זה יעלה לכולנו dasides וכמה אתה חושב שאני מקבל עבוד ציוצים לא פחות מ1000 לציוץ שמגיע ל1K shnaiderman כמו בלוטו בארצות הברית חילקו לי את הסכום ל20 שנה עם כל הביקורת על התנהלות הממשלה תודה לאל שנכנסים לסגר הזה אחרי שקיבלנו את ה750 שקלים Rereshef Abutir ישר כשעלה הדב לשיר אני ידעתי שזה עודד בן עמי Nehoray81365797 YuvalKarni sbyifat עוד חבר כנסת או שניים מחוץ לקבוצה ואנחנו ממגרים את הקורונה YuvalKarni sbyifat זה נראה שבליכוד עסוקים בעיקר בלפתוח קבוצות וואטספ talialin מה זה פה גבעת התחמושת chaimlevinson בבחירות הבאות אני מצביע לך sefiova Israelkatz תהיה חזק תתכונן לזה שהחל מהערב  אתה נציג השמאל הקרן החדשה בעצם עזוב chaimlevinson עושה את זה יותר טוב ivgiz אז זה אורי תירוש  ivgiz בושה ילד קצת הפריע לשיעור בגלל זה לשלוח לו חמוש שינתק אותו מהזום doronaviram YehoshuaYosi 12 זונות kenegozi yakhinzik YehoshuaYosi 1989 לא הצלחתי לקלוט מה המפקד אומר אתה מדבר איתי על קליטה של סלולר yakhinzik YehoshuaYosi והרבנים שחטפנו בקבטייה הם חטפו סוכריות טופי amihai72 YehoshuaYosi בושה YehoshuaYosi פעם קראו להם כוסיות ובצדק BenCaspit YehoshuaYosi haimslutzky זה רק כי נכשל בגיבוש YehoshuaYosi לא הבנתי למה גדוד 13 לא עובר לחיל נשים akivanovick דעה למי אכפת איפה ואיך שרה נתניהו עושה כביסה שתשלח מאה מזוודות מדי חודש לאיזו מכבסה שתבחר ברחבי הגלובוס הרבה יותר חשוב… צרפת או שוודיה בדוק  OfirRichman NoaShpigel בוא נאמר ככה אם המצב יצריך הפגנות גם כשיהיה אסור צריך להפגין כרגע במצב התחלואה כשחיילי…  OfirRichman NoaShpigel קטונתי אבל לא עכשיו אפילו כמה מנהיגים מהשמאל ביניהם עופר שלח הודיעו שבשלב הזה עם כל ה…  dasides אתה יודע שיש מסיבות אנדרגראונד בתל אביב כבר כמה חודשים שלשום שמעתי והייתי בהלם ושם לא נדבקים  לגבי רשי…  Orengerman לכולם שנה טובה OfirRichman NoaShpigel אז אולי זה הזמן של המפגינים להחליט על דעת עצמם לא להפגין ובכך לא לתת לו את התענוג לחוקק את זה dasides מעולם לא טענתי שהם הבעיה המרכזית אני אומר שיש הדבקה בבלפור נקודה אין מצב של התכנסות של אלפים של אלפים…  ShuliMR שולי תתפללי חזק תתפללי הרבה כי ממני לא תבוא הישועה  Orengerman לא נתתי שום תחמושת לראש הממשלה הוא לא צריך אותי בשביל פרופגנדה יש לו מספיק אנשים שעושים את זה מצוין…  dasides ראיתי נורא זה למה ניסו את תכנית הרמזור וזה לא עבד כי ישראלי לא יכול לראות ישראלי אחר חוגג כשהוא מטר ו…  NoaShpigel ואנשים יוצאים מהבית לים כי הם רוצים להתאוורר ולמשפחה כי הם רוצים לראות את ההורים ולבית הכנסת כי הם רוצ…  Orengerman במצב התחלואה הנוכחי אין מנוס מסגר אומר לך את זה אחד שנפגע מזה קשות שלא קיבל שקל מהמדינה שכועס על ההת…  Orengerman לו היתה הפגנה של חסידי גור ערב ערב ושוטרים היו אמונים על הסדר מניח שגם שם היתה הדבקה וגם אז הייתי מביא את אותה דוגמא koderius ובלי ריחוק koderius רק לא בנטפליקס תן לסיים כמה סדרות ואחכ לא אכפת לי שיגעו גם בסדרות ההודיות JoshBreiner אתה חייב קצת אינסטגרם מדהימה ההתעקשות הזו של מפגיני בלפור לטעון שאין שם הדבקות יש מקום בלי הדבקות יש הדבקות בים בבתי ספר בתי כנסת יש…  ebatman1 איך אני אוהב לחסום אנשים שקוראים לי אפס BokerIris הולך לפינה בתקווה להשתפר gontarzn שמע אני שומע יותר ויותר על אנשים שנחשפו לחולי קורונה ולא קיבלו שום הודעה פשוט החליטו על דעת עצמם להיכנס…  gontarzn הרבה יותר מזה שלא לדבר על זה שכשאתה מפקד אתה נפגש עם יום יום שעה שעה עם שוטרים שהיו בשטח גם הם נדבקו oferjos נמוך זה עדיין מדבק אם סגר אז לכולם דיו אחד לכולם למתפללים למפגינים ולבליינים אם לא בהצלחה לכולנו gontarzn arielplaksin1 בטוח בהרבה אין ספק כשאתה בהופעה ויש פקחים שעוברים בין קהל ומוודאים שאנשים עם מסיכות אז…  debkob1 הפתעתי מה יש פה להפתיע למישהו בכלל יש ספק שנדבקים בבלפור כמו גם בחופי הים בבתי כנסת כמו בכל מקום…  BokerIris לדעתי הוא נדבק מהתקופה ששירתנו יחד בצבא רק היום התחיל לפתח תסמינים HagayN מהטוויטר YasmineGil אמרתי לו לא קיבלת את החיסון של מפגיני בלפור  אמר לי אין לי קשרים תבדוק לי BokerIris לדעתי הוא נדבק מההפגנה של הילדים לפתוח את גני החובה debkob1 כזה אני BokerIris הוא נדבק מביבי בדקתי עכשיו gontarzn יגיע yarivop יריב תביא לנו כבר את החיסון שלכם gontarzn מה אתה טוען פה בעצם שבין המפגינים אין חולים  שבין המפגינים לא חלה הדבקה  הבנאדם עובד 247 בבלפור כמעט…  Ariav אתה יכול לתת לי את החיסון הזה שיש לכם נגד קורונה חייב אותו רק לחגים ומחזיר לך הרגע דיברתי עם קובי יעקובי מפקד תחנת מוריה חבר מהצבא אח נדבק בקורונה סליחה לא נדבק חולה חום חולשה כאבים…  davidhalevi Yossieli לא 8200 ruthelbaz כי לא מצאת חצאית מקסי Yossieli כפרה על קובי חבר שלי מגולני אין כמוהו ruthelbaz בטח בגלל חצאית קצרה מידי AvrahamBoimel ivgiz אפשר גם להרוג אותי בעונה שניה ולהחזיר אותי בפרק האיחוד זה כבר פרק איחוד מושלם AvrahamBoimel ivgiz למה לחכות עד לפרק האיחוד כדי להדיח אותי ivgiz לא אכפת לי גם 10 עונות רק בבקשה בלי פרק איחוד shnaiderman GuyGold3 רק הוא נשאר לנו כרגע GuyGold3 shnaiderman כמו שזה נראה כרגע אפשר בשקט להוסיף ומהשנה הקרובה קלל במשטרה מודים אם המצב יחמיר נאלץ להורות לשוטרים במחסומים גם לעצור מכוניות ולשאול נהגים לאן הם נוסעים ראש הממשלה צלצל לנדבק ה200000 והעניק לו מכשיר הנשמה במתנה KnessetT חכ AyeletShaked תזמנה שעה וחצי מתל אביב לירושלים בתגובה לטענותיה של חכ מyeminaparty על מחסומים מיותרים בכבישים אמר יו… origra92 N12News inbartvizer רק שלא יגייסו אותי ZiatMoshe azironen N12News inbartvizer הלוואי Ariav N12News inbartvizer ברור ZiatMoshe N12News inbartvizer רוב המתים היו חולים קשה רגע לפני מן הסתם N12News inbartvizer נראה לי די הגיוני שחלק מהמתים היו חולים קשה מה שמוריד את מספר החולים ומעלה את מספר המתים RonelAdani moransamun TzurMaor שנה כיוןן TzurMaor מצפה שזה יפתח מהדורה RonelAdani moransamun TzurMaor אז סתם אמא שלה נכנסה לכלא TzurMaor בהמשך נטלי דדון מגלה שהחומצה ההילוארונית שדחפה לשפתיים זו חומצה שבכלל מיועדת לשטיפת רצפות דמוי פורצלן לא שיש ChenSror ורק לי מפריע שהיא כתבה ״יהיה זו אות קלון״ orenankava ברור ItayBlumental shushanavi מטופל קל עד 15 דקות לא ישלם על חנייה ItayBlumental shushanavi משפחות לא היו מוצאות את המאושפזים החולים yesnomabyyes judash0 שלא תדע קבוצות judash0 בקבוצה של הילדים יש את ברבש הבת eladrosenfeld judash0 בכינים judash0 עשו לי את זה קבוצת הגן של הילד עצוב HillelSommer אני הגעתי לשלב שאני מביא להם סירים yossidavidov10 מה לגבי דוחות חנייה ומי ששכח להפעיל פנגו dovikco בושה kaisos1987 המדינה הזאת מאוהבת בפיצוצים ועשן CynicalDe איפה חשבונית אני עם ההורים עובד שנים רק בשחור Jeremlib ראיתי שוטרת משחק ״טום החתול״ Pitzynivly אוסטרו הונגרים PinkPantherIL המחסום הזה ספציפית זה התרעה על חשוד בנסיעה לחוף בית ינאי בלי סירים לראות את השוטרים פרוסים בכל המחסומים דוקרנים על הכביש כאילו עוד רגע יקבלו התרעה על מכונית חשודה של אנשים עם סירים על הברכיים בדרך להורים PBeinish roysharon11 זאת אומרת PBeinish roysharon11 זרת אומרת סאממק PBeinish roysharon11 סאמר התיקון האוטומטי roysharon11 מעניין שההודעה שלך יוצאת בדיוק יומיים אחרי קלמן שלושה אחרי עקיבא ויום לפני יאיר הבן אם תיקח את כל הי…  BarashiKinneret שלא כמו ביבי טועה ותמיד מתנצל אה בעצם maormaz netalishemtov הפוך גוטה אם יש מישהו שדאג ועדיין אכפת לו ממי שנפגע בכל הכאוס הזה זו היא netalishemtov ככה תמיד רציתי שיתחילו איתי ראיון hunyuc netalishemtov לא לא מעבר לתחזיות בהתאם להגבלות לרגעים הוא היה נשמע לי כמו מרים בנימיני shaharamano Thioret תוסיף את הדוגמא האישית שלא קיימת בסביבתו דבר שגרם וגורם לציבור לא להקשיב לו netalishemtov אז תביאו אותי netalishemtov שאשא עושה את עבודתה נאמנה ומייצגת אותך ואותי וכל אחד אחר שואלת שאלות ולרוב לא מקבלת תשובות כי הכל…  Thioret shaharamano לשים את פרופסור לס יחד עם יפעת שאשא ביטון ובנט זה שקר הוא טוען משהו אחר לחלוטין ואני אגב מ…  duduassor אני לא מתלהב מחיבוק של התקשורת זה הוכח כמעט תמיד כרע לחברי הכנסת אבל היא עושה את עבודתה ברבש גם נתן ת…  duduassor קוראים לזה לעשות את העבודה יור ועדת הקורונה שואלת בודקת מקשיבה  ברוסיה היא אמורה לשתוק hebmeme מסכים אם כי זה התבקש הפעם דבר אחד טוב בגל הזה לעומת הגל הקודם אין מחסור בביצים  GLZRadio glicksh למי זה לא קרה HauserTov בתקופה האחרונה עברתי כמו לא מעט להופיע לכל מיני חברות בזום כשהגיעה הצעה להופיע מול אינטל הבנתי שזה לא…  koderius moshenayes zoharm7 או באומן זזה הכי קרוב לאומן</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  swid4 KseniaSvetlova עצוב מאוד תנחומי כמה ההבטחות של netanyahu מופרכות במבט לאחור המציאות לא מתרשמת מההנחיות של ראש הממשלה והציוצים שלו זחוחים ומביכים…  מאות מכוניות בהפגנה בקיסריה   דורניקו זה עוד אחד מכזביו של netanyahu אסור להאמין למילה שיוצאת מפיו אני מכיר את המהלכים לקראת המינוי מוזי סיפר…  RafiMann חיפוש בארכיון בעניין אחר העלה את זה 90 מן הטקסט יכול להיכתב גם כיום  המלצת קריאה תמלילים  מתוך חקירת נתניהו שמפרסם היום גידי וייץ במוסף ״הארץ״ אם ראש הממשלה הנאשם בשוחד יתמיד בגרסה ש…  נתניהו ״המפגינים רק עוזרים לי פוליטית״ להלן מצבו בסקרים והנאצות  41 מנדטים  פוגעים בסמלי המדינה  37 מנדטים …  JoshBreiner הכוונה של נתניהו להביא את הגבלת ההפגנות כתקנה לשעת חירום רק כי הוא לא הצליח עדיין להעביר אותה כחוק בכנסת היא עדות נוספת לכ… בכל זאת הציבור אשם הרי אנחנו בחרנו בנאשם בשוחד ומרמה לראשות הממשלה מה ציפתם שאתכם הוא לא ירמה רמאי הוא רמאי הוא…  אחרי הנאום של netanyahu השתכנעתי סופית שחייבים לפתוח את בתי הכנסת ראש הממשלה הזה לא יציל אתכם אולי השם יעזור נתניהו ״כולם אשמים חוץ ממני צאו לבלות״  מה לעשות עכשיו 🟠 לסגור את כל בתי הכנסת 🟠 לסגור את כל ההפגנות 🟠 לסגור את netanyahu מאחורי סורג ובריח 🟠 אין צורך…  faniaoz ניגפנו פושעי הקורונה לדין זהו אפילו ועדת החקירה מיותרת מי ששלח ילדים למדגרות 25 מהנדבקים בבתי ספר מי שאישר תפילות …  במילה אחת מחדל בשתי מילים בנימין נתניהו  ishmuli אמירה הזויה היקף הבקשות לסיוע במזון בחגים זינקה פי 2 השנה ל12 מיליון בקשות את התקציב הגדלנו פי 3 וזו רק דוגמה אופס השקר נחשף עוד לפני תום השנה  האיום האמיתי על מדינת ישראל לא מגיע מטהרן אלא מהבית ברחוב בלפור בירושלים  MeravMichaeli צער גדול  itamarbz שרשור ארוך אך עמוס תופינים תבדקו אותי  מהו גוף התקשורת שעושה הכי הרבה כסף מפרסום של תעמולה ממשלתית סמויה נתוני אמת שנחשפי… גמר חתימה טובה  סיכום ביניים של הסגר בחג הציבור ברובו המכריע יותר נבון ממנהיגיו ומתנהל הרבה יותר בחכמה מממשלתו המטומטמת Ayeletnnv שנה טובה מקסימים RoyIddan  הבחירה כעת היא בין חיים למוות לא בין ימין ושמאל נתניהו וממשלתו הכושלת הפקירו אותנו במחדליהם האיומים לגורלנו אנחנ…  Eladingo זה בלתי נתפס זה אלי זעירא מתראיין עם אשתו בלבוש חג בגליון ה 9101973 על המלחמה הקשה בחזית מדהים  subtext100 faniaoz  ברור שnetanyahu לא מסוגל לנהל את המשבר הזה פשוט גדול עליו הוא מדינאי  לא מנהל לא איש עשייה הכי טוב למדינת ישר…  שנה טובה שנאמין היום בפרוייקט הציוני כמו שהאמינו אז כסבא שלי ואחרים בנו את הנמל בת״א  ובצדק מזל טוב יקירה שנה טובה בריאות טובה בשורות טובות וציוצים שהופכים את הבטן  שאלת הדיוט אם כולם משוכנעים שהסגר לא יעיל  למה לא מודיעים על ביטולו והחלפתו באיסור התקהלות של מעל 10 אנשים ונתניהו הוא לגמרי לא כשיר התדרדר כל כך עד שהוא בניגוד עניינים עם עצמו  Haaretz ך צודק  הודעת אחרונה בהחלט ממזכיר הממשלה ההחלטה היא לא להחליט בעניין הסגר עד שתיכנס לתוקף החלטה אחרת שתחליט מה שיחליטו הפוליטיקה הישראלית פשטה את הרגל הסקטוריאליות ניצחה את הממלכתיות והזלזול בתהליך קבלת החלטות הרס את אמון הציבור יהי…  talibo8 שר הבריאות מעז לדבר על הציבור שלא ציית כמה חצוף הוא יכול להיות בכל מקום נורמלי הוא היה מחזיר את המפתחות ומתפטרYuliEdelstein  השלום מדבק  השלום עם המפרציות חשוב מאוד בפני עצמו  אבל הוא חשוב שבעתיים בגלל ההבטחה שנתן netanyahu להקמת מדינה פלשתינית חבל…  limormoyal EmilieMoatti שתיכנן  33 וכמובן אודי אנג’ל הוא עד מטעם התביעה במשפט  netanyahu  ואני שואל איפה amitsegal כשיש דיון על ניגוד עניינים בפרקליטות 22 נתניהו יודע שצריך בקרוב מאוד לקבל החלטות בקשר למכרז של הפקת אשלג בים המלח המכרז אמנם יתקיים  סמוך לסיום העשור…  12 שאנחנו צועקים ״הוןשלטוןעולם תחתון״ אנחנו מתכוונים בדיוק לזה ראש הממשלה התכוון לטוס לארצות הברית במטוס פרטי ה…  איך הציונים בתעודה עוד לא בדקתם עם הילדים תברכו אותם על סיום שנת הלימודים שבת שלום    yayafink YoavKisch כדי שnetanyahu יוכל לנסוע להצטלם בוושינגטון ולחזור סגר הוא דבר נורא גם שחיתות היא דבר נורא מדינת ישראל לא מצליחה להתמודד עם מפירי הכלללים בעיקר במגזר החרדי והערבי …  TomerNaor בואו נצא למסע נוסף בעקבות יצירת תודעה כוזבת מוכנות ומוכנים לפני שעתיים מפרסם עמית סגל את הציוץ הזה שמספר שמנדלבליט מקיים… zionnenko ראש ממשלה שעסוק רק בענייניו האישיים המשפטיים ולא מצליח לנהל את המשבר הגדול ביותר מאז מלחמת יום כיפור צריך לצאת לנבצרות עכשי… אומר זאת כך יונית הסרחון במח״ש איום ונורא בלי קשר  ואולי עם  התיק של amitsegal נסגר אבל הוא בסך הכל המיקרופון  אם המספרים מצביעים על מחדל וההנהגה חסרת אונים מול המחדל  ואין תכנית להתמודד עם המחדל זה מחדל 2020  כל ישראלית…  Urieldenn מגלגל עינים עמית הוא מדווח תחת הכותרת החשד לטיוח חקירות נתניהו  ואין בדל הוכחה לטיוח Urieldenn  22 זכותו של סגל לחשוב שתפרו תיק לביבי אבל בשביל לבטל משפט או לסגור תיק צריך הוכחות והוכחות אין סגל רמז בדיווחיו…  12 בשפה המקצועית קוראים לזה אינאונדו הצגה של דברים בדרך של רמיזה והוספת פרשנות שמצוצה מהאצבע וזה בדיוק מה שעושה…  מזל שהמשפט של netanyahu יתנהל בבית משפט בפני שופטים ולא בכיכר העיר בפני בית הדין של טוויטר acrionline סמי מיכאל נשיא האגודה  לנוכח המשבר הבריאותי הכלכלי והמוסרי הפוקד את החברה הישראלית אנו באגודה זקוקים לתמיכה במאבקנו למ… תכירו האיש שלא לקח מעולם אחריות  aviadglickman baruchikra עזוב תבקש ישר חנינה אסטרטגית יציאה לקראת הכניסה  arik3000 דיקטטורה אאוצ׳  amitbentzur תודה יקירי OmerLubi תודה  guylerer תודה גיא אתה מגזים ובכל זאת  Syechimovich תודה שלי  RavivDrucker  LeviYonit  DanyCushmaro  Syechimovich  KerenMarc היום קפצה התזכורת הזו מלפני 12 שנים תמונות מהקרנת הבכורה של ״שיטת השקשוקה״ בסינמטק בתלאביב מאוד מטריד שהאליטה הת…  נתניהו אעמוד איתן מול הלחץ החרדי למנוע את הסגר כמו שמנעתי מאיחוד האמירויות מטוסי F35 ובדיוק כמו שעצרתי את מכירת הצוללות הגרמניות למצרים עכשיו ברצינות ברור לכם שהבריאות שלכם והחיים שלכם שווים בעיני netanyahu פחות מהמשך שלטונו  השפןימין חזק שוב ברח Shiritc פרויקטור הקורונה נשלח לוועדת חוקה הבוקא ובמשך ארבע שעות מנסה להגן על הסגר הצפוי שאושר כבר על ידי הממשלה ונתניהו  שעתיים אחר כ…  עמוד שער מצויין  הלוואי שמשטרת ישראל היתה ״מתנפלת״ ככה על חקירת השחיתות של netanyahu בפרשת הצוללות האמיתיות היס״מ חכמים רק על צולל…  פורח החצב ועולה ליד ביתנו השנה הבאה תהיה טובה מהחולפת  AmirHaskel כל מי שחרד לעתידה של הדמוקרטיה הישראלית נקרא להגיע הערב לכיכר פריז בירושלים  shiramakin חמישי 1050 מיקי זוהר מאשים את המפגינים בהפצת הקורונה חמישי 2043 יאיר נתניהו מאשים את השבכ בהסתרת ״נתוני ההדבקה בהפגנו… זה שבת שלום תמורת שלום או שוב רימית  מתגעגע ל״מסיבות העיתונאים״ של netanyahu  אומרים שהוא ישוב לתת כשנגיע ל4000 שבת שלום Irisleal15  יגון קודר שאלה בלוגיקה האם שקרן שמשקר אומר אמת או שהתוצאה היא שוב שקר התשובה 100 אלף במוצש בבלפור  RazShechnik נציב קבילות החיילים בצה״ל פתח בהליך בירור בגל״צ בעקבות מכתב אנונימי ובו תלונות חיילים בתחנה נגד ראש חטיבת החדשות אמיר איב… הוןשלטון ובעיקר כישלון  משטרה פוליטית מטורף  ZmanIsrael אנחנו שופטים את מנהיגינו עפי מוצא פיהם במקום עפי מה שיוצא תחת ידיהם גנץ אמר שלא יילך עם ביבי ועשה הפוך נתניהו הבטיח ס… איך לבחור לך פוליטיקאי  דרך zmanisrael שיתוק לאומי שניהם הביתה  rutirutiiii תבור  22 מי שחושב שבאמצעות כריתת בריתות עם מדינות ערביות ניתן לדלג על הבעיה הפלשתינית טועה ומטעה או שנפרד מהם בהסכם או…  12 אני מפרגן לראש הממשלה netanyahu על ההסכם עם איחוד האמירויות טובים סיכוני השלום מסיכוני המלחמה בלי קשר  האמי…  תעודת 100 ימים של הממשלה 🟡 הטיפול בקורונה  נכשל 🟡 המצב הכלכלי  נכשל 🟡 מערכת החינוך  בלתי מספיק 🟢 יוזמות שלום …  טיטאניק הקפטן עסוק בהישרדותו הצוות המקצועי נוטש את הספינה והנוסעים הסמויים השתלטו על הפיקוד  כל צמרת האוצר עוזבת או מושתקת אחרי החשב הכללי גם הממונה על התקציבים מדובר בסכנה אמיתית לכלכלת ישראל לא תמיד הדרג…  33 בסך הכל ההפסד המצטבר של העתון בעשור האחרון היה למעלה ממיליארד שקל  החינמון המכונה גם ״ביביתון״ מהווה שופר לעמ…  23 ההפסדים של העשור האחרון שולמו במלואם על ידי המיליארדר אדלסון  לחינמון ״ישראל היום״ יש הכנסות ממודעות והוא אף מ…  13 המיליארדר האמריקני שלדון אדלסון הזרים בעשור האחרון למעלה ממיליארד שקל כדי לקדם את netanyahu   לידי הגיעו נתונ…  מיליארדר אמריקני הזרים בעשור האחרון למעלה ממיליארד שקל לקדם את netanyahu  פרטים בקרוב הנאשם netanyahu ישיב  RinoZror בהצלחה חביבי  Irisleal15 ההפגנות נגד נתניהו יצליחו מעגלי המצטרפים יגדלו גם מצביעי הימין יגיעו ברגע מסויים תווצר מסה קריטית והשלטון שלו לא יהיה לג… NuritKoren תודה נורית אני מאוד נרגש שבת שלום UriahCanaff אופס  אולי זה ישמע מוזר  אבל לדעתי צריך להנהיג פה בדיקה נפשית של ראש הממשלה אחת לשנה מנהיג שחלילה יוצא מדעתו מאבד את ה…  itayr2  רגעים מופלאים תודה  kannnews hadover1 shemeshmicha בריאות שלמה ofracarmi1  תודה יקרה GlickmanPaz Shiritc בדרך כלל האמת והעובדות אין שום דיון עיתונאית מצויינת ואין בעיה עם העובדה שיש לה דיעות מגובשות גם אין בעיה עם כתבים בעלי דיעות ימניות הב…  Shiritc בהצלחה sharonkarni תודה שרון יקרה  YossiYonah תודה יוסי  talibo8 תודה טלי  guymeroz תודה רבה חבר הציפיות שלי ממנו הוא כמו ההסכם עם ילדי תהיו מאושרים ואני אדאג לכל השאר 🤨 GilliParann שערוריית שיפוט nissimdouek תודה יקירי  רק בשורות טובות Ohsolomio2 רון subtext100 זהו פורש בשיא miki1650 תודה רבהרבה  ryabetz1 liorchorev רודף בצע liorchorev תודה רבה חביבי תביא לי מתנה את סילוקו של השקרן ShuliMR תודה רבה שולי רק בשורות טובות ושמחות Mickeygitzin תודה מיקי  אפ36 אפ37  MICHELLELITTAUE תודה רבהרבה  smadarp תודה רבה סמדר בשורות טובות ושמחות  ramivered תודה רבה רמי  shaquedmorag תודה רבה יקרה  yanivba7 תודה רבה יניב שמחות ובשורות טובות בהצלחה בשנת הלימודים החדשה Eyalo365 Syechimovich תודה רבה נראה לי שאקים קבוצת תמיכה עלפי מספר הפונים בסוגייה  MKmeircohen תודה רבה מאיר בשורות טובות ושמחות sabbabale בקרוב AmitTali ברכות טלי איזה כיף המון נחת drAnatBerko תודה רבה ענת אני מאוד נרגש tamarzandberg תודה רבה תמר אושר גדול baruchikra תודה ברוכי  שמחות ובשורות טובות francescabraun1 תודה רבה יקרה  Syechimovich תודה יקרה  אני מתקשר לבן ולבת שלך 🥴 Irisleal15 תודה מקרב לב איריס  רק שמחות ובשורות טובות Ayeletnnv תודה איילת אהובה רק שמחות ובשורות טובות MikiMiki1949 תודה רבה חביבי כך שמעתי  PolakR10 תודה חביבי OrlyAzoulay תודה אורלי אהובה  AviAmit26 דווח בהזדמנות gideonallon תודה גדעון  רק בשורות טובות TomerMichelzon תודה תומר ykarniel תודה רבה יובל AviAmit26 תודה אבי יקירי  מה שלומך עוקב בדאגה אחרי קורותיך yayafink תודה יקר שלי  בשורות טובות mgenelevi תודה רבה רבה MKMickeyLevy תודה חבר רק בשורות טובות eransinger תודה רבה יקירי בהזדמנות זו  הסדרה על השפה הערבית חשובה ומעניינת מאוד  oizreel  ItaiVered תודה איתי  mreshef1  ybhlashon תודה רבה  AmirP77 תודה  dinadayan תודה דינה יקרה מבטיח לדווח בהמשך  רק בשורות טובות giladmeir חן חן  תודה limormoyal תודה מקרב לב לא חושב שהעוגה המשמחת תקהה את שיני  mkorlyfroman תודה אורלי  hkim14050017 תודה חני רק בשורות טובות yigal1957 תודה מקרב לב KElharrar תודה קארין  amitbentzur תודה עמית subtext100 כל העניין הזה של הפתעה ידועה מראש מצריך באמת בירור מעמיק נולד לי נכד  אני לא מאמין שהפכתי לסבא אני סבא בטח קשירת קשר להפיל אותי RinoZror מחכה לספר בהצלחה הבחור סובל מדמנציה או שזה הלא היה כלום החדש  schatzah סנצ גוואטה מכה שנית סרטון חדש חושף שגוואטה חזר לתקוף העצור בשנית אחרי שכבר נעצר ובנוסף תוקף צלם  מה שהכי עצוב הוא שזה כבר לא משנה אם מכריזים על בחירות או עניין הבחירות נדחה יש אדם אחד שנמלט מאימת הדין ונאחז בקרנ…  השקרן שאמש אמר שהוא לא מתערב במינוי פרקליט המדינה אוחז היום במינוי הזה בדיוק כאמצעי סחיטה אירגון פשע השתלט על בלפור אחרי כל הבדיקות שיקלול היתרונות והחסרונות  יש לנו ממשלת שיתוק לאומי היינו יכולים לשים עציץ בראשה ולהציב אדניות ס…  ימין חזק   אירגון פשע ממשיך לשלוט בממשלת ישראל החלו התשדיר של הליכוד לכבוד חגי תשרי השופרות הגבירו את הפצת הדיבה והספינים אסור להתפשר עם אירגון הפשע של בלפור ועם העלילות שהוא מפיץ באמ…  ״רק ביבי״  ממתין בציפיה דרוכה    שרשור חשוב בבלפור מתנהל אירגון פשע  זה ידוע לאירגון יש פלנגות של פעילי מקלדת המתחזים לעיתונאים המפיצים חצאי אמית…  almogychen1 JDNsg6sw0Hamed4 שבת שלום גם לך EmilieMoatti חברים אנחנו צריכים להביו שהרגע שבו נפלת לפה של שופרות הבלאי ושחייני הביוב מבלפור הוא רגע של גבורה לא של שפל נגמרו הימי… ShaiCohen13 תודה חביבי שבת שלום פורסם כעת  כלומר פורסם ב2017 אתה עיתונאי  כמו שאני חבר ליכוד  אני מתעב את הצבועים ומגלגלי העיניים לשמים שמצד אחד מצפצפים על החוק קוראים שלא לקיים את החלטות בית המשפט יושבים עם…  תראו ציפור  אפילו הרעיון למנות את האיש המושחת הזה פגום בעיני  פה קבור הכלב פה קבור הכלב זהו עצם העניין לא זה העצם של הכלב אבל הכלב מת מזמן טוב זה עצם העניין  2017 netanyahu מכחיש שאישר לגרמניה למכור צוללות למצרים 2019 ביבי מודה שאישר מכירת צוללות למצרים 2020 נתניהו מכח…  נתניהו לא מדובר בחמקנים אלא בחמגשים  MaximovNatan amitsegal RavivDrucker לפי עיתונאיי וצייצניי הימין אני חריגת בניה עצומה  בפועל ובמציאות מעולם לא… </t>
-  </si>
-  <si>
-    <t>מאז ומתמיד אני מכבד כל אדם באשר הוא אם לא הובנתי התייחסתי לכך שמוקדי ההתפרצות לפני שבועיים היו בערים מסויימות וכע…  אני מברך על החלטת ארגוני המחאה שלא לצאת להפגין במהלך סוף השבוע מול בלפור וקורא לציבור כולו הישמעו להנחיות הישארו…  עלינו למגר את המגפה שגובה מחיר כבד מאזרחי ישראל תוך שמירה על דמותה של המדינה שלנו עלינו להציל חיים ולהחיות מחדש…  זו תקופה לא פשוטה לאף אחד מאיתנו בפעם השנייה אנחנו נאלצים להיכנס לסגר הפעם אפילו מהודק עוד יותר נתוני התחלואה לא…  לא נאפשר להפעיל תקנות שעת חירום למניעת הפגנות או תפילות זו תהיה דריסה של הדמוקרטיה  כחול לבן תפעל להשלים את החקיק…  מביש לראות שגם הערב נתניהו בוחר להמשיך להסית נגד המפגינים כחול לבן מנהיגה קו אחראי של סולידריות חברתית ונתניהו ממש…  Kachollavan19 כחול לבן התנגדה נחרצות לניסיונו הפסול של השר אוחנה לכפות השתתפות יועץ משפטי חיצוני בקבינט הקורונה ולהפיץ חוות דעת חלופית… אנחנו מחוייבים לעשות ככל שניתן כדי להבטיח שנפגעי הקורונה הכלכלית יוכלו להתקיים בכבוד המתווה המיוחד שהצגנו הנשיא ו…  אני מברך על החלטת בית המשפט וההכרזה על מלכה לייפר בת הסגרה לאחר שנים של ייסורים יזכו סוף סוף נפגעות העבירה לעשיית…  בפתח השנה החדשה סיירתי היום בין יחידות משרד המשפטים כדי להודות לעובדות ולעובדים על עבודתם המסורה למען הציבור   עו…  תראו לי רודנות אחת שבה קיימת מערכת משפט חזקה ההבדל בין המדינות שבהן יש זכויות על הנייר לבין מדינות שבהן יש זכויות…  הסכמי השלום הם ציון דרך היסטורי ברכות לעם ישראל ולאזרחי איחוד האמירויות ובחריין   עלינו להמשיך ולחתור לפיוס עם כל…  הוועדה לבחירת שופטים בראשותי התכנסה היום לישיבתה הראשונה השופטות והשופטים יבחרו על בסיס ניסיונם כישוריהם ומקצועיו…  המהלך ישפר משמעותית את השירות לאזרח ייעל את המערכת ויפחית מהעומס המוטל כיום על בגץ ועל בית המשפט המחוזי לעניינים…  בדומה למדינות אירופה כמו גרמניה וצרפת גם בישראל תהיה מערכת נפרדת של בתי דין מנהליים בעלת שלוש ערכאות כך יושלם המ…  רפורמה נוספת יוצאת לדרך הפצתי היום טיוטת חוק להקמת ערכאה שיפוטית חדשה בישראל  בתי משפט שלום לעניינים מינהליים…  במקביל עלינו להבטיח שלצד הבדיקה המערכתית יוכלו מפוני הכפר לשקם את חייהם באופן מיטבי לכן יחד עם השר amirperetz…  הבדיקה המקצועית תסייע לחזק את המערכת ואת אמון הציבור בה אבל אסור להתבלבל כל ניסיון לקשור את האירוע הטראגי באום אל…  הדיווחים בעניין מקרה אום אלחיראן עוררו שאלות בנוגע להתנהלות הפרקליטות ומח״ש בקשר לאל קיעאן ז״ל והעלו סוגיה חברתית…  בתקופה שבה שלטון החוק נתון תחת מתקפה נטולת רסן שכל מטרתה לייצר דהלגיטימציה לשומרי הסף עלינו לבור את המוץ מן התבן…  הניסיונות המכוערים לקחת את המשטרה הפרקליטים והשופטים ולהפוך אותם לנחקרים לא יצליחו   לא סתם התעקשנו על תיק המשפטי…  משרד המשפטים מחוייב למימוש זכויותיו של כל אזרח גם כשמדובר בנאשמים ובעצורים דלי אמצעים פרקליטי הסניגוריה הציבורית…  ומצטרפות לקריאות  מסיתות נוספות  שיש לחקור את השופטים את החוקרים את היועמ״ש ועוד ועוד לכל אלה מטרה אחת  ריסוק…  המערכת מחויבת לבדוק את עצמה כל הזמן לתחקר לתקן ולהשיב באופן ענייני על כל ביקורת וכך ייעשה   הדיווח אמש בחדשות 1…  כשר המשפטים של אזרחי ישראל אמשיך לדאוג ששומרי הסף יפעלו באופן עצמאי לא תהיה פוליטיזציה של מינויים שיקולים זרים ל…  אמרתי הערב בוועידת המשפט התשיעית   הנסיונות לקדם חוקי התגברות על בגץ לא מבקשים לחזק את תשתית הבלמים והאיזונים…  כמו בכל תחומי העיסוק גם בספורט אנו מחויבים להיאבק למיגור הטרדות מיניות יחד עם השר חילי טרופר החלטנו לאמץ את המלצת…  תלמידי ישראל שנת לימודים פוריה ומוצלחת  אנחנו מתמודדים עם פתיחת שנה מאתגרת במערכת החינוך השמעו למורים ולהנחיות מ…  החובה החלה על פושט רגל לשלם את חובותיו לא יכולה לפגוע בזכות היסודית למחיה בכבוד הצוות שהקמתי היום יחד עם שר העבודה…  שאול מרידור הוא איש מקצוע מצויין הגם שלא תמיד ראינו עין בעין הכרתי תמיד בערכו ובמחויבותו לציבור מרידור תרם תרומ…  לכן בכוונתי לפנות ליועץ המשפטי לממשלה ולבקש ממנו לשקול הגשת בקשה לדיון נוסף כמובן שיש לכבד כל הכרעה של בית המשפט…  החלטת בג״ץ מאמצת לראשונה את עקרון הסדר תקנת השוק ששימוש בו יאפשר הסדרה של מאות רבות של בתים באיו״ש אני מברך על כך…  הרצח הנתעב של הרב שי אוחיון שהותיר אחריו אישה וארבע בנות צעירות פשוט שובר את הלב   אני רוצה לשלוח תנחומים למשפחתו…  נתניהו התבלבלת המסע המתוזמן של הסתה ושקרים לא ירתיע אותי אני אמשיך לשמור על שלטון החוק ועל הדמוקרטיה הישראלית…  JusticeGov המחלקה לחקירות שוטרים פתחה בחקירת המקרה שתועד אמש בהפגנה בירושלים של תקיפת מפגינים עי קצין משטרה בדרגת סנצ הבדיקה נפתחה… לכל מי שמנסה להפיץ שקרים מופרכים ולהמציא פרשה לא תרתיעו אותי לרגע מהגנה על שלטון החוק  עלובי נפש המתקפות שלכם רק מחזקות אותי gantzbe אנחנו לא אנשים של משחקים ותרגילים אנחנו אנשים של כבוד ותקווה  עבודה קשה יושר וערכים נפגשנו הבוקר כל כחול לבן להתרכז שוב… כך נמגר את התופעה המזעזעת של התעללות בפעוטות  החמרת הענישה  עונש מינימום של מאסר בפועל על מתעללים החקיקה בעיצומה…  האונס המזעזע באילת בלתי נתפס לקרוא את העדויות ולא להאמין כמה עמוק הוא השפל המוסרי  המדינה חייבת להעניק את כל התמי…  יחד עם השמירה על מערכות החוק והצדק חלה עלינו החובה לדאוג לריסון הכוח השלטוני אל מול האזרח   הצגתי היום שורה של צע…  לא יוטלו הגבלות נוספות על המסעדות  אני מברך את שר הבריאות YuliEdelstein ואת הפרויקטור פרופ רוני גמזו על שקיבלו א…  לפני מספר שבועות נפגשתי עם פרופ רות גביזון מהמרשימות והמשפיעות בתחום המשפט והחברה בישראל עם כניסתי לתפקיד זכיתי…  שמירה על שלטון החוק ועל שפיות מדינית בהחלט מחיר ששווה לשלם  שבת שלום  מהלכים מוצלחים עושים במשא ומתן ישיר בין שני הצדדים אני מברך על ההסכם החשוב עם איחוד האמירויות ועל ההימנעות מסיפוח…  נאבקים בתופעת ההתעללות בפעוטות יחד עם ishmuli הבאנו בשורה חשובה שתחזק את ההרתעה ותחמיר את הענישה נגד מי שפוגע ביק…  אני מברך על החלטת הפרקליטות לאשר למשטרה לפתוח בחקירה בעקבות התבטאויותיו של יונה אברושמי   אם היו חסרות נורות אזהרה…  ועדת השרים לחקיקה לא תתכנס היום  סיכמנו כי בשלב זה יקודמו בוועדה רק חוקים הנוגעים לקורונה אבל לצערי בליכוד מסרבים…  על ההגנה על שלטון החוק בתקופה שהדמוקרטיה שלנו שברירית מתמיד על זכות ההפגנה ועל שמירה על עצמאות הכנסת ובתי המשפט…  הדגשתי בפני כבוד השייח מוואפק טריף את המחוייבות שלנו לקידום חקיקה שתעגן את עקרון השיוויון עבור כל אזרח בישראל יוצא מסיור חשוב בבית הדין הדרוזי בעכו ובבית העדה הדרוזית בגוליס יחד עם alonschustermk  בקרוב אכריז על מתווה בנו…  הכנסת הצביעה היום ברוב מוחץ בעד הדמוקרטיה ונגד הנסיון להחליש את האזרח מול כוחו של השלטון  בעיצומו של משבר לאומי צר…  המפגינים מייצגים ציבור גדול מאוד זה לא מיעוט הזוי זה עם ישראל שמודאג שאכפת לו מהמדינה שלו   בתקופה הקשה הזו כש…  מה קרה לנאום לא פרנסה  לא מעניין נפתלי איילת אין דבר שמעניין אתכם יותר מלרמוס את שלטון החוק והדמוקרטיה לא יקרה شرفني ان أزور بلدة كفر قرع بمناسبة عيد الأضحى المبارك  أتيت إليكم مع رسالة المساواة لكل سكان اسرائيل بيد واحدة، م…  תודה גדולה לדר איאד זאחלקה מנהל בתי הדין השרעיים על האירוח הנפלא לנשיא בין הדין השרעי הקאדי עבד אלחכים סמארה ו…  לכבוד הוא לי להתארח בכפר קרע לרגל חג הקורבן   יחד עם צאת תשעה באב הערב מתחזק המסר החשוב של אחדות ושותפות הגורל בי…  גם אני הורדתי את אפליקציית מגן 20 ככל שנחזק את השימוש בטכנולוגיה אזרחית במאבק בקורונה יופחת הצורך באיכוני גופי ה…  אלו שתקפו את המפגינים אתמול  הם האנרכיסטים האמיתיים בחוק המענקים הבאנו גם בשורה חשובה וצודקת למען ציבור הנכים הדיסריגארד לזכאים לקצבת נכות יעלה לא תהיה כל הפחתה מסכו…  נפגשתי היום עם ראשי המטה החברתי להשבת הבנים מור חאייק וגולן פרחי השבתם של הלוחמים סמ״ר אורון שאול וסגן הדר גולדין…  בחוק הקורונה עמדנו על כך שזכות ההפגנה לא תיפגע כך פועלת דמוקרטיה חזקה בשעת חירום    כל ניסיון לעקם את ההחלטה הזו…  שיתוף פעולה אכן בנוי על אמון לכן תמוהה החלטת הליכוד להפר משמעת קואליציונית לטובת פגיעה בשלטון החוק וחקירת שופטים…  הממשלה תעביר היום 15 מיליון שח לטובת תנועות הנוער נמשיך לפעול כדי שתועבר אליהם יתרת התקציב הנדרשת לפעילותם התקינה הערכית והחשובה אף אדם לא זקוק להמרה סטרייטים ולהטבים אתם טובים בדיוק כפי שאתם ‍ רק לעשות סדר כחול לבן ואני דאגנו שחוק הקורונה הגדול לא יפגע בעצמאות הכנסת בבתי המשפט ובזכויות האזרח הבסיסיות כל…  כדאי לזכור למה שמסוקר היום כבלאגן בין הממשלה לכנסת קוראים הפרדת רשויות  ועדת הקורונה מוסמכת לבטל החלטות מסיבה…  ביקורת היא לגיטימית אבל ההתלהמות נגד משרתי ציבור חייבת להיפסק   בימים האחרונים ראינו מופעי השתלחות ברז ניזנרי לי…  בעקבות דרישת כחול לבן המדינה תעביר סיוע ישיר לאזרחים אבל בתוכנית דיפרנציאלית עם רגישות חברתית חצי מיליארד שקלים…  תודה לcohenmeirav ishmuli KerenBarak omeryankelevitc YSegalovitz עשינו היום עוד צעד חשוב למאבק באלימות נגד נשים אישרנו כעת בוועדת השרים את החוק שקידמתי ויסדיר לראשונה בדין הישראלי…  מענק כספי שיגיע ישירות לציבור הוא צעד נכון להנעת גלגלי המשק אבל לא נחלק מענק עיוור נתמוך בתוכנית סיוע דיפרנציאלית…  פרסמנו היום את התקנות לחוק איסור צריכת זנות כדי לאפשר אכיפה מדורגת ומאוזנת התקנות יאפשרו להמיר את הקנס בסדנה חינוכ…   בפעם הראשונה יתכנס היום הצוות הבין משרדי שהקמתי לגיבוש הרפורמה בקנאביס   הצוות יבחן בשבועות הקרובים את כלל השיקולי…  חתמתי עכשיו על תקנות סדר הדין האזרחי החדשות לראשונה מאז 1963 אנו מביאים רפורמה מקיפה בתשתית ניהול המשפט האזרחי ביש…  Kachollavan19 נוכח חשיבות תפקודה של הכנסת כגוף מפקח אין זה ראוי להדיח את יו״ר ועדת הקורונה יפעת שאשא ביטון   אם הליכוד יקדם הצבעה בנ… פניתי לשר האוצר Israelkatz כדי שתוכנית הסיוע תכלול גם העלאה של הדיסריגרד לאנשים עם מוגבלויות סיכמנו שלא תהיה כל…  נשים אינן סחורה ומעכשיו צריכת זנות היא עבירה פלילית   שתפו את קמפיין משרד המשפטים  המפגינים מביעים מצוקה אמיתית וצודקת   חבילת הסיוע היא צעד בכיוון הנכון אך עלינו להציג תקציב שיביא ודאות כלכלית ומ…  אני רוצה לברך את חברות וחברי הכנסת מכל קצוות הקשת הפוליטית על חקיקה חשובה זו ליו״ר מרצ לשעבר זהבה גלאון לשרת המשפ…  נשים אינן סחורה וגופן לא מיועד להשכרה לכל המרבה במחיר   למרות הלחצים לא הסכמתי לדחות את החלתו של החוק לאיסור צריכ…  נפגשתי היום עם שגריר האיחוד האירופי בישראל מר עמנואל גופרה דיברנו על שיתוף הפעולה המשפטי הפורה בין ישראל למדינות…  gantzbe נלחמים בקורונה שומרים על הדמוקרטיה  גאה בAviNissenkorn  שר המשפטים של מדינת ישראל  כל עוד אני שר המשפטים שלטון החוק לא ייפגע ומערכת המשפט תפעל בעצמאות מלאה למען כל אזרח במדינת ישראל נקודה יש בישראל מיליון מובטלים ובכל יום מאובחנים יותר מאלף חולים חדשים בקורונה ויש מי שהכי דחוף לו עכשיו זה לחרב את שלטו…  נפגשתי היום עם השייח׳ מוואפק טריף המנהיג הרוחני של העדה הדרוזית בישראל ונשיא בית הדין הדרוזי לערעורים שוחחנו על ד…  גם בזמן משבר הקורונה כנסת ישראל ובתי המשפט ימשיכו לפעול   בשגרה ועל אחת כמה וכמה בשעת חירום מוסדות הדמוקרטיה חי…  זו בשורה ענקית שתחזק את הנגב ותצמצם פערים בין המרכז לפריפריה זה מהלך אסטרטגי חשוב עבור מערכת הבטחון  קיבלנו עכשיו בישיבת הממשלה מספר החלטות קשות בנוגע להגבלת הפעילות במשק אלו צעדים הכרחיים למאבק בנתוני התחלואה במקב…  כל עוד אני שר המשפטים שומרי הסף ומערכות שלטון החוק יפעלו בעצמאות מלאה  אתמול ב pgoshMTP  מוטלת עלינו האחריות לשמור על בריאות הציבור מבלי לקחת את הכלכלה חזרה לאחור בדיוק בשביל זה ולמען שמירה על שלטון הח…  I expressed to him my firm commitment to ensuring that the Malka Leifer case would be handled expeditiously In add…  I had the pleasure of meeting today with Australias Ambassador to Israel Mr Chris Cannan We discussed matters of…  נפגשתי היום עם שגריר אוסטרליה בישראל כריס קאנן AusAmbIsrael דיברנו על הקשר החזק בין המדינות ועל שיתוף הפעולה המשפ…  השוויון הוא עמוד תווך בדמוקרטיה והזכות להורות חייבת להיות שוויונית ללא הבדל דת גזע מגדר ונטייה מינית כדי לסיים א…  מנדלבליט לא רודף אף אחד הוא מבצע את תפקידו מתקפה על שומרי הסף פוגעת בדמוקרטיה והחלשת הדמוקרטיה תפגע בזכויות של כל אזרח במדינת ישראל חוק איסור צריכת זנות ייכנס לתוקף במועדו 10 ביולי אני מודע לחששות ולקשיים ניישם את הפתרונות הנדרשים לטובת שיקום…  הגעתי הערב לאירוע הגאווה בירושלים מאבק הקהילה הלהטבית הוא מהחשובים והמוצדקים זה מאבק מהותי על שוויון חירות סוב…  יוצא מפגישה חשובה עם נציגות איגוד מרכזי הסיוע לנפגעות תקיפה מינית  אי אפשר להפריז בחשיבות המאבק באלימות המינית מא…  נתוני התעסוקה המדאיגים שיצר משבר הקורונה מחייבים אותנו לסייע לאלו שמתקשים לחזור למעגל העבודה אני מברך את…  חופש הביטוי והזכות להפגין הן אבני יסוד בדמוקרטיה שאין להגבילן אלא במקרי קיצון אני מברך על החלטת בית המשפט לשחרר את…  המתקפה על אמנון אברמוביץ׳ מקבל צל״ש הרמטכ״ל היא ביזוי חופש העיתונות ותמרור אדום לכולנו הבוקר קיימתי בלשכתי פגישת עבודה ראשונה עם נציגים מארגוני הלהט״ב יחד עם EitanGinzburg   אמרתי לנציגי הארגונים ואנ…  אני מברך את הרשות השופטת על צעד חשוב לקידום השקיפות זוהי עדות נוספת לכך שהתברכנו במערכת משפט איכותית ומקצועית  הנחיתי את הנהלת משרד המשפטים ואת הנהלת בתי המשפט לדאוג כי 5 אחוז מכלל העובדים יהיו אנשים עם מוגבלות  אנשים עם מוגב…  המתקפה המתמשכת על מערכת המשפט מסוכנת  ומסכנת את חוסנה של מדינת ישראל יש שופטים בירושלים והם ימשיכו לבצע את עבודתם…  הבעייתיות בחוק ההסדרה היתה ידועה לממשלת ישראל כבר מהרגע הראשון ופסילתו היתה צפויה לכל הגורמים במערכת הפוליטית  הכר…  סיימנו הבוקר את סבב התיקונים על טיוטת חוק שעת החירום  נלחמים בקורונה שומרים על הדמוקרטיה  לרשויות ינתנו הכלים לאכוף את ההנחיות אולם שוטרים לא יתפרצו באופן שרירותי לבתי תושבים  בימים הקרובים נמשיך בעבודה מ…  החקיקה בנושא הקורונה הכרחית אבל זכויות הפרט ימשיכו להיות נר לרגלנו גם בעת חרום  יחד עם אנשי משרד המשפטים ושותפיי ב…  ערב חג השבועות אני בוחר להתמקד ברעיון החסד והנתינה לזולת השזורים במגילת רות כי גם זו אפשרות חג שמח לראש הממשלה עומדת חזקת החפות ואני מאחל לו שיוכיח אותה בבית המשפט   התברכנו במערכת משפט איכותית וללא משוא פנים אין…  אני שב ומבהיר יש לי אמון מלא ביועץ המשפטי לממשלה שרי ממשלה רשאים להביע ביקורת עניינית אבל מתקפות נטולות רסן הן חציית קו אדום gantzbe עדכון קצר ממני אליכם 1 החל מהחודש חברי הכנסת של כחול לבן יתרמו 20 משכרם  2 עם הקמת הממשלה נפעל מול גורמי המקצוע כדי להור… הישראלים לפני הכל בעקבות השיח שניהלתי בתקופה האחרונה עם הממונה על שוק ההון והביטוח ד״ר משה ברקת סוכם הבוקר כי הק…  מחר מיד לאחר הקמת הוועדה המסדרת נוביל פתרון הצבעה לחברי כנסת השוהים בבידוד בימי משבר כאלה הכנסת חייבת לתפקד באופ…  יעל גרמן היקרה כנסת ישראל נפרדת היום מאישה ישרה ערכית בעלת הישגים שהכנסת והציבור הישראלי התברכו בה יעל מגלמת בא…  חייבים להציל את מדינת ישראל רק כחול לבן   EitanGinzburg מה אומרים לא אומרים מצביעים  הבחירות ביום שני הן שעה גורלית לעתיד המדינה אם כחול לבן לא תהיה המפלגה הגדולה ביותר אנחנו נתעורר למציאות מסוכנת שב…  באירוע שבת תרבות בחולון בהגשת NechamaDuek אמרתי כי אין אדם ראוי מבני גנץ להנהיג את מדינת ישראל עבדתי קרוב עם כל…  חרפה ההתנהלות הגזענית של השוטרים המוצגים בכתבה כלפי יוצאי אתיופיה ונוער במצוקה מזעזעת אין להתנהגות כזו מקום במש…  ניר למה דמגוגיה בגרוש העובדות הן שאתה הובלת את ים לירידה בדירוג הסוציואקונומי בזמן שאני העליתי את שכר המינימום…  המאבק שלנו הצליח ומיזם הביטחון התזונתי ימשיך לפעול בהמשך לפנייתי לחשב הכללי תאושר בקשת משרד הרווחה ותימנע הפגיעה…  פרופ׳ רות בן ישראל כלת פרס ישראל הלכה לעולמה זכיתי להכירה כמרצה מופלאה בפקולטה למשפטים ונפלה בחלקי הזכות להקשיב…  הבטחנו וקיימנו שלטון החוק ניצח היום את הקומבינה הפוליטית בדמוקרטיה כולם שווים בפני החוק וכעת גם נתניהו נאלץ להכיר בכך Kachollavan19 יו״ר הוועדה המסדרת ויו״ר סיעת כחול לבן ח״כ אבי ניסנקורן פנה לפני זמן קצר לייעוץ המשפטי של הכנסת בבקשה להבהרה דחופה בנו… אנחנו מכבדים את יו״ר הכנסת ומחכים להודעתו על כינוס המליאה בהקדם כל פרסום אחר חוטא לאמת על יו״ר הכנסת להתנהל כעת בצורה הממלכתית המתחייבת אפעל להקמת ועדת הכנסת החל ממחר ונקיים את דיוני החסינות בצורה הוגנת עניינית ויעילה אין מקום לדחות את הקמת ועדת הכנסת יש לקיים דיון ענייני בבקשת החסינות נתניהו הפך הערב לאויב הדמוקרטיה הישראלית אני קורא ליו״ר הכנסת לכבד את מעמדו הממלכתי ולאפשר את כינוסה של הוועדה המס…  רק החלטה נחושה לממש את ההסכמות אליהן הגעתי בנושא תצמצם את מגפת תאונות העבודה האדישות של הממשלה הנוכחית היא מזעזעת…  תמונה עגומה עולה מדוח העוני שפורסם היום עצוב ובלתי נתפס שראש הממשלה דואג לחסינותו האישיתבמקום לחסינותם של הקשישים…  Kachollavan19 עקב כוונת יו״ר הליכוד בנימין נתניהו להגיש בקשת חסינות מפני העמדה לדין באשמת שוחד מרמה והפרת אמונים הודיע כעת ח״כ אבי נ… מבחינת ביבי כל מה שמגן עליו הוא אבן יסוד ובירור האמת בבית המשפט היא אבן ריחיים בילבול בערכים בזמן שאחרים מצייצים אנחנו עובדים הגענו הערב להסכמה עם משרד האוצר שתשים סוף לאפלייה כלפי החינוך המיוחד במגזר החרדי…  האזרחים לפני הכל הוועדה המשותפת בראשותי ובראשות ח״כ גפני אישרה כעת העברה של 242 מיליון שקל מיתרות תקציב הכנסת לטוב…  מנכ״ל משרד הבריאות הודיע לי על אישור תוספת של חצי מיליארד ש״ח לסל הבריאות אני מברך על כך אסור שנושא כל כך חשוב ומ…  הוועדה המסדרת בראשותי תוודא שהתוספת לסל התרופות תעמוד על 500 מיליון שקלים ולא שקל אחד פחות אני עומד בקשר רציף עם ר…  gantzbe אם בסופו של יום נידרדר בגלל נתניהו  לבחירות אזרחי ישראל מימין ומשמאל שנמאס להם מהמצב הקיים ילכו איתנו אנחנו ננצח ונרכיב ממש… הייתי היום בכנסת אבל המחשבות היו בדרום אני שמח שהצלחנו להקל ולו במעט על המסעדנים ובעלי האולמות בעוטף עזה בזכות שי…  אנו מחזקים את ידם של צה״ל וכוחות הביטחון במלחמה הנחושה נגד הטרור ביטחון המדינה וביטחון אזרחיה לפני הכל אין גבול לחוצפה שר המשפטים מנצל לרעה את החסינות הפרלמנטרית תוך הפרת צו איסור פרסום חרפה המסעדנים ובעלי אולמות האירועים בעוטף עזה מחכים כבר חודשים לפיצוי שהבטיחה להם המדינה בגין הנזקים הקשים שהם נאלצים לס…  חוזרים לכיכר להגיד נגד אלימות ונגד הסתה  הניסיון הבזוי של נתניהו לפגוע בבחירות דמוקרטיות וליצור תוהו ובוהו  נכשל כפי שאמרנו לאורך כל הדרך ועדת הבחירות תפ…  peretzsami לצמצם את אי השוויון זה בעיניי משימה מתחייבת ועליונה גם לחוסן החברתי שנוגעת באלו שהכי זקוקים ובוודאי…  חינוך לגיל הרך אי שיוויון בחינוך והכשרות מקצועיות  בהן משקיעה הממשלה שיעור נמוך מידי בתקציב כמו גם היעדר הכשר…  הובלתי גם קיצור שבוע העבודה רפורמות במשק החשמל מכון התקנים ומשק המים שישפרו את הפריון וצמצמתי משמעותית את ימי השב…  peretzsami אל תתן לעובדות להפריע לך בסיסמאות הקבועות אני תרמתי לצמצום פערים   במעשים ולא דיבורים שכר מינימום ש…  ביבי מה נתפסת לוונצואלה קל לקבל שם חסינות  תודה חברים  ביבי בלחץ  יכלת למצוא תמונה טובה יותר הנה העובדות   כך לא צריכה להיראות הרפואה הציבורית בישראל תת תקינה שאינה תואמת את העומסים מביאה לזעקת האחיות הנשמעת כעת אני מחז…  מתפלא עליך בנט כשנאבקתי למען צמצום פעריםשיפור משמעותי בתנאי עובדי שמירה וניקיון למען הקשישים והנכיםהעלאת שכר המ…  אחרי החלטה בלי בירור מעמיק של ההשלכות אחרי שבועות של הולכת שולל של תושבי אילת והערבה החליט הערב נתניהו באופן סופי…  אזרחי ישראל צריכים לזכור דבר אחד  הבחירות האלה הן בין ביבי נתניהו לבני גנץ ורק בין שניהם ישראל ניצבת לפני החלטה…  הבוקר אצל DaphnaLiel בשבתרבות חזרתי ואמרתיביטול הבחירות היה עוד תעלול אחיזת עיניים מבית נתניהוזו מציאות מאוד מצע…  ועדת הכספים אישרה הבוקר את דחית סגירת שדה דב ובכך הצטרפה להתנגדות של כחול לבן ולמחאת תושבי אילת עכשיו זה לפתחו…  עכשיו מול בית רהמ בירושלים סיעת כחול לבן עומדת לצד תושבי אילת נגד סגירת שדה דב צינור החמצן של אילת  רהמ הוא שאחראי לגרעון בחוסר התפקוד שלו בהתמקדות בבעיותיו האישיות במקום באזרחים הייתה לי הזכות לפעול לצמצום הפערי…  פניתי הבוקר  ליור ועדת כספים לכנס בדחיפות את הועדה למנוע את סגירת שדה דבעלינו להבטיח שאזרחי אילת והדרום אינם מופק…  מדינת ישראל חייבת לחבר בין אילת למרכז הארץ באופן אפקטיבי ונגיש וכל עוד לא נמצא פתרון יש להפעיל את שדה דב באופן סדי…  נתניהו ממציא שיטה  מביא לבחירות ב5 מיליארד שקל על חשבון האזרחים בשביל לדחות שוב את השימוע שלו זילזול מוחלט בא…  בזכות הדיון הבוקר בועדת הכספים בראשותו של ח״כ גפני שנערך בעקבות פנייתי בנושא הצלחנו להביא לעצירת הקיצוץ בקרנות הפ…  בלב כבד נפרדים היום מהגב׳ נחמה ריבלין רעייתו של נשיא המדינה ראובן רובי ריבלין  נחמה הקדישה את חייה לפעילות ציבו…  intxchlxrine תודה לעם ישראל שהגיע הערב והצביע ברגליים יחד הצבנו את הקו האדום לשמירה על הדמוקרטיה   הערב הייתה ירית הפתיחה למאב…  תכף מתחילים הצטרפו אלינו למלחמה על הדמוקרטיה הישראלית  יוצאים להיאבק על הדמוקרטיה הצטרפו אלינו מחר ב2030  מחזק את ידיהם של לוחמי האש היקרים הנאבקים בשריפות הקשות ברחבי הארץ שולח חיזוק גם לכל התושבות והתושבים הנמצאים בקיר…  זה ימין שפוי ימין שפוי לעולם לא היה נותן יד לריסוק הדמוקרטיה הישראלית  נתניהו לא בוחל באמצעים למען הישרדותו עשרות מיליוני השקלים שהוא מתכנן לזרוק לפח הם חרפה לקואליציה שתקום לכל השרים…  לא ניתן להפוך את מדינת ישראל לדיקטטורה הניסיון הבזוי והמתמשך לחרב את מערכת המשפט עבור ראש ממשלה שנגדו תלויים שלושה…  צפו בסרטון קצר על חלק ממה שעשינו ב 3 השנים האחרונות  חיכיתי עד הבוקר בכדי לראות האם היא תתנצל על הבושה ותיקח אחריות על הקומבינה את שלי מעניינת רק שלי – ולא שום דבר אחרgt  אני מודה ליוגב עשור יור הועד של ברינקס והעובדים על תמיכתם בי לתפקיד יור ההסתדרות  ביחד ננצח למען העובדים ולמען ה…  אני מודה לקרן אופק יור ועד עובדי פרטנר והעובדים על תמיכתם בי לתפקיד יור ההסתדרות ביחד ננצח למען העובדים ולמען הח…  עם מוטי חזיזה היקר בפרי הגליל סמל ומופת למאבק למען התעסוקה בצפון  קולטים את עובדי הקבלן להעסקה ישירה ומחוייבים ל…  הגענו להסכם הבנות באלעל בחברה כ 6000 עובדים מסורים אנו נפעל למערכת יחסי עבודה טובה בחברה ולפתרון בעיות בכל הסק…  חתמתי עכשיו הסכם קיבוצי להסדרת הרפורמה בבורסה ההסכם כולל הגנה מפני פיטורי צמצום וקליטת עובדי קבלן להעסקה ישירה ככ…  פועלים לקידום שינוי חברתי נוסף העברנו לקריאה ראשונה הצעת חוק למתן תנאי עבודה הולמים לעובדי אבטחה המטרה להעביר את…  לפני מספר דקות חתמנו על צו הרחבה המשפר משמעותית את תנאי העסקה של כ7000 עובדים סוציאליים בישראל מעשים ולא דיבורים…  אני מודה על הבעת התמיכה לשר חיים כץ לוחם חברתי אמיתי מבטיח שיחד איתך ועם רבים אחרים נמשיך להוביל לשינוי חברתי במדינה אני רואה מול עיניי את העובדים המוחלשים פעלתי להעלאת שכר המינימום ב1000 שקלים ואמשיך עד שנשנה את החברה הישראלית ונ…  אתמול התקיים דיון ראשון בוועדת העבודה והרווחה בכנסת בהצעת החוק לתנאים הולמים בתחום האבטחה המטרה היא להעביר את החוק…  שחררנו את השכר מכבלי הקיפאון  מתחילת הקדנציה שלי עלה השכר הממוצע במשק ריאלית ב 88 ובשנה החולפת הייתה עליה של כ…  מאיר בנאי נפטר איש צנוע רגיש יוצר ישראלי מופלא אני אוהב את יצירתו היא באה מהלב ונוגעת בלב ומאחדת יהי זכרו ברו…  אני משתתף בצער משפחות ההרוגים ושולח ברכת החלמה מהירה לפצועים יום קשה לכולנו בנמל אשדוד שמים את הויכוחים על הרפורמה בצד וחותמים על הסכם להעסקת עובדים עם מוגבלות קוגנטיביתנפשית בהעסקה ישירה זו אמירה חברתית סיימנו עכשיו טקס העברת 69 עובדים להעסקה ישירה בבית החולים וולפסון נר תשיעי של חנוכה  ממשיכים בשינוי החברתי גם ב2017  בשעה טובה מצטרף לטוויטר  בואו נכניס את נושא צמצום הפערים וקידום השוויון חזק לשיח</t>
-  </si>
-  <si>
-    <t>Normalizing SudanIsrael Relations Now is a Dangerous Game write paytonknopf and JeffreyFeltman   arielelharar עשיתי ראיון לעיתון החג עם אחד מפעילי השמאל המוכרים הרגשתי בתור חרדי בדיוק את מה שהוא הרגיש כל הקורונה מעניין AfifAbuMuch הטור שלי הבוקר בYediotAhronot  על הסכמי הנורמליזציה הכישלון הפלסטיני תחושת המיאוס בעולם הערבי ושימור הסטטוסקוו של… JoshBreiner אפשר להיות פוליטקלי קורקט ואפשר להתייפיף אבל האמת המרה כפי שכותב AnshelPfeffer  שרוב המגזר החרדי מוביל אותנו להדרדרות מט… chaimlevinson  האום מאבד את זכות קיומו  האום מסתכן באבדן הרלוונטיות והלגיטימציה שעוד נותרו לו  הארגון היוקרתי והמנופח חייב… AnshelPfeffer כתבתי הבוקר בהארץ על טיול רגלי בבוקר כיפור בשכונות החרדיות של ירושלים  המסקנה המרכזית ההנהגה החרדית ברובה החליטה במ… IshayShnerb הצעת חוק שבעה חודשים מתחילת המגפה פוליטיקאים לא יורשו להשתמש בלשון עתיד בהודעות לעיתונות המבשרות על מהלכים שהצורך בהם יד… VeredLee1  talschneider פופי הרלו לדובר הבית הלבן הנשיא לא פרסם מסמכים שיסתרו את הפרסום של הני״ט תפסיק לתקוף את העיתון כאילו עשה יד עם המפלגה ה… KseniaSvetlova שלא תדעי עוד צער חיבוק גדול NadimKoteich كل التمنيات لفايروس كورونا بالشفاء من جبران باسيل EladStr On YomKippur we are dedicated to reconciliation with ourselves God and each other We commit to selfreflection and inner ch… On this Yom Kippur I wish all my followers in Israel and around the world Gmar Hatima Tovah To all of you who are…  IvankaTrump As Yom Kippur begins tonight I wish all the Jewish people observing this sacred day of atonement an easy fast and meaning… noamfathi גמר חתימה טובה נעם becktalia וגם מהדורות חדשות ופאנלים שפתאום לא שלמים בלי אנטידמוקרט נלהב אחד לפחות SecPompeo Wishing a blessed and sacred Yom Kippur to all the Jewish people May your fast be easy and meaningful Gmar hatimah tovah… גמר חתימה טובה לכל עוקביי בישראל ובעולם צום קל מועיל ומשמעותי לכל מי שצם והעיקר תהיו בריאים hagarsi yairlapid BenCaspit MeravMichaeli tamarishshalom בשמחה zalmanovitz תן בראש amirtibon Chasing AOC is a waste of time for liberal Jewish Zionists It would be better to focus on political leaders who actually wa… amirtibon Liberal Zionists it’s time to admit AOC just doesn’t want to be your friend And thats OK    מי שמסתמן כבר עכשיו כתגלית השנה הקרובה הוא zalmanovitz ממליץ לכם לעקוב אחריו AfifAbuMuch מציע ביום זה ללא מעט עורכיםות לבקש סליחה מהציבור הערבי על הדרתו המתמשכת מהאולפנים יש לי חדשות בשבילכם אפשר להזמין רופא… itzikelrov למה נתניהו עושה השוואה בין החרדים למפגינים אני מבין לגמרי  מייצר ספין  למה אנחנו החרדים נופלים למלכודת הזו כשברור לכל י… המפגינים בבלפור עשו הכול כדי למנוע מנתניהו תמונת ניצחון כותב danieldolev  נדב מנוחין כשמאות אלפי מובטלים יושבים בביתם בחרדה עצומה לעתידם הכלכלי המהדורות העדיפו לעסוק באובססיביות בשאלות…  newsisrael13 לא נכון זה ממש לא מה שכתוב בדיווח מדויק  כל השירשור  razshlomo חתן פרס נובל פרופ ישראל אומן בראיון לנחום ברנע  DanielBShapiro Very disappointing decision now confirmed by AOC not to attend this event A mistake to give in to pressure a misse… jacobkornbluh אזרחי ישראל היקרים  עם כל הקושי שבדבר אני מאוד מעריך את שיתוף הפעולה של רוב אזרחי ישראל   חייבים לעצור את שרשרת ההדבקה… BenCaspit מי שהוציא את ההמונים אתמול לירושלים לקיסריה לצמתים לגשרים למחלפים ולכל מקום מי שגרם לבני 90 לצאת מהדיור המוגן עם ההליכו… oronrazz לא יכול לפרט על החלק הזה Ygygygyg17 לא יכול לפרט על החלק הזה segaleran נראות ערבות הדדית וסולידריות בגלל זה צריך להשהות כרגע את ההפגנות הגדולות לא בגלל ההשפעה הזניחה כרגע על התחלואה  אז בי… segaleran חשבון פשוט אחרים גם עשו מראה שלהפגנות יש כרגע השפעה זניחה על התחלואה ועדיין לדעתי כרגע צריך להשהות אותן  הנה חשבון מוגז… בתחילת האינתיפאדה ה2 כמה ימים אחרי הלינץ ברמאללה היו אינדיקציות שעיראק של צדאם שוקלת לשלוח כוחות הטלוויזיה העירא…  מי שחושב שאת הקורונה מנצחים עם עובדות מדעיות ועם נתונים ולא באמצעות ספינים פוליטיים חייב לקרוא את הכתבה הזו הממשלה…  yaakovkatz מנהיגות מודל תשפ״א משסע מפלג ומפצל  עמוס הראל כותב בזמן שנתניהו ממוקד בדיכוי במחאה התחלואה בחברה החרדית מזנקת מספר הנשאים החרדים מטפס כבר יותר מחודש…  AfifAbuMuch לא יודע נראה שבבלפור יצטרכו לעדכן את התגובה הקבועה לאהוד ברק  chaimlevinson וזה בדרך למשדר סליחות שאלוהים יעזור לי  horowitzb בערב יום כיפור חייבים להיות אמיתיים עם עצמנו אין שום סיכוי שממעל 8000 נדבקים ביום נראה ירידה דרמטית בתחלואה לכמה מאותעשרו… axios  The fact that world leaders couldnt gather in person for this years General Assembly was another setback for Palestinian le… AfifAbuMuch darkenuIL כל הכבוד אחי התנהלות נתניהו בימים האחרונים תידלקה את זה  amirtibon אמא של אשתי עלתה לארץ מרוסיה לפני 30 שנה מעולם לא הלכה להפגנה לא התעניינה בפוליטיקה התעסקה בפרנסה ומשפחה וסמכה על השלטון… BenCaspit לבין עתונאי כלומר בועז כהן השופר מערוץ 20 המשפט האחרון נאמר עי קרעי טוב אז גייסנו את בועז שפשוף נעים  BenCaspit טוב בבירור הכי מרגש היום דיירי הדיור המוגן ברמת השרון יצאו להפגין אחד מהם שמואל כסלו ערך סרטון אלה האנשים שבנו את המדי… AnshelPfeffer עכשיו סופגים את העלייה במבדקים מהתקהלויות הסליחות בימים הקרובים יהיה את הגל של תפילות ראש השנה בשבוע הבא נקבל תפילות י… anerhaim1 גיליתי שבמהלך השבת שני אנשים יקרים לליבי נכנסו לקו האש אלו הן דעותיי בנושא   חיים לוינסון לא צריך עזרה הוא אוכל את פתחי כ… Shiritc אפשר לעזור freyisrael1 Shiritc במקרה במקרה ההגבלה היחידה שהממשלה רוצה לבצע ללא הכנסת היא ביטול ההפגנות נגדה צירוף מקרים ItayBlumental כ 20 בני אדם שהפגינו הערב במסגרת הדגלים השחורים בשכונת שפירא בדרום תא הותקפו על ידי שני רוכבי קטנועים שעברו במקום נדב… GrandmomLiza BarakRavid RMatsliah pgoshMTP N12News ברק שאפו לא נותן  לדמגוג פתחיה לגנוב דעת עם שקרים הזויים itaizil עכשיו בפגוש noamfathi טוען שהציוץ הזה של BarakRavid הוא עידוד עלייה להפגנה בבלפור ולכן לא אכפת לו מהנפטרים מהקורונה אני י… בעוד כמה דקות אדבר אצל RMatsliah בpgoshMTP בN12News מוזמנים לצפות  כל כביש 1 קילומטרים על קילומטרים של שיירה במסלול הימני אלפי כלי רכב של מפגינים  כביש 1  לכל נוסעי השיירה לירושלים כבו בבקשה את הווייז האפליקציה חושבת שכל כביש 1 פקוק ולא מזהה שזה רק המסלול הימני היועץ המשפטי של משרד הבריאות אורי שוורץ העביר אתמול למזכירות הממשלה חוות דעת לפיה קיימת מניעה משפטית להגביל הפגנות…  Ibishblog tabacoffd Many people dont think it is a non issue talshalev1 עכשיו ב WallaNews  גם במהלך הסופש נמשכו השיחות בקואליציה על העברת תקשח להגבלת הפגנות במשאל טלפוני בכחול לבן הבהירו לאד… במהלך סוף השבוע המשיך נתניהו לקדם תקנות לשעת חירום להגבלת ההפגנות במטרה להעביר אותן בממשלה לפני יום כיפור הדיווח ש…  chaimlevinson מישהו יודע מי החברים של גיימס פאקר בישראל אביעד גליקמן לא גיא פלג לא מעניין 🧐  בעקבות לחץ מצד פעילים פרופלסטינים אוקסיוקורטז ביטלה את השתתפותה באירוע לזכר רבין  בתחילת השבוע קיימה משלחת סודאנית שיחות באבודאבי עם בכירים בבית הלבן בנושא הנורמליזציה עם ישראל והוצאת סודאן מרשימת…  אלבורהאן לא התייחס ישירות לסוגיית היחסים עם ישראל אך ציין כי סודאן עומדת בפני הזדמנות חסרת תקדים להסרתה מרשימת הטר…  דבריו של חמדוק הבליטו את המחלוקת בין הפלג האזרחי של השלטון בסודאן לבין הפלג הצבאי בראשות יור מועצת הריבונות הזמנית…  ראש ממשלת סודאן עבדאללה חמדוק שעומד בראש הפלג האזרחי של השלטון הזמני במדינה אמר היום כי סודאן מתנגדת ליצירת קישור ב…  גם באיראן מחזירים את הסגר  jhaboush BREAKING Lebanon’s PMdesignate steps down after failing to form a new govt Sanctions likely to follow from France now t… מה שנדב אומר  שחקנית בריטית טוענת שהמיליארדר האוסטרלי גיימס פאקר מקורב למשפחת נתניהו ואיש מפתח בתיק 1000 כפה עליה לקיים יחסי מ…  chaimlevinson יתרה מכך הערך הועמד למחיקה היוזר האנונימי נאבק בדף השיחה נגד המחיקה הרחיב את האייטם במידע רב שלא ימחק טען שטען שהרדי… chaimlevinson למי שתהה למה נעם פתחי קורא לעצמו סאטריקן בויקיפדיה זה כנראה בזכות הסאטירה המשובחת הזו תנו לו לייק רחמים AnshelPfeffer halbfinger AOC It’s not really about the Palestinians or about Rabin It’s an internal squabble between tiny factions… halbfinger New peak reached in IsraelastoxicissueforDems aoc pulls out from Peace Now event honoring Rabin’s legacy under fire… amirtibon ArthurLenk 90 of elected Democrats including many of the young congresswomen first elected in 2018 would love to attend… tcwittes In which a US official who says she supports a peace agreement between Israelis and Palestinians shuns the US affiliate of Is… chaimlevinson אוקיי רבותיי כשכתבתי את הציוץ המקורי לא ידעתי שהקמפיין המבריק עם ההומור הבריטי הצונן והדק של שוקה זה של נעם פתחי  סל… A must read  YairRosenberg AOC Ill give the last word to a progressive Israeli and Egyptian You dont make peace between friends you do it by… YairRosenberg If AOC cant even do an event with Peace Now remembering Yitzhak Rabin the general turned peacemaker killed by a fa… mkoplow If you can’t recognize and honor the Israeli PM who recognized the PLO ceded Israeli sovereignty for the first time in parts… mkoplow Enormously disappointing decision by AOC to withdraw from PeaceNowUS Rabin event There is no such thing as a peacemaker wit… issacharoff bariweiss It’s sad that instead of strengthening the moderates on both sides she supports the extremists on one side… Ahmadtibi לזכרם  StavShaffir AOC alexbkane When we stand for peace there will  be those who will tell us its impossible even threaten us Rabin st… פתיחה חזקה ביותר של DanyCushmaro באולפן שישי בN12News bahdiplomatic وزارة الخارجية ترحب بنتائج الاجتماع التنسيقي الذي عقد في العاصمة الأردنية لإحياء عملية السلام في الشرقالأوسط  tcwittes ilangoldenberg BarakRavid AOC alexbkane PeaceNowUS Dear AOC Rabin shook hand w his lifelong enemy declared “enough of… ilangoldenberg BarakRavid AOC alexbkane Also PeaceNowUS is a great organization that is true to progressive values ilangoldenberg BarakRavid AOC alexbkane AOC I hope you do this Rabin was assasinated for pursuing peace He was a military man e… MChesterB BarakRavid AOC alexbkane I second this It was such a hopeful event It may didnt turn out as expected but it was a move… chaimlevinson אתם חושבים שגם עליהם יגיד מיקי זוהר שהם מפיצי מחלות כפי שאמר על המפגינים בבלפור ונתניהו יוסיף שמדובר במדגרת קורונה… RonenManelis BarakRavid PeaceNowUS FarkashOrit אין ספק שלשמוע לדבר ולנסות להשפיע גם עם מי שלא מסכים איתנו היא הדרך שאנחנו מאמיני… I hope not  chaimlevinson חשבתי שראיתי הכל בימי חיי אבל קופרייטר כושל שלולי היה מלקק לביבי היה כותב היום ברושורים למאפיות טוען שקלמן ליבסקינד הו… Suvanji לעתים רחוקותביבי צודק נקווה שהיא לא תתקפל  AOC alexbkane I hope you do attend the event You make peace with your enemies This is what Rabin did He was assassinated for doing this מסכים עם כל מילה של ראש הממשלה  chaimlevinson פרסום ראשון בעקבות פרסום תמליל מחקירות נתניהו  השבכ הגביר האבטחה סביב ראש הממשלה  shemeshmicha יזהר שי היום בזום לפעילים של כחול לבן  ״נתניהו עשה לנו תרגיל פוליטי אני משוכנע בזה  עוד פרטים בטלגרם  אירוע מעניין מאוד אגב  זו בדיוק הדרך להילחם בBDS לדבר עם המבקרים ולמצוא נקודות הסכמה כל הכבוד לPeaceNowUS מ…  jacobkornbluh Rabin signed the Oslo Accords Rabin signed a peace treaty with Jordan Rabin sacrificed his life for peace Rabin was a… eliorlevy חייבו את כל המנהיגים לשלוח נאום מוקלט של 15 דקות ולא יערכו אותם galberger תוספת קטנה בעיקר מחכה לאחרי הבחירות באמריקה ומתפלל שביידן ינצח Important thread  BREAKING Palestinian President Abbas called in his UNGA speech to convene an international peace conference on the…  הנשיא הפלסטיני מחמוד עבאס אבומאזן בנאומו בפני העצרת הכללית של האום אני קורא למזכל האום להתחיל בהכנות בשיתוף…  chaimlevinson פרסום ראשון של יערה זרד  talshalev1 1מנכל משרד הבריאות חזי לוי על המכתב שנשלח לבקשת אדלשטיין הנקודות הועלו בישיבת הקבינט ואף היו חלק מעבודת מטה עם המשטרה וה… avischarf טוויטר שמקום מושבה מעבר לים מאפשרת ביזוי והשפלת ישראלים היא שוכרת משרד עוד מקומי שינסה לא לאפשר לישראלי שנפגע להתגונן ש… מאמר מדוייק של KalmanLiebskind על חבורת ריקליןברדוגותדמור ושות למרבה הצער יש עוד הרבה כמותם טוב שקלמן כתב או…  بالضبط  נתניהו האשים את הציבור  בלי גרם של חשבון נפש כותבת KerenMarc  MarkZlochin אפשר לשער שנתניה ינסה להשתמש בחוות הדעת של חזי לוי כדי להצדיק מגבלות קיצוניות על ההפגנות לכן חשוב לשים לב לחלקים המודגשי… chaimlevinson נתניהו בתגובה   בכל הקריירה שלי היו מצבים רבים שלא שמעתי לאנשי המקצוע וצדקתי במאה אחוז kaisos1987 עסקת המאה כבר לא תהיה בקרוב אבל הטרלת המאה אולי תארו לכם שהיום בזמן נאום אבו מאזן באום טראמפ מעדכן על עוד מדינה שמצטרפת… SefyHendler נשמח לקרוא את הנתונים והמחקרים המדעיים עליהם מתבסס מנכל משרד הבריאות במכתבו AlonPinkas אה ״מענה״ מענה זה יפה ומנומס talshalev1 פניתי בשאילתא למנכל משרד הבריאות כדי לשאול מה מטרת המכתב שנשלח באופן חריג ביום שישי בצהריים והאם הנקודות לא הועלו בישיבות… בלשכת שר הבריאות מאשרים כי הרקע למכתב ששלח מנכל משרד הבריאות חזי לוי לנתניהו הוא מענה לבקשה של השר אדלשטיין השר…  aviadglickman ובגלל זה נתנו למשטרה סמכות בהפגנות לתת קנסות על אי שמירת מרחק ועל מסכות וגם סמכות לפזר הפגנות זה אותן תקנות שלפי חישוב… לפי המכתב הזה חייבים לסגור את בתי הכנסת ביום כיפור  אני מאוד רוצה לקוות שזה לא מכתב מוזמן של נתניהו ואדלשטיין כדי לקבל כסות מקצועית לדיכוי ההפגנות אבל זה מריח לא טו…  ברייקנג מנכל משרד הבריאות לנתניהו ומנדלבליט כל התקהלות בלתי מבוקרת ונשלטת בוודאי בחללים סגורים ובמידה פחותה א…  talshalev1 נתניהו אומר שההפגנות מחזקות אותו בינתיים נראה שהוא עושה לא מעט כדי לחזק אותן בחזרה erancherpak והעמוד השלישי שנשמט  erancherpak מוטב מאוחר מאשר אף פעם הטור של קלמן מהיום  talshalev1 עכשיו בצומת נתניה ועוד צמתים ברחבי הארץ שיירת תקווה של המחאות יוצאת למסע בין ערי ישראל  prokooter גידי וייץ פרסם היום תמלילי חקירות ארוכים מסמרי שיער אבל את הקטע הזה אני אקח איתי גבירותי ורבותי זה האיש שבגללו ישראל נכנס… בהחלטתה על הסגר שיעבדה הממשלה את עתידנו הכלכלי למצבו המשפטי של נתניהו כותב peretzsami  avischarf The Haredim have a strategy for dealing with the plague Change nothing It may cost more lives but once over they believe… אחרי שיחה עם בני גנץ יזהר שי לא יתפטר מהממשלה זה מומלץ תמיד  אבל עכשיו בסגר עוד יותר תעקבו אחרי freyisrael1 תענוג צרוף adiryanko כל הסיפור בשתי תמונות אחרי ההכרזה על סגר הרמטי שיחל מחר מהו ההבדל בינו לבין זה שנכנס לתוקף ביום שישי האחרון תראו בעצמכם… Nefolet החל ממחר תשבו בבית ותחשבו על מה שעשיתם לביבי freyisrael1 arielikobi רגע כל הזמן היית נגד הפגנות בלי לדעת על מה הם chaimlevinson  שאלה לכתב לוינסטוןNews  אדוני ראש הממשלה איך זה שאתה כל כך מושלם כל כך מנהיג כל כך חכם מנצח הקורונה משחרר יר… kann היינו שאננים בעיקר מוני  בהצלחה עם העם הבא   פרק חדש מהניילונים של זהוזה2020 2115 בכאן 11 ואיפה עוד בדיגיטל   עמוס הראל כותב ראש הממשלה כבר נמצא בעיצומו של גיהאד נגד המחאה ואם לשם כך צריך לסגור בסגר חונק את המשק כולו צעד…  JoshBreiner קיצר אנחנו אשמים RuthiLandau BarakRavid האיש המובטל המתגורר בבלפור ירושלים NadavEyal ההצהרה של נתניהו הציגה מצג עם הגיון פנימי לגבי מצב החירום לקח אחריות על ההחלטה וזה עליו  ואז הוא תקף את האופוזיציה ואת המ… chaimlevinson אגב חוק הקורונה עבר על 4 קולות אם ימינה היו טורחים לבוא החוק היה נופל מעניין אותי מי בלשכת ראש הממשלה כותב את השאלות לערוץ 20 נתניהו הוכיח הערב שבאמת אין גבול לבריחה מאחריות מי שפתח את המשק בלי חשבון ובלי תכנון קפדני וקרא לכולם לצאת לבלות מ…  ariehkovler To put it another way more Israelis were killed by the coronavirus in the last ten days 214 than were killed by terrori… ariehkovler According to Israels Health Ministry 1376 Israeli residents have died of Covid19 surpassing the death toll of 20 years… jacobkornbluh Scoop Jared Kushner speaks to AIPAC for the first time in his White House role  The White House senior advisor spoke ye… BenHowardIL לא מצליח להבין  אנשים רואים את הטיטניק טובעת ואף אחד לא קופץ BarakRavid rshamir אחת הכתבות היותר מפחידות ומטרידות שתקראו הערב BarakRavid מתאר את ישיבת הממשלה מאתמול ואת הדרך בה מתקבלות החלטות של חיים ומוו… NadavEyal פרסמתי הערב משרד הבריאות וקבינט הקורונה מנסחים אסטרטגיית יציאה השאלה הגדולה האם לאמץ אסטרטגיה של דיכוי הנגיף עד אפס או ק… gabibarh כולם בדיכאון כולם בחרדה כולם עבדים של הילדים בזום כולם מפחדים מהעתיד מחשבון הבנק המתרוקן מהנפש שמטרללת אמסלם קראו לי ש… עצבני אפוקליפטי ונרגן נתניהו דרס את אנשי המקצוע והשרים בדרך לסגר השני קראו את הפרשנות שלי בWallaNews עם הרבה פ…  NaamanStavy בשואה כמו בשואה אנקדוטה מישיבת הממשלה הלילית שר החוץ גבי אשכנזי צידד בהחלטה להשאיר את בתי הכנסת פתוחים ביום כיפור והשתמש באנלוגיה…  גנץ ימסור הצהרה בנושא הסגר ב2015 המשוואה הפגנהשווהתפילה של נתניהו היא שקר מרושע שיעלה לנו ביוקר כותב baruchikra   להקיא  wasilalitaha The article by jakesNYT appears understandably so very sympathetic to the terror victims but doesnt make any mention… OdehBisharat BarakRavid יש כאלה שמאוד עצובים שחיים ראה את המודעה בעיתון talshalev1 מה שכן איזה מזל שבני גנץ נסע השבוע לאמריקה YakiAdamker למי שלא קרא פה    YakiAdamker כשהושבעה הממשלה יזהר שי סומן כאחד האויבים הפוליטיים של נתניהו חשדו בו לא האמינו שיעבוד כתף לכתף ובחנו אותו משל היה מיש… DaphnaLiel נוצר פה ניגוד עניינים בעייתי רק במצב של סגר כללי ניתן לאסור לגמרי את ההפגנות בבלפור כשבשאר הזמן המפגינים יצטרכו לשמור על… talibo8 איזה פחד איזה פחד איזה פחד ViciousVictim המסמך הזה של Izhars7 ראוי שיהיה לו מקום של כבוד ב׳ועדת אגרנט של משבר הקורונה׳ שתוקם בוודאי בעתיד הלא רחוק אני מצדיע לו goldman1007 השר Izhars7 הוא אחד האנשים ההגונים והרציניים שאני מכיר אם יורשה לומר הוא מתון באופן קיצוני לכן המכתב שלו קריאת חובה אם… jw17061 לשמור לוועדת חקירה rolbishaul מטריד ביותר איזה מזל שחיים ראה את המודעה הזו בעיתון הוא נכס לעיתונות הישראלית  קו ברור וחד מחבר בין מכתב ההתפטרות של שאול מרידור לבין הדברים שאמר אתמול יזהר שי בישיבת הממשלה המסקנה לגבי התנהלות…  מחכה לעדכון  WallaNews חוסר טקט על המסך לא ברור אם צבי יחזקאלי הוא יותר חצוף או יותר חסר מודעות  natitucker אחרי חודשים של שליטת רשת 13 בטבלת הרייטינג בזכות הישרדות המומנטום כל כך התהפך לטובת קשת 12 עד שאתמול המרוץ למיליון עש… השתקת מומחים עקיפת שרים זגזוג בהחלטות סלחנות לגבי התפילות ואובססיה לגבי ההפגנות השר Izhars7 בעדות מבפנים על הכ…  השר יזהר שי צפוי להיפגש עם יור כחול לבן בני גנץ בשעות הקרובות כדי לדון באפשרות שיתפטר מהממשלה לאור ההחלטה על הסגר הכולל zalmanovitz אני מחבב את השר יזהר שי הוא מהאנשים הרצינים היחידים בממשלה  באיחור לא אופייני הוא גילה כמה הממשלה הזאת לא שווה את הדף על… alonkes חובת קריאה חברים וחברות erant יזהר שי הוא היחידי בממשלה שמבין משהו בבלימת הקורונה והאדם הכי פרקטי שם כדאי לקרוא את מה שהוא כותב DoronHorowitz מדינת ישראל עומדת על קצה המצוק ומבצעת צעד אחד קדימה BarakLS לקרוא ולבכות chaimlevinson כל דקה שגמזו לא מתפטר הוא משתתף בהונאת הציבור כאילו יש אלמנט מקצועי בהחלטות ItamarKatzir אני באמת לא מאלה בדרך כלל אבל סו קריאת חובה אנחנו בני ערובה של ממשלה שפועלת נגדנו  כולנו  בלי הבדלי דת מוצא מגדר וש… idanlandau בניכוי הטפיחה העצמית על השכם יזהר שי מסביר כאן במילים פשוטות שנתניהו פועל כדיקטטור oferdann מילים כדורבנות של השר Izhars7  אבל אין לזה כל משמעות אם אחרי כל זה הוא ממשיך לשבת בממשלה הזו asaflib זה מה שקורה כשאדם רציני כמו יזהר שי מבין באיזו ציניות מנהלים כאן את המדינה כדאי לקרוא השר יזהר שי הצביע נגד החלטת הממשלה על הסגר זה מה שהוא אמר לפנות בוקר בישיבה קריאת חובה לכל מי שאכפת לו איך מתקבלו…  AnshelPfeffer מעולם לא התקיים בממשלת ישראל בשעת חירום לאומית דיון כל כך עקר ומנותק מהמציאות מסגירת בתי הכנסת פרשנות שלי הבוקר ב ⁦Haa… benirabin דווקא עכשיו מיליון אנשים שיצאו להפגין בכל יום ויום בכל עיר ועיר בכל פינת רחוב בשעה קבועה itamareichner ממשלה מתנהלת כמו מתנס 4 שעות אחרי סיום ישיבת הממשלה אין עוד הודעה לא יודעים מתי הסגר מתחיל לא יודעים מתי נתבג ייסגר… amirtibon החילונים ייתקעו בבית אסור להם ללכת לפארק או לחוף הים אסור להם לעבוד עכשיו אסור גם להפגין אצל החרדים יהיו עסקים כרגיל ביש… NadavEyal אין אפשרות ליצור אמון בציבור אם מסתבר שגמזו והגורמים המקצועיים לא תמכו בסגר הזה במתכונתו החריפה ואם שורה של שרים מדווחים ש… avischarf מישהו הוציא בחול את הכביסה המלוכלכת על הכביסה המלוכלכת של ביבי</t>
-  </si>
-  <si>
-    <t xml:space="preserve">מהדורת החדשות של N12News במוצאי הצום הייתה תצוגה של רדידות מביכה hodayakh   עשרים שנה לאינתיפאדה השנייה  הפסקול שצמח מתוך הכאב shmunitz   רוצים לשקם את ענף התיירות הפסיקו להנשים אותו מלאכותית  ״נחזיר את האנשים למפלגה עד הבחירות נצליח״ שר ירושלים והמורשת realrafiperets בראיון   47 שנים אחרי ״ידיעת זהב״ נוספת נחשפת ממלחמת יום כיפור הפעם מכיוון סוריה  noamamir74   המחלץ המחולץ והטנק שני הלוחמים נפגשים אחרי 47 שנים ונזכרים ברגעי האימה והגבורה במלחמת יום כיפור   שכחנו מה זה להיות אופוזיציה נטשנו את יו״ש לא עזרנו לרווקים היינו אליטיסטים לא גיבשנו תפיסת עולם כוללת הגזמנו ב…  arielschnabel חמישה ישראלים שלא יכלו לוותר  אולי הטור העצוב ביותר שכתבתי בMakorRishon   ירדן בר כוכבא מסכמת את חמישים השנים הראשונות  הוועדה שתקבע אם תחוברו למכונת הנשמה  RikiRath1   השמאל ימשיך לשסות נגד הימין האידיאולוגי גם הרבה אחרי נתניהו  orlygogo   חסרת שחר תמימה לא מעשית לוקה בעיוורון פוליטי RanBaratz לא התחבר לרעיון עסקת הטיעון עם נתניהו תמורת פרישה מהחיי…  הכינו את המצרכים המנות המושלמות לסעודה המפסקת   האזהרה שמשמיע הרופא הבכיר מחלימים מקורונה עלולים להיות פצצה מהלכת yairkraus   KoheletForum כתבה של ayeletkahana  ב MakorRishon וראיון עם דר אביעד בקשי ראש המחלקה המשפטית בפורום קהלת על חוות הדעת שחיבר עם עו… OrDemb זה נוער זה מפגיני בלפור  הגיע הזמן לפזר את המסיבה batelkol   מלחמת יום כיפור השנייה  arishavit   מי צריך לגלול את כל הפיד כשmoshemem מסכם כל כך יפה את הטוויטר של השבוע   נמאס לכם להיות הפראיירים של הבנקים וחברות הביטוח תקראו את הכתבה הזו  כך ניצחו יהודי שיקגו את הקורונה  JTAnews   יפה בן דוד מטפחת פצצה מתקתקת budarach  מחסוםווטש   הערב ב2030 yairkraus    עד אוקטובר 80 אלף ביום בנובמבר 100 אלף כך מתכוון צה״ל להשתלט על מערך בדיקות הקורונה  noamamir74   למשך שבועיים עם אופציה להארכה אלה ההחמרות של הסגר שיוחל ממחר על ישראל  hodayakh   haggaisegal בחזרה ליום הכיפורים ההוא  MakorRishon  צמד לא חמד קורונה ואנטישמיות  ADL קרול נוריאל דעה  לא נותנים לנגיף לעצור אותם הפלסטינים ממשיכים לבנות שלא כחוק בשטחי C ayeletkahana   ״מבינים שבקרוב תהיה לנו הרבה עבודה״ קברני הקורונה מדברים yairkraus   השלום ממשיך בתוכם נסיונות גישור משמעותיים בין פת״ח לחמאס בעקבות התקרבות ישראל והמפרציות assafgibor   כתב האישום כבר מוכן ממשלת ישראל ופרויקטור הקורונה  כשלתם yairkraus דעה  הנקודה השחורה של איחוד האמירויות  hodayakh   בצה״ל שוקלים סגר מלא על החיילים noamamir74   ״tadmorerez48 וחבריו אינם שונים מהפריקים של בלפור הם תמונת הראי שלהם״ מיכאל טוכפלד דעה  ״את גסטפו״ עובדי מוקדי הבריאות חוטפים אש מהציבור  rathriki   13 אלף הצעות לחיסול הקורונה אחת מהן חייבת לעבוד ד״ר ניר לונדון מכון ויצמן  טראמפ תוקף סין שולטת בארגון הבריאות העולמי  hodayakh   כפי שפרסם yehuday30 כבר בסוף השבוע    למרבה המזל נותר עיתון אחד במדינה שבו לא תיאלצו לקרוא מילים כאלה  מנוי למקור ראשון כוכבית 9248  ויש גם צד שני לפרשה הזו shlomopyuter    חוות הדעת החלופית אם לממשלה אין סמכות גם למנדלבליט אין ayeletkahana   למה בלשכת ראש עיריית טייבה תלויה מפת פלסטין assafgibor   AskAnshul As an Indian its overwhelming to be featured in an Israeli newspaper  Thank you MakorRishon ZvikaKlein  We Indians sta… AskAnshul ZvikaKlein  ZvikaKlein הם לא יהודים ולא נולדו בארץ אבל הנשים והגברים שתכירו במיזם שלפניכם שמו לעצמם מטרה אחת לעמוד לצידה של ישראל ברשתות החברתיו… כך הפך Avrigi לפרזנטור של הפרעות הקשב ZvikaKlein   ובינתיים אצל הפלסטינים  תחושות בגידה ועלבון  assafgibor   מאתרגים את הפגנות בלפור אתם מועלים בתפקידכם העיתונאי hodayakh  מחסוםווטש  הגרעין האיראני טראמפ איתנו וזה חשוב אבל לישראל יש בעיה מול האיש הזה noamamir74   רכבת לילה לדובאי assafgibor   שופטי בג״צ נגד הרב שמואל אליהו אמירות שאינן חוסות תחת חופש הביטוי  ayeletkahana   גלעד שרון בנו של ראש הממשלה לשעבר אריאל שרון ״הסטטוס קוו בהר הבית הידרדר לרעת היהודים זהו שטח ריבוני שלנו״…  האיש לא מושלם אבל הוא התקווה היחידה לניהול המשבר רוני גמזו חייב להישאר בתפקידו yairkraus   ZvikaKlein מזפזפים בין בתי הכנסת כשתפילות ראש השנה הפכו לנטפליקס  בתי הכנסת שאינם אורתודוכסיים מצאו פתרונות טכנולוגיים לשיתוף המתפללי… כשכל הצדדים מחופרים עמוק בפוזיציה המאבק על מינוי מחליפה לשופטת העליון בארה״ב רות ביידר גינסבורג  שנפטרה בסוף השבו…  שוב מזהה תהליכים ח״כ YairGolan1 מזהיר בטור מיוחד ״העולם פתוח ומלא בהזדמנויות ויש גבול עד כמה הצעירים המוכשרים ש…  איך ומדוע קיבלו חריגות בנייה של האו״ם בירושלים הכשר מהמדינה  hodayakh   מנדלבליט ״מעולם לא טענתי שאי אפשר להגביל הפגנה משיקולי שלום הציבור״ yehuday30   שנה טובה ומתוקה לעוקבי הטוויטר של עיתון מקורראשון ולכל עם ישראל בארץ ובעולם תשפ״א  ברוכה הבאה והיי ברוכה כולנו חטאנו כולנו חייבים לתקן ועכשיו  arishavit   השנה שבה התפרקה הקהילה הפיזית סביבנו משה קלוגהפט דעה   למה עשינו את מיזם החיבורים המוזיקליים דווקא עכשיו  YHepstein   זמני החג  זו הייתה השנה הפוליטית שהייתה  Shiritc   השבוע בטוויטר עם moshemem   הילדה מקריית ארבע שחיממה מופע של סטינג  rathriki   IshayShnerb haggaisegal אין ברירה תצטרך לקנות אחת יותר גדולה בהחלט  פסק הלכה מותר לעשות התרת נדרים דרך זום  יוזמה תקיעת שופר ארצית באותה השעה  moshemem   הרב שי פירון ״יש מרכיבים בדת שלא מתכתבים עם קשיי קשב וריכוז״ ZvikaKlein   זה לא סגר זה ישראבלוף yairkraus   שופט בפנסיה שמקבל 90 אלף שקל בחודש קצינים עם קצבה מגיל 42 פצצה מתקתקת ושמה פנסיה תקציבית שרובצת על כתפינו כתפי י…  כשעסקני ההסתדרות נוהגים באלימות shlomopyuter   ״חיזבאללה מורתע״ ריאיון חג עם IDFSpokesperson תא״ל הדי זילברמן  noamamir74   הרגע ההיסטורי שחילק את העולם האסלאמי לשניים assafgibor   ארבעה אורחים במקום תשעים כך מתמודדים בתי חב״ד בעולם עם משבר הקורונה ZvikaKlein   לא פשוט לייצר קאבר לשיר של מאיר בנאי אבל נראה ששולי רנד וכנסיית השכל הצליחו למצוא דרך חדשה לגמרי לשער הרחמים מוזמ…  פרקליטי נתניהו נגד הפרקליטות ״עושה דין לעצמה״ ayeletkahana   מנהלי בתי חולים ישראל אינה ערוכה לגל תחלואה בחורף Shiritc   noamamir74 שוב פעם הפלסטינים הבטיחו הפגנות זעם ןהפגינו בעיקר אדישות אבו מאזן ואנשיו ביקשו לתת ביטוי לתסכולם מחתימת הסכמי השלום עם איח… גורם בטחוני ישראלי בכיר ״הסכם עם סעודיה הוא תסריט אפשרי לגמרי״ hodayakh   מבוכה גדולה ושמה דנה ויס arielschnabel N12News מחסוםווטש  זכות ההפגנה היא זכות יסוד אבל הזכות לחיים יסודית יותר הפגנות בלפור חייבות לעבור שינוי יאיר שלג דעה  הארכת סל הקליטה והבטחת הכנסה כך תסייע הממשלה לעולים חדשים שנפגעו בתקופת הקורונה  ZvikaKlein  pninatamanosh   yehuday30 הם רק ברגים במערכת  צוות קו כחול  התחקיר המלא עלה לרשת   אביתר בנאי ורביד פלוטיניק קיבלו על עצמם לבצע קאבר מרגש להריני של רביד פלוטניק במסגרת פרויקט החיבורים המוזיקלי…  שופר עולמי כך תחגוג יהדות התפוצות את ראש השנה בצל הקורונה  ZvikaKlein   באמירויות חוגגים הפלסטינים מתאבלים assafgibor   עצומת הרבנים בעד עמרם בן אוליאל  מסוכנת הרב יעקב מדן דעה  מנהל ארגון הבריאות העולמי באירופה ״הולך להיות קשה יותר מספר המתים מקורונה ביבשת יגדל בחודשים הקרובים״ AFP   לקראת הטקס ההיסטורי הערב בוושינגטון גורם בבית הלבן ״אופטימי לקראת מדינות נוספות שיצטרפו בהמשך״ hodayakh   תזכורת לליכודניקים naftalibennett bezalelsm וAyeletShaked  עושים בדיוק את מה שמצופה מהם להיות אופוזיציה דע…  מסמך דוקומנטרי מרשים על הסדרה של roysharon11 וgalberger בkann שחוזרת לימי האימים של האינתיפאדה השנייה…  כדי להפיל את נתניהו ליברמן יגרור את כולנו לאנרכיה קרני אלדד דעה   הציבור החרדי לא אשם מנהיגיו כן מיכאל טוכפלד דעה  גורם בפמליית נתניהו ההסכם לא כולל הקפאת ההתיישבות hodayakh   אנחנו גאים להציג שיח סליחות מסוג חדש פרויקט זההזמןלסלוח מביא עיבודים מחודשים של המוזיקאי יעקב אסרף לשירי סליחה מו…  המתכונים שיסגרו לכם את ארוחות החג  המשטרה משבר הקורונה מביא לעלייה חדה באלימות על רקע כלכלי yairkraus   בג״צ בביקורת על מנדלבליט ההדלפות בתיק 4000 הן פגיעה מערכתית ודורשות חקירה ayeletkahana   יום לפני החתימה עדיין לא ברורים פרטי ההסכמים עם איחוד האמירויות ובחריין hodayakh עם פמליית netanyahu בוושינגטון  לא באמת חשבתם שהטור הזה יישאר בלי תגובה חדה של gershuni שטוען  האג׳נדה הסביבתנית הקיצונית מנוגדת לתורה…  כך הגיעו מאבקי השליטה בעכו לנקודת רתיחה מסוכנת  yairkraus   ״הישרדות״ היא מראה מדויקת לכל מה שמכוער בנו מחסוםווטש  משרד התקשורת לחברות הסלולר השלימו את הפריסה ביהודה ושומרון   הישרדות 2020 האם כחוללבן והעבודה יתמזגו  Shiritc   ממותות במקום מטוסים  AFP   קבינט הפיוס שדווקא כן מתכנס  YHepstein   קורה עכשיו ערב שיח וזיכרון לקורבנות הזנות בישראל הצטרפו לשידור החי בפייסבוק ובאתר מקורראשון   אג׳נדה ירוקה היא מצווה מהתורה דעה adamteva   מהדורות חדשות סוף השבוע הפכו לגיא פינס וזו לא מחמאה  aviyashklar   מפתח המודל שצדק עד כה ב25 מתוך 27 מערכות בחירות לנשיאות ארה״ב מעניק כעת לטראמפ 91 אחוזים לעומת תשעה אחוז בלבד לבי…  ריבונות לפני החורף habithonistim טוענים שזה אפשרי hodayakh   כמה זה עולה לנו חשש בימין מההסכם עם בחריין hodayakh   batelkol תראו מה aviyashklar  הרימה ערב שיח וזיכרון לקורבנות בזנות ב 2100 בפייסבוק ובאתר MakorRishon  האם נמל חיפה יעבור לידי האמירתים  assafgibor   רוצים להימנע מסגר תנו סמכויות לשלטון המקומי ERSpeiser   מאיים באקדח ריק המפלגות החרדיות לא ממהרות להצטרף לאיומי הפרישה של ליצמן  Shiritc   מסיבת טבע אינה משחררת היא יותר דומה למאסר עולם orlygogo   אז אולי בכל זאת יש בתקינות הפוליטית המאוסה הזו משהו נכון arielschnabel   YotYotam גילה מחדש את הגוגואים זה נגמר בדמעות  matanamirr akivanovick השאר פרטים כתובת וטלפון בעיקר בדיאם ונדאג לך ״החזקים ישרדו״  סיור מדאיג בערים האדומות במגזר הערבי  assafgibor   ארי שביט הפרקליטות רואה בנתניהו אויב  דעה תרבות האונס קיימת גם בציונות הדתית  batelkol   הבעיה עם שומרי הסף RanBaratz   המסכה ירדה האופי הישראלי התגלה והוא לא משהו haggaisegal   מעבר להררי הפוזיציה האם מחאת בלפור תורמת להתפשטות הקורונה או לא  yairkraus   רבים כבר הספידו את כוחה הפוליטי של הציונות הדתית ובכן רבים טועים Shiritc   עמדה ראש השנה צריך לחזור ולהיות חג של יום אחד בלבד  מי באמת קובע את הכללים בנוגע להתיישבות ביו״ש לא בטוח שתאהבו את התשובה תחקיר מאת yehuday30   המדריך השבועי לטוויטר הישראלי  moshemem   מרגרינה היא לא מילה גסה ראיון מפתיע עם גיל חובב rathriki   יורדים ליגה למה הפלסטינים מאיימים לפרוש מהליגה הערבית  assafgibor   סגר הוא האופציה הגרועה ביותר והיחידה שנותרה כתב הבריאות שלנו yairkraus בטור זועם  את השאילתא הגישה חברת הכנסת MichalShir הכן מאחזך לחורף השר MichaelBiton4 התחייב לפיילוט חיבור לחשמל לשלושה מאחזים ביו״ש hodayakh   המטרה לפצח את מנגנון הקורונה  ״הדברים שנאמרים נגד נתניהו גרועים בהרבה מאלה שנאמרו על רבין לפני הרצח״ הרב חיים נבון דעה  הוליווד החליטה תקינות פוליטית חשובה ממקצוענות budarach   החוקר שהביא להרשעת זדורוב מודה בראיון ראשון יש ברצח של תאיר ראדה תעלומה שלא פתרנו  גם פחמימות הן סוג של נחמה מתכוני לזניה שיסייעו לכם לצלוח את הפיד   מטוסים עמוסי קוקאין מעל חורבות המאיה כך נראה נתיב הסמים העמוס בעולם  washingtonpost   משכילים אאוט פליטים אין משבר ההון האנושי של טורקיה   לימין ישראל ארה״ב מטילה סנקציות על חיזבאללה  assafgibor   חושבים לקחת הלוואה תחשבו שוב ושוב   בכירים במח״ש נגד המפכ״ל לשעבר אלשייך ayeletkahana   נקלעה לסיטואציה למי בכלל יש זמן לקורונה בשנת בחירות  Shiritc   למה השר AmirOhana לא חותם על החוק לאיסור צריכת זנות  aviyashklar   מקדימים תרופה מבצע מעצרים נרחב וחריג ביו״ש  noamamir74   התלוננתם על אלימות משטרתית ברוב המקרים כאן זה ייגמר  ayeletkahana   הפאנל מרוט ומתיש המערכונים המצולמים מצויינים ספיישל אמש הראה ארץ חצי נהדרת ואיך היה yanivbiton99…  זוהי צפירת ארגעה לתושבי חאן אל אחמר ממשלת ישראל לא תפנה אתכם  noamamir74   בראש טבלת התלונות ביטוח לאומי  ayeletkahana   כך מקרב המשבר הכלכלי ברשות בין הפלסטינים לישראל assafgibor   kerenmelamed רשמנו לפנינו מחפשים אסקפיזם הסדרה הזו ממש לא בשבילכם kerenmelamed   דיכטר נגד נתניהו חייבים לפנות את חאן אל אחמר מיד״ Shiritc   150 שוטרים נדבקו בהפגנות פייק ניוז yairkraus   מנאייכ על ספידים למה הפרשה שחשף אמש amitsegal מרתיחה במיוחד  shlomopyuter   בעקבות חשיפת amitsegal הערב  שימו לב לכתבתו של פרשן המשפט של מקורראשון yehuday30 לפני למעלה משנתיים  Shiritc ביקשתי את תגובת שר המשפטים לחשיפת עמית סגל בחדשות 12 על מעללי ניצן וצמרת הפרקליטות ומחש היא לא צפויה להתקבל הערב שייקספיר צדק משהו רקוב בממלכת דנמרק  ZvikaKlein   ישראל השנייה תמשיך לחכות כך מוסמסו החלטות ועדת ביטון במשרד החינוך    Shiritc אצל סוכני החיברות הטלוויזיוניים דבר אחד עדיף שהן לא יבחרו – להתלבש בצניעות תהיי מי שאת העיקר שזה יהיה בביקיני  אב…  ואיזה יופי שאולי אף פעם לא נדע   talshalev1 Shiritc אנחנו בקטע טל תודה מתואמים בינהם או לא זאת השאלה   לכל המעריצים החדשים של RoyIddan   איילת כהנא כתבת המשפט שלנו עושה לכם קצת סדר בראש  ayeletkahana    החברה הערבית בישראל נמצאת באחד המשברים הרפואיים הגדולים ביותר שחוותה מתוך רשימת 23 היישובים האדומים בישראל שבהם כמ…  ZvikaKlein הקומיקאי היהודי שרוצה להתמודד לנשיאות ארהב  הקורונה הביאה לצומת דרכים את הקריירה המצליחה של הקומיקאי היהודי–אמריקני מודי ר… Game over חביבי  noamamir74 צה״ל לא תוקף הלילה ברצועת עזה ומאותת לחמאס שהוא נותן צ׳אנס להרגעה האם העלייה בתחלואה בנגיף הקורונה בעזה תביא את השקט עכשי… כל עוד מרידור היה מסוגל לבצע את הנחיותיו של השר  גם אם תוך חריקת שיניים הוא היה יכול להישאר בתפקידו ברגע שהמצפון…  צד אחד אנחנו דורשים בכל תוקף לחיות חיים נורמליים – ומצד אחר אנחנו מתלוננים על שהמגפה לא הודברה מצד אחד אנחנו רוצים…  yairkraus פייק ניוז תוכניות סאטירה מחליפים בשלט בטח אם מדובר בערוץ מסחרי שכל שיקוליו נתונים לפרסומת הבאה שנכנסת כך מצא את עצמו אביר…  בכל מקרה בלי שתי בדיקות שליליות  שבועיים בידוד  משהו לאכול אל תגיע yairkraus  למערכת תודה   שני יהודים הגיעו לאי בודד ורצו להקים בית כנסת לא תאמינו מה קרה אחר כך  Shiritc  מה שמות האסירים הביטחוניים המשמשים כדוברים ומתווכים בין שלטונות הכלא לבין שאר האסירים הביטחונייםהאם מדובר באסירים…  קוים לדמותה של החגיגה הצהובה והחולנית של אמצעי תקשורת שמפרסמים תיאורי אונס קשים ונוראים תחת הכותרת איך זה מרגיש א…  איך כתב RoyIddan   צהל הצבא הכי מוסרי בעולם וגם היחיד שמשתתף בתחרות הזאת hodayakh מתחברת מחסוםWatch   לא רק שעיירות פיתוח כדוגמת בית־שאן קופחו בשטחים שבעבר שימשו רק לחקלאות והיום משמשים את בעליהם גם למטרות מסחריות אל…  להיות או לא להיות    הנה בא השלום בכפוף לפס גלישה רחב   לבנט ולמפלגות בראשותו יש היסטוריה של התרסקות בסיום מסע הבחירות לאחר פתיחה גבוהה הוא ואנשיו צריכים לעת עתה להשקיע…  נטפליקס כבר על זה  איפה שאתם רואים פקקים אנחנו רואים מחלפים חדשים   מילה לא תצא מאיתנו yairkraus  yoavr ZvikaKlein IsraelDiaspora omeryankelevitc davidbitan מי זה יקי קוראים לי אוריך yoavr ZvikaKlein IsraelDiaspora omeryankelevitc davidbitan יש סעיף תקצוב לפודקאסטים של מארק מארון היא יודעת שזה לא כל כך קול אבל לא ממש אכפת לה  יעלי נגיד מזרחי ממש שמחה לראות את ההפגנה אתמול נגד היהודים באים…  איש לא שאל שאלות קשות ואיש לא פצה פה חוץ מאישה אחת אמיצה וחכמה אשר חשבה שמה שמתרחש בארץ לא ראוי ולא נכון והחליט…  לא יכולים לדבר על זה יותר מדי אבל פרויקט מיוחד שלנו נמצא על האש בקרוב גם אצלכם   shlomopyuter דבר מה אתה צריך hananamiur אז מה היה לנו שם ריגולז ברקס פלגים פלטינות ריבונות עסקת המאה   אבל על מי האלמנט  חישוב המחיר והתועלת של…  מישהו </t>
-  </si>
-  <si>
-    <t>כולם פה עם המלצות קריאה אז זה מה שאני קראתי ביום הכיפורים  amsterdamski2 יש בארץ לא מעט רופאים שמחכים לתקן שיתפנה למשל כאלה שמחכים לפעמים שנתיים שיתפנה מקום להתמחות במחלקה מסוימת וכמובן הכפלת משכורת לצוותי הרפואה במחלקות הקורונה כפול ועדיין יישאר הרבה עודף מה20 מיליארד 12med865 איך אין ווינר לזה איך  Irisleal15 יפ Irisleal15 הטרלה של צייצנית ותיקה בדיוק במקום לשפוך לביוב 20 מיליארד שקל על סגר פוליטי קחו את הכסף הזה ושימו על מערכת הבריאות 500 תקנים לרופאים 2…  בנט לפני כמעט ארבעה חודשים  למה לא ליוו אותו למעצר זה מה שלא ברור לי  avigrin10 לעדכונך היועמש הוא ראש התביעה הכללית לא בדיוק פקיד אחד ואם אתה כבר רוצה ללמוד מארהב בוא תתחיל עם…  eitanzeliger למשל Doco28 מקסים DavidLifshitz מי שהכניס לארץ טיסות של אברכים מברוקלין האדומה מי שלא סגר ערים חרדיות בגלל שיקולים פוליטיים ובמקום זה סגר בסוף את כולנו… avigrin10 אתה מבין שאתה עושה בדיוק מה שאתה מבקש שלא יעשו נכון motiszuszan1958 הרגע קלטתי שאתה גם מאיית שוּשן בכתיב פולני motiszuszan1958 שימחת אותי מאוד עם כתיב יידישאי מדויק מול מיליארד אנשים שחושבים שביידיש פשוט תוקעים ע פה ושם חתימה דלוקס מוטי תביאו לי את האנשים האלה אני רוצה לשמוע מה הם אומרים עכשיו  odedkramer שר שדקה לפני שנכנס הסגר השני ארגן מסיבה וטען ההוראות עדיין לא בתוקף יוצא נגד אנשים שעשו בדיוק אותו הדבר אין גבול לחוסר… ב8221 אם לגבי כל מאומת מגיעים במהירות ל10 מגעים עשרה ימים אחורה זה קצב של כמעט 3 מיליון איש בבידוד בחודש זה…  Ronkofman1 למי שתוהה מהו הרוטב הסודי המופיע במתכון  BenCaspit הראשון שזיהה קישון הגדול עע זהוזה  idoefrati1 קורונה מספר מתים יומי למיליון נפש ממוצע שבועי  24 באפריל  ישראל   084 בריטניה – 121 ארהב – 72 האיחוד האירופי –… Niro זה פאה haaretzcom AnshelPfeffer Who has  who’s Not whose EstyS גבירותי ורבותי ראש הממשלה שלכם  hagitw כן 1966 אבא שלי אליק היום תשע שנים למותו  zionnenko BenMittelman HaOshIa ranboker את זה כל ילד יודע אתה רוצה להרשים  תן שעה מדויקת ומספר רישיון טיס VigyRotem akivanovick moshenayes הלוואי שגם אני הייתי akivanovick moshenayes  הילדים שלי יושבים בחצר עם פיצה והראש במסכי הסלולרים אני מתקרב לברר מה יש שם שדחוף להם לראות קרן מרציאנו לא סלחתי לא אסלח N12News מי היה כאן ראש הממשלה בחצי השנה האחרונה אולי גם לו יש אחריות כך הגיבה KerenMarc  להצהרת ראש הממשלה  Nefolet קרן מרציאנו תמצתה את הנאום של ביבי במדויק ״זה נאום אני מאשים  אתכם״ amsterdamski2 AyeletShaked הלוואה מהמלצרית של ריקלין dimikolo YairNentanyahu זה לא הוא תסתכל על היוזר הבהרה חשובה הכוונה לתלמידי ישיבות שמאלנים שמפגינים בבלפור  shiri19801 BershadMr seerpico1 אנחנו גם עושים חילופי זוגות liorchorev קומה שנוצטרה subtext100 NaimNaor קצב ממוצע של 155 תווים בשנייה  כולל רווחים וסימני פיסוק מילה ממוצעת בעברית היא 5 אותיות כ…  shiri19801 seerpico1 זאת הייתה כתבה של מוסקו NeriaKraus הצעת פשרה שם הרחוב יוסב לרחוב מלכה לייפר chardimk שייקספיר מקבת כמובן יפה שעלית על זה גם מיליון כביסות בכל מרככי הכביסה המבושמים של אמריקה לא יצליחו לכסות על סירחון מחדל הקורונה AmichaiStein1 זעקת גמזו בישיבת הממשלה  פאקינג לא ייאמן  yaircherki ״מי שמתקשה בצום יוכל להתפלל במבנה סגור״  מי שבקבוצת סיכון יוכנס למקום שימקסם את סיכוייו להידבק איפה ההיגיון אבל המפגינים בבלפור  hamakom סיור בבירה החרדית מגלה שיירות של ילדות בילקוטים מוסדות תלמוד תורה שוקקים ומחנכים שמתחננים שלא נחשוף את הסוד בזמן שהקבינט דן… אבל בכיכר פריז זאת מסיבת הדבקה  asafkfir אופס  ברייקינג פרס נובל ברפואה יוענק השנה למגלי התרופה לווירוס הקורונה  איסור על הפגנות נגד נתניהו מעריך שד״ר שרון אלרועי עשתה אתמול צעד גדול לקראת מינויה לפרויקטור ב111 baruchikra בדיוק אין לתאר  יבוא אישי  JordanUhl checkmate fauci  BarShemUr העצוב זה שטופז דווקא כן בגיל guyzo ניצחנו בפער לדעתי יאללה לפתוח את הקווים תביאו את השאלות מכל העולם תקשיבו לגלצ ביום חול רגיל יום אחד יספיק ותדעו בדיוק איך להתקבל לתחנה של דקלאלקבץ באמת שקורס זה הדבר האחרון שצריך GadiTaub1 Riklin10 כן זה באמת מנהג חדש שם gilicohen10 יועצו של רהמ נתניהו טופז לוק שהה בהפגנה בסמוך לבית ראש הממשלה בבלפור לאחר שביצע את בדיקת הקורונה  כך עולה מנתוני הציל… zionnenko זה מעגל שני לא רואה סיבה שעופר גולן ייכנס לבידוד בעיני השימוש בבידוד כאמצעי ענישה נקמה השתקה או הרחקה פוליטית מסוכן מאוד naimleee בדרך לבדיקת קורונה עוצרים בהפגנה המונית talschneider בתגובה לעיל יש כמה בעיות א דוברות הליכוד לא ענתה לשאלה אם לוק היה שם ולאיזה מטרה ב מתחם הבדיקות לנוסעי מטוס רהמ היה לי… Nefolet טופז לוק היה בדרכו לבצע בדיקת קורונה אצל המלצרית של ריקלין LevineHagai ישראל צריכה סדר לא סגר סגר זה עוצר עם יחסי ציבור צריך לעצור התקהלויות בחלל סגור לא את התנועה האקורדיון הוא אסון הוא מוע… NitzanWaisberg אורן קיבל דוח על מסיכה ערער ויצא זכאי  איך הוא עשה את זה  הוא הציג תמונות מחודש אוגוסט של הנאשם השר לבטחון פנים וב… Shualaravot אמרתי בפירוש אין עדיין חיסון וגם כשיהיה חיסון הוא לא יהיה מה שאתם חושבים אני חושב שלא ייחדנו מספיק תשומת לב להצעה של ריקלין להמתין לטעות של הנגיף ואז לתקוף nadavabeksis ruthelbaz yigal1957 שעה לפתוח אצלך את הדלת בבית שעה אם יש שריפה וצריך לברוח אל תנסה את הדלת או חלון או ישר לשמע ישראל amsterdamski2 אפרסק כתום כלומר אמיתי בטעם של שנות ה70 כלומר כשעוד היה לו טעם לפני שהפך לקולורבי עטוף זמש עם חיי מדף jamesbb25 אני יכול להגיד לך את היצרן של השתל 12med865 גם הפרס ברפואה ההצעה להכליל מיסופוניה בDSM לא ממש מגוחך אני מכיר מישהי שסובלת מזה וזה אכן מקשה מאוד…  12med865 פסיכולוגיה לא פיזיולוגיה ובהנחה שיש מיתאם במה זה יותר מגוחך או פחות מועיל מאינסוף מחקרים על זיהוי שקרנים לפי מחוות גוף yairlapid קשה לחבק ולהצדיע בוזמנית Riklin10 ההומור שלך משהו Riklin10 שכחת להגיד שמפגיני בלפור אשמים מהמקפצה  Riklin10 מי בדיוק אמרת שלא דואג לעם ישראל מי מסכן את חיינו מי יגרום להארכת הסגר  segaleran העברנו לנובי גוד alonbeer1 ההיגיון כולו על רגל אחתהשרה מרב כהןתלך לאכול ארוחת ערב עם ההורים היום כי מחר אסורהוירוס לא עובד בחמישימתחיל משמרת רק מחר… לידיעת כלבי הדשבורד  haimhz שאלה לי אליכם idfonline  למה נועה קירל חיילת בשירות סדיר מופיעה בסרטון של נבחר ציבור שהועלה לעמוד האישי והפוליטי שלו לא ל… ErelSegal YakovSela אם ההלכה הייתה מכירה את הקורונה המקווה היה איסור חמור הרעיון של מקווה הוא טהרה לא הפצת מחלות עם חצי אחוז תמותה MeytalinkaVan  rottemd משרד הבריאות שלום לאחר שנודע כי ישנה התפרצות קורונה בבית הלבן ברצוני לדווח כי ראיתי מספר לא מבוטל של ישראלים אתמול באותו המק… danakarni Yesssssssss ברור לכם שריבלין נושא נאום שהוא כתב לנתניהו כן shimritmeir yaronavraham כי זה הגיוני OferFarandyan galit577917912 amitsegal ועכשיו רואה הבדל  OferFarandyan galit577917912 amitsegal המספרים שונים לחלוטין אני מבין שהיית מעדיף וירוס מהונדס בדיוק לאירועים…  OferFarandyan amitsegal לא שכחתי צא מהפוזיציה אם תביא נתונים שבהפגנות יש אחוז הדבקה שמתקרב לישיבות חתונות ומו…  amitsegal קחו שני מיליארד מתוך ה20 ותנו למערכת הבריאות ותבטלו את הסגרדמיקולו הזה הרבה יותר מועיל נגד הווירוס…  NehemiaGA לא כי תפילות זה באופן כללי מופת של לוגיקה GadiTaub1 הפנה אותי בבקשה לספרי הלימוד בישראל שבהם מופיעים שטחי הרש״פ shimritmeir טוב יאללה אחרון ודי shimritmeir ראש הממשלה כשינחת יצטרך לחתוך בסכין או שמבטלים את הסגר במתכונתו המגוחכת הנוכחית או שמבטלים לאלתר את כל ההחרגות סגרסגר… N12News דפנה ליאל מפרסמת כשנתניהו כבר בארהב התברר שרק שר חוץ מוסמך לחתום על ההסכם DaphnaLiel RinoZror זה בשביל הפרק החיובי של השבחים רינו בקיצור חילונים בערים ירוקות ושמאלנים מפגיני בלפור  תסתגרו בבית דתיים ומצביעי ליכוד  יאללה שנה טובה משוחררים חבר…  NitzSha ברור shimritmeir זה עדיין פרמטרים טכניים סוגרים את הים ופותחים בתי כנסת אבל בלי לקבוע אם יגיעו לשם דתיים או חילונים ייצא מה שייצא avishaiz NehemiaGA זה בקטע סאטירי TheMaya IlanLukatch  סגר בראש השנה על ערים ירוקות הגיוני כמו סגר על בני ברק בנובי גוד NehemiaGA בוא תצטט גם את כתב הצרכנות של הדי אולגה אבל דחוף להכניס את קיבוץ שפיים לעוצר סגרפוליטי   יש שתי אפשרויות או שהבידוד לא דרוש כשהבדיקה שלילית  או שמאבטחיו ורופאו האישי של האדם המאובטח והשמור ביותר במדינה…  roysharon11 כמו שכולם יודעים שאחת שתיים שלוש ארבע  מגרמניה היטלר בא הוא שיר עממי משנות ה50 נכון רועי עכשיו…  DaphnaLiel מאות אנשים ישתתפו בטקס בוושינגטון ועדיין נתניהו ופמלייתו לא יחוייבו בבידוד עם שובם יסתפקו בבדיקת קורונה לך תשכנע אחרי זה… NehemiaGA זה מדויק לחלוטין שמעתי מרופאים בכירים את שתי הדעות מנתונים עולמיים גם של הקורונה וגם של אפידמיות שקד…  מה נסגר עם השופטים האלה לא קלטו שעמירם בן אוליאל שרף את משפחת דוואבשה בקטע סאטירי שמישהו יעדכן את יגאל עמיר 20 שינון התכוון לסאטירה zionnenko ועוד דבר אפשר רק לדמיין את הדיונים הדחופים בכנסת והקריאות לפיטורין לו גיא פלג באותה תחנת רדיו או RinoZror בגלצ היו מאומרי… ShiraHN Riklin10 neoraytal BarakRavid אני בדיוק עובדת על קטע יותר ארוך על ההבדל בין עיתונות לאמנות אבל להגיד סאטירה זה לא כמו … idogur קודם כל אני רוצה להגיד תודה ענקית לתוכנית הספורט של 103 שנתנה לי במה מרכזית במשך כמה שנים טובות נהניתי מכל שנייה בכל שיחה לצע… Riklin10 YonatanKit חחח הרגת  magazineLiberal הכותבים המשתתפים בגיליון ״משפיעים 2020״ של ליברל EliBitan Meravbenari avrahamdov NechamaDuek AmalyaDuek YaronD… odaskal זה היה קטע סאטירי  לא יאמן  אשמים הם האנשים שנותנים לו את הבמה ב103   לא פאקינג יאמן AssafYNews OferHadad יש מישהו ספציפי שהיית רוצה לציין במיוחד בכישלון הזה או שזה כל הממשלה ככה יחד כמיקשה אחת odaskal המגזר העסקי יושב בבית ולא באמת יכול לעבוד כי הילדים על הראש שלו אבל לפחות המדינה עשתה הסדרי תפילה להמשך הדבקה בבתי כנסת הגיונ… ISudri איציק אני זוכר שהגבת באופן דומה להוגה המדיני אלירז שדה ואני מקווה שהעיסוק שלי אשלח בפרטי רזומה מאפשר לי ב…  ShaniAshkenazi בתי כנסת  מהמקומות שהתרחשו בהם הכי הרבה הדבקות יפעלו כמעט כרגיל עד 120 איש בחלל סגור בעיר אדומה בית קפה בעיר ירוקה… praklitut גם הבוקר לצערנו ממשיכים לפרסם פייק ניוז לגבי בני משפחתה של ליאת בןארי שווקי למען הסר ספק הפרסום בגלי ישראל IsraelGal… nadavabeksis zionnenko סיריוסלי נדב לא הייתה פעם אחת שמנהל בי״ח אמר שחסר לו תקציב ולא בצדק אם יש הבדל אז הוא ל…  סגר על כפר מל״ל דחוף  mossiraz היום הבנתי מה פירוש הביטוי האירוניה התאבדה כששמעתי את עמיר פרץ אומר שהבעיה שלנו היא אובדן האמון nadavabeksis zionnenko כן נדב זה באמת נורא שבתי חולים יקבלו תקציבים בואו ניזכר לרגע בפעם האחרונה שמישהי מחתה נגד הרעבת מערכת הבריאות בפריפריה ובתגובה הספונטנית של ביבי ״את משעממת או…  טים רינה  אפקט הפרפר 2020 בוויזניץ עושים חתונה המונית ועל קיבוץ קליה מוטל עוצר סגר פוליטי מיותר זה בפרטיטורה של רסיטל הנשפנים ״תפילה חשובה יותר מהפגנה״ כותב ריקלין ״רוצים סגר כי קורונה מאה…  GalDeLevie עוצמים עיניים עכשיו תדמיינו את אהוד אולמרט נוסע לטקס בוושינגטון באמצע מלחמת לבנון כל מילה  הכוונה לעזמי בשארה למי שלא הבין  GadiTaub1 יאיר גולן צודק ולא בפעם הראשונה אגב GadiTaub1 OrenNahari בוא נדבר על חברים באמת  segaleran האם יש אנשים שמחוסנים טבעית לקורונה מבלי שנחשפו  מחקר חדש שלנו מצא תגובה חיסונית צולבת בין הקורונה ה׳רעה׳ לבין קורונות עו… DaphnaLiel מכל החרא שאנחנו שקועים בו עד צוואר המחשבה האופטימית היחידה היא שעוד חודשיים תיגמר הטעות ההיסטורית האיומה ששמה הנשיא דונלד טראמפ amsterdamski2 tamarishshalom לא צנוע דברים לחשוב עליהם בזמן שאתם נחנקים בסגר מיותר  לרבים ששואלים על עמוד ההשוואות המדהים של אוקספורד הנה הלינק  ממדליסטים למחדליסטים gorodezk amsterdamski2 כשביבי ובוגי יהיו רופאים יפנו גם אליהם בתואר אגב לפרופ׳ גמזו יש שני דוקטורטים שני מאסטרים ותואר במשפטים amsterdamski2 אגב ממתי זה מר גמזו הוא פרופסור הזדכה על המר ביציאה מביס לרפואה לפני 26 שנים amsterdamski2 יושב וקורא את פרוטוקול ישיבת קבינט הקורונה מחמישי ופתאום קולט שנפלה שם טעות סופר פרוידיאנית  chaimlevinson נישתי hadarse פרופ׳ חגי לוין ברור וחד משמעי הפקירו אותנו הכל פוליטי גם הסגר הצפוי  זה פשוט עצוב  chaimlevinson מאמי צרחותתתתת ואני על האלגנט הספורטיבי orenaharoni1 zionnenko unh axuck vo fnuci vjukho zionnenko הרגת לי את משפט הסיום לכתבה של מחר ivgiz בגימטריה  אדוה דדון רוברט ג׳ונסון  672 חיים אתגר  672 ממנשן את המומחה  shlomokarhi שנון הדוקטור  הלם  פצצת אטום 20 וכמו כן בוקר טוב אליהו  מתלבט בין ריקלין לאלירז שדה  gilshil yoelituv כמדד אמין כל השאר הרבה פחות אמינים אבל ברור שיש להם משמעות YoazHendel1 ריאלי כמו משהו מאוד ריאלי NehemiaGA yoelituv חשיבות כן אבל האינדיקציה האמינה למגמות היא מספר המתים מספר המאומתים יכול לשמש אותך להערכה …  yoelituv מספר המאומתים אינו אומר דבר מלבד זה שעושים יותר בדיקות וממקדים אותן איפה שצריך ואלה דווקא חדשות טובות ס…  MDarabaner פה ניסיתי להסביר את ההבדלים באופן שלא מצריך רקע מדעי    celestialannihi אכן דיוק חשוב תודה זה החיסון של אוקספורד אסטרהזנקה והוא מבוסס על אדנוֹוירוס כמו החיסון הרוסי אירוע מעניין מאוד  guyro13 מכירים את החברים כאן גם אני לא אבל הם זכו באליפות העולםבמקצוע הכי נוראי אבר במתמטיקה  הם גברו על רוסיהארהב ספרד אנגלי… yaronavraham BenMittelman עיקר הסכנה אכן נשקפה מסצינת המועדונים של בני ברק ומהפאבים הטרנדיים של טייבה CohenAsaf בשר טחון עם חציל בפיתה כמה הבהרות  1 היטלר בא מאוסטריה 2 אפשר לאכן סלולרי גם כשהוא כבוי 3 מי שפועל הפוך מדרישות המומחים שהוא עצמו מינה לא רשאי להטיף לאחרים YoavRibak יו״ר הכנסת יריב לוין בתגובה לליברמן זה חוסר אחריות במדינה דמוקרטית אי אפשר לעודד אי ציות למוסדות שהם לא בית המשפט העליון igalmosko המסיבה על הטיטאניק ממשיכה כרגיל  yaircherki קראתי ומכיר ועד כמה שהבנתי זה כבר לא נספר ככה yaircherki אסימפטומטי הוא עדיין מדבק ומדבק הרבה יותר מחולה תסמיני כי הוא לא יודע שנדבק והוא לא בבידוד freyisrael1 בעזרת הקומבינה ננצח את הקורונה תושבי בני ברק קיבלו הודעה קולית מלשכת ראש העיר בה התבקשו לצאת ולהיבדק מומלץ להביא ילדים… ayakorem יש סרט שלם ג׳מפינג ג׳ק פלאש סביב זה שבסטונז תמיד דחפו את השירה למעמקי המיקס עד שלפעמים קשה לאמריקאים…  radio103fm אוהד חמו ohadh1 חדשות 12 מחבר הספר פני השטח המגמה כרגע בשטחים שאני שומע בעיקר מכיוון הצעירים זה ויתור על מדינה פלסטי… תתחדש  aradnir ״האומץ הוא מה שנדרש כדי לקום ולדבר אומץ הוא גם מה שנדרש כדי לשבת ולהקשיב״ ווינסטון צ׳רצ׳יל פרופ׳ אייל לשם איש אמיץ  עומד… N12News סגר כללי  כישלון של החברה הישראלית וההנהגה שבראשה  פרופ אייל לשם דעה gt   צילום אוליבר פיטוסי  פל… לציוץ שהעליתי בתאריך 247 בעניין אבנר נתניהו שממנו משתמע שהוא הריע לשירי הלל ליגאל עמיר לא היה כל בסיס והוא נמחק…  rabeabader עד היום נדבקו בקורונה בכנסת ממשלה יותר אנשים מאשר בהפגנות ניסיון רצח  Nefolet משוכנע שהם גם עושים ניסויי צ׳לנג׳ דיקטטורה זה לא פיקניק attilus ובכן אטילה כפי שכתבתי  רסיטל פחות מוצלח של ריקלין  roysharon11 מכתב ששלחה תושבת איתמר בתפוצה פנימית הרגע שבו היא הבינה שרעולי הפנים שיידו עליה אבנים בדרך הביתה היו יהודים  hadover1 מהמם אבל מביני דבר מעדיפים מוקה YoavNews1 netanyahu זה יפה איך אתה ממנשן את נתניהו בסוף כל רסיטל רוצה להסביר למה sinnerinnorth GadiTaub1 איזה מחקר אתה צריך יש נתונים מסתכלים על הנתונים אין גם ״מחקר״ על ההדבקה בטייבה ובאלע…  sinnerinnorth GadiTaub1 יש לי יותר מאשר מושג היו לי שיחות עם חוקרים יש נתונים אין עלייה בהדבקה הנתונים מארה…  RotemShtarkman יש עוד תשובה אתה יודע ולוּ רק בשביל הפריים הזה היה צריך להמציא את המימרה תמונה אחת שווה אלף מילים  sinnerinnorth GadiTaub1 אני לא בדיוק עובד אצלך אתה יודע הנתונים מירושלים נמצאים אין לינק נתונים מההפגנות בא…  sinnerinnorth GadiTaub1 יש נתונים בהחלט וחוץ מזה  כמה לדעתך ממפגיני בלפור באים מבני ברק טייבה אלעד וג׳לג׳וליה GadiTaub1 שום חלק גדי הפגנות באוויר הפתוח לא מייצרות עלייה בהדבקות גם פה גם בארה״ב נבדק אמפירית שוב ושוב ביולוגיה ללא פוזיציה AssafYNews גורם בכיר תכנית הרמזור הייתה רלבנטית לפני חודש עכשיו אין מנוס מסגר מיידי 🤔 האם זה הגורם הבכיר שמרח את מינוי הפרוייקטור… EHaski2 שמח שנהנית מחקתי כי החלטתי שאתה לא מספיק מעניין בשביל לספק לך טראפיק מי שמסתיר יש לו מה להסתיר בדיוק כמו שמי שמסרב לבדיקת ינשוף נשפט כמי שנהג שיכור ככה ישיבה שתסרב לבדיקות צריכה להי…  urieltzaitlin yoch21 ספר לי בבקשה מתי החולירות מאילת הציגו את עצמם כצדיקי עליון מורים רוחניים ומטיפי מוסר עם שעות קבלה לצאן מרעיתם PlotkinYuval לכאורה גיזס איזה סתומים אבל 1 בוא תיזכר לרגע מה קרה לשיר All Along the Watchtower אחרי שהנדריקס ה…  DaphnaLiel הוא ימין מדיני ושמאל מגיני</t>
-  </si>
-  <si>
-    <t xml:space="preserve">menishwartz הטענה שלי לא נוגעת להתנהלות הציבור החרדי אלא לכך שפוסקים לציבור הרחב על פי הפלגים שלא מצייתים להוראות…  shlomohohoyzer אבל שס ודגל קיבלו החלטות על הציבור הרחב על פי התנהגות הצפויה של בעלזא ויזניץ  shlomohohoyzer בוודאי אבל לצערינו ההחלטות לא מתקבלות על פי החרדי המתון אלא על פי הקיצוניים ההוראה להשאיר את בתי…  wV1XDpZBurJa8Y4 לא הבנת אני לא כותב שהציבור הרחב צריך לקבוע לחרדים אלא  שהחרדים לא צריכים לקבוע לציבור הרחב RozenblatDavid Orfadid נשמע פוטנציאל לשיחה משעשעת Kirilon1 לא סותר זה חוסר הבנת הנקרא כנראה ניסחתי מסורבל אז האחריות עליי   הכוונה שההפגנות מאפשרות לחרדים להימלט מביקורת מוצדקת Kirilon1 די יקירי עם כל הכבוד לא מכיר אותך ולא זוכר שדיברתי איתך ואם אמרת דיברי טעם ודאי שהייתי שמח ללמוד מהם…  BenMoalem אני לא עשיתי את המפגינים בבלפור שעיר לעזאזל כמעט להפך כל פרשנות שלי על ההפגנות בבלפור בטלויזיה נפתחת ב…  DanK92542410 דווקא זה לא מנותק בסאב טקסט מדובר פה גם בסיפור הדרת ישראל השנייה המתונה והממלכתית והאחראית ממוקדי קבלת ההחלטות BenMoalem  moransimon5 עם כל הכבוד שב תלמד הרבה שנים ואז תוכל להעיר הערות זה נחמד הטוויטר הזה אבל באמת שזה מגוחך שבתודעתכ…  itzikelrov כבוד לשמוע ממך ראה המצורף כאן שפרסמתי הבוקר יעניין אותך אני חושב   itzikelrov התמונות מהריכוזים החרדים שונות ב 180° כל חצר עושה דין לעצמה כל רב מחליט אם לסגור פעם זה לא היה קורה גדולי הדור קבעו קו… EGz9LDzwXiJ9wsI לא נכון קרא שוב מה שכתבתי לגבי מעמדה של מדינת ישראל כקהילת העל של העם היהודי הם ועוד איך מתחשבים בהוראות המדינה moransimon5 אם היית קצת יותר מעמיק היית מבין שועוד איך שכן מתינות מתינות 929292m1 בוודאי אם לא הפסיקה לכל מדינת ישראל על פי החרדים לא המתונים שבהם הקיצוניים היו מחליטים שבתי הכנסת סגורים ביום כיפור Orfadid לא יכול זה כאילו צריך פה קורס שלם אי אפשר לצייץ את זה אם רוצה תתקשר ואנסה להרחיב באישי 0523112149 Israelh אתה טועה אני שנים עושה הבדלה בין תפיסת הרב שך קודם כל לשמור על פך שמן טהור וקטן ולהציל את החברה החרדי…  Moshe68625488 לא הבנת קרא שוב  ואתה כותב שגיאות היחידים שלא מקשיבים להוראות זה חלק מהחרדים אנשי ישראל השנייה א…  Orfadid לא משקיע בך יותר הסברתי בדיוק אי אפשר לנהל את כלל ישראל על בסיס מדיניות שמירת פך שמן טהור אם היית לומד…  050Leag אתה מגיב בלי לקרוא הרי אני מסביר שקבעו על פי הרב לאו שלא לסגור את בתי הכנסת כי הציבור לא יציית אבל זו טע…  050Leag קרא שוב נראה לי פספסת הרעיון אם היו מחליטים על כלל ישראל על פי הקו של הרב עובדיה ובנו הרב דוד זה היה סבב…  nzeuZ8kzNZuJ8BV Dganit85945554 mendygruzman ariyederi אני לא מאשים את החברה החרדית כולה אלא אומר שהיא ובראשה…  Orfadid הסברתי קרא 050Leag הסברתי אז באריכות התגובה הפרדוקסלית להתפרקות היא הקצנה בזרמים מסויימים בוודאי ביחס לחילונים תמונות יום הכיפורים מהריכוזים החרדיים לא מותירות ברירה ומאשרות מסקנה שהממשלה כולל החרדים בה מוכרחים לקבל   אי אפ…  OritDouek naomilster כתבת פה דיבה ופרסמת תמונה ממועד אחר מציע לך למחוק OritDouek BarashiKinneret זה פייק לא חצי שיה אחרי אלא שבוע לפני מציע שתמחק את השקר JHulaty זה פייק זו תמונה ממועד אחר מציע שתמחק Createfreedom התמונה הזו היא פייק היא מערב אחר ערב לפני ראש השנה מציע שתמחק Riklin10 BoazCohen לא שמעון התפיסה הבסיסית שלי היא שישראל הראשונה אנשים טובים  ותפיסת ההגמוניה שלי היא שלכן הי…  SabaryYoram Riklin10 זה מקסים ופרופ בן זקן נפלא אבל זה לא בדיוק אותו דבר בוודאי אותה משפחה netanelgla Riklin10 תחשוב על מה שכתבת אתה מסכים איתי מבחינתם הגיוני שהם יהיו פריבילגים זה דיי הגמוניה שאי…  NaorMeningher Riklin10 נורא ואיום כתבתי לפני מספר ימים מאמר חריף מאד נגדם אולי יתפרסם מחר Riklin10 לגבי הסיפא שלך אני מסכים בשפה אחרת Riklin10  זו טענה מרכזית שלי  כל ההיסטוריה של ישראל מאז מהפך 77 לא…  Riklin10 לא הגיוני שהם מודעים אחרת היה להם לא נעים והם היו מרגישים שזה לא מוסרי  העוולות שהם גורמים  דוגמא ההפ…  georgygeorge11 מדובר בשקר מכוער אלה תמונות מלפני שבוע סליחות ערב ראש השנה לא מהאירוע המדובר של סליחות ערב יום כ…  Qp4fQ2eIcbwA7Df אתה ראשונה תהיה רגוע TimtumAtzmi בוודאי שידרנו למהדורת החדשות nolaori hadarse הלוואי לצערי לא נראה כך שנה טובה ומתוקה V5yyiqXr9CypYTZ זו תמונה משבוע שעבר סתם שקר מכוער או טעות  ortis78 זו תמונה משבוע שעבר לא מאתמול מקבל התנצלותך למפרע teslererez hadarse לא הוא לא היה מפרסם כזה דבר אם היה יודע שמדובר בשקר ושזה בכלל וידאו משבוע שעבר razsauber hadarse תגיד אתה רציני אסור לי למחות נגד הדיכוי כי יהיו כאלה שיגיבו בדרך שאני מגנה וסולד ממנה ותוקף א…  TheIsrabot sagihadas hadarse לא רק פרסמתי גם שידרנו אותן בשידור חי עם צופית גרנט ואיתי hadarse TheIsrabot אמן כן יהי רצון הלוואי הלוואי למרות שאני לא יודע מה השביל שיוציא אותנו מזה בעבר הייתי בטוח…  hadarse אתה מתוק בציוץ הזה אבל הציוץ הגדול שלך שטוען שככה נראתה רחבת הכותל אתמול בלילה הוא שקר כנראה שמישהו הטעה…  TheIsrabot hadarse היה סגר שבגללו אושרו סליחות מצומצמות של 2500 איש על פני כל הרחבה בערב ראש השנה במקום עשרות אלפ…  hadarse זה אירוע שמתחיל משעות הערב בכל שנה יש הפנינג של עשרות אלפים בכל רחבי הרובע היהודי לכיוון הכותל עשרות אלפ…  razsauber hadarse לא הניסיונות לעצור את המחאה נגד הדיכוי במניפולציות כאלה הן כלי דיכוי לא הגון ולא מוסרי Eddie7701 ברור הכי סבבה לשמור על הדיכוי והסדר הישן ואז לא תיטרפו שנוגעים לכם בפריבילגיה לדכא hadarse הבדל בין אמת לשקר שבוע שעבר לא היה סגר עדיין היו סליחות מצומצמות אתמול היה סגר ולכן במקום אירוע של מאה…  tzvikagonen זה שקר מכוער אלה תמונות מלפני שבוע לא מאתמול בערב Eddie7701 רק המדכא הפריווילג רואה ברעיון השוויון שנאה hadarse לתשומת לבך מישהו הטעה אותך ככל הנראה אלה תמונות מהסליחות בשבוע שעבר לא מאתמול בערב אתה מטעה את הציבור codswallop מדובר בשקר מכוער אלה תמונות מלפני שבוע לא מאתמול בלילה  מקווה שהטעו את הכותב ולא שהוא החליט לשקר adirosenfeld123 זו תעמולה מכוערת ושקרית מישהו הטעה את הכותב אלה תמונות מהסליחות מלפני שבוע לא מאתמול Nadav1Levy kzipi100 זה שקר אלה אינן תמונות מאתמול אלא משבוע שעבר לפני הסגר pdoron שקר וכזב תתביישו אלה תמונות משבוע שעבר לפני הסגר Nadav1Levy kzipi100 מוכן שאתבע אותך דיבה תפרט מה אני משקר  התמונות שהשמאל מפיץ הן לא מאתמול אלא משבוע שעבר kzipi100 אין שידרנו שידור חי אפשר לראות מה זה השקרים האלה של השמאל kzipi100 צילמתי בשעה תשע בערב שבה שידרתי ושבה בדרך כלל יש כבר אלפים רבים בכותל ציינתי שניתן אישור ל200 בלבד באירו…  pdoron חייכתני שנה טובה ומתוקה  לא צריך שתקבלו סליחות צריך שתקבלו את רעיון השוויון אבל באמת זה אתגר קשה למעמד…  MichelZaherEye אני מקבל את הביקורת הזאת אבל יש מהלך קבוע של השמאל הישראלי להשתיק את הדיון בדיכוי המזרחים על ידי…  pdoron העובדה שאתם מבינים את רעיון השוויון והפסקת הדיכוי כשנאה כלפיכם חלילה היא שיעור עצוב על תודעת ההגמוניה הישרא…  DanielBursan תודה יקר נעים לשמוע alivson זו גישה חוכמולוגית מתנשאת שנובעת מבורות גישה שמבטאת את הבוז העמוק שלכם ליהדות המסורתית וחוסר הבנה מוחלט ש…  amittali מתנצל לא הבנתי מה הקשר יש לי כבוד עצום למשפחתך אבל זה לא מכשיר עוולות דוגמת שימוש באלימות לגלית כדי למ…  asafkfir לא הטענה היא באשר לתגובה של ישראל הראשונה לכניסת המזרחים למשחק הפוליטי ב77 מאז ועד ימים אלו ממש mendygruzman ״בימים הללו״ זה מאז 1984 כשהרב עובדיה זיהה את הפוטנציאל של הצעיר בן ה24 ושם אותו לידו malitusha efrattolk אם אנשים מקדישים זמן ומגיבים לדברים שכתבתי גם במלים רעות אז אני משתדל לכבד את הזמן ותשומת הלב ולענות am4327 efrattolk זו הפריבילגיה של ההגמוניה לא קראת אותי מספיק סיום סמלי לשנה הזו  היום מתפרסם בהארץ ריאיון מקיף שאיתי שטרן   שנראה קשוב למרות שהוא ממש מהעבר השני של המתרס…  ShlomiEi פשוט נורא דיברתי נגד זה בחריפות בפרשנות שלי yanivtwig בשום אופן להפך אבל אני חושב שיש חשיבות עצומה שהציבור יבין את הפריבילגיות של ישראל הראשונה efrattolk זה ממש לא יפה ולא הגון כמה מניפולציות מכוערות אתם עושים בשעות האלה בערב יום כיפור רגיל כל האיזור מלא כ…  DanielM רעיון השוויון איננו שינאה הפריבילג שמרגיש מאויים מרעיון השוויון ונוח לו עם הדיכוי ועם המשך העוולות מ…  matticar אתם ממשיכים במדיניות עלילות הדם ורצח האופי לכל מזרחי שמעז להרים ראש מולכם איך זה קשור אליי אין לכם גבולות Ronkofman1 קופמן Ronkofman1 יקר לי כתבתי מאמר חריף עד כדי קריאה להוציא מידי החרדים את היכולת לקבוע לכלל החברה הי…  ranninglife OriginalGavish אתם פריווילגים שמבינים או יותר נכון מרגישים את רעיון השוויון כאיום עליכם וכשינאה…  1379bac849584d4 לא יאומן כמה אתם לא פריבילגים בתפיסת העולם העמוקה שלכם  לכם מותר להפגין ולקבל שידורים חיים מההפגנ…  sigalit87724912 גמר חתימה טובה נשמה חזק ונתחזק בעד עמנו אל תיכנסו לבתי הכנסת יש לקח מבהיל שלמדנו בימים האחרונים שמירה על ההוראות לא מספיקה נגד הקורונה   אנחנו מכירים ח…  mosheifargan שנה טובה וגמר חתימה אהוב מעריך ומתפעל idayan68 תודה יקירי זה חשוב לשמוע OriginalGavish העובדה שאתה מבין את אהבת ישראל השנייה כשינאה כלפיך היא עיוות שרבים במחנה שלך לוקים בו כאילו שלילת…  ערב יום הכיפורים הכותל ריק   מידי שנה בערב הזה שהוא ערב השיא של ישראל המסורתית עשרות אלפי מתפללים הערב ניתן אישו…  dz050228 eli19 חס ושלום אני לא אמרתי שום דבר כזה להפך כל פרשנות שלי בנושא ההפגנות בטלוייזיה נפתחת במ…  arikarielpopper juldush yishaym בוודאי שאשמים פאסיביים ונחמדים וממלכתיים AaronNurani תודה נו נראה מרחיב נפש כל מה דעביד רחמנא לטב עביד arikarielpopper aizenkraft ברור השסניקים נחקרו והורשעו בשנות השיא של שס יותר מכולם לא כי המערכת החליטה לבלום…  arikarielpopper juldush yishaym ההגמוניה חזקה זה בסיס הטענה שלי שכל ההיסטוריה של ישראל מאז 77 כרוכה במהלך של י…  bnyiroz ילמדנו רבנו במוצאש  גיט שאבעס Moshe68625488 איזה יופי אשריהם ישראל תודה 135790poiuy nbjovsr88 תודה נשמה חשוב לשמוע RafiRodnik12 כלומר derieliran מגניב ores1111 איפה זה סוציולוגית הכוונה Eliot1817 איפה זה נשמה yesnomabyyes אז זה לא לפי ההוראות בתי הכנסת אמורים להיות סגורים  MoshikoRan המחאה דמוקרטית אחלה אמרתי אלף פעם לגבי המשפט אסביר מהי אלימות לגלית להפוך את ראש ממשלת ישראל ליעד מ…  h6402000gmailc1 ליטאים חסידים לא מבחין nbjovsr88 וואלה בקיצור בתי כנסת כרגיל אצלכם Mry05961431 למי משתייך  0Ew1QrRvevGENE0 ומה אצלך oMVfhF8kl7gnCee תפרט שאלמד h6402000gmailc1 וואלה כך מעריך שיהיה אצלכם מעודד nbjovsr88 אבל מישהו יסגור את בתי הכנסת או שיהיו פתוחים 0Ew1QrRvevGENE0 מה זה לפי הרב שלו יפתחו בתי כמסת בניגוד להוראות חופשי BenYairdhn איזה כללים הערכות בבקשה איך ייראו בתי הכנסת השבת בכל אתר ואתר gal09094007 ביבי חייב מפלגת מרכז כזו שתקלוט את אלה שהשתכנעו ממסע התעמולה נגדו לא לכולם יש את החוסן האידאולוגי והז…  aizenkraft אדרבה אז אפילו את בגין עם מידותיו המופלאות השמיצו ורמסו ישראל הראשונה תבין מה המוטיבציה האמיתית שמניעה אותם hagaihofer מלך aizenkraft כשבחרו בבגין האליטה של ישראל הראשונה ציירה אותו כסכנה פשיסטית למדינה כשבחרו בדרעי האליטה ציירה אותו כש…  almonimi PoeticRg ronen5956 נשמה זה רק האליטה שלא מסוגלת בחיים להקשיב לביקורת ותמיד ממסגרת עמדה מזרחית כמשהו שנ…  tinypainfulspa1 תעבור על הנתונים המצורפים ותבין את התמונה גם בדרך הזאת העשירים ששולטים בתקשורת באקדמיה במשפט בהון…  juldush yishaym ברור גם אתה מבין זאת כמתבקש ההגמוניה כה חזקה אז ודאי שיש לה אחריות הן על דחיפה לבצע מדיניות מז…  ilanitshaked תבדקי את עצמך למה את מבינה את רעיון השוויון והמחאה נגד עוולות כשינאה חלילה AvishayBenHaim המכינה הקדצ המלהיבה תבור העלתה ביוטיוב הרצאת זום שנתתי לפני מספר ימים  ניסיתי להסביר את תיאוריית ישראל ה2 לעומק ב… GilTuchman יקר לי אני לומד ומלמד כל חיי על התגובה הגזענית הקבועה שלכם  לכל מזרחי שמעז לעמוד מולכם לא היו ציפיות…  yishaym אני חושב שאי אפשר יהיה להמשיך להכחיש את האחריות של ההגמוניה לשיתוק המערכת הפוליטית ולהחלשתה  מתי שהוא נפתח את הנושא הזה ועוד כמה o55224926 נשמה אני התחלתי בה לפני הרבה הרבה זמן segevomri די עם המניפולציות האלה מותר להשתמש בפראפרזה מפסוק מוכר בלי שתעניקו לה פרשנות מרושעת ChauleMoshe אתה לא סולידרי איתו אלא עם בוחריו בהנחה שאכפת לך מהם ChauleMoshe זה המאבק הלאומי הכי חשוב היום מי שלא מזהה את הסנטימנט של העם שבשדות או מזהה ומנוכר כלפיו צריך להעיר לו ParshanLeumi כוונתי הייתה שהתנהגותם בלתי מתקבלת על הדעת ורק הפגנות בלפור משמשות בהצלחה להסחת דעת SivtaT כל הציוץ הזה סובב סביב הגמוניה לא הבנת באמת Urieldenn בא לי לחסום אותך על המדרש המטופש והמרושע הזה omermic רק פריווילג שהדיכוי והעוול נוח לו רואה ברעיון השוויון והפסקת הדיכוי רעל Easternprince לישראל השניה אין מספיק כוח לנהל מאבק לבד למעשה אין לה שום כוח ושום אמונה בכוחה לכן חייבים בריתות ע…  zachsivan matankaplan מבחינתך סתם שוויון והפסקת העוולות של האליטה לא בא בחשבון זה או המשך הדיכוי או פילוג למה לא פיוס tomerskurnik מה קרה נשמה nohraba המחאה נגד העוולות שהאליטה עושה נתפסת כמשהו רע רק אתל מי שהעוול נוח לו ואין לו בעיה מוסרית עם דיכוי שנה טובה ומתוקה matankaplan כשהצביעו בגין עיניתם את נפשו ושברתם את לבו בכוח שהגמוניותכם נותנת לכם כשהצביעו דרעי הכנסתם אותו לכלא…  Isaiah00493765 Soloph0ne nosseihdegel1 אני לא חושב שאני אומר לאנשים שהם משרתים את ההגמוניה לא נראה לי לגבי ״מג…  PoeticRg ronen5956 מעריך את זה באמת AshkeloniS nitlachman תודה יקר זו תגובה חשובה לי PoeticRg ronen5956 מציע שתאזין פה אם באמת מעניין אותך וחשוב לך אני מסביר את זה   D1VhQyjw4N9A0yD נשמה עוד לא נולד המזרחי שהעז להרים את הראש מול ישראל הראשונה וישראל הראשונה הגיבה בצורה מכובדת וק…  orenba בקיצור חוץ מגידופים לא אמרת כלום גמר חתימה טובה yarwax אם היית חי את השיח היית יודע כמה מאמרים כתבו אנשים מהצד שלך במפה שכפרו בנתונים הברורים הללו mostene זה פנימי שלהם אני לא מחנך חרדים ולא רוצה לפגוע בה אבל לא מוכן שבשביל איזה גחמה שממציא עסקן חרדי יפגעו בע…  gmarkovich3 nosseihdegel1 אתה מדחיק מתרחש בישראל עוול גדול כלפי בחירה של ציבור גדול צריך לפתור את זה בדרך יפה ו…  nitlachman לא יודע ברור שזה לא עבד כמו שחזיתי ורציתי nosseihdegel1 אני אבוא נשמה סדרה הבאה אני בא לצלם אצלכם אתה יודע שגם במרוקאים החדשים רציתי לבא אליכם gmarkovich3 nosseihdegel1 אתה בבעיה מוסרית למשל אתה שותף לדיכוי של ציבור שאין לו ייצוג במערכת המשפט באקדמיה ובת…  nitlachman אני דיי מסביר פה מה המטרה שלי פיוס אבל מתוך שוויון והפסקת הדיכוי   gmarkovich3 nosseihdegel1 ראה הנתונים המצורפים ותפסיק להיות לא מוסרי ולהתעלם מהדיכוי eli19 אנשים לא טפשים ביבי הוא הבחירה הדמוקרטית המובהקת שלהם תכבד אותם nosseihdegel1 אל תשחק אותה דואג להם הם דואגים לעצמם ובוחרים דמוקרטית מה שבא להם ולא מה שבא לך תכבד את הבחירה שלהם ואל תתנשא ronen5956 מה זה אין תקרא שוב ותפסיק לעצום עיניים ולהתעלם בצורה לא מוסרית מעוולות  בתקופה זו ממש האליטה מנסה לגנו…  shalomkamil מדהים כמה מדרשים אתם צריכים לעשות בשביל למצוא אצלי את הטקסטים שאין  מותר להשתמש בפסוקים בפרפרזה בלי…  המאבק להפלה אלימה לגלית של נתניהו הוא מאבק של ישראל ה1 נגד הבחירה הדמוקרטית של ישראל ה2 ראו הנתונים  על האליט…  WeissInbar מציע שתראי באיזו הערכה עצומה דיברתי עליה אתמול בשידור שלנו בגלל הדברים שאת מציינת ולכן גם דחיתי את הסיפ…  rothmar תקשר כשיהיה לך זמן אסביר פרשנותי לגבי הדינמיקה של נורמות ההקצנה הדתית והחרדית  איזה חרדי ממציא חומרה חדשה…  yinonidan כוונות טובות asafb2k rothmar נשמה גם אני חשבתי שאין סיפור וגוננתי על דר עליזה בלוך בהתלהבות בטלוויזיה עד שהתברר לי שאשכרה חר…  ParshanLeumi אתה יודע שבן אדם צריך להיות לא מאד חכם בשביל להבין את מה שכתבת ממה שכתבתי SrulikKlein דווקא על המצבה שלה במרוקו בבית העלמין בפז ראיתי שכתוב חגואל brafman מקווה שלא יכעיס אותך אלא ירגיע אם אתם לא נרדמים  wlhdPcAeDW4Hbty ציוניים OrHeller NeriaKraus  roeilach רועי אהוב  ו״האחים״ כדי לא לומר  אוריאל ואלירז פרץ ו״יונתן״ כדי לא לומר יוני נתניהו וחגואל כדי למחו…  nachumehrlich מדוייק gadymz BeeriMor אכן מאשים אותך בדיכוי ובתמיכה באלימות לגלית ובגזילת זכותה של ישראל השנייה להשתתף במשחק הדמוקרטי וכיוב בוודאי אכזבת סוף השנה ד״ר עליזה בלוך  כגודל הציפיות  mzahavi1 אתם כרגיל מעלילים עלילות כל פרשנות שלי בטלוויזיה בנושא זה מתחילה באמירה שההפגנות הן חגיגה דמוקרטית ומדוב…  gadymz BeeriMor ביקורת על הדיכוי בוודאיאבל פה הוא האשים בדברים אחרים winerez לא נותן הכשר בשום אופן MosheRahmani תודה יא אהוב מאד שמח שתפס אותך davidbenporat רק בעייני המדכא שנוח לו הדיכוי ואי השוויון  רעיון השוויון נתפס כמו הסתה נגד הפריבילגיות שלו  חלי…  winerez אם היית קורא יותר טוב היית מבין שזה לא מצדיק אותם אלא ביקורתי כלפיהם zlildror Erella11 GiladGendelman איזו מין המצאה דיבתית זאת בחיים לא אמרתי דבר כזה ממש הפוך אשמח לציטוט אחד של…  kidrong לצערי אין באפשרותי להתווכח על זה kidrong אני חושב שפספסת מה כתבתי eladshpier לא הבנת כלום ממש Tamarhamagniva אבל אנחנו לא עוסקים באיכות ההשוואה אלא בעובדה שהיא קיימת בשיח הציבורי ומצילה את החרדים ואת גוש הימין מביקורת חריפה BeeriMor יא מתוק הכל טוב אין כעס וגם כשיש זה בסדר אני אומר דברים מכעיסים שנה טובה ומתוקה BeeriMor אני מאד משתדל לא לעשות את מה שטענת שאני עושה כלומר להתמקד ברהביליטציה לישראל השנייה ולא בהתקפות על הראשו…  GiladGendelman asafb2k Erella11 אז על הסעיף הזה בתיאוריה הסכמנו שיש מגמה כזו גם טוב  שאר התיאוריה זו טענה…  ambivalentiut אני לא מנסח ככה אבל אני בהחלט מבואס GiladGendelman asafb2k Erella11 מה זה לא מה אתה לא לומד על מגמה מהנתון הזה למשל  אין שום מקום בישראל השנייה המ…  BeeriMor אני לא אמרתי את זה אני אמרתי שהתמיכה בנתניהו איננה תמיכה בשחיתות חלילה אלא נובעת מעמדה לאומית אחראית ומ…  GiladGendelman asafb2k Erella11 מבדיקת כל הקלפיות בישראל אין שום מקום בישראל השנייה המובהקת שבו ביבי הפסיד אין…  8eSnINY1aOMQpGQ מזרחיות איננה שד זו תפיסה קולוניאליסטית גזענית שלכם שאתם צריכים לעקור אותה כבר  אני מסביר פה קצת…  BeeriMor זו הוצאת דיבה שלך ממש חמורה לא אמרתי כזה דבר   לא מבין למה אתם קוראים דברים חיוביים על ישראל השנייה כא…  realDolevYaniv אם היית מעט יותר נבון או מעט פחות כועס היית מבין שהטקסט שכתבתי הוא ביקורתי מאד כלפי ההתנהלות החרדית  באמת לא הבנת Erella11 GiladGendelman נגמרה לי הסבלנות לשיח הזהויות המפלג הזה זה את מעידה על עצמך עצם הזהות של המזרחים לא מ…  assafazaria אכן ואלמלא ההפגנות בבלפור זה היה הסיפור שאי אפשר לברוח ממנו Erella11 GiladGendelman לא שינית בזמן האחרון יקרה זו הנוסחה דה לגיטימציה מוחלטת ורצח אופי למזרחי שמעז להביע עמד…  ZeppeliN0007 אני לא אבל הדיון הציבורי כן Kirilon1 זה ממש מה שאני טוען לכן אני אומר שרק בזכות ההפגנות בבלפור החרדים נמלטים מהביקורת הציבורית החריפה שהי…  AvishAb12 yesnomabyyes ruthelbaz אבל זה לא קשור הסברתי לך  זו הרצאה על בית שני שבהקדמה ציינתי את חורבן בי…  roeep86 לא אמרתי שזה לא בסדר אתה לא קורא נכון אני מעולם לא קראתי להגביל את ההפגנות או משהו דומה חלילה  אני רק מ…  AvishAb12 yesnomabyyes ruthelbaz אתה לא הצעת פה שום דבר מועיל סתם זרקת דבר הבל  קורה  ועם כל הכבוד לביקור…  Iaskquestions30 YuvalCo80807283 מקבל כך פרשנתי גם בשידור גם אם יבוטלו ההפגנות בבלפור החרדים לא יקבלו ההוראות GiladGendelman מביך לא אחראי ולא סולידרי AvishAb12 yesnomabyyes ruthelbaz אבל אתה מדבר הבלים לצערי היא שאלה על נקודה בהקדמה להרצאה שעוסקת בנושא א… </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NoaLiberator Rutshapira זה משחק גאווהסקריפט אז פשוט אפשר להעתיק את הקוד ולהריץ מקומית לא NadavPerez DorDugy הם מספרים בכתבה שהמילים נכתבו שנים קודם בעקבות פיגועי שנות התשעים  וואי הלוואי שאני אקפוץ קדימה בזמן איזה 50 שנים ככה  למה בגלל הקורונה   לא כדי שאם מישהו שם גיף של I underst…  DorDugy איך קוראים לאהבה שלי לא נכתב כתוצאה מהאינתיפאדה השניה מבחן האזרחות שהממלכה המאוחדת עושה למהגרים  מתי פותחו רעיונות חדשים במתמטיקה  1 לא ביוון העתיקה טפו 2 לא בעולם ה…  OdedFire האםםםםם שמעת על מצילינו ומושיעינו הקדוש האדס ישתבח שמו IraImmergluck ZmanIsrael היי אירה אין לי תלונות לכתבה שלך שכתובה היטב יש לי תלונות לבחירה של העורך למצב בכותר…  AnerOtto איך מוגדר ויטמין AnerOtto אני רואה שהציוץ שלי על ויטמין D משך קצת אש שזה מעניין כי הייתי בטוח שהחלק המעניין שלו הוא שויטמין D הוא לא ויטמין אלא הור… ZmanIsrael IraImmergluck לא רוצה לסכסך אבל יש מצב שניו זילנד הצליחה קצת יותר noamginger מוגלגלי סליחה ia42 MemeR Shluli אם אני פונה לאדם וקורא לו מישהו במקום להשתמש בשם הספציפי שלו שם שאני צריך לזכור בעל פה יש…  dinadayan זה ללא ספק מרכיב מהותי בסיפור האם זה כל הסיפור אני לא בטוח דווקא בגלל פגיעות היתר של האוכלוסייה הזו ק…  MemeR ia42 Shluli כן בזרה לנו דיברתי עלי ועל עירא מקווה שלא השתמע אחרת תמצית הדינמיקה הטוויטרית    האם יש דבר מיותר יותר מאריות ים   סליחה אדוני אריה ים הציל את חיי בוייטנאם משפחה ש…  ia42 MemeR Shluli מטאפורה יפה הנה הצד השני שלה זו חוויה שזרה לנו לגמרי אבל יש אנשים שהעברית שגדלנו בה דופקת להם מכות פטיש ISudri מר סודרי אתה מבין שהרעיון בקפסולה הוא לא שהנמצאים בה חסינים מהמחלה אלא לצמצמם את ההדבקה למי שנמצאים ב…  dinadayan לא קשור ללצחוק קשור לנבואה שמפריכה את עצמה הגל השני לא הגיע מעצמו בגלל הכוח הגרביטציוני של הירח הוא ה…  Wlrving considerthefish לא הוא לא אבל כן יש חשש לבעיות בריאות כרוניות אצל אחוז לא מבוטל Gili95664232   אוהבים לדבר על שבדיה כמדינה שהצליח לה עם חסינות העדר זו לא הטענה של שבדיה עצמה  העניין הוא שחסינות עדר זה לא מ…  idan315 יש לנו הנחה  adistav ברור שזה היה יכול להיות אם היו מגלים כזה דבר זו הייתה הפתעה מדהימה בלי קשר לדרך אבל בתיאוריה גם ייתכן…  adistav זה כמו המשפט האחרון של פרמה היה ברור לכולם שזה נכון כבר מאות שנים אבל היה גם ברור שאין שום סיכוי שבעולם…  adistav אה ההתלהבות כאן לגמרי תהיה לא מהתוצאה אלא מהטכניקה המטורללת שיצטרכו כדי להוכיח משהו כזה idan315 Solance מדבר כל היום על מג מג מג ואף פעם לא על דוזה שרץ שאול טיפוסי אז יש תחקיר של ענייני המיסים של טראמפ שהוא כנראה עבודה עיתונאית פנומנלית ואני מתקשה להבין מה הביג דיל בו כי איכשהו…  AidaTuma שרון נכנס אל תוך המסגד לא הצלחתי למצוא מקום שבו זה נאמר אפשר פירוט DorDugy גורמים בממשלה מדברים על מתי יהיה חיסון אילוסטרציה  RanBalicer אני תוהה כמה אנשים צריכים למות פה מדי יום כדי שיפסק המינהג השערורייתי לעניות דעתי של הקריינות בסגנון ׳מתו עם קורונה או ב… BenDror4 לא מבין בזה מספיק אבל להבנתי זה לא לינארי אלא קשה בהרבה BenDror4 הם יהיו רועשים ולא יהיה אפשר לעשות איתם כלום צריך לזכור שרוצים שתתאפשר סופרפוזיציה של כל הקיוביטים הללו…  chonye91 YaelSherer אה התפיסה שלי היא שהדת היהודית היא תועבה מיזוגינית ששומר נפשו ירחק ממנה ואסור שתהיה נתיב החת…  שמאלן מצביע בבחירות אילוסטרציה  ExMaahal AvinoamY נראה לי שזו עמדה בלתי נמנעת גם לסתם חילוני שגדל פה הדת נכנסת אלינו עמוק מדי מתחת לעור lilyoftheyard אוקיי זה יצא ממש אגרסיבי בצורה שלא התכוונתי אליה מה שרציתי לומר הוא שממש משמח אותי לשמוע את זה  lilyoftheyard לא נכנסתי שם למתמטיקה theconfigurator תהיה אותה שיחה גם ב5000 אנשים אחרים כותבים ציוץ אחרון בסדרת ציוצים פיקטיבית וכולם מגיבים לזה כאילו זה היה עמוק נורא כדי לעבוד על הדתיים…  mipcodes שעון קיץ כאן מסמל לא איזור זמן מסויים אלא את הקונספט להזיז את השעון שעה אחת קדימהאחורה בהתאם לעונה שנת 2000   וואי כמה אפשר למה הם נלחמים כל כך על לעבור לשעון חורף לפני יום כיפור אני מת פה  עזוב המפלגות האלו…  LongtimeNut dubikan האמת שאחרי הMCU ותאנוס נהיה הרבה יותר קל להסביר את אלוהים פשוט בתור נבלעל עם דרך משונה מאו…  dubikan CrazyVet noamginger gilgu oferron מעניין בארץ אין לחץ מיוחד להכיר את המיתולוגיה היוונית אבל די באופן…  JenAshleyWright realDonaldTrump Thats also pretty much the story in Israel dubikan CrazyVet noamginger gilgu oferron הם מכירים את המיתולוגיה היוונית eyal6699 אני לא מנתח קומיקס בעיקרון גיבורי על הם מן הסתם אלגוריה לשלל טיפוסי סלבים ואלמנטים קלוקלים בתרבות gil73965867 Obar06485129 אני מקווה שאתה יודע שמים זה חומר רעיל בכמות מסויימת ובטח שזה רע לילדים שנופלים לבריכה ולא יודעים לשחות whtstar2 tessartype כבר לא מרגישים הבדל בין כיפור ובין סתם סגר shirlior asafabcde MatanHolzer FakeYoel למה בלי להניד עפעף לפני הקורונה מה שצעקנו עליו כל הזמן הוא ללכת להתחסן נגד שפעת כי זו מחלה קשה MatanHolzer asafabcde FakeYoel מהיכן המידע רובם משתחררים תוך יום eyal6699 אגב Hades הוא באופן טבעי רפטטיבי כי זה הזאנר אבל הסיבה שכולם נשפכים ממנו היא הבית ספר שהוא עושה לגבי…  eyal6699 ואם אתה כן במצב רוח למשהו קצת יותר נסיוני Return of the Obra Dinn התחייבות שלי לינארי לא מבוסס שוטטות…  eyal6699 ביושוק אינפיניט Nowa לא יודע אותי זה הצחיק jonobarel IdanDekel DanielleBN MemeR כן חוץ מאלו שבהם הספין אוף מתבסס על דמות שקיימת בחומר המקור ומקבלת במה מש…  מתחשק לי לאמץ את אבח ולהגיד שהוא מדמחניק זה הרי מתאים לתיאור שלו לא פחות מכל תואר הזוי אחר שהוא מייחס לעצמו  mashkazg perryallon Amitna87 roeer היה לי רק את ציפורי לילה בננטקט בתור ילד וכל כך אהבתי אותו  Amitna87 ואן דייק לדעתי התנצל פומבית מרוב שזה היה נורא hyuvii כן כן אני יודע את כל זה אבל זה לא משנה את העובדה שהתפילות הללו טרחניות בעיני בצורה קיצונית והתוכן שיש בה…  FakeYoel MFaibis רק מציין שהחשבון של 1 ל1000 על מדינה של 9 מיליון איש מתורגם ל9000 מתים וזה בלי להיכנס לנזק…  FakeYoel MFaibis איך פתאום קפצת לדיבור על סגר FakeYoel MFaibis זו אותה מגמה בדיוק למה אתה מעיק  FakeYoel MFaibis האמירה זה עצר בכל מקום אחר בעולם היא שגויה  Amitna87 לדעתי זה פשוט שייך לעידן שבו כשעיבדו ספרים לא הבינו שחייבים לקצץ על ימין ועל שמאל TalGoldman במקרה הנוכחי פשוט תכתבו בגדול הירשמו והתחברו לאתר על מנת להזמין צמיד TalGoldman tomer תודה גולדמן אני יודע שאתם אנשים טובים שעובדים קשה ורוצים שיהיה טוב לכולם ומקווה שלא משתמע אחרת  eyal6699 זה חשוד מאוד משחק שמשאיל בצורה כל כך מובהקת את הסגנון הגרפי הייחודי של משחקים אחרים זה בדרך כלל סימן…  eyal6699 שיחקתי קצת אמרתי וואו איזה מגניבבבבבב נתקעתי באיזה קרב שלא הצליח לי לא חזרתי מאז  אוקיי רגע מה הכוונה היא יותר מכניסה אחת בבת אחת או שיש לי רק פעם אחת לראות את כל הכנס ואחר כך זהו אני מניח שה…  גם מהמחשב לחיצה על הזמנת צמיד כניסה מקשרת לתוכנייה שבה אין שום הסבר איך מזמינים צמיד כניסה  האם אני אסתדר בוו…  saralegliksberg כדאי לבדוק מה הנתונים המעודכנים על החודשיים האחרונים   קשה לנצח את הבוס האחרון ב Hades יותר קשה לטפס על האוורסט עוד יותר קשה לעצור את הקורונה הכי קשה להבין איך נרשמי…  ClarkMcFly מפלצות העל  FakeYoel מתנצל לא הבנתי תוכל להסביר במילים למה הכוונה ולהדגים איך זה תואם את הגרף שיש בארץ FakeYoel מה זה אומר שטוח המונח לא מוכר לי בהקשר הזה FakeYoel אנחנו רואים גל כזה במקום אחד בעולם ישראל אז המינימום שאתה צריך לעשות הוא להבין שאם אין דבר כזה ביתר העו…  omeresh לא כי אני לא חושב שזה ייגמר ב5000 אם לא נעשה כלום כמו כן הסגר עכשיו הוא לא פתרון והדיון הוא לא על סגר…  אגב מקדים תרופה למכה רוצים לומר לי שזה לא מיוחד לתפילות יום כיפור אלא זה ככה בכל תפילה ותפילה כן אני יודעעעעע FakeYoel חשבתי הרבה זמן בדיוק כמוך על הנתון הזה אבל הוא מטעה כי אנחנו לא יודעים מה הולך לקרות במדינות שיחטפו גל ש…  omeresh rutihersh אבל אתה אמרת לפני רגע שאי אפשר לדעת מה יקרה בעתיד מה גרם לך לשנות דעה כל כך מהר היית צריך לענ…  omeresh rutihersh אגב לא הבנתי איך להתעלם מהמגיפה יציל אותנו מהמשבר הכלכלי את שוודיה זה לא הציל omeresh rutihersh אתה לא יודע בודאות את העתיד מכחישי קורונה אל תעשו סגר זה יהיה אסון כלכלי המדינה תיחרב העתיד   מתנגדי קורונה אוקיי אבל חייבים צעדי מ…  omeresh rutihersh אתה לא יודע את העתיד אבל אם אתה רוצה לדבר על המחלה אתה חייב לנסות ולהעריך אותו בצורה שמחוברת…  omeresh rutihersh בוא תסביר לי אחת ולתמיד את הקטע הזה  אתה אומר 1500 בחצי שנה למה הנתון הזה הרי אתה יודע ב…  geifmany למשל לא להתקהל במקומות סגורים זה רעיון חדשני אני יודע אבל הוא טרם בוצע פה FakeYoel אני לא חושב שהתמותה תחומה ב5000 ומציע לא לתת תחזיות של חסמים עליונים כי אנחנו אולי יודעים איך זה מתחיל…  rutihersh omeresh הטענה שקשה יותר להשפיע על שיעור התמותה כי זה תלוי בדמוגרפיה עוד איכשהו ברורה לי למרות שגם זה לא…  NoaLiberator אני מהמר על או אחרי החגים אם הממשלה ממש מטומטמת או עוד חודשיים מה אנשים כנראה רואים בתפילות יום כיפור חשבון נפש בקשת כפרה שיפור עצמי יופי  מה אני ראיתי בתפילות יום כיפור כשהל…  ehmaimon צחוק צחוק אבל יש לי הרגשה שפספסנו את הOregon Trail הישראלי פה nitayp Sstoyaabulafia עם זה אני מסכים דברים שאני חושב שאסור לעשות למידה בטכניון בכיתה סגורה קפסולות שמקסולות…  Sstoyaabulafia אני לא רואה בעיה במפגשים בחוץ עם שמירת מרחק ומסיכות Sstoyaabulafia נראה לי שכולנו נסכים שבערך כל הצעדים של הממשלה נגד הקורונה הם אסון ושגם הסגר הזה מבוצע בצורה…  ia42 MemeR גם חברים יכולים לפגוע אפילו בלי כוונה לפעמים כשהמכה מגיעה מכיוון אנשים שאנחנו פתוחים אליהם היא חזקה…  hadarinke מאז כבר הרגתי אותו שוב ושוב ושוב rutihersh nitayp אני מאמין שהייתה ירידה משמעותית אבל שכדי שזה לא יסתיים באסון היה צריך יותר מירידה משמעותית eranbe אני לא מתערב עם אף אחד אני מבטא את ההיסטריה שלי MynaHodit רק מזכיר שאנחנו לא הולכים למודל השבדי כי בשבדיה היו זהירים יותר מאיתנו HuffiMuffiGuffi Idanyo יאפ זה אקסקום הישן והטוב adlerizm CactusBavarius אתה כנראה לא תופס משהו בסיסי  אחרי הסגר הראשון הייתה הזדמנות להימנע מגל שני אם כלל הציב…  Idob82 NucleusDawn אני שונאאאא את הקטע הזה של לקנות בונוסים זמניים תמיד זה נגמר כשבאמת צריכים את זה maayanef מתנצל  זו הייתה בדיחה אני לא הצלחתי להבין את ההערה של ההוא בעצמי maayanef מתנדב להיות עוד נודניק שמסביר לך שילדים הורסים את הכיף  RikerGoogling can a dermal regenerator fix a leather couch shmuelfarkash לא Elinorigby אצלי הרבה פחות לשמחתי אנשים אחרים שונים ממני בדרכים שאני לא מתיימר להבין ובוודאי שלא לשפוט Sammyd453 אני מקווה שכולם יתעשתו ולא נגיע ל5000 אבל זה לא יקרה מה Elinorigby אני הייתי בעיקר בודד יותר  התעלקתי על אנשים ספציפיים שאלוהים יודע איך סבלו אותי Sammyd453 אם הסגר נמשך כמו כרגע לא רואה איך זה יציל אותנו ואם תפילות יום כיפור הלכו גרוע כמו שאני חושב אנחנו נחטוף גם עם וגם בלי סגר Jenny666Beans מלוא כל הארץ כבודו eyal6699 אז מה אמרנו העמדה שלך בנוגע לHades אני לא אפידימיולוג ולא פיזיקאי עם מודלים ולא חתן פרס נובל 2013 כך שכשאני זורק תחזית לאוויר היא לא מבוססת על כלום חו…  Jenny666Beans הוא מהאלו שנכנסים לתפילה עם מסיכה ומורידים אותה בדיוק כשמגיעים לקדוש קדוש קדוש PazFeed TRIGGERED EdGorinstein Well you managed to recreate the feeling of one of my favourite boss fights Thanks AradFirer זה כמו התנך מלא קסמים והרפתקאות ובעיקר חטפנו מנה גדושה מזה בתור ילדים וקשה להשתחרר אם השטן היה קיים האקט הראשון שלו היה להמציא את אלוהים רק אומר אני מנסה להבין מה עובר לאדם כזה בראש ופשוט לא מצליח אנחנו כאלו פסיכופתים  SupergiantGames Artemis told me she digs my Coronacht Case closed   Also deflecting the witches with its special is SO satisfying adlerizm CactusBavarius להיטפל לאלפי כאילו אם היו אומרים אלף ארבע מאות זה לא היה נוראי באותה מידה זה מטומטם…  Icel אתה משתפר בכל פעם תמשיך amph מתנצל בהנחיות נפלה טעות צל כאשר אתן מדברות עם מעריצי אבישיה מתיה מוטב כי תהיו לא מנומסות chonye91 YaelSherer כפייה כזו פירושה מתן גט ללא הסכמת הבעל או סתם לגיטימציה להפעלת אלימות כלפי הבעל YaelSherer אל תדאגי לא ייתן גט ישימו אותו בכלא זה כבר יראה לו NeuOmer יודעים לתת מדדים עם גרפים יפים   Stillwa16458825 לא NeuOmer מה אתה מודד MyHactana דקה לפני כן הוא יוצר באופן חופשי זוויות של תשעים מעלות הוא יודע ליצור ריבוע Hofshia GrimBeholder AviRabina הוא מדבר על ניסוי אפידימיולוגי שתלמידי הישיבות מפעילים על עצמם כל חיי רציתי לראות שלט כזה שבו לא עומדים בדדליין תודה קורונה  AvishayBSG idan315 DenisVi אני משחק בעיקר בhandheld האדס ספציפית אבל גם כל דבר בכללי eman70y Nefolet PhysicsRocks3 יש oblong למלבן שאינו ריבוע אבל הוא כן מלבן לא מרובע כללי idan315 DenisVi AvishayBSG בסוויץ זה רץ חלק ונראה מעולה Nefolet אני לא בטוח למה את מתכוונת אני מכיר עיגול בתור החלק שתחום על ידי המעגל עיגול הוא העוגה מעגל הוא שפת העוגה yuvalv yoavgo eyalbhaim צריך טיפה להיזהר כאן  אחד מהדברים המרכזיים שעושים כרגע בתחום הוא לנסות ולבצע אבסטרקציה…  yoavgo eyalbhaim אני לא יכול לומר אם אני מתנגד או לא כי אין לי הבנה אסטרטגית של השיקולים והמטרות של ישראל אני יכ…  קוראים באי התעלומות ופתאום המהנדס מחשב זוויות על ידי חלוקת מעגל ל360 חלקים   למה למה מעגל שלם למה למה לא לי…  yoavgo eyalbhaim לדעתי זה בדיוק אומר שלא הולכים לבנות מחשב אלא רק ללמוד איך להשתמש בו ולפתח דברים אליו yoavgo eyalbhaim אגב גם כדי ללמוד איך להשתמש כדאי שיהיה תקציב מהמדינה כן yoavgo eyalbhaim לא בונים מחשב אני לא מבין איך הגעת לחוקרים איך להשתמש שאת זה עושים גם כרגע בלי קשר כבר מתו יותר מ1400 אנשים וחובבי הקורונה עדיין מנהלים ויכוחים על קוצו של יוד בסגנון התחזית מופרכת הבטיחו היום 8…  eyalbhaim yoavgo בניית מחשב קוונטי היא תחום נפרד מפיתוח אלגוריתמים קוונטיים וכדומה בשביל שיהיה לך מחשב קוונטי את…  NoamsArk זה הדגל NucleusDawn מקווה שיש לך קצת דם מנחים כי זה פותח שדרוג לאקסל שמסייע להתקפה הקריטית adlerizm CactusBavarius יאללה יאללה אלפיים מתים כבר יהיו ושום דבר שנעשה לא יכול למנוע את זה מציע להפסיק עם ההתפ…  eyalbhaim yoavgo כיום המחשבים הם של סביבות החמישים קיוביטים אבל זה לא המדד הכי מעניין יבמ למשל כל הזמן משפרת את…  yaelrashlin NoaLiberator זה בגדול הרעיון מאחורי רעש קוונטי אבל הפרטים מסובכים יותר eyalbhaim yoavgo זה לא מירוץ במובן של למי יהיה קודם וגוגל עושים יחסי ציבור בעייתיים מאוד לתחום לדעתי אלא פשוט…  yoavgo eyalbhaim בשלב הנוכחי מחשבים קוונטיים לא מאפשרים לנו לעשות כלום שהוא גם מועיל וגם לא ניתן לביצוע במחשב קלא…  eyalbhaim yoavgo קטונתי מלהגיד לישראל איך לנקוט ברמה האסטרטגית ומן הסתם ישמח אותי אישית אם הם ישתפו פעולה עם יבמ…  yaelrashlin NoaLiberator אני לא יודע מה זה ריקבון ומה בדיוק קורה בשבבי 7 ננומטר יש בעיות שבזרגון המקצועי מכ…  yaelrashlin NoaLiberator הרעיון למחשב הגיע מהחתול של שרדינגר כמובן eyalbhaim yoavgo יש בגישה הזו שתי בעיות ראשית אפשר יהיה לעשות עם מחשב קוונטי גם דברים שהם לא האלגוריתם של שור…  yoavgo לשאלות עניתי eyalbhaim yoavgo אם נגיע לרמה של האלגוריתם של שור כן כרגע נראה מאוד לא סביר שנגיע לאלגוריתם של שור בעשור הקרוב…  yoavgo כי כאמור לבנות מחשב קוונטי זה לא לעשות קופי פייסט למחשב קיים בפרט כזה שאין לך גישה אליו מלכתחילה UdiQimron horowitzb amsterdamski2 ArielMunitz GerlicL aradnir NadavEyal נניח שהתחזית הייתה רק של 700 ולא…  yoavgo אז בבקשה תנסה לנסח את השאלות שלך בהתאם ולא לטעון טענות על בסיס תמונה שגויה שיש לך בראש yoavgo השאלה היא למה שישראל תרצה טכנולוגיה חדשנית yoavgo זו לא נחיתה על הירח שבה רק מי שמגיע ראשון זוכה yoavgo לא yoavgo זה השלב שבו אני תוהה מה ההבנה שלך בעצם כי אנחנו בעולמות שונים לגמרי yoavgo יבמ כבר בנתה מחשב קוונטי וכבר משכירה זמן חישוב זה לא אומר שאם מחר הם מפתחים מחשב שמריץ את שור ישראל תקבל גישה חופשית אליו yoavgo מי מוכר כמו כן זה לא משהו שמחברים לשקע וזהו אתה צריך אנשים מיומנים לתחזוקה שוטפת של זה yoavgo זה לא פיתוח מדעי זה פיתוח טכנולוגי אי אפשר לעשות קופי פייסט Icel חושב שהמשחק היה מתסכל אותי הרבה יותר אם לא הייתי במקביל משחק עם הילד בGod mode ומתרגל אליו שם עכשיו ניצחתי…  Jenny666Beans זה הדבר שיש לי ואני מרוצה ממנו אין לי היכרות עם התחום מספיק טוב כדי לקבוע איך הוא ביחס לאחרים   therealkingonly MadaGadol בהתחלה הייתי על מיוט כמו טמבל וחוץ מזה חישוב קוונטי זה מגניב אבל ממש ותודה לNoaLiberator שהאיורים שלה מראים עד כמה lt11  חלק ממה שצריך לזכור פה הוא שמחשב קוונטי זה לא 0 או 1 וסליחה על בדיחת האבא האלגוריתם של שור הוא הדבר הכי מפורסם א…  אז האם ישראל אומן צודק כשהוא מזהיר את נתניהו מפני השקעה במחשב קוונטי קטונתי מלחרוץ דעה בעניינים אסטרטגיים שכאלו ו…  האם אי פעם נוכל להגיע לשם כאן אין תשובה חד משמעית המתמטיקאי פרופ גיל קלעי למשל חושב שלא נוכל ויש לו טענות לא ט…  ראשית צריך הרבה קיוביטים פיזיים כדי לקודד קיוביט לוגי חסין רעשים בודד אז צריך מחשבים גדולים יותר שנית וחשוב…  אולי תגידו  אבל רעשים זה משהו שקיים גם בחישוב קלאסי ויש קודים לתיקון שגיאות שמתגברים עליהם זה כמובן נכון ויש גם…  סתם להגיד יש לנו מחשב קוונטי עם 1000 קיוביטים זה חסר משמעות צריך להבין מה אפשר לעשות עם הקיוביטים הללו בצורה שא…  העניין הוא שמידע שמיוצג בצורה קוונטית הוא מאוד רגיש לקלוקלים מבחוץ בשיטת הייצוג שמשתמשות בה כיום חברות כמו גוגל ו…  אלא שהאלגוריתם של שור הוא תיאורטי הוא אומר אם יהיה לנו מחשב קוונטי חזק נוכל לעשות בו את זה מחשבים קוונטיים כאל…  הדבר שכנראה פרסם את החישוב הקוונטי יותר מכל דבר אחר הוא תוצאה תיאורטית לגמרי מ1994 של פיטר שור שמצא אלגוריתם קוונט…  מה זה חישוב קוונטי יש לי פוסט שמתאר את זה בפירוט אבל הרעיון הבסיסי הוא לנצל אפקטים פיזיקליים מגניבים כמו סופרפוזי…  הסיפור האווילי הזה של ישראל אומן על השקרנות הפתולוגית של נתניהו הוא בעיקר הזדמנות טובה בשבילי לקשקש קצת על חישוב קו…  מחקתי כי גיליתי שאומן עצמו אמר את ובכן זה יצריך ציוץ נפרד זה לא מבחן אלא שאלה אין לי מושג וגם לא למשתף המקורי AvinoamY או כמו שאנחנו קוראים לזה בחיפה יום ראשון eyalrh בכנות לא אכפת לי מה היו הכוונות שלו אני רוצה שהוא יסתום פשוט יסתום HuffiMuffiGuffi OmerLahav idan315 האהוב עלי מבין 49 הוא 9 ואחריו 6 ואחריו 7 לדעתי הוא ממצה הכי טוב את האופי…  EdGorinstein Got to ask Is the TheseusAsterius battle a nod to Dark Souls OrnsteinSmough battle  Also the Hy…  HuffiMuffiGuffi OmerLahav idan315 תודה כבר יש לי את 789 וכדאי שקודם אגיע אליהם HuffiMuffiGuffi אני קצת לא מאמין שאני אומר את זה אבל עדיף החידוש מה דעתכן קובי אריאלי יתחיל עכשיו לסתום פשוט לסתום  כשהייתי קטן ושיחקתי בxcom המקורי אני זוכר איך זעמתי על מדינות שהחליטו לחתום על הסכם עם החייזרים ולהפסיק לתמוך בנו…  LitalCohen אלופות הניו מדיה האמיתיות עושות שרשור מיץ תפוזים ברמת אביב ג OdedFire Icel GadiAleks SupergiantGames אתה עיתונאי רק אם משלמים לך על זה אני גיימר מבעבע DrMelodyPond עשית לי נוסטלגיה  DanaGat1 תיקון יש מצב שברמה האישית ההפגנות מרגיזות מאוד אותו ואת המשפחה והוא רוצה להיכנס בהן אבל אני לא חושב שהו…  DanaGat1 לא חושב שההפגנות מזיזות לו חושב שהוא עובד הרבה על להטיל את כל האשמה בקורונה עליהן זה בוודאי מה שהשופרות…  DanaGat1 בנט כנראה יקבל משמעותית יותר מנדטים וכידוע בנט שונא את נתניהו שנאת מוות אז בהתחשב בכך שהאלטרנטיבה הוא…  odedkramer אתה אשכרה רוצה שנגלול בפיד של קובי אריאלי האימה Hey SupergiantGames thanks for an amazing game Question When crosssaves come and I load my Switch save on the…  smallweed michaelzil לא קרן טטנוס תוקף סליחה </t>
-  </si>
-  <si>
-    <t>DavidLifshitz די ראיתי אתכם ביחד בהופעה של אוזי roykatz פנדמיה של אמת ולפני הקורונה היתה פה ממשלה ולפני הקורונה מישהו דאג לכם ולפני הקורונה קיבלתם תמורה למיסים במקום לתפוס… Mickeygitzin מיקי  נראית 66 avivatlas odedkramer barzik vlvl היי אביב זה פרוייקט עצום תפעולית ופיננסית ומתבצע בארץ מאד מהר ביחס למקומות אח…  nivshai שי תודה cch444444  ומי ידאג לך לטלויזיה  avivatlas היי אביב שלח לי מספר טלפון ואבדוק zako74 עודכנתי בבוקר zako74 בן מצטער על עגמת הנפש שלח לי מס׳ טלפון ואטפל TomerLotan אנחנו אלופי העולם ב״לתפור״ פתרונות לאלתר להמציא לקמבן וליזום הכי טובים כש״יורים עלינו״ ככה הפכנו למדינה ממציאה מובילה… yonibloch שלח כתובת ב DM yonibloch היי יוני  באתר שלנו אפשר לבדוק תחזור yonibloch  תומר מדייק  akivanovick כל כך חבל   אחד העיתונאים היותר חכמים סקרנים והגונים NoamGershony If we can do it so can you WearAMaskSaveALife  jessfeet  ZShilon  amsterdamski2 שאול רק סלקום tv השילוב הנכון של מוצר אינטרנטי ומתקדם הרבה תכנים כולל HBO ומחיר מצוין עושים גם הובלות cch444444 cellcomil ויקטור תודה חיפשנו משהו מדויק חול שוויצרי נבדוק את זה שבת שלום barkomforty היי בר  בודק את זה בינתיים מחזיר לך את הפתק  rahelibindman daveden11 נדב  תודה רחלי תודה   ofercorn תודה עופר Undercontrol200 barzik LaviShiffman מדויק zeevelkin מזל טוב זאב kann כאן מתרגשים לחשוף את הקליפ המלא של שחור לבן כחול לבן   בפעם הראשונה בשילוב של תחקיר עומק כוח מחשוב עצום ויוצרי וידאו וטכנ… michallovo akivanovick מיכל תודה וחג שמח MosheIce תודה מטפל akivanovick עקיבא רבי  אני אמנם מספק קווים כשרים אבל לא מאזין להם gadperez נראה שרשתות התקשורת עמדו בעומס והחשש מפני תקלות לא התממש סלקום מעריכה כי 100 אלף משפחות עשו שימוש בזום בליל הסדר מדובר בגי… arielschnabel תהיו יוסוף  Irisleal15 לצד המגלומניה של אתה בחרתנו ואור לגויים אין לפרטים בתוך החברה שלנו שום תחושה של זכאות האין זה מדהים חברה שלא חושבת שמגיע… במענה לבקשת אנשי הוראה הודענו אתמול שהגלישה ל zoom וסקייפ תהיה מחוץ לחבילה ובהמשך לפניות גם ילדים חרדים שלומדים דרך…  974jxh Dannyhbrown YoavCM טופל  ילדים שלומדים וכל מי שרוצה להאזין לשיעורים יוכל לעשות זאת ללא עלות בתקופת המשבר…  menachemgerst Dannyhbrown YoavCM אם אין בעיה טכנית נוסיף אשתי רכזת וחושבת שהמשוב עדיף 974jxh Dannyhbrown YoavCM היי אנחנו לומדים איך הדברים עובדים בדיוק בכדי להתאים פתרון שיאפשר לתלמידים להקשיב כאוות נפשם Dannyhbrown YoavCM דני  תודה שהפנית את תשומת ליבי  לא יהיה ילד שלא ילמד משום שאין לו גלישה  בעקבות זאת הודענו…  Irisleal15 פעם פעם בסבב הבחירות הראשון באפריל 2019 היה אחד אבי גבאי שלמד את כל בעיות מערכת הבריאות הוא הסתובב בבתי חולים דבר עם רו…    אז איך ייראו החיים שלנו אחרי הקורונה  הגירסה האופטימית RonHuldai הממשלה החליטה להפסיק את עבודת המורות והמורים בלמידה מרחוק לא ייחסך כסף רק יתווסף עלבון לציבור שהוכיח את מסירותו הפעם בחז… roykatz רועי אני חושב שזו היתה יונה 10elilevi zviashkenazi HavodaParty תודה אלי zviashkenazi HavodaParty תודה רבה לך צבי  dandayan דני יקר תנחומיי YoazHendel1 תודה יועז YaakovLebi תודה יעקב kunikran תודה חבר cohenmeirav תודה מירב אשמח לשמוע וללמוד 10elilevi תודה חבר רעיון מבריק   Shmuelbenzvi כשצפיתי בזה לפני חצי שעה חשבתי ש GabbayAvi קצת מגזים ואז קיבלתי טלפון ממישהי שנמצאת עכשיו במיון בשערי צדק ואמרה לי בדיו… kunikran קשה להאמין אבל הולכים לבחירות מה שנורא זה שאנחנו אדישים אין כח להילחם מקבלים כל גזירה בהכנעה עכשיו יריבו מי אשם ומה זה מ… BihariGilad ״גיוס החרדים״ הוא ישראבלוף בדיוק כמו חוק הגיוס עליו לפיד וליברמן שמו את יהבם זה טריק שלא היה מגייס אף חרדי באמת חבל ש… EldadYaniv תודה אלדד RavivDrucker ׳חבר בארגון לא נקי׳  תיזהר שלא תישאר הצדיק היחיד בעולם  אחרי הבחירות אספר מה יש שם ואתה תתבייש בכל…  RavivDrucker אם אתה חושב שהסרטון הוא אס ולא הרוטציה אז תתרחק מטקסס הולדהם RavivDrucker ואגב הסרטון לא ברשותי מאחר והוא נעשה למטרה מסויימת שלא התרחשה ומעבר לזה כמי שצילם אותו אני יודע שפי…  RavivDrucker דרוקר  מה קרה שחזרת להיות עיתונאי נחרץ  ראיתי אותך ביום שישי בערב אצל איילה חסון ממלמל משהו מבולבל…   ruthelbaz גם אני נשמה תומר מדייק   ליברמן נסיך האופל  מדויק   sshahar OrHeller ואתה חושב שלא הבנתי את השאלה  sshahar OrHeller שנתיים ושמונה אלא אם יילך לקצונה OrHeller תודה  Irisleal15 ההתלהבות מליברמן מפליאה אותי נפלתם על הראש אתם רוצים להחליף ראש ממשלה עם שלושה כתבי אישום בראש ממשלה שהצליח להמלט מכתב אי… amitsegal מזל טוב  אושר ובריאות ותוסיפי שהאקרדיטציה לקחה מהן את הזכות לטפל בחולים לטובת ישיבה אינסופית מול מחשב והקלדת נתונים שאף אחד לא יראה  SylvieKeshet זה באמת יעבור לך הרשעות תמיד תישאר לך עצוב מאד עם פטירתו של יוסי שבו ז״ל לשעבר ראש העיר נס ציונה איש נפלא ישר וחכם שכל מיפגש איתו היה מלמד ומעשיר  Syechimovich את משאירה חותם של ממש בחברה הישראלית   חותם שנובע מהיכולת המפלאה ומהאומץ  לראות את הקשר בין הנושאים…  נתנו להם אצבע לקחו את כל היד  כל תיאוריית מתווה הגז היתה שתהיה תחרות ולכן לא צריך לפקח על המחירים  צלצול השכמה לרגולטורים  BiranMichal מזל טוב מיכל כל כך שמח בשבילך  תודה לכולם מאחל לכל אחד שותפי דרך יקרים ומוצלחים כאלה   שוחחתי לפני זמן קצר עם היור הנבחר עמיר פרץ ואיחלתי לו הצלחה בתפקיד החדש מאחל לו שיוביל את המפלגה להישגים הראויים לה Irisleal15 לא משנה לי את מי ליברמן מתקיף אם הוא צודק או לא אם הוא משרת את עמדותי הפוליטיות אם בדרך נפתלת הוא עוזר למחנה שלי לעולם… צאו להצביע  ברכות NitzanHorowitz שמח מאד בשבילך אתה הקול הנכון למרצ הערב בועידת מפלגת העבודה אחרי שנתיים סוערות אנחנו עומדים כעת בפני מערכת בחירות חדשה ומפתיעה ואני קורא לכל המועמדי…  TheProletariat אסף אין ספק בגללי אנשי שמאל עברו להצביע לביבי Benadam2019 אבישי גם אני חשבתי לתומי שתיתן לעוקביך גילוי נאות שביקשת לעבוד איתי וסורבת  אבל תרגיש נוח אתה לא לב…  שבתאי שביט ומתנשאים שכמותו הם מבוני שלטון הליכוד והמתחזקים המרכזיים שלו  הם גורמים לכך שישראלים רבים מצביעים בהתאם…  ZeevKam מזל טוב  מיכל יקרה תודה על הדברים  אור לי יקרה  תודה  תמשיכי באומץ הנפלא שלך  doonch z1jgCrJzgLmBzKM EldadYaniv דנה תודה על הדברים לאה יקרה  תודה רבה   EmilieMoatti תודה מקסימה  חיליק תודה ושיהיה בהצלחה   GideonMeir benirabin גדעון תודה על הכל  selaudi1 benirabin אודי תודה  ofercorn עופר תודה על הכל  אלדד תודה רבה   ראשת העיר תודה רבה   תודה אורית זכיתי לראות אותך נלחמת לטובת הציבור  TomerPersico תודה תומר benirabin בני תודה רבה על הדברים  לתומכים ולחברים שלום  לאחר התלבטות ארוכה החלטתי ללכת עם הלב והאמת שלי ולהסיר את עצמי מהרשימה לכנסת הבאה  כמובן שה…  לתומכים לחברים ולשותפים היקרים והאהובים  לאחר מסע ארוך ורצוף באתגרים מורכבים החלטתי שלא אתמודד על ראשות המפלגה בב…  ביום 29718 פרסמתי בחשבון הטוויטר הודעה שבמסגרתה כיניתי את איתן ברושי עבריין מין והודעתי על השעייתו מפעילות במפל…  היתה לי הזכות להכיר ולהיות עם טל בתקופה שלפני ואחרי הבחירות מרגע שהצטרף טל עבד ועבד בלי הפסקה הגיע לכל מקום שבו…  חבריי וחברותיי המוסלמים בני החברה הערבית   לרגל חג עיד אל פיטר אני מבקש לברך אתכם בברכת חג שמח ומבורך ושנזכה לחי…  המומים וכואבים את לכתה של נחמה ריבלין שולח חיבוק ותנחומים לנשיא ולבני משפחתו הצניעות ואהבת האדם של נחמה ילוו אותנו תמיד יהי זכרה ברוך טל רוסו הודיע לי שהוא מוותר על השיריון שלו כמספר 2 ברשימה   פגשתי אנשים רבים בפוליטיקה וטל הוא אחד המרשימים שבהם…  מר ליברמן מסכים בתמורה תגלה לעם ישראל מי ולמה שילם 3 מיליון דולר  למיכל בתך כשהייתה רק בת 21  Amos123Biderman בידרמן  בקשה אחרונה אל תהרוג אותי בלי תבלינים טובים כשנכנסתי למערכת הפוליטית הבטחתי לילדיי שבכל החלטה שלי אראה לנגד עיניי רק את טובת המדינה וזה בדיוק מה שאני עושה יש כאלו שמסכימים שנכון היה להיכנס לממשלה ולעצור את חוק החסינות את הפגיעה במערכת המשפט ובדמוקרטיה הישראלית ויש שחול…  MoavVardi לא אמר כלום עמדתנו נותרה שאין מקום לבחירות נוספות ועל הנשיא לתת את המנדט להרכבת הממשלה לחבר הכנסת בני גנץ במהלך החודש האחרון מפלגת העבודה קיבלה  מספר הצעות להשתלב בממשלה   ההצעה האחרונה אמש כללה התחייבות לחבילת צעדים לשמ…  roussotal באתי לכאן להיות שומר סף של הדמוקרטיה לקבל את רצון הרוב ולא פחות מכך לשמור על זכויות המיעוט חברים חוקים נועדו להגן על כ… אם נתניהו יכשל בהרכבת ממשלה המנדט חוזר לנשיא  נתנגד לבחירות הן משרתות רק את נתניהו ולא את המדינה  לא ניתן למי ש…  אתם הצעירים שהמדינה מפקירה אתכם ליוקר המחיה למחירי שכירות מטורפים ולשכר נמוך – אם לא תצאו לרחוב נאבד את הדמוקרטי…  AviBenayahu החשבון הקטן והאישי מאוד שלי עם barakehud מוכר וידוע  אבל ביום השנה ליציאת צה״ל מלבנון  צריך לברך ולהודות לברק על היו… חתמתי ותומך במאבק כל כך צודק להחזרת הבטחון האישי ל 20 מאזרחי המדינה  הצעירים הנפלאים של ישראל המבוגרים שנתנו את הכל כדי להקים כאן מדינה לא יעמדו מנגד בזמן שישראל תהפוך לדיקטטורה  אנ…  עוד משרדי ממשלה עוד שרים עוד בירוקרטיה עוד טירטור של האזרחים שיעברו מעכשיו בין משרדים נוספים ועוד מיסים כדי לממן…  זוהי שעה אפלה לדמוקרטיה אחרי החסינות לנתניהו תגיע גם חסינות לטייקונים שתומכים ונתמכים על ידו  תרבות של חסינות היא…  אחי הצעיר יהודה הוא אחד המרגשים שבשירי הזכרון  היום בבית העלמין בבנימינה השיר הפך לחצי מציאות כשפגשתי שניים מחבר…  תפילה  גיורא פישר  מִי יִתֵּן  וְאֶהְיֶה כְּבָר זָקֵן  מְבֻלְבָּל  אִם אָז אֶשְׁאַל  לָמָּה הוּא לֹא בָּא לְבַ…  מברך על הפסקת האש ושולח תנחומים למשפחות ההרוגים ואיחולי החלמה לפצועים אחרי עשרים שנים שנתניהו מחזק את החמאס  שחרו…  משתתף בצער משפחתו של משה אגדי מאשקלון שנהרג מפגיעת רקטה ושולח איחולי החלמה לפצועים לתושבי הדרום מגיע לחיות בשקט וב…  אינני מכיר ומעולם לא פגשתי את גיל מסינג דובר צהל המיועד  רק אלו שרואים את המשטרה והפרקליטות כאוייבים יכולים לצאת…  גם השנה נעמוד יחד לזכר המיליונים שנרצחו רק בגלל שהיו יהודים למען מי ששרדו ונושאים עמם צלקות שאי אפשר אפילו לדמיי…  התרגשתי לומר מתחייב אני בטקס ההשבעה היום בכנסת זאת זכות וחובה גדולה לשרת את עם ישראל נמשיך להילחם על הדמוקרטיה…  למי שכבר הגיע ולמי שעוד בפקק למארחים ולמתארחים למי שקורא כל פסיק בהגדה ולמי שרק מחכה לאוכל   חג שמח שנדע לא רק…  הגענו לנשיא והמלצנו להטיל על בני גנץ את הרכבת הממשלה למרות הסיטואציה הפוליטית  הדגשנו שנילחם מהאופוזיציה שהדמוקרטי…  אנחנו כאן בטירה כדי לאמר בקול רם שלאזרחי ישראל הערבים יש זכות לבחור ולהיבחר ואני קורא להם לממש אותה ולהשפיע על עתי…  אנחנו היחידים ששואלים את ביבי את השאלות הקשות באמת  איציק שמולי הספיק לנחות אתמול בארץ עם הרכש החדש למשפחה ומילא את כולנו בגאווה והתרגשות  ככה זה כשמחויבים לשינוי תי…  שרונה הנהדרת הצטרפה והתחייבה לשינוי וכמוה עוד הרבה אחרים שהצביעו היום בפעם הראשונה לעבודה אל תאבדו תקווה אף פעם…  עוד 100000 מצביעים של מפלגת העבודה שיכולים לעשות את השינוי צאו להצביע העבודה  barakehud עוד שלוש וחצי שעות  מחיקת או גימוד העבודה ומרצ אם חלילה תתרחש  תוביל בהכרח לממשלה קיצונית בראשות נתניהו זוהי גם שגיאה פ… אם העבודה תימחק  ביבי ראש הממשלה  תודה אורי  nadavabeksis Irisleal15 לך אחרי איריס Irisleal15 הצבעתי למי שמרגיז אותי כל יומיים למי שיש לו ראש בארד ולפעמים הולך איתו ישר בקיר למי שהכי מתאים לראשות הממשלה מוכשר ונחוש… גאה בבן שלי חניך מכינת רבין הולך עם האמת שלו  נתניהו צא כבר מהגזענות שלך זכותם של ערביי ישראל לבחור ולהיבחר קורא לכם צאו להצביע בהמוניכם  נתניהו גזען ושקרן שקר המפלגה הגדולה ושקר הדיל שלא היה ערביי ישראל הם אזרחים שזכותם לבחור ולהיבחר נגד השקרים והגז…  צאו מהספינים צאו מהשקרים  צאו להצביע ולכו עם האמת שלכם רק מפלגת העבודה  RamiHod ראיתי עכשיו תוצאות של מספר סקרים שבוצעו היום הסיפור פשוט מה שכחוללבן עושים מצליח התוצאה הניתוח יצליח החולה ימות במצב כ… roussotal מסתובב בקלפיות תל אביב ופוגש את מפקדי היקר ראש הממשלה לשעבר barakehud אהוד ברק  שהלך גם הוא עם האמת שלו  אמא שרה היקרה מצביעה לראשונה בחייה  אמת העבודה והיא לא היחידה רבים אחרים קראו את התכניות שלנו התאהבו בנבחרת של…  GabbayAvi אני מבקש מכל חברי מחנה השינוי להקשיב היטב לראש הממשלה ושר הבטחון לשעבר אהוד ברק האיש שהוביל עשרות מבצעים מעבר לקווי האויב… בוקר נפלא לכולם הולכים עם האמת שלנו שמים אמת בקלפי למען השינוי בגלל הדרך בזכות הנבחרת  יחד אנחנו נעשה את זה תאמינו העבודה תודה ילד  AnshelPfeffer אצביע עבודה כי היא מייצגת היום את התקווה הטובה ביותר לאיחוד החברה הישראלית סביב מכנה משותף שהוא לא רק סגידה לכוח אבי גב… מצמצתם קבלו את זה  סיכום הבחירות ב90 שניות  חוזרים לדרך חוזרים לעבודה  השיחה האינטימית בין ביבי ולפיד נחשפת  נתניהו ולפיד משקרים  שקר המפלגה הגדולה  בלי מרפסת אבל עם נשים חזקות הנבחרת הכי טובה בישראל יחד כל הדרך לשינוי אל תפלו לספינים לכו עם האמת שלכם  רק קו…  אני מבקש מכל חברי מחנה השינוי להקשיב היטב לראש הממשלה ושר הבטחון לשעבר אהוד ברק האיש שהוביל עשרות מבצעים מעבר לקו…  כדי שהקול שלכם באמת ייקבע לכו עם האמת שלכם תצביעו לדרך אמיתית לנבחרת שאתם סומכים עליה לשינוי שאתם מאמינים בו כ…  דינה היקרה תודה רבה   RomanBronfman תודה רומן אלדד   תודה רבה   MatanAlcalay אשמח אם מישהו יסביר לי באמת איך הצבעה לרשימה שיש בה את טל רוסו איציק שמולי סתיו שפיר שלי יחימוביץ רויטל סויד מרב מיכ… נתניהו יספח את כחול לבן לממשלה ויספח 25 מיליון פלסטינים לישראל  אומרים לא לסיפוח  מצביעים העבודה  אתמול בלילה נתניהו הכריז על המהלך שעלול להוביל לחיסולה של מדינת ישראל  סיפוח של יהודה ושומרון וכחול לבן במקום ל…  לפיד עלול להקים את ממשלת נתניהו הבאה  zionnenko הספין על חשיבות המפלגה הגדולהשמקדמות הליכוד וכחוללבן הוא כל כך מטופש ורחוק מהמציאותשברור שהוא יתפוס   גם אם אחת מהן תקבל… drorbin זה הפתק שלי לעוד יומיים למה כי אני רוצה בכנסת אנשים שיעבדו בשבילי ראינו בכנסת הקודמת כמה עשו החכים של העבודה ועכשיו קיבל… granot בשמחה עידו  yitzy4 אני ימין מדיני וימין כלכלי אך אצביע GabbayAvi למה תקראו את grolnik   GabbayAvi פעם שקרן תמיד שקרן  GabbayAvi מי שחונה בכחול לבן  יגררו אותו לליכוד  גם ב0904 הולכים עם האמת שלנו  הנבחרת הכי טובה הכי לוחמת והכי מקצוענית בישראל רגע לפני הבחירות על עתידה של המדינה amirperetz MeravMichaeli…  עם הנבחרת המעולה שלנו מציגים את התכניות שלנו לשינוי פני המדינה על גבי מסכי ענק בתל אביב מוזמנים להספיק להגיע עוד…  מי שחונה בכחול לבן  יגררו אותו לליכוד  kannnews יור מפלגת העבודה GabbayAvi בשבתרבות בתא אני מסתכל על ראש הממשלה מפטר אנשים מפתה אנשים הכל כדי לתת מיליארדים לטייקונים… kannnews חכ StavShaffir ממפלגת העבודה בשבתרבות בגבעת שמואל צריך להחליף את נתניהו אם לא תהיה מפלגת עבודה חזקה אז המנוע האידיאולוג… גפן הבת המקסימה של הילה הדוברת שלי  אני חייב לה המון שעות אמא  GabbayAvi 7000 שח שכר מינימום מבינים לביבי אין ארנק איך יבין צפו ורטווטו  aradeyal כל פעם אותו הדבר  מתי הם ילמדו  פעם שקרן תמיד שקרן  איזו נבחרת הבוקר בתל אביב בדרך לאירוע הצעירים שלנו לדבר על הנושאים שחשובים באמת לצעירים בישראל ועל התכניות שלנו…  התקבלנו במטח סוכריות בשוק הכרמל מרגישים את השינוי באוויר  10elilevi ברכות אלי יקר מהפרסים המוצדקים שניתנו  תרשה לי להוסיף שאתה לא מביא רק נושאי פריפריה אלא גם הרבה שכל יש…  7000 שח שכר מינימום מבינים לביבי אין ארנק איך יבין צפו ורטווטו  TheProletariat סיימתי הדרכת קלפיות לכ100 חברי ועדת קלפי  מרגש בכל פעם לדבר על טוהרהבחירות ולשתף בטיפים ודגשים לתהליך ההצבעה והספיר… eransinger על רקע הקריאה להחרים את ההצבעה בחברה הערבית איך בונים קמפיין בערבית לקראת הבחירות במה מתמקדת מפלגת העבודה ומה מייחד את ה… sharonidan אבי גבאי GabbayAvi מגיע לכרמל אינעל העולם באקסטרים  נרגשים על החזרת גופתו של זכריה באומל זל הלב עם משפחתו ועם שאר משפחות הנעדרים שממשיכות להמתין בכאב ברכות לכוחות הביטחון על המבצע ההרואי עכשיו בשוק הכרמל מתקבלים בממטרי סוכריות זה לא רק הסוכריות זה האור בעיניים של האנשים זה הרצון העז בשינוי וזאת ה…  HavodaParty מטח סוכריות ואהבה עכשיו בשוק הכרמל  עם ישראל רוצה שינוי ולעם ישראל מגיע שינוי זה מה ששמענו וראינו בסיור הבוקר עם יור… שולחים איחולי החלמה לגברת הראשונה נחמה ריבלין גם אחרי כנס בגבעתיים  המנה הטובה ביותר ביקום  נתניהו ממשיך לתקוף את ריבלין שיתבייש  תומכים בממלכתיות תומכים בנשיא  לא דרמטי איבדתם את הביטחון ב0904 תאבדו את העם  חברת חשמל מוותרת על מיליארד וחצי דולר מהכיס שלנו ובתמורה חברות הגז ימכרו גז למצרים המשך של שוד הגז רק אנחנו במפלג…  נתניהו שוב נכנע לחמאס שתפו  barakehud אמור לי מי הם חבריך ואומר לך מי אתה  yoavkeren2  איך יודעים שנתניהו יעשה הכל כדי לגנוב את הבחירות  ככה  צחצחים נתניהו אתה לא מתבייש אתה שאמרת שחיילי גולני טובים כל עוד יש להם קצינים לבנים אתה שהקמפיין והבית שלך מ…  KnessetT יור מפלגת העבודה GabbayAvi לפרלמנט צהריים עם mazalm3 בהתנהלות של netanyahu אין קווים אדומים ונועדה להציל אותו מכתבי…</t>
+    <t>אין סוף חרדים מחרטטים פה על ניראות ההפגנות מול המגבלות עליהם איפה היתה הניראות הזו כשמערכת החינוך החילונית נסגרה ל…  eranetzion DramaSkills אתה טועה התפטרות של שרי כחול לבן כמו שכולכם דורשים בלי השלישיה הזומשאירה את נתניהו ראה…  YakiAdamker מציע ללמוד דבר או שניים על הליכים פרלמנטרים ועל תפקיד האופוזיציה ציוץ מביך idaholloway הרבה קודם כשלא סגרו את הטיסות מארהב כי פחדו מתגובת טראמפ שכל חרדי שמגיע לחדר מיון ומתאשפז בגלל קורונה יודיע בקבלה שהוא פה בגלל ההפגנות  SuperDori סליחה tzvidanieli פוקס ככה קוראים לזה moshemenachem1 shacharbm ברור אצל שמאלנים יש 25 חיובי בבדיקות הקורונה מדהים לראות שגם אחרי כל כך הרבה התפרצויות בישיבות יש פה עוד חרטטנים שמתווכחים על מתווה הקפסולות אין דבר כזה מתו…  elicoh itainathaniel logreisas לא היה צריך בכלל להיפתח השנה מד וצפונה כל מי שיכול להישאר לבד בבית בדמוקרטיה ממשלה לא יכולה למנוע מאזרחים להפגין מולה בטח כשאין לזה שום הצדקה בריאותית את ענייני המשמעת והנראות צרי…  logreisas אלו לא מוקדי התחלואה איזה סגר  YakiAdamker אולי קצת פחות עיסוק בהפגנות ויותר בהתפרצות במגזר ישראל לעולם לא תיחלץ מהמגפה כשהחברה החרדית מתעקשת על קיום המנהגים והנהגתה עוסקת בהפגנות במקום בתחלואה קראו את אנש…  sinister314159 כנראה שפיספסת את הסרקאזם שלי DramaSkills אם יתפטרו הנדל האוזר ויענקלביץ ישארו ויתנו לביבי ממשלת 62 זה נהדר  ksoko123 לדעתי צודק רבים חושבים שלא bnyiroz אתה לא עסוק במפגינים zsiroka72 לא טעה אתה מביך את עצמך  zsiroka72 שמע אתה לא אמיתי  zsiroka72 itzikelrov גם פה  zsiroka72 אתה חושב  itzikelrov לפני שבועיים וחצי דיווחו על עשרות נדבקים בישיבה הזו רק לפני שבועיים וחצי דיווחו על עשרות חולים בישיבה הזו  nitayp Nefolet ISudri וסגל ישיבה שבא הולך prokooter הוא שופר מלא בסהכ משתמש בפסאודואקדמיה להפצת המסרים prokooter אתה חדש פה EranAzoulay נתראה במאי מי היה מאמין  Rereshef אמרו משהו על מוזיקה מזרחית karmelhaifa YoavShani1 swathyeald הנדל האוזר ויענקלביץ maayanef וואו itayalmogbar zashaked אין ויכוח שחייבים להילחם לא נותר להם עוד דבר אחר להצדיק את קיומם שם zashaked itayalmogbar זה לא עדיף עם ממשלת62 נתניהו מקים דיקטטורה ב5 ימים manuelbaz יומולדת שמח  atsra בלי ספק freyisrael1 חלאות BenCaspit להשעות יכולים רק המוחים לא הממשלה מולה הם מפגינים keren38013683 לא SamionBuchas natifried4u אין לזה רוב לצערי Justhadto BenKapl06079542 יש לו ביד את המדל האוזר ויענקלביץ GalYoffe itayalmogbar הם אותם אנשים אפרופו המונולוג של דני קושמרו ביום שישי  GalYoffe itayalmogbar זה כבר קרה מי את חושבת הניח את האקדח על שולחנו של גנץ וגרם לו לפרק את כחול לבן ולהיכנס לממשלה natifried4u לא ממש GalYoffe itayalmogbar נראה לך אם יערקו ויאפשרו ממשלת ימין ימין הם יהיו מלכים ilanbentov TheOnlyLiron ויענקלביץ natifried4u חוץ מזה שההתפטרות תשאיר את נתניהו עם ממשלת 62 GalYoffe itayalmogbar אין להם עתיד במרכז שמאל רק בימין שם האינטרס GalYoffe itayalmogbar עכשיו המצב גרוע פי כמה shoshgru itayalmogbar הנדל האוזר ויענקלביץ לא יתפטרו GalYoffe itayalmogbar כי הם לאומנים ימנים וגזענים יגידו יש קורונה ואסור ללכת לבחירות בדיוק כמו שאמרו לגנץ בסוף מרץ SargonoffAkkad הטימטום הזה מתחלק שווה בשווה עם הגיבורים החדשים לפיד ובוגי Orengerman הצבעתי לגנב קולות אחר לא דרמה itayalmogbar יש אין סוף ביקורת עליהם כמעט כולה מוצדקת אבל בסוף היום ההתפטרות שלהם לא תשרת אף אחד מאיתנו רק יש…  BenKapl06079542 לאופוזיציה אין משמעות אתה כבר יודע את זה הכנסת סורסה לגמרי בעשור האחרון צא קצת מהרומטיקה Orengerman אתה לא מבין האוזר התכוון להיבחר בשביל לסכל את מאיר כהן ואת חוקי הנאשם הוא והדביל השני שמו אקדח על השו…  itayalmogbar הם לא יכולים להפיל איתי אם יתפטרו ביבי יישאר עם ממשלת 62 SargonoffAkkad אתה אשכרה לא מבין במי מדובר 3 גזענים לאומנים שנכנסו בקולות השמאל עריקה הופכת אותם לכוכבים במחנה שלהם BenKapl06079542 ממשלת 62 הופכת את ישראל לדיקטטורה בשבוע itayalmogbar אתבאס מאוד אבל מה אתה רוצה שאומר אני לא תומך שלהם ולא הצבעתי להם הם תקועים שם כשההתפטרות שלהם רק…  SargonoffAkkad 59 של הבלוק בתוספת הנדל האוזר ויענקלביץ או שאתה בונה על ההגינות שלהם Orengerman כל הפרשנים הפוליטיים דיווחו את זה עופר שלח אמר את זה אתה מעדיף להמשיך ולצעוק למרות שהמציאות בסוף מרץ…  SargonoffAkkad השפיעו מאוד במשפטים השפיעו בסיפוח השפיעו קצת בחיי היום יום האלטרנטיבה היא ממשלת 62 של נתניהו גם את זה צריך לזכור ksoko123 כל אחד רואה ומתרכז במה שאין לו OGolobov TheOnlyLiron איך תעיף תהיה לו ממשלת 62 בלי בלמים BenKapl06079542 מה תיתן ההתפטרות נתניהו יישאר בראש ממשלת 62 Orengerman האחטרנטיבה גם אז הייתה ממשלת 61 של ביבי אתה לא מצליח לזהות את המורכבות הנדל והאוזר לא איפשרו את מאיר כהן ואת חוקי הנאשם Orengerman אז אתה חושב שממשלת 62 של נתניהו עדיפה כן אוחנה במשפטים בתי משפט סגורים כל חוק עובר אוטומטית TheOnlyLiron יתפטרו  נתניהו נשאר עם ממשלת 62 זה עדיף בעיניך RanBalicer 4 תובנות ממידע ומחקר הבאתי הערב בשידור  1 שיעורי התמותה בישראל מהגבוהים בעולם והתמותה המצטברת מטפסת בחדות  2 20 מהנדב… Orengerman מה תיתן ההתפטרות נתניהו יישאר עם ממשלת 62 צריך להילחם מבפנים giladbaum אבל לא היה לא רוב הנדל והאוזר לא איפשרו כתוב YoavShani1 swathyeald כותב לך זמיר שהנדל והאוזר לא איפשרו את מאיר כהן ואת חוקי הנאשם אתה הפכת לניהיליסט מעדיף מ…  IamYaure  yhalevy פוסט מדוייק בלא מעט דברים swathyeald אין ספק עשו המון טעויות rapoporthila גם אני לא EnTT לא יעבור EnTT לא יעבור פוסט יום כיפור של אסף זמיר אישית התחברתי להמון דברים שכתב שווה קריאה  AmirDolev1972 ממש yhalevy נכון עם כל הכבוד לקליפים הסיפור עם בני הישיבות הוא לא האוטובוסים והצפיפות בהסעות הסיפור הוא בני נוער וצעירים שחוזרים מ…  yoslevy למה לספר לו מהיכרות אישית איתו אם יקבל פקודה בלתי חוקית הוא יעשה את הדבר הנכון gilgu ליקוק סטנדרטי RamiHod משוכנע שהקורונה תשנה RamiHod עוד יבואו איתם חשבון yakov57v מחיל אל חיל liranofek מסכים רמת ניתוק מהמציאות הצימרים בבחריין  Teodor1 גם לא יידבק משוכנע בזה tommybor גם שלי Teodor1 לא חריג שמעת את מנכל משרד הבריאות את נציגי משטרת ישראל בתקשורת את הרופאה ההיא ממשרד הבריאות שטענה שהמפגינים לא ציונים Teodor1 שאל את דעתו על ההפגנות אמר שזה לא תפקידו ושישראל היא דמוקרטיה אל תלך לשם מתוך הראיון של בן כספית עם האלוף אורי גורדין מפקד פקע״ר בדיוק ככה צריך לענות כל לובש מדים ופקיד ממשלתי בישראל בעני…  NoamC aviadglickman כל הכבוד D5887610 AnshelPfeffer פספסת את הסרקאזם Lewafcb1 אתה לא מרגיע אותי משלב מסויים אנשים מתים בכמויות בשל חוסר היכולת לתת טיפול לכזה עומס של חולים אנחנו לא רחוקים משם MatanAlcalay מלך uv1709 limormoyal בלי ספק Yoglas74 אין עליך aviadglickman במידה בהרצליה ורמת שרון ככל שראיתי הכל היה פתוח והתפללו בפנים anatnh ברור הם לא סתם מחזיקים שם מעון עם מנקות ומבשלת Teodor1 המנהיגות שלהם כושלת הרבה יותר שלהם מסכנת את חייהם  ביודעין מהמרת על הגיל הצעיר של בחורי הישיבות ומפקירה את החלשים והמבוגרים YaneevM הוא שילם בחייו על ההסתה של המחנה שלך הייתי סותם קצת במקומך AnshelPfeffer אנשיל אתה טוען שהסיכום עם רוני נומה לא  יחזיק מים  YaneevM רצית לומר עסקאות נשק שלום עושים עם מדינות שיש לך עימות איתן anatnh נורא הא איך מעיזים פה להפגין מול הקיסר ומשפחתו YaneevM לא עוזר וזה לא שלום שלום עושים עם מדינות שיש לך עימות איתן זו עסקת נשק limormoyal ממשלה פושעת bnyiroz מדהים שהתחלואה המשתוללת בריכוזים החרדים לא מלמדת אותך לשתוק לפעמים אולי זה יקרה מתישהו בהצלחה לכולנו  JoshBreiner גם ברמת השרון והרצליה בכל בתי הכנסת התפללו בפנים Eden61mandatim יודע קרא אצל נייט סילבר Idollete שבועיים פחות או יותר Eden61mandatim ממליץ בחום לעקוב אחרי ממוצע הסקרים ולא סקר בודד ב317 חצינו את 500 המתים זה לקח כ20 שבועות ב59 חצינו את ה1000 מתים זה לקח 5 שבועות הערב אנחנו ב1500 מתים 3 שבועות ויומיים Eden61mandatim שנשים כסף על העימות הזה האתגר של ביידן לפמפם למצביעים במדינות המתנדנדות ולמעמד הביניים האמריקאי שיש להם נשיא נוכל איש עסקים עלוב ובעיקר אחד שמעלים מס על חשבונם odedkramer ״שחקן״ 1499 מתים אתמול בעדכון האחרון לפני הצום היו 1450 עליה של 49 בקצת יותר מיממה odedkramer עולים עם נערים ג׳ Arspoeti אני דומע פה תודה ששיתפת danielpet4 אבל זה מבעיר אותה danielpet4 זה בדיוק מה שצוקרברג רוצה תביא לו עוד כמה הייטרים לפלטפורמה litigilad תגידי את אמיתית זה קליפ הסתה זה נשיא פתאט לא נתפס שאת לא מסוגלת לקלוט מה אתם עושים מושל טראמפיסט  YoavShani1 Yashar2U edvalotan rikycohen4 הו הם צריכים להתעורר עוד רגע גם תגיד שאם רק נביא איזה ימני לייט לרשי…  YoavShani1 Yashar2U edvalotan rikycohen4 להדהד את הקליפ שלה זה וואחד גול עצמי Yashar2U edvalotan rikycohen4 אני הכי בעד להתייחס ולמסגר את זה נכון רק לא להפיץ את הקליפ שלה כמו שהוא ברשתות זה גול עצמי עצום YoavShani1 Yashar2U edvalotan rikycohen4 והתעלמתי מהוואטאבאוטיזם YoavShani1 Yashar2U edvalotan rikycohen4 רגע אתה לא זה שטוען פה כבר חצי שנה שהכל אבוד פתאום אתה דני האדום Yashar2U edvalotan rikycohen4 את טועה כל הפצה חושפת אותו לעוד אנשים שאומרים לעצמם לגיטימי לדבר ככה בפרהסיה ואפי…  Soloph0ne אתה שוב הולך לאדם הבודד מי שמפרש ככה ומי שמפרש אחרת אני לא מדבר על זה בכלל האלגוריתם של הרשתות ובמיוח…  Yashar2U edvalotan rikycohen4 לא להדהד את קליפ הרפש שלה מה לא ברור בזה על כל 3 שמאלנים שיצקצקו ויקוננו יחד אית…  SchibyAmir מעולה Yashar2U edvalotan rikycohen4 ברור אמרו לך לעצום עיניים ולהתעלם זה מה שנכתב פה SweetCapsule שעה אחרי תחילת המום עשרות כלי רכב טסים בכבישים כולם בדרך למיון זה נהדר  Nefolet רעיון Soloph0ne אבל לא צייצתי עליך יש פה מאות שיתופים של הסרטון הזה משמאלנים כולנו פעם חשבנו כמוך שחשוב לחשוף את הצביע…  Soloph0ne לא מבין מאיפה הבאת את יחבקו אותנו הבעייה לא תיעלם פשוט לא צריך לסייע להפצת הרפש אפשר לצייץ ללעוג ולה…  GilTevet גלול את הפיד אין סיכוי שתפספס את זה שותף פה מאות פעמים Soloph0ne בקבוצה של חברים זה סבבה אין שם אלגוריתם שמזהה עניין ומקדם ברשתות החברתיות זה משחק לידיים שלה Soloph0ne כל העולם יראה  עוד שמאלנים שיצקצקו ועוד הרבה יותר פאשיסטים שיזדהו ויקבלו לגיטימציה לקליפים דומים ככה ז…  Soloph0ne האלגוריתם לא מבחין בין שמאלני נסער שמצקצק לימני פשיסט שאוהד הוא רואה עניין ומקדם זו המציאות RTsipris misscorina2 מיקי זוהר נראה ממש טבעי Soloph0ne אתה מסרב להפנים איך הרשתות עובדות אתה מסייע להם להפיץ שנאה זו עובדה chellig היא ולא אחרת המון תגובות לציוץ הזה ובאיזשהו שלב השתקתי נוטיפיקציות זה לא הכפייה הדתית זה לא החוק זה לא החופש לעשות מה שבא לך…  yaniva הצימרים בערבות הפרסום בNYT על דוחות המס וההפסדים הכבדים שתאגיד טראמפ צבר עם השנים סיכוי לא רע שעוד הערב יכריזו בבית הלבן…  AdamAlbag LiorTayler nirbenz TrinityZ20Z למה שילמדו הם קראו בפייסבוק איפשהו litigilad RTsipris זה בדיוק מה שצריך לעשות להגחיך למסגר לא להדהד את הרפש שלה HiggsBozoEffect הבנת מצויין אתה סייען של הביביסטים בהפצת הרפש litigilad רק שכמוך יש מאות אם לא אלפים אם אתה לא מבינה את זה את לא מבינה איך רשתות חברתיות עובדות litigilad האלגוריתם לא מבדיל בין אוהדים למצקצקים הוא מזהה עניין ומקדם litigilad אין לך מושג איך האלגוריתם של הרשתות עובד הא חלק גדול מהקידום מגיע מהמזדעזעים באותו עניין ככה ממסגרים בלי להדהד את הרפש  TheSocialist9 NiflaPo יאפ NiflaPo המטרה כמו שקרמר אמר היא לצקצק ביחד במציאות ההידהוד מאפשר לאכולי השנאה לגלות שהם לא לבד בעולם ונותן להם לגיטימציה ופרסום ShaniAshkenazi odaskal לא חושב שאנחנו המיעוט היא המיעוט הצרה עם הידהוד השנאה הזה שאנשים כמוה מגלים שהם לא לבד ומקבלים לגיטימציה edvalotan ברור שלא תוצר של מכונת הסתה ודלגיטימציה משומנת למה להדהד אותה NiflaPo אין דיכוטומי מזה שמאלנים מוכנים להדהד את הרפש נגדם תמורת כמה לייקים עלובים מחבריהם shoshgru emmanuelrosen2 של יוזף Eden61mandatim גלול את הפיד emmanuelrosen2 שתפו שכולם שיראו את הצביעות שלו odaskal עמוק אבל ההידהוד של זה מטומטם לא פחות guyelster אני שם לפניך guyelster נמות צודקים חברת כת ביביסטית שאיש אינו מכיר מעלה בערב יום הכיפורים קליפ מחליא ומלא רפש על שמאלנים לפייסבוק בתגובה עשרות שמאלנ…  davidrozental carmelkamin לא סתם היוונים העלו את המכסות לישראל בספטמבר פי 20 אחרת התיירות שם מתה YossiDorfman אפשר למסגר עם תמונת מסך לא להדהד את הרפש הזה davidrozental carmelkamin לא בספטמבר אוקטובר זה כמעט בלעדי של ישראלים YossiDorfman אבל למה להדהד אותה nirbenz TrinityZ20Z תגיד לא נמאס לך עם חירטוטי היד הנעלמה הקורונה הוכיחה שאין דבר כזה כוחות השוק ובלי התערבות מ…  carmelkamin איזה תיירים רק ישראלים מגיעים עכשיו nirbenz TrinityZ20Z מה לא ברור בפיקוח זמני למה הכל צריך להיות מטומטם פה זו מגפה ואנשים חייבים מיגון לא מחיר הבמבה בפיצוציות nirbenz TrinityZ20Z אתה כנראה לא מכיר את הסיפורים אנשים מכרו ב150 מה שקנו ב5 מחיר המסכות אצל היצרנים השתנה מעט מאוד ilanbh89 אם אתה חושב שעשרות כלי רכב פרטיים ב3 שעות רכיבה מיהרו כולם למיון שיבא יש לי ראש ממשלה ישר למכור לך nirbenz TrinityZ20Z כלכלה עובדת ככה בדיוק בגל הראשון אנשים פרטיים ויבואנים הפקיעו מחירים הרוויחו אלפי אחוזים…  TrinityZ20Z נו אז פיקוח עושים כשהמחירים משתוללים ומסירים כשהם יורדים קוראחם לזה צו זמני בגל הראשון אנשים שילמו 150 שקל לחבילת מסכות יום כיפור  בול בפוני  liran2020 לכבוד הציוץ של דודו שרשור טעויות שלו לאורך הקריירה התחלנו Yosinive העיקר שלמד לרכוב ilanbh89 ההתרשמות שלי היא שהרוב המוחלט נסע מבחירה נהג בודד בכלי רכב בלי מהבהבים לאותת על חירום Yosinive קרוקס תקראו לי נביאה  ShaniAshkenazi חשבון פארודי לא שלו מיליון מתים מדווחים מוירוס הקורונה  GRachmani MatanAlcalay אבל ממש LeBlueFlame זו ידיעה מלפני 3 ימים בדיוק שבועיים אחרי העצרת אדם שלקח חלק בעצרת של טראמפ במישיגן שחלקה נערך באולם סגור אובחן עם קורונה  danielpet4 היה המח״ט שלי Yanix2Go רכבתי גם בגימל ואזורי חן גם תל אביב חיפה נסעו בלי סוף מכוניות Banboonsdum מותר לעשות ספורט טרחני</t>
+  </si>
+  <si>
+    <t xml:space="preserve">שמאלנים אלימים ארורים  hovevamim העבירה של ליאת בן ארי היא עבירה קלה יחסית ועדיין היא חמורה פי כמה מהעבירות שהיא המציאה לנתניהו   שווי של עוד חדר בבית gtgtgtgt… BittonRosen מפגיני שמאל תקפו פקחים ושוטרים כעת סמוך לכנסת ואף פצעו שוטרת לאחר שהכו אותה באמצעות מקל RubiYona חשיפה חכ אלי אבידר מישראל ביתנו בשיתוף פעולה נוסף עם הדגלים השחורים ‍  קרדיט 2346479Orna  IlanTsion פרשת ליאת בן ארי ובנה משטרת שדות מעכבת טיפול בשתי תלונות שהוגשו כנגד תומר שוויקי בגין תקיפת המפגין והשוטר התלונות הוגשו…  BarashiKinneret תהיו מוכנים עם פוש גליקמן  בטעות פולמוס עשה גזור הדבק להודעה של משרד המשפטים אולי  הוכחה כמה הם מהנדסי תודעה אנו… RubiYona ראש הממשלה מר בנימין נתניהו מאוים ללא הרף הסתה לרצח שלו ושל בני משפחתו איום בהשלכת רימונים כיתור בית רהמ עם התפרעויות וחס… KoheletForum ראש מחלקת הליטיגציה בפורום קהלת בטור נוקב על האיומים ניגודי העניינים סוגיית הסמכות ומסרים בעייתיים נוספים שהגיעו מהיועמ… hovevamim למיטב זכרוני עבירת ההשבחה הבלתי חוקית של המבנה בראש העין היא רק אחת העבירות של ליאת בן ארי ישנה עבירה נוספת של עצם הרישום… LiberalRiWo דנמרק  מדינה מאוד מאוד מסודרת פתחו את הלימודים ללא מסיכות וללא ריחוק וחשבו עד לפני שבועיים שהכל מוצלח עכשיו המספרים מוכ… galidalal איך אפשר להאמין לליאת בן ארי שווקי כתובעת אמינה ישרה וצדיקה בתיק התקדימי נגד בנימין נתניהו כאשר השופט רוזן טוען שהיא אמורה ל… yotameyal בואו נניח שבאמת רוב פיצולי דירה מאושרות בן ארי הודתה בעבירה בתחום האכיפה שהיא בראשה מה הייתם אומרים אם ראש התנועה היה נתפס… hovevamim חריגה מינורית שגדולה בשוויה הכספי מ100 פרסומי כתבה בוואלה קל וחומר סיגרים ושמפניות ErezZadok1 להבנתי השופט בעניין ליאת בן ארי קבע שהיא עברה עבירות בניה אבל היא לא עברה עבירות בניה או שהיא עברה עבירות בניה אבל זה לא ע… וואו  elizipori ליאת בן ארי מודה אני עבריינית בנייה  ״מן הראוי שהשינויים המסויימים שנעשו בבית כמו גם הפיצול ל2 יחידות דיור ייעשו רק לאחר… elizipori דוד רוזן במסר ברור לליאת בן ארי ולמנדלבליט בפרשת ראש העין משרת ציבור בטח ובטח משרת ציבור במשרה בכירה מצווה להקפיד ולהיזה… avribloch התמונות המזעזעות של הפרות הנחיות הקורונה ההמוניות מבני ברק הן תוצאה ישירה שההפגנות לא מוגבלות  יש דתיים וחרדים שיתעצבנו וי… BarashiKinneret השרלטנים גליקמן ודרוקר לא יספרו לכם ש היום ניתן דוח שלילי עי רוזן שקובע ליאת בן ארי מודה בעבירה בניגוד לחוק תכנון… avribloch בהולנד מתכנסים לקראת סגר שני ומטילים הגבלות לאור העלייה בתחלואה במדינה הכל בגלל נתניהו נכשל בניהול הקורונה  rothmar וזה ממשיך  האירוניה הוסיפה ארבע קומות לא חוקיותפרגולה לבית שלה פיצלה לעשרים דירות עלתה למעלה וקפצה אל מותה  rothmar ואז ליאת בן ארי טענה שמדובר באכיפה בררנית  וזהו דוקטור יותר אני לא זוכר כלום  ושאני פרסמתי את הכתובות שלהם קיבלתי צו הטרדה מאיימת מ״שופטת״ כנגד אנשים שקראו לרצוח אותי דרך אגב  MidaWebsite בזמן שמנדלבליט כובל את ידי הממשלה אך לעולם לא יתן על כך דין וחשבון עוד zeevlev מזכיר לשרים היועץ הוא רק יועץ gtgt  גמר חתימה טובה LiberalRiWo עכשיו כשיודעים שהישראלים לא מתחברים לחקירות האפידיומולוגיות מה עם איזו סליחה של מערכת המשפט ותנועות השמאל על הפסקת האיכונ… YuvalKarni רק מזכיר  mohsaud08 Lol thank you Mohammad  George Orwell described the leftwing agenda perfectly in his book Animal Farm  All animals are equal but some ani…  ronisassover לא מכיר מעריצים של אבא שלי מכת המטורללים האמרכיסטים של פרעות השמאל  yanircozin ו5 מתוך 9 חברי הוועדה הם שופטים או חברי הגילדה של לשכת עורכי הדין אשר מתואמים בינהם  וגם הוועדה הזאת…  yanircozin לא ממש לא ההשוואה היא שראש ממשלת ישראל יבחר איזה שופט עליון שבא לו לפי האג׳נדב שבשמה בחרו בו אזרחי ישר…  rothmar שופט בית המשפט העליון יוסף אלרון ביקורת חריפה על שרגא ותנועתו קובע שהתנועה לאיכות השלטון פעלה בחוסר נקיון כפיים חמור בהפגנה… avigrin10 בדמוקרטיה הגדולה בעולם הנשיא הנבחר ממנה שופט עליון מינוי שלישי שלו על בסיס פוליטי מובהק  כדי להעמיק את הרוב השמרני בבית… 2346479Orna יועמ״ש מפלגת העבודה לשעבר עו״ד דני כהן למתי טוכפלד בגלי ישראל אהוד ברק נמצא במסע נקמה נגד נתניהו הוא אדם ציני ומשתמש בש… CarolineGlick Now that its game on for Republicans with AmyConeyBarrettSCOTUS its important to understand whats at stake Israel… giladzw מחקרים בארהב מלמדים שאין הדבקות קורונה בהפגנות לא נכון  להלן מחקר מאוגוסט שמצא קשר ישיר בין הפגנותהתפרעויות להדבקות  המחקר… spiderchen ולעומת זאת יש מדינות פדרליות עם משטר פרלמנטרי כמו גרמניה spiderchen אין שום קשר בין היותה של ארהב מדינה פדרלית להיות מדינה עם משטר נשיאותי בצרפת יש ממשטר נשיאותי והיא לא פדרלית gtgt והדרך היחידה להדיח אותו מתפקידו היא עוד רוב של מעל 23 גם בבית הנבחרים וגם בסנאט ע״י נבחרי העם ולא ע״י פקיד וחצי במשרד המשפטים ולכל הטרולים השמאלנים שכותבים ״באמריקה יש הגבלת 2 קדנציות לנשיא״ אכן אך זה בא לצד משטר נשיאותי אני ממש בעד שינוי…  ptrdvd קוני מזכירה את מורה ורבה הש המנוח סקאלייה ומציינת ששופטים אינם מתווי מדיניות כי אם מיישמי החוק דבריה של איימי קוני ברט הם כמ… איזו מדינה מוזרה ארה״ב שם העם בוחר את הנשיא והנשיא בוחר את שופטי בית המשפט העליון אשר עוברים שימוע ע״י נבחרי העם…  ronisassover וראית את מי הוא מעריץ netanelgla נראה שלמברגר שועט בחקירת המימד החמישי ותראו איזה יופי יש חקירות  שאין בהן הדלפות יש מישהו שעוד לא ברור לו שכחול לבן והחו… LiberalRiWo גם על בגין הם כתבו שהוא זרע פירוד ושנאה  taliaeinhorn רפורמהתקנותסדרהדין 14 בהמשך לעצה הטובה שקיבלתי מעמיתי המלומד מאוד עוד chaimindig שאציג בפניכם מידי יום תקנה מתק… rothmar עוד שש דקות טראמפ מכריז על המועמדת לבית המשפט העליון בארהב  מדהים איך האמריקאים האלה לא מבינים כלום בדמוקרטיה מהותית ולא יו… Arieliluz לא ייאמן צפו עד הסוף תראו בן אדם דיי מבוגר שעושה לייב פייסבוק ופשוט נותן בוקס לשוטר עם מעיל אופנוענים הילוך איטי בסוף… KastelMoti דקה לפני יוכ כך נראתה אמש הפגנת השמאל בבלפור בהמשך אעלה תיעודים עם קריאות גנאי קשות זריקת חפצים ואלימות פיזית כלפי שוטר… ptrdvd הצצה לדמוקרטיה המועמדת לכהונה בערכאה החוקתית זו שיכולה בשם החוקה לפסול חקיקה מוצגת על ידי ראש הרשות המבצעת לאישור בית הנבחר… netanelgla הם לא רוצים שחיילים יוכלו להגן על עצמם מפני מחבלים הם לא רוצים ששוטרים יוכלו להגן על עצמם מפני מתפרעים הם רוצים אנרכיה ה… ronisassover  התמונה שתהיה המסמר האחרון בארון הקבורה הפוליטי של מחנה השמאל למעלה  רחבת הכותל הריקה בערב שלפני יום כיפור למטה…  netanelgla אשכרה מנדבליט בגלל קלטת בכספת אתה מביא את המדינה לאנרכיה אשכרה בגלל קלטת בכספת אתה מחרב את הדמוקרטיה הישראלית אתה מסכן את… AviNissenkorn קפץ לך הסטאלין mohammadkabiya 3 هويات مجتمعة في شخصية واحدة لخدمة الوطن جندي في ساحة القتال، مواطن عربي إسرائيلي، وبدوي مسلم  arutz20 בזמן שאתם בסגר השתוללות עימותים ותקיפות שוטרים בבלפור gtgt   YinonMagal החלמה מהירה BoazGolan לפני זמן קצר בקיסריה  מעניין אם החמוצים בשמאל שרדפו אחרי טופז ידרשו מהמשטרה לקנוס גם את הג׳ינג׳ בגין אי עטיית מסכה  iairLevy כעת בבלפור צפיפות מטורפת תוך כדי שהמפגינים רודפים אחרי השוטרים ודוחיפים אותם  shlomokarhi זה הסיפור המרכזי של הימים האלו הכותל בערב היום הקדוש ביותר לעם ישראל מול ההפגנות המטורללות בבלפור  אין לב יהודי שלא מחס… AvishayBenHaim ערב יום הכיפורים הכותל ריק   מידי שנה בערב הזה שהוא ערב השיא של ישראל המסורתית עשרות אלפי מתפללים הערב ניתן אישור ל2… shiraaedri מה עם המימד החמישי משאירים את התיק פתוח כדי שישמש שוט נגד החליפי זה תיק שלעולם לא ייסגר ולעולם לא יבשיל רפובליקת בננות שמתם לב שהשמאלנים האחרונים שהיו עם שכל והוגנות עברו גם הם לימין ועכשיו לא נשאר שם אפילו אחד עירית לינור ד״ר גדי טאוב כנרת בראשי וכו BT909  ItsikSaban חובת צפייה  המפגינים רוצים אלימות הם רוצים להתפרע הם רוצים לשרוף את המדינה קדימה עיתונאים קדימה תעשו לזה יחסי ציבו… לא הבנתי מי הדובר הרשמי של האנרכיסטים ענבר טוויזר או משה נוסבאום giladzw 14 החשיפה של איילה חסון  לפיה המפכל דאז דודי כהן דיווח לרמטכל אשכנזי ולפצר מנדלבליט ששומרים עליהם  פותחת מחדש את הקל… זוכרים בסך הכל לפני כמה חודשים RMatsliah  פרודיה   YoavNews1 חשיפת News1  מה מסתירים בפרשת כלי השיט  דרושה חקירה ומעמד עד מדינה לאיש סודו של ליברמן שרון שלום שדרש ממיקי גנור 300 אלף ד…   hofitsh מה השורה הזאת למטה זה ציטוט של מישהו הוא גחמה של העורך  סעיף 252 לחוק העונשין קובע כעבירה פלילית איסוף כספים לשם תשלום קנס שהוטל על אחר  התרמה למען תשלום קנס א128  2…  anatnh חבורת השקרנים מרעילי המוחות מורעלי השנאה מחדל יום כיפור עאלק במשך חודשים הם יושבים באולפנים וצועקים שאסור להטיל סגר שפרופ…   זוכרים  דני קושמרו איכשהו חמק לימין מתחת לראדר למרות שאמנון אברמוביץ הוא מלאך צחור כנפיים ועיתונאי אובייקטיבי לעומתו הוא…  shelegbeleg הגשתי תלונה למשטרה היום בין היתר על הסעיף הזה הוא יצורף כנתבע לתביעת הנזיקין של השוטרים והאחרים שנדבקו וידבקו בהפגנות … NissimSofer הפרקליטות ממשיכה בהתנתקות המוחלטת שלה מהתפקידים של פרקליטות במדינה דמוקרטית וחושבת שמתפקידה עתה גם להגיב לאמירות פובליצי… Arieliluz אזרחי ישראל חייבים לדעת מה קרה בכנסת ב24 השעות האחרונות אזרחי המדינה חייבים לדעת שמשבר המשילות הוא הדבר הכי מסוכן שקיים הי… RubiYona אלי אבידר מישראל ביתנו לעשות שיירות לבלפור מי שייקנס  נעשה לו הדסטארט   סעיף 252 לחוק העונשין קובע כעבירה פלילית איסוף כס… להעמיד אותו לדין על סעיף המרדה  cshlomit מכל השנאה ההסתה ושיסוי שימו לב מי מנהיגי העתיד שלו לפיד אייזנקוט חולדאי  ובנט  jennush10 איך כחול לבן שומרים על הדמוקרטיה  מעבירים את כל הסמכויות לאדם אחד שאינו נבחר ציבור היועמש ובמקרה גם ממ פרקליט המדינה cshlomit הסתה חמורה קבלו את הפרופסור שקורא לראש הממשלה היטלר פני השמאל הנאור בושה וחרפה   מעלה את הסרטון בעקבות הודעה שקיבל… זה פשוט הזוי מככ הרבה בחינות הפכנו לרפובליקת בננות מרכז אמריקנית של שנות ה70  mosheifargan תגידו לי רק באיזו רפובליקת בורקס דובר משרד המשפטים כותב דבר כזה בפומבי והוא נותר בתפקידו איזה כשל מערכתי צריך לקרות כדי… ramikeren הציבור משלם שכר למנדלבליט ולחברי כחול לבן והם בתמורה מקריבים את הציבור לגחמותיהם הפליליות והפוליטיות  לא נתפס מביאים לא… BarakRavid הסתה נגד שומר סף מפקפק בפקידים המקצועיים תהליכים של שנות ה30 shlomokarhi והעובדות הן הגשנו 4 הסתייגויות מהותיות מתוך כמה אלפים שהוגשו  בלי ההסתייגויות האלו החוק הופך את המצב לגרוע יותר  מי ש… haggaisegal האם yehuday30 שוחח עם מנדלביט על תיקי משפט  נתניהו  צפו ושתפו את התוכנית השבועית  avribloch לא תשמעו קצין משטרה שאומר למפגין בבלפור מבחינתנו זוהי הפגנה מפוברקת כרגע אתה ואשתך מקבלים דוח על יציאה ללא צורך חיוני מע… dovikco מהדורות חדשות שהביאו את יורם לס שאמר שזאת ״רק שפעת״ ואת עידית מטות שסיפרה לנו שבכלל אין גל שני ואת אירה דולפין כדי לקדם אנר… nfsgalibh רק בשמאל אפשר להסית כנגד ראש ממשלה עי האשמתו בהסתה ולקרוא לאנרכיה ולהתגודדות שמסכנת את כולנו בעת מלחמה במגפה תוך האשמתו בח… RonenRt דרך אגב בתור המפעיל של בובה גנץ יש לך תעוזה לרמוז על קופות שרצים ודי לחכימא ברמיזא Onetruth011 להזכיר לכם שקצת אחרי התחקיר הזה בר סימן טוב התפטר לא כולם כמו נתניהו עשוים מברזלהיום ידיעות שואלים איפה הואהתקשורת בישר… IlanTsion תת הרמה של התקשורת הישראלית מגולמת כולה בפוסט למטה   לטענת כאן 11 בארגנטינה סגר ממושך מאד לא מצליח אבל מחמיאים להם על כך… YaaraZered לקלמן מפריע שאנשי תקשורת היו בפעילות בליכוד וחזרו לתקשורת הוא כנראה שכח שהיה פעיל פוליטי והוצב ברשימת התחיה לכנסת בשנת 92… RonenRt אה גם אני רוצה לסבר את אוזניך במדינה דמוקרטית יש חוק ראש ממשלה נבחר ע״י מליון וחצי איש ההתייחסות היחידה…  RonenRt פחחחחח אתה מאיים עלי נראה לי יש סעיף על זה בחוק העונשין ואתה מפחיד אותי באותה רמה של החתולה שעברה הרגע לידי AvishayBenHaim המאבק להפלה אלימה לגלית של נתניהו הוא מאבק של ישראל ה1 נגד הבחירה הדמוקרטית של ישראל ה2 ראו הנתונים  על האליטה הצ… arisade94 פאק ההפגנות שלך יא בן אדם חליפי במה אתה מתעסק אנשים מתים הכלכלה קורסת ואתה והמפלגה המקושקשת שלך ממשיכים להתעסק בנושא ש… BoazGolan חב׳ פייסבוק שלחה לצל  יואב אליאסי התראה לפני סגירת הדף ההודעה בעקבות פוסט שהעלה על שמאלנית ברחוב עם שלט גועלי על יאיר נתנ… shiraaedri לישראל היה עשור עם הישגים רבים 20092020 כולל במלחמה נגד הקורונה עד שהבולשביקים הצטרפו לשלטון ב17 במאי 2020  זה דפוס קב…  elchananz תמו הריסות בתי מחבלים  בקיצור מזוז פוגלמן וברון ניצחו למרות שיש רוב בבגץ נגד עמדתם  היועמשים החליטו לאמץ את עמדת השופט… omeraricha מאחורי ריב קלמןריקלין עומד משהו נוסף לדעתי שעמית סגל הצביע עליו בשבוע שעבר בגלובס רוב עיתונאי הימין מזוהים עם ימינהבית… HSajwanization Hamas is a terrorist organization YaaraZered ראיתי הבוקר שלקלמן ליבסקינד מפריע שהייתי בפעילות בליכוד וחזרתי לתקשורת תגידו שמעתם את קלמן אומר את זה פעם על הנדל יחימוב… DdongISR למה אתם חסום mosheifargan אני לא יודע למה התכוון מי שניסח את זה אבל מה שאני לומד מכאן זה שארגנטינה נחרבת גם בגלל הפגנות חוזר על למה לכל הרוחות… BarashiKinneret היי שלי מצאתי ראיות לתלונה שהגשת נגד יור ההסתדרות בעבר ויור המפגינים בהווה  אסי ניסנקורן  אעזור לך לחדש את החקירה… RonenRt חחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחחח אמר מפעיל המריונטה של גנץ 🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣🤣 YinonMagal מתוך הספר המתריע של עמוס גלעד אחד היועצים היותר נחשבים מתברר שלא תמיד היועצים צודקים לפחות לא בעידן נתניהו  shiraaedri אם זה היה הפוך המהדורות הערב היו נפתחות עם הודעה דרמטית על אלימות קשה שמפעיל הימין הקיצוני ממלא מקום מפכל המשטרה היה מוצ… AronRabino1  yaronavraham N12News אתם בדיחה  ivgiz  sbyifat אכן הזמן לסלוח לחכית אנונימית שנכנסה לכנסת רק בזכות נתניהו הוא כבר לא היה מחוייב להכניס אותה לרשימה ההסכ…  BarakRavid אותו אחד שכתב באל ג׳זירה 1213 את השאלות לגנץ כל ה3 מערכות בחירות ivgiz  ivgiz ואני אזרח במדינה דמוקרטית שמותר לו לבקר את הביקורת שלך ivgiz תלמד לקבל ביקורת יפה  פותח לוע על אבא ואמא שלי 🤣🤣🤣 אולי בכלל אתה דווקא צריך דרגת אביעד גליקמן למודעות עצמית ivgiz בלאט עכשיו שודרגת בערוץ לדרגת ענבר טוויזי תמשיך ככה אולי אפילו תזכה לדרגת גיא פלג יום אחד ivgiz  בונוס מאבי ניר בדרך ArielKallner התפקיד האמיתי של gantzbe בכחולבן הוא יור המפלגה החליפי היור בפועל הוא AviNissenkorn ניסנקורן מושך בחוטים והבובה גנץ… gtgt לו לעשות אותו דבר לא חשוב אם אתם כבר חברי ליכוד או לא תיכנסו לקישור מלאו את הטופס הצטרפו לקבוצות הווצאפ וכש…  gtgt השיטה שלהם פשוטה הם פוקדים כמה שיותר ישראלים לליכוד ובאמצעותם מפעילים לחץ על חכים במפלגה שלא להתפרס בפני הפקי…  האקטיביזם השיפוטי מכרסם את הדמוקרטיה הישראלית שופטים ופקידים מקבלים החלטות במקום נבחרי ציבור הימין מתוסכל מהמצב ה…  AviNissenkorn תרגע הוגו צ׳אבז   arisade94 אני מצטער אבל אני לא יכול להתאפק מר בוזגלו כדמות ציבורית לא כוס התה שלי אבל אקדחי צעצוע וספריי לניקוי חלונות פתחו פה מ… מת לדעת מה יש להם על הרשקוביץ  Onetruth011 תרגום  לא נתניהו לא תכליתי  ivgiz אתה מודע לזה שאנחנו לא באמת חיים הדמוקרטיה ולכן הבוס בפועל  של המשטרה הוא הפקיד הרועץ מנדלבליט שמחזיק אותם קצר באמצעות שליטתו במחש ivgiz ברור לך שהם יחליטו שהפגנות ״תכליתיות״ הן אך ורק הפגנות שמאל אנרכיסטי פשוט טירוף במילים אחרות  ממ המפכל האח של זה של המימד החמישי אומר הפגנות שמאל ימשכו כסדרן ואפילו את ההגבלה של…  אתם מדמיינים איזה שבוע שידורים מיוחד היה באל ג׳זירה 12 אם היה הפוך  yehudaamrani חשבו שמגיפת האקטיביזם המשפטי היא בעיה של מי שמעניין אותו מנהל תקין של סעיפים וכללים חשבו שזה מציק לתזה השמרנית ומיועד לד… BoazGolan לא הפתיע אותי  אמש פניתי ליועמ״ש מנדלבליט וביקשתי לראיין אותו בתכניתי ״האולפן הפתוח״ בערוץ 20 ראיון מוקלט או בשידור חי  ב… haggaisegal האם מנדלבליט דיבר בשיחה שלו עם yehuday30 על משפט נתניהו  תיקי נתניהו  מדובר בעבירה פלילית של הדלפה…  YairGolan1  avribloch הפרקליטות חושפת בתגובה לעתירת התנועה למשילות ודמוקרטיה  מי שכתב את הודעות הדוברות לפיהן התובעת במשפט נתניהו ליאת בן ארי ל… MidaWebsite אמש הוכח סופית אצל גנץ ניסנקורן ושות ישראל היא אחרי הכל gtgt  DaphnaLiel לקח לי שנייה להבין אם זה ציוץ של ״עיתונאית אובייקטיבית״ או חיים שדמי mclbgn shimritmeir 🤣🤣🤣🤣 giladzw 15 עברתם על החוק תגידו שמאיימים על חייכם  ותיהנו מחסינות זוהי השיטה של ליאת בןארי להסתרת עבירות הבנייה שביצעה לכאורה בבית… אין מספיק 🤦‍🤦‍🤦‍🤦‍🤦‍ בעולם נתניהו הוא פוליטיקאי מותר וגם רצוי לפוליטיקאי לדבר עם עיתונאים מנלדלבי…  mclbgn אז אפשר לפחות להוריד מהשולחן את הוויכוח למה עברנו את הגל הראשון טוב יותר מכל העולם כמעט זה לא בגלל שאנחנו אוכלוסיה צעירה ל… OferShelah  LiberalRiWo ציוץ של שלח מיוני אחרי הגל הראשון  היום אגב הצפי הוא למעל 8000 מאומתים לפי שיעור המאומתים כרגע shlomopyuter היועמש מנדלבליט נבהל מהפרסום שהוא התנה הגבלת הפגנות בסגירת המשק ודאג שתפורסם מטעמו הודעה שלפיה היועמש לא קבע בשום שלב… haimmisgav חשד עוד עבירות בנייה של בן ארי  newsbuzznet ronisassover newsbuzznet המסר שהוסר מספר הקורונה שפרסם חכ נפתלי בנט כל הזמן מכניסים אותנו לתבהלה שתיכף המדינה קורסת אבל הנתונים מראים הפוך h… amitsegal  cshlomit הנה בגין שכל כך מתגעגעים אליו תקשיבו טוב מה אמר על הדגל האדום  avribloch ניסנקורן מתגאה שבכחול לבן הצליחו לטרפד את הכוונה של נתניהו להגביל את ההפגנות גם אחרי שהסגר יוקל  אתם מבינים את האדיוטיות… netanelgla הפגנות ימין בבלפור נגד רבין היו מותרות רק שעה וחצי ביום עד 500 איש אם איני טועה הפגנות שמאל בבלפור מותרות כל היום  עד 2000… dogly1900 יעקב ברדוגו בכירי ימינה פעלו לייצר עם אנשי תקשורת פגישות עם אביחי מנדלביטי כדאי לשנות את דעתם   bardugojacob YaaraZer…  RahavRan gantzbe netanyahu IsraeliPM Israelkatz GabiAshkenazi רני הכלכלה של כלללללללללל המדינות בעולם בקרשי…  BittonRosen קצין המשטרה האחראי בשטח על הפגנות השמאל הקיצוני בבלפור נמצא חיובי לקורונה לפי חדשות 13 מעניין מה מקור ההדבקה judash0 דיווח מדהים של ירון אברהם נתניהו וכץ ביקשו להשאיר חלק קטן מהמשק פתוח בעיקר במגזר הפרטי ואנשי כחול לבן מתנים את ביטול ההפגנ… RahavRan gantzbe netanyahu IsraeliPM Israelkatz GabiAshkenazi אבל אנשים לא מקפידים ואי אפשר לאכוף שאנשים יו…  RahavRan gantzbe netanyahu IsraeliPM Israelkatz GabiAshkenazi אז אתה דן לפחות 3000 אנשים למוות בחודשים הקרובים mosheifargan נעשה את זה קל לדבילים מצטער על הבוטות אין ברירה חוק לא יכול לומר נתיר ל 10 אנשים לסחור בסמים הנזק לא כל כך כבד בגל… למה השמאל ירה על הימין ועל מנחם בגין באלטלנה למרות שידע שאם הימין ירה חזרה תפתח מלחמת אזרחים וישראל תושמד ע״י צב…  YinonMagal נזכר שאלה שמפגינים עכשיו בבלפור ומכחישים הדבקות בקורונה בהתקהלויות הם אותם אלה שדיברו יותר נכון לא הפסיקו לדבר על שוד ה… זוכרים  yitzhak55 משתתף בצערך המלחמה ההזויה של מנדלבליט למען המשך ה״הפגנות״ של השמאל האנרכיסטי למרות שהוא יודע שזה יוביל לאלפי מתים מחזקת את הש…  BarashiKinneret בקיצור כחולבן רוצים שרובנו נחלה ורובנו נמות אחרת אין הסבר מניח את הדעת למה הקרקס הזה ממשיך  akibigman אגב השאלה אם איילת שקד מתווכת לעיתונאים פגישות או מסרים ממנדלבליט בנוגע לפרישה של נתניהו הרבה יותר מעניינת וקריטית מהשאלה א… f7FEPCkXfGH3sBU 1285 נפטרים  1010 נפטרים מאז נכנסה כחול לבן לממשלה כמה מפתיע ״קבינט הקורונה האזרחי״ של בנט מעודד המשך הפגנות בסגר ronisassover  netanelgla למה לעד כמו אילן שלא חשוד בכלום להדליף לעיתונאים על חומר חקירה אולי בגלל ש״שביבי אסון וצריך להוריד אותו״ העד שחומר מאוד ס… במילים אחרות מנדלבליט נתן עדות שקר לבית המשפט כמה שנות מאסר זה  elizipori המדליף הפלילי מס 1 – מנדלבליט 1 מפברואר 2016 ועד אפריל 2020 נפגש מנדלבליט 99 פעם עם אנשי תקשורת אבל לא ציין את שמם… yoyoeldad סתם בשביל ההבחנה  ביבי בממשלת מעברמנהל הכל למופת מקבל החלטות קשות ומהירות מציל את חיי אזרחי ישראל מודיע על סגר בזמן א… ronisassover כן שמענו על המערך הזה הוא ביקש לתת אותו לצהל וזה מה שעשו נתנו לצהל והיום אנחנו ב6000 חולים והמערך הצהלי קורס זוכרים  netanelgla בנט אסור לתת לצבא לנהל את זה  בנט זה חרטטן המאה הדבר המדהים שתומכיו מחזיקים ממנו כי נערי מוזס מרימים לו כמה אפשר לא להב… haggaisegal tadmorerez48 gtgt לעיתונאי לחשוף עם מי הוא נפגש לשיחות רקע haggaisegal האם אתה מבין ש״שיחות רקע״ של יועמש על תיקים שהוא מנהל הינה עבירה פלילית מצידו שדינה 3 שנות מאסר בראי…  Meshilut חבר הכנסת HaleviAmit היום בווועדת חוקה  הנה נחשף לעינינו שמערכת שלטונית השתמשה במשאבי הציבור כדי לסתום פיות של אזרחים כד… ArielKallner אנו נמצאים במדרון חלקלק להפוך מדמוקרטיה לאוליגרכיה משפטית ופקידותית בדיון בוועדת חוקה היום הצבעתי על המצב האבסורדי בו המ… mosheifargan אם נתניהו היה מכריז על תוכנית התנתקות הוא היה מחולל תהליך ריפוי פי מיליארד גדול בהיקפו מהחרפה שהציעו חברי כת קטנה שבמ… netanelgla לא מבין למה כחול לבן יושבים בדיוני הממשלה בשביל מה הם צריכים את הישיבות תיאום בינם לבין החונטה סתם בזבוז זמן ואנרכיה שימ… ramikeren בנט חייבים סגר בנט חייבים לפתוח את הסגר בנט צריכים סגר חלקי בנט לשחרר את כולם מהסגר בנט רק סגר בנט קראתם את הספר… aviadglickman  jennush10 43 נפטרים ביממה   האם הגברת sbyifat עדיין רוצה לפתוח הכל  האם היא עדיין חושבת שהתחזיות שהציגו לה הן מופרכות   בשביל 15… avribloch אלה תנאי ההפגנות מול ביתו של מנדלבליט  עכשיו תדמיינו הוראה לקיים מחאה שקטה של עד חמישה אנשים בבלפור מול ביתו של ראש הממש… Arieliluz תמצית הסיפור בישראל הימין מתריע gtgt התקשורת מכחישה gtgt השמאל דוהר לאסון gtgt 1000 ומעלה מתים gtgt הציבור מבין את גודל האסון  ה…  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">בשעת חירום לאומית זו אין מקום לפוליטיקה קטנה אף שההפגנות רק מסייעות לליכוד מבחינה פוליטית הן מסכנות את בריאות הצי…  כיוון שלא ניתן להשלים את חקיקת החוק עד יום שלישי הליכוד הציע תקנות לשעת חירום לימים ספורים כדי למנוע הפגנות המוניו…  החוק ממילא לא יכל לעבור היום בכנסת עם 4000 הסתייגויות של האופוזיציה שמתנהלת בחוסר אחריות בשעת חירום לאומית זה קורה…    הערב שמענו את יאיר לפיד פוגע באמון הציבור בזמן חירום ובכך מסכן את חייהם של אזרחי ישראל   זה אותו יאיר לפיד שאמר ש…  rothmar קחו לעצמכם כמה דקות ותקשיבו לנאום הפתיחה של HaleviAmit בכנסת   העלות הכוללת של טיסת שני המטוסים לוושינגטון היא 50 פחות מעלות הטיסה הקודמת לוושינגטון במטוס אחד   השמאל והתקשורת…  ראש הממשלה נתניהו ימריא לפגישה עם נשיא ארהב ולהסכם שלום היסטורי שיביא למדינת ישראל רווחים מדיניים וכלכליים אדירים…  השמאל והתקשורת מחפשים כל תירוץ להקטין את ההישג ההיסטורי של ראש הממשלה נתניהו ואף לסכן את בריאותו רק בגלל שהם לא מוכ…  סיעת הליכוד רק חקירה עצמאית ובלתיתלויה תגלה את האמת על תפירת התיקים נגד ראש הממשלה נתניהו ישראל צריכה מערכת אכיפ…  מדהים לגלות שמי שעומדים מאחורי הקמפיין השקרי הזה הם אותם אנשים שתמכו בעסקת הגרעין המסוכנת עם איראן ובעקירת יישובים…  בשום שלב בשיחות בין ישראל לארהב שהובילו לפריצת הדרך ההיסטורית עם איחוד האמירויות ב138 ראש הממשלה נתניהו לא נתן…  לשמאל קשה לראות איך ראש הממשלה נתניהו ריסק את תפיסת שטחים תמורת שלום והביא לראשונה ״שלום תמורת שלום״ ולכן הם מנה…  חברת הכנסת לשעבר שולי מועלם מצטרפת לליכוד   ראש הממשלה נתניהו   ״אני שמח מאוד ששולי מועלם חברת הכנסת לשעבר ו…  הפגנות השמאל הן ההפגנות ״הספונטניות״ המאורגנות ביותר אי פעם מי שעומד מאחוריהן ומממן אותן הם טייקונים מהשמאל וביניה…  שווה קריאה   גבי אשכנזי ממשיך להיות חתרן בלתי נלאה עד הרגע האחרון אשכנזי ממשיך לעשות כל מאמץ לגרור את ישראל לבחירות כדי להדיח א…  אנחנו נמצאים כ100 ימים אחרי כינון הממשלה וניסנקורן מסרב אפילו להקים את הוועדה תוך הפרה ברורה של ההסכם הקואליציוני סעיף 3ד ״מעבר ל100 ימים צוות שוויוני של הליכוד וכחול לבן יגבש בהסכמה כללים לביצוע מינויים בכירים בשירות הציבורי…  הנה הסעיפים בהסכם הקואליציוני שניסנקורן הפר ברגל גסה  סעיף 3ג  ״במשך 100 ימים כל המינויים הזמניים יוארכו״   מייד…  האם יש פה סגירת תיק תמורת מינוי ומינוי תמורת סגירת תיק מנדלבליט וניסנקורן חייבים תשובות לציבור  ומייד 1 מתי החליט מנדלבליט לסגור את התיק נגד ניסנקורן  2 מדוע הסתירו מנדלבליט וניסנקורן את קיום התיק וסגירתו בפני הציב…  עכשיו מתברר שמנדלבליט סגר תיק פלילי נגד ניסנקורן וניסנקורן לאחר מכן הדיח את מ״מ פרקליט המדינה דן אלדד שהחל לחקור נ…  האם אבי ניסנקורן גורר את המדינה לבחירות בגלל עסקה סודית עם מנדלבליט שסגר את התיק נגדו  ניסנקורן מפר את ההסכם הקו…  כל פעם שבנט לא מקבל את הגוב שדורש הוא מגלגל עיניים ותוקף את ראש הממשלה הוא כינה את תוכנית הריבונות תוכנית כליה…  כחול לבן שוב נלחמים בממשלה בזמן שראש הממשלה נתניהו נלחם בקורונה היום בועדת הכספים הם עצרו כסף חיוני לפתיחת שנת הלי…  הרבה פייק ניוז בתקשורת סביב הסכם השלום ההיסטורי  ראש הממשלה נתניהו מחוייב לריבונות ולארץ ישראל בפעם הראשונה בתולד…  dudiamsalem אתם יודעים את האמת כל אזרחי ישראל יודעים את האמת אתם לא מצליחים לנצח את נתניהו בקלפי אז אתם בשמאל מעלים חוקים אנטי דמוק… במקביל  ראש הממשלה נתניהו מכנס את קבינט הקורונה מקיים ישיבות עבודה על החזרת הכלכלה לשגרה נפגש עם אנשי תחום התרבו…  24 השעות האחרונות השמאל מפגין בבלפור עם שלטים נגד נתניהו ו״הכיבוש״ יאיר לפיד בכנסת מעלה הצעת חוק להדחת נתניהו אחר…  בתוכנית יועברו 700 מיליון שקלים בעבור הבטחת ביטחון תזונתי למשפחות מוחלשות ו600 מיליון שקלים לטובת הארכת מענקי ההסת…  ישיבת הממשלה לא תתכנס מחר בשל סירובם של כחול לבן להעלות לסדר היום תוכנית סיוע כלכלית ממשלתית של ראש הממשלה ושר האוצ…  ראש הממשלה נתניהו ימשיך לעבוד מסביב לשעון להילחם בקורונה ולחזק את כלכלת ישראל ראש הממשלה קורא לכולם להתלכד במאמץ…  לעומת זאת הם מתעלמים מהאופי האלים של ההפגנות ומהקריאות הנשמעות בהם לרצוח את ראש הממשלה ובני משפחתו   הטלוויזיה בצ…  ערוצים 12 ו13 ממשיכים לשמש זרוע תעמולה להפגנות השמאל האנרכיסיטיות   הם עושים מאמץ נואש לשטוף את המוח של הציבור ב…  שפל נוסף לאיימן עודה שהשתתף היום בכנס עם אנשי חמאס שקראו לרצוח ישראלים זה האיש שאיתו יאיר לפיד ובוגי יעלון רצו להק…  NaorIhia אבדה הבושה ועוד על חשבוננו yoavgallant במקום להעביר ביקורת מוטב ששר המשפטים יפעל לחשיפת הקלטות מנדלבליטאשכנזי והתנהלותם בפרשת הרפז פתאום כשפעיל שמאל נעצר כשהוא מפר את החוק וחוסם כביש בהפגנת שמאל שמאורגנת על ידי אהוד ברק חברו ושותפו של הפדופיל המ…  התקשורת לא אמרה דבר על מעצרה המזעזע של פעילת הימין שפי פז או על מעצרם של פעילי ימין רבים אחרים בהפגנות ימין  יאיר לפיד צריך להסביר לציבור איך דחף למנות את מאיר כהן ליו״ר הכנסת למרות שידע על עברו המפוקפק לפיד וכהן צריכים להס…  הביקורת הטוקבקיסטית של בנט מהיציע לא תמנע מראש הממשלה נתניהו להמשיך לפעול במלוא המרץ כדי להחזיר את מקומות העבודה ל…  בניגוד מוחלט לרצון בוחריהם בנט ומפלגתו סירבו להמליץ לנשיא על נתניהו לראשות הממשלה זרקו 6 מנדטים של הימין לאופוזיצ…  האובססיה של בנט לקחת קרדיט על דברים שלא עשה לא יודעת גבול ״תרומתו״ של בנט לביטחון הייתה בכך שלא הפריע למדיניות התק…  AmirOhana עדכון חשוב  כוחות המשטרה פתחו במבצע אכיפה מקיף בביר הדאג  14 חשודים נעצרו 3 כלי רכב נתפסו ציוד וכסף מזומן הוחרמו   ישר… מצער שבג״צ התערב ופסל חוק חשוב להתיישבות ולעתידה נפעל כדי לחוקק את החוק מחדש TopazLuk שקר  רמדאן שלח נקבר בבית הקברות אלשהדאא במחנה הפליטים אלירמוכ בדמשק שבסוריה   להבא ממליץ לבדוק dudiamsalem מי אתה מר סגלוביץ שתתקוף את ראש ממשלת ישראל ותקרא לו מושחת טול קורה מבין עיניך אם אתה רוצה לדבר על שחיתות תסתכל במראה… בדמוקרטיה האזרחים מצביעים בקלפי ובוחרים את ראש הממשלה מי שרוצה להחליף את ראש הממשלה יכול בוודאי להתמודד בבחירות ולתת לאזרחים להחליט בעצמם אזרחי ישראל בחרו בראש הממשלה נתניהו ברוב עצום כשהליכוד קיבלה את מספר הקולות הגדול ביותר שקיבלה מפלגה בתולדות המדינ…  המעון של ראש הממשלה החליפי לא עלה במו״מ כדרישה מצד הליכוד וראש הממשלה נתניהו בזמן שראש הממשלה נתניהו יחיל ריבונות על יהודה ושומרון כפי שמופיע ומתחייב בהסכמים הקואליציוניים בנט יבלה באופוזיצי…  בנט זרק את כל מפלגתו לאופוזיציה רק כי לא קיבל את תיק הבריאות הוא יודע שזאת האמת ולכן הוא מזיע ומשקר מי שפרש מגוש…  בבחירות מועד א׳ בנט לא עבר את אחוז החסימה ובזבז קולות לימין בבחירות מועד ג׳  רק בגלל כיסאולוגיה  בנט העדיף לזרוק…  אם בנט היה מקבל את תיק הבריאות הוא היה אומר שזו ממשלת החלומות של הימין בגלל שלא קיבל הוא החליט לגרור את ימינה לאופ…  חבל  לצערנו בנט דחה את ההצעה בשל המאבק הפנימי בתוך ימינה על חלוקת התיקים ומכיוון שמה שחשוב לו זו כיסאולוגיה ולא אידיאולוגיה ראש הממשלה נתניהו עשה כעת ניסיון אחרון להכניס את ימינה לממשלה לפני הנחת ההסכמים הקואליציוניים הלילה  ראש הממשלה ה…  shlomokarhi סיפורו של טיוח פחד והתעלמות  מנדלבליטampאלדד  מדוע המבקר לא מגן על אלדד כחושף שחיתויות ואיך ייתכן שמנדלבליט הנמצא בניגוד…  בעוד שרוב עצום של אזרחי ישראל ומנהיגי העולם מכירים בהצלחה של מדינת ישראל בהובלת נתניהו בטיפול במשבר הקורונה בוגי י…  החוצפה של אליעד שרגא לכנות ״יצור״ את ראש הממשלה נתניהו שהציל את חייהם של אלפי ישראלים רק עכשיו במשבר הקורונה היא עו…  סיכמנו לכם את הדיון בדקה  ההפגנות הביריוניות של השמאל הקיצוני בחולצות שחורות ובקריאות קרב מזכירות הפגנות פאשיסטיות לכל דבר  במקום לגלות אחריות ולהיכנס לממשלת חירום לאומית שפועלת להצלת חייהם ופרנסתם של אזרחי ישראל יאיר לפיד העדיף להישאר בא…  בשעה זו נחתם הסכם להקמת ממשלת חירום לאומית בין ראש הממשלה בנימין נתניהו לבין יו״ר כחול לבן ראל במיל ח״כ בני גנץ תנועת הליכוד שבה ומבקשת מהנשיא ריבלין להעביר את המנדט לראש הממשלה נתניהו ראש המפלגה הגדולה בכנסת ועם 59 ממליצים ב…  ברגע שכחול לבן תחזור להסכמות המקוריות ניתן יהיה להשלים את ההסכם ולהקים ממשלת אחדות  ספינים תקשורתיים כוזבים של כחו…  מהרגע הראשון הוסכם כי ממשלת האחדות השיוויונית תקום על שני קווי יסוד ברורים קבלת החלטות משותפת בכל הנושאים וקידום ה…  יונתן בן ארצי מסית למותו של ראש הממשלה גם כשראש הממשלה מציל את חייהם של אזרחי ישראל אין גבול לשנאה אתם חושבים שמי…  NaorIhia לא הבנתי לפני שבועיים באת בטענות שאומרים לאזרחים לא לצאת מהבית עכשיו אתה בא בטענות שאנחנו בפיגור מודה שאני קצת מבולבל ראש הממשלה בנימין נתניהו שוחח בטלפון עם כל ראשי המחנה הלאומי והבהיר להם ששימור המחנה הלאומי חשוב יותר מתמיד במהלך ה…  השותף של כחול לבן מהלל מחבלים  מצדיעים לך יולי   יושב ראש הכנסת בא תמיד מהמחנה של ראש הממשלה אם כחול לבן רוצים להחליף את יושב ראש הכנסת שיקימו ממשלה וימנו את היבא…  מי שמחפש קרקס בימי הקורונה מוזמן לראות איך ליברמן מקפץ מצד לצד בפקודות מלמעלה  netanyahu  לאור התנהלותם המבישה הליכוד והמחנה הלאומי החליטו להחרים את דיוני המליאה ושלא לקחת חלק בהליך בזוי זה עם זאת ומתוך…  לא יעלה על הדעת שברגעים מכריעים וקריטיים למדינת ישראל במקום להיכנס מתחת לאלונקה בוחרים כחול לבן בהתנהלות דיקטטורית…  מדינת ישראל והעולם כולו נמצאים במשבר הבריאותי המורכב ביותר שידעה האנושות במאה השנים האחרונות בזמן שראש הממשלה עסוק…  כחול לבן רומסים את הדמוקרטיה על חודו של קול באמצעות הרשימה המשותפת וביניהם תומכת הטרור היבא יזבק   במשך כל שנות ק…  arielikobi גם הבוקר ראוי להזכיר יש גוש שזכה ברוב בבחירות אבל אין לו שום דרך להקים ממשלה כי הוא לא רוב בעצם על כן הוא מנסה לבצע ת… צעדים אלה יביאו לזעם ציבורי עצום ולריסוק הדמוקרטיה הישראלית דווקא בעת שאנו חייבים להתאחד למען הצלת חייהם של אזרחי…  חוקי איראן אלה ימנעו מראש הממשלה נתניהו לכהן כראש הממשלה ולהתמודד בבחירות ישירות לראשות הממשלה שלפיד מתכנן לקיים כ…  ראש הממשלה לא יוכל לעשות זאת מול יו״ר כנסת לעומתי יאיר לפיד יודע זאת הסיבה האמיתית שהוא מתעקש על הדחת יו״ר הכנסת…  לאחר מכן בתקופת כהונתו של בני גנץ כראש ממשלה התפקידים יתחלפו   הסכם הגיוני זה נקבע כדי לאפשר לראש הממשלה המכהן ל…  הצעת האחדות המוסכמת עם ״כחול לבן״ קובעת שראש הממשלה נתניהו יכהן שנה וחצי ולאחריו יכהן בני גנץ לתקופה זהה   בזמן שר…  הדחת יושב ראש הכנסת תחסל את ממשלת האחדות ותביא בהכרח לבחירות רביעיות   זה יהיה צעד של חוסר אחריות מזעזע בזמן מגיפת…  זו לא העת לפוליטיקה העם מצפה שנגלה אחריות ומנהיגות נתאחד כולנו ונקים מייד ממשלת חירום לאומית רגע לפני כניסת השבת אנו מחזקים את כל אזרחי ישראל ובראשם את הצוותים הרפואיים וכוחות החירום שפועלים יום ולילה במלחמה…  assafgibor הדובר רמי מנסור בלד  הדיוןמי גרם לבלד להמליץ על גנץ  1 הרשפ רוצה להפיל את נתניהו  2 ועדת האינטראקציה ניסתה להשפי… rothmar אגב הויכוח על גודל הוועדה המסדרת ועל היתרון המספרי של הגוש הוא ההוכחה הכי ברורה שכחול לבן יודעים שאין לגנץ ממשלה  אם המספר ה… חרפה  arutz20 ללא בושה חכ טיבי סימן תנועת ניצחון להורים השכולים מחוץ לבית הנשיא  צפו בתיעוד gtgt  NaorIhia רמטכ״ל לשעבר דורש משני ח״כים להתפטר במידה ולא יסכימו לשבת בקואליציה עם תומכי טרור  סה״כ הגיוני מבדיקה ראשונית עולים פערים וסטיות חריגות בהליך הספירה לא ייתכן שלא תינתן האפשרות לבדוק בזמן סביר האם הייתה פגיעה בטוהר הבחירות הליכוד רואה בחומרה רבה את הצבת האולטימטום של יועמ״ש ועדת הבחירות לכנסת להגשת פערים ובעיות בהליך ספירת הקולות עד הער…  elirazsade מחר לא לוותר לצעירים כולם בקלפי מחל מחל מחל מחל פתק ועוד פתק אף אחד לא הכריח את יועצו הבכיר של גנץ לחשוף את האמת ש״גנץ מפחד לתקוף באיראן ומהווה סכנה לעם ישראל״ כל הקשקושים מסב…  NirBarkat רשמו לפניכם מחירי המזון יירדו משמעותית  כדי שנוכל להוביל כלכלה חופשית ופתוחה שתאפשר לחקלאים ולכל אחד לשגשג ולצמוח אנחנו צ… גנץ חי בסרט אין לו איך להקים ממשלה   gantzbe איזה מומנטום אין לך איך להרכיב ממשלה gantzbe א אתה משקר ב אתה כבר מכרת את המדינה לתומכי טרור ותעשה זאת שוב אם לא נעצור אותך מחר בקלפי  גנץ מקשקש ימצאו חיסון לקורונה לפני שהוא ימצא דרך להקים ממשלה בלי אחמד טיבי אנחנו מנדט מניצחון שימנע בחירות רביעיו…  מצפים מבן גביר לגלות אחריות ולא לשרוף קולות ולפגוע בניצחון הימין עוד מנדט אחד לליכוד ואנחנו מנצחים ומקימים ממשלת י…  שני מנדטים מפרידים בין ממשלת שמאל מסוכנת של גנץמרצ וליברמן שתלויה באחמד טיבי לבין ממשלה לאומית חזקה צאו להצביע ל…  הצבעה לגנץ או לליברמן היא הצבעה לממשלה מסוכנת לביטחון ישראל שתהיה תלויה באחמד טיבי ובמשותפת רק הצבעה לליכוד בראשות…  רעידת אדמה עמיר פרץ מאשר בקולו ״סיכמתי עם גנץ על הקמת ממשלת מיעוט של כחול לבן גשר ומרצ בתמיכה מבחוץ של ליברמן והרשימה המשותפת״ אמרנו לכם  LikudParty Kachollavan19 אנחנו רואים בסקרים שבכל יום אתם מאבדים מנדט כי גם הבוחרים שלכם יודעים שיש יותר סיכוי שבני גנץ ישרוד ראיון א… Kachollavan19 אנחנו רואים בסקרים שבכל יום אתם מאבדים מנדט כי גם הבוחרים שלכם יודעים שיש יותר סיכוי שבני גנץ ישרוד…  HauserTov yairorvieto אתה לא באוסטרליה ולא לא הועברה שום הקלטה אם ההקלטה של יועצו של גנץ מבושלת ושקרית כדברי גנץ למה גנץ פיטר אותו 🤨 ראו הוזהרתם  ayeletsl יאיר גולן מזהה התהליכים נוהג באלימות כלפי אילוז שלנו חכו שתראו איך אמילי מואטי התנהגה ליגאל מלכה הם מ פ ח ד י ם  igal… יועצו הבכיר של גנץ בהקלטה ״לגנץ אין אומץ לתקוף באיראן הוא סכנה לביטחון ישראל״   גם האנשים הקרובים ביותר לגנץ יוד…  המנוח ואני  כחול לבן בפאניקה הדבר היחיד שצולל היום זה המנדטים של כחול לבן כי גם המצביעים שלהם יודעים שגנץ לא יכול להקים ממשלה…  Israelcohen911 אסור לימין לבזבז קולות רבני חב״ד בקריאה מפורשת נגד עוצמה יהודית ומגלים דעתו של הרבי מלובביץ׳ ״לא להתפתות להצביע עבור… גנץ נראה מאוד לא רגוע הערב אנחנו קוראים לו להירגע לשתות כוס מים ולהגיע לעימות לא להתבכיין ולא להשתולל פוליטיקה…  i24NEWSEN Prime Minister Netanyahu had done more for the Arab citizens in Israel than anyone else — definitely more than the Arab pa… GabiashkenaziMK אם תמשיך לשקר נאלץ לפרסם את הניסיונות שלך להצטרף לליכוד ואת הסירובים שקיבלת בגלל הדברים הנוראיים ש…  AmirOhana יש פה אמירה חמורה מאוד הנובעת מחוסר הבנת יסודות הדמוקרטיה במקום איזונים ובלמים ההכרעות החשובות ביותר תתקבלנה על ידי המערכת… כשההקלטות של גבי אשכנזי ייחשפו הוא יפרוש מהפוליטיקה הוא לא יוכל לכהן ולו יום אחד גנץ לא מסוגל להיות ראש ממשלת ישראל רק חלק קטן נחשף פרטים בהמשך GolanOfer משנכנס אדר מרבין בשמחה  ההבטחה של גנץ למנות את גבי אשכנזי לשהב״ט ריקה מתוכן כל מי ששמע את הקלטות אשכנזימנדלבליט יודע שהוא לא יוכל לכהן כש…  גנץ לא יטיף לנו מוסר  KnessetT ראש הממשלה netanyahu בריאיון מיוחד בתוכנית ברדוגו ויניר מתחייב בנוגע לחוק הצרפתי אני לא מתכוון לחוקק שום חוק  bardugoj… משמעות הסקר הערב בחדשות 12 אם בן גביר פורש יש 61 וממשלת ימין  GolanOfer gantzbe  GLZRadio בדיוק ב1620  רהמ netanyahu מודיע נבחן את ייבוא המודל הקנדי להסדרת קנאביס לישראל yanircozin  רוב יהודי לגנץ אין ממשלה בלי תמיכה של הרשימה המשותפת ממשלה כזאת היא סכנה אדירה לביטחון ישראל  גנץ לא יכול לנהל מדינה  לגנץ היה ניסיון אחד באזרחות עמד בראש חברת ״המימד החמישי״ לחברה היה מוצר אחד החברה פשטה את הרגל ונפתחה נגדה חקירה…  בשעות האחרונות כחול לבן מפיצים פייק ניוז הקורא לתומכי הליכוד להסיר את אפליקציית ״אלקטור״ אל תסירו את האפליקציה המ…  yoavgallant אני יודע היטב מה היה לפני עשור במה שמכונה בטעות פרשת הרפז אך צריך להיקרא פרשת אשכנזי לאחר שיוסר צו איסור הפרסום תהיה רעיד… GadiTaub1 איפה פרופ מרדכי קרמניצר שדרש בתוקף שיפורסמו החשדות נגד נתניהו לפני הבחירות כדי שנצביע באופן מושכל ולמה הוא לא דורש שנדע א… yossidavidov10 22  yossidavidov10 למה הפעם החלטתי להצביע אחרת 12  netanyahu אני צריך את העזרה שלכם כדי שננצח בבחירות סמסו עכשיו מחל למספר 0529996226 בן גביר אף פעם לא עבר וגם לא יעבור את אחוז החסימה אסור לבזבז עליו אפילו קול אחד ממשלה שתלויה ברשימה המשותפת תהיה סכנה לביטחון ישראל   רק ליכוד גדול יקים ממשלת ימין חזקה ישמור על ישראל ויבטיח של…  הבחירה בידיים שלכם כלכלה חופשית של ברקת והליכוד או כלכלת הסתדרות של גנץ וניסנקורן  לגנץ אין שום אפשרות להקים ממשלה בלי התמיכה או ההימנעות בכנסת של אחמד טיבי והרשימה המשותפת ממשלה שתלויה ברשימה המשו…  NirBarkat ב23 בוחרים נכון  תבחרו  netanyahu שידור חי  חושפים את תוכנית ברקת להורדת יוקר המחיהgtgt  זוכרים זה כבר כמעט קרה זה יקרה אם מצביעי הליכוד לא יצאו להצביע  netanyahu ליכודניקים זה תלוי רק בכם הפעם אתם חייבים לצאת להצביע  הסיכום שהושג בין הליכוד וצומת נועד לתת מענה לסוגיות החשובות של ההתיישבות הכפרית בכלל והמושבים בפרט מדובר בצעד חשוב…  מפלגת צומת הסירה את מועמדותה לכנסת ותתמוך במפלגת הליכוד  ראש הממשלה נתניהו נפגש הבוקר יחד עם שר הכלכלה והתעשייה אל…  עשו טובה אל תגלו לגנץ שהבחירות ב2 במרץ  איימן עודה צודק  על פי התוכנית הממשלה תעלה את כל מי שזכאי לעלות לישראל כ7500 יהודים יועלו מאתיופיה עד סוף שנת 2020 העלאת כל שארית יהודי אתיופיה תיכנס לתוכנית 100 הימים של ממשלת הליכוד  הליכוד מתחייב להעלאת שארית יהודי אתיופיה בת…  Michael50616567 מה גרם לדר GadiTaub1 הנפלא  להתפכח מאשליות השמאל ולמי הוא הולך להצביע הפעם  לא  Slonim91 אחחח איפה הימים של פעם שהיו פה עיתונאים  netanyahu אני מציג הערב שש רפורמות ענקיות בכלכלה ובבריאות שהממשלה הבאה של הליכוד תביא לישראל ולהודיע שניר ברקת יהיה שר האוצר הבא של המ… netanyahu  היום בראש העין ואור יהודה  בואו  בני גנץ מטעה בלי תמיכה בכנסת של אחמד טיבי ו״המשותפת״  אין לגנץ ממשלה  יש לו מקסימום 53 מנדטים 36 גנץ  10 מרצפ…   LiberalRiWo מספר נפגעי הטרור בתקופת נתניהו הוא הנמוך בתולדות ישראל  LiberalRiWo ראיון חובה עם מנכל איכילוב רוני גמזו  על המספר 5000 ומאיפה צץ ועל ליצמן כשר בריאות הכי טוב שהיה כאן  מומלץ מאוד … חשבון פשוט לגנץ אין ממשלה בלי אחמד טיבי רטווטו  gantzbe גם אתה יודע שאין לך איך להקים ממשלה בלעדיה  לגנץ אין ממשלה בלי הרשימה המשותפת אחרי ההחלטה היום מי שרוצה את היבא יזבק באופוזיציה ולא בממשלה  חייב להצביע רק לליכוד לגנץ אין דרך לגנץ אין ניסיון  לגנץ אין ממשלה בלי טיבי  בלי אחמד טיבי אין לגנץ ממשלה  arielschnabel משהו ברצינות לגבי מערכת הבריאות ברור שיש גם בה כמו בכל מערכת בעיות ואתגרים אבל כשהדירוג העולמי של בלומברג ל2019 מצ… Arieliluz יועז הנדל הסרטון הזה מוקדש לך לצפות עד הסוף  יועז הנדל הוא גרבוז של 2020 הוא מתייחס למצביעי הליכוד כ״מנטליות של דרבוקות״ זה היחס שלו לאנשים שחזרו הביתה לארץ…  לגנץ אין עמדה  לגנץ אין תשובה  לגנץ אין ממשלה בלי המשותפת  בושה לפי יאיר גולן שותפו הטבעי של גנץ לממשלה הימין אחראי לטרור נגד חיילי צה״ל ואזרחי ישראל כל אחד מבין שגולן וג…  אנו קוראים לבני גנץ להבהיר לחברו ויועצו הקרוב אהוד אולמרט שזה לא הזמן להיפגש עם אבו מאזן כדי לפעול נגד ״תוכנית המ…  GYevarkan אני מברך את חברי השר אמיר אוחנה על קידום המהלך להקמת ועדת חקירה ממשלתית לבדיקת מח״ש בתקופתי במפלגת כחול לבן ניסיתי לקדם חק… Onetruth011 אממ לא נגענו ודש מכונס הנכסים  כחול לבן  קומסי קומסה  סכנה לישראל  הטרמפיסט גנץ מנסה לתפוס טרמפ על ההישגים האדירים שראש הממשלה נתניהו הביא לאחר שלוש שנות עבודה מאומצת מול ממשל טראמפ בדיחה בלי הרשימה המשותפת אין לגנץ ממשלה  bogieyaalon ד״ש מגרמן  tadmorerez48 כל המהות של כחוללבן בציוץ מדהים אחד לעזאזל המדינה האינטרסים הלאומיים והחשיבות האסטרטגית של בקעת הירדן למי איכפת משעת… בדיחה  כפי שאורלי לוי מצאה את עצמה באותה מפלגה עם תמר זנדברג ממרצ וכפי שברשימה המשותפת חברו קומוניסטים ואיסלאמיסטים לרשימ…  השמאל התאחד  הם לא הולכים לאבד אף קול עכשיו הימין חייב לעשות הכל כדי למנוע בזבוז קולות   לצערנו בנט בזבז קולות ב…  לכחול לבן אין שום הישג להציג לאזרחי ישראל אז הם ממשיכים לעסוק רק בדבר אחד ״רק לא ביבי״ הם ימשיכו לעסוק בשטויות ו…  מילה זו מילה  EliadAmar אמא כתבה פוסט שהזמין את השר אלקין למשחק שחמט מול אבא בזמן הנישוב כי אבא בן 80 עם מחולל חמצן ולא יכול להתפנות ואם אין סכנה… אמממ דווקא כן פוליטיקה    netanyahu ניצחון ענק תודה לחברות וחברי הליכוד על האמון התמיכה והאהבה בעזרת השם ובעזרתכם אני אוביל את הליכוד לניצחון גדול בבחירות ה… yairlapid יאיר בהצלחה בפריימריז ביש עתיד  nadavabeksis זוג חדש בביצה  הפנים של עקיבא נוביק אומרות הכל  לצערנו יאיר לפיד טירפד ממשלת אחדות מהרגע הראשון  כדי למנוע בחירות מיותרות ולהקים ממשלת אחדות ראש הממשלה נתניהו הציע לעגן בחקיקה יצירתית את הסדר הרוטציה שמונע מכל…  מצער שבני גנץ לא מרים את הכפפה לממשלת אחדות שתממש הזדמנויות היסטוריות למדינת ישראל  וביניהן ברית הגנה עם ארה״ב והח… </t>
   </si>
 </sst>
 </file>
@@ -501,10 +501,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="B2">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -518,10 +518,10 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="1">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="B3">
-        <v>80</v>
+        <v>142</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -535,16 +535,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1">
-        <v>51</v>
+        <v>147</v>
       </c>
       <c r="B4">
-        <v>51</v>
+        <v>147</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>23</v>
@@ -552,16 +552,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="1">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="B5">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -569,16 +569,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="B6">
-        <v>23</v>
+        <v>139</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
         <v>25</v>
@@ -586,10 +586,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="B7">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -603,16 +603,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1">
-        <v>45</v>
+        <v>133</v>
       </c>
       <c r="B8">
-        <v>45</v>
+        <v>133</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
         <v>27</v>
@@ -620,10 +620,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B9">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
@@ -637,16 +637,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="B10">
-        <v>81</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
         <v>29</v>
@@ -654,10 +654,10 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="B11">
-        <v>84</v>
+        <v>109</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
@@ -671,10 +671,10 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B12">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
@@ -688,10 +688,10 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="B13">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
         <v>15</v>
@@ -705,16 +705,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1">
-        <v>8</v>
+        <v>91</v>
       </c>
       <c r="B14">
-        <v>8</v>
+        <v>91</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
         <v>33</v>
@@ -722,16 +722,16 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="B15">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15" t="s">
         <v>34</v>
@@ -739,16 +739,16 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="1">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="B16">
-        <v>92</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" t="s">
         <v>35</v>

</xml_diff>